<commit_message>
model runs with stored results
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DC3E00-6740-4639-8879-01CD7B9834FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C36D27-DEF4-4627-BC39-E0447BA5EE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{28F97023-1D5E-44FA-A19C-A9B15763E968}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{28F97023-1D5E-44FA-A19C-A9B15763E968}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="full_model_set" sheetId="2" r:id="rId1"/>
+    <sheet name="reduced_model_set" sheetId="1" r:id="rId2"/>
+    <sheet name="no_capacity" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="99">
   <si>
     <t>id</t>
   </si>
@@ -319,6 +321,18 @@
   </si>
   <si>
     <t>101005</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>vehicle_capacity</t>
+  </si>
+  <si>
+    <t>starter_08_gmaps</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -348,7 +362,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -436,11 +450,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -455,6 +493,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,11 +810,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE80E51-CF44-4883-A8E2-7FBF5966048F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52608AA2-C70E-466C-93EB-B7FB869EB03E}">
   <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -854,7 +896,9 @@
       <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="12">
+        <v>13</v>
+      </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -883,7 +927,9 @@
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="12"/>
+      <c r="E3" s="12">
+        <v>13</v>
+      </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -912,7 +958,9 @@
       <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="12">
+        <v>13</v>
+      </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -941,7 +989,9 @@
       <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="12"/>
+      <c r="E5" s="12">
+        <v>13</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -970,7 +1020,9 @@
       <c r="D6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="12">
+        <v>13</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -999,7 +1051,9 @@
       <c r="D7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="12">
+        <v>11</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -1028,7 +1082,9 @@
       <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="12">
+        <v>11</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -1057,7 +1113,9 @@
       <c r="D9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="12">
+        <v>11</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1086,7 +1144,9 @@
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="12">
+        <v>11</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -1115,7 +1175,9 @@
       <c r="D11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="12"/>
+      <c r="E11" s="12">
+        <v>11</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -1144,7 +1206,9 @@
       <c r="D12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -1173,7 +1237,9 @@
       <c r="D13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="12"/>
+      <c r="E13" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1202,7 +1268,9 @@
       <c r="D14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -1231,7 +1299,9 @@
       <c r="D15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -1260,7 +1330,9 @@
       <c r="D16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -1289,7 +1361,9 @@
       <c r="D17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="12">
+        <v>12</v>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1318,7 +1392,9 @@
       <c r="D18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="12"/>
+      <c r="E18" s="12">
+        <v>12</v>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1347,7 +1423,9 @@
       <c r="D19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="12"/>
+      <c r="E19" s="12">
+        <v>12</v>
+      </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1376,7 +1454,9 @@
       <c r="D20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="12">
+        <v>12</v>
+      </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -1405,7 +1485,9 @@
       <c r="D21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="12">
+        <v>12</v>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -1434,7 +1516,9 @@
       <c r="D22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="E22" s="12">
+        <v>12</v>
+      </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -1463,7 +1547,9 @@
       <c r="D23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="12"/>
+      <c r="E23" s="12">
+        <v>12</v>
+      </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -1492,7 +1578,9 @@
       <c r="D24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="12">
+        <v>12</v>
+      </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -1521,7 +1609,9 @@
       <c r="D25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="12">
+        <v>12</v>
+      </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -1550,7 +1640,9 @@
       <c r="D26" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="E26" s="12">
+        <v>12</v>
+      </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -1579,7 +1671,9 @@
       <c r="D27" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="12"/>
+      <c r="E27" s="12">
+        <v>14</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -1608,7 +1702,9 @@
       <c r="D28" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="12"/>
+      <c r="E28" s="12">
+        <v>14</v>
+      </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -1637,7 +1733,9 @@
       <c r="D29" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="12"/>
+      <c r="E29" s="12">
+        <v>14</v>
+      </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -1666,7 +1764,9 @@
       <c r="D30" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="12"/>
+      <c r="E30" s="12">
+        <v>14</v>
+      </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -1695,7 +1795,9 @@
       <c r="D31" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="12"/>
+      <c r="E31" s="12">
+        <v>14</v>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -1724,7 +1826,9 @@
       <c r="D32" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="12"/>
+      <c r="E32" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -1753,7 +1857,9 @@
       <c r="D33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="12"/>
+      <c r="E33" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -1782,7 +1888,9 @@
       <c r="D34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="12"/>
+      <c r="E34" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -1811,7 +1919,9 @@
       <c r="D35" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="12"/>
+      <c r="E35" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -1840,7 +1950,9 @@
       <c r="D36" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="12"/>
+      <c r="E36" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -1869,7 +1981,9 @@
       <c r="D37" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E37" s="12"/>
+      <c r="E37" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -1898,7 +2012,9 @@
       <c r="D38" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="12"/>
+      <c r="E38" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -1927,7 +2043,9 @@
       <c r="D39" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="12"/>
+      <c r="E39" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
@@ -1956,7 +2074,9 @@
       <c r="D40" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="12"/>
+      <c r="E40" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
@@ -1985,7 +2105,9 @@
       <c r="D41" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E41" s="12"/>
+      <c r="E41" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
@@ -2014,7 +2136,9 @@
       <c r="D42" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="12"/>
+      <c r="E42" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
@@ -2043,7 +2167,9 @@
       <c r="D43" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="12"/>
+      <c r="E43" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -2072,7 +2198,9 @@
       <c r="D44" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="12"/>
+      <c r="E44" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -2101,7 +2229,9 @@
       <c r="D45" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="12"/>
+      <c r="E45" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
@@ -2130,7 +2260,9 @@
       <c r="D46" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E46" s="12"/>
+      <c r="E46" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
@@ -2159,7 +2291,9 @@
       <c r="D47" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="12"/>
+      <c r="E47" s="12">
+        <v>13</v>
+      </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
@@ -2188,7 +2322,9 @@
       <c r="D48" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E48" s="12"/>
+      <c r="E48" s="12">
+        <v>13</v>
+      </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
@@ -2217,7 +2353,9 @@
       <c r="D49" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E49" s="12"/>
+      <c r="E49" s="12">
+        <v>13</v>
+      </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
@@ -2246,7 +2384,9 @@
       <c r="D50" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E50" s="12"/>
+      <c r="E50" s="12">
+        <v>13</v>
+      </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -2275,7 +2415,9 @@
       <c r="D51" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E51" s="13"/>
+      <c r="E51" s="13">
+        <v>13</v>
+      </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
@@ -3742,11 +3884,2053 @@
       <c r="S101" s="10"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2:A101" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE80E51-CF44-4883-A8E2-7FBF5966048F}">
+  <dimension ref="A1:U25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="T12" sqref="T12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.54296875" style="1" customWidth="1"/>
+    <col min="2" max="5" width="15.6328125" customWidth="1"/>
+    <col min="6" max="20" width="10.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="7">
+        <v>40</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="6">
+        <v>8</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" s="6">
+        <v>6</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" s="6">
+        <v>5</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>5</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="7">
+        <v>40</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="6">
+        <v>7</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="6">
+        <v>5</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" s="6">
+        <v>6</v>
+      </c>
+      <c r="N3" s="6">
+        <v>9</v>
+      </c>
+      <c r="O3" s="6">
+        <v>5</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>5</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="7">
+        <v>40</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="6">
+        <v>9</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" s="6">
+        <v>6</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4" s="6">
+        <v>6</v>
+      </c>
+      <c r="N4" s="6">
+        <v>9</v>
+      </c>
+      <c r="O4" s="6">
+        <v>5</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>5</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="10">
+        <v>40</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="U5" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>100205</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="7">
+        <v>40</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="6">
+        <v>5</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="6">
+        <v>4</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="O6" s="6">
+        <v>4</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>4</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="S6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>100405</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="7">
+        <v>40</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="6">
+        <v>6</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" s="6">
+        <v>4</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M7" s="14">
+        <v>5</v>
+      </c>
+      <c r="N7" s="6">
+        <v>9</v>
+      </c>
+      <c r="O7" s="14">
+        <v>4</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>4</v>
+      </c>
+      <c r="R7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="S7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>100505</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="7">
+        <v>40</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="14">
+        <v>8</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="14">
+        <v>6</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M8" s="14">
+        <v>5</v>
+      </c>
+      <c r="N8" s="14">
+        <v>9</v>
+      </c>
+      <c r="O8" s="14">
+        <v>4</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>5</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="U8" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="10">
+        <v>40</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="U9" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="7">
+        <v>60</v>
+      </c>
+      <c r="F10" s="12">
+        <v>11</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H10" s="6">
+        <v>7</v>
+      </c>
+      <c r="I10" s="14">
+        <v>5</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="6">
+        <v>6</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="P10" s="14">
+        <v>7</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>4</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="S10" s="6">
+        <v>14</v>
+      </c>
+      <c r="T10" s="7">
+        <v>12</v>
+      </c>
+      <c r="U10" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="7">
+        <v>60</v>
+      </c>
+      <c r="F11" s="12">
+        <v>12</v>
+      </c>
+      <c r="G11" s="6">
+        <v>8</v>
+      </c>
+      <c r="H11" s="14">
+        <v>8</v>
+      </c>
+      <c r="I11" s="14">
+        <v>6</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K11" s="14">
+        <v>13</v>
+      </c>
+      <c r="L11" s="7">
+        <v>12</v>
+      </c>
+      <c r="M11" s="14">
+        <v>6</v>
+      </c>
+      <c r="N11" s="14">
+        <v>6</v>
+      </c>
+      <c r="O11" s="14">
+        <v>5</v>
+      </c>
+      <c r="P11" s="14">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="14">
+        <v>4</v>
+      </c>
+      <c r="R11" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="S11" s="14">
+        <v>15</v>
+      </c>
+      <c r="T11" s="7">
+        <v>13</v>
+      </c>
+      <c r="U11" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="7">
+        <v>60</v>
+      </c>
+      <c r="F12" s="12">
+        <v>12</v>
+      </c>
+      <c r="G12" s="14">
+        <v>9</v>
+      </c>
+      <c r="H12" s="14">
+        <v>8</v>
+      </c>
+      <c r="I12" s="14">
+        <v>6</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K12" s="14">
+        <v>13</v>
+      </c>
+      <c r="L12" s="7">
+        <v>12</v>
+      </c>
+      <c r="M12" s="14">
+        <v>6</v>
+      </c>
+      <c r="N12" s="14">
+        <v>7</v>
+      </c>
+      <c r="O12" s="14">
+        <v>5</v>
+      </c>
+      <c r="P12" s="14">
+        <v>8</v>
+      </c>
+      <c r="Q12" s="14">
+        <v>5</v>
+      </c>
+      <c r="R12" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="S12" s="14">
+        <v>15</v>
+      </c>
+      <c r="T12" s="7">
+        <v>12</v>
+      </c>
+      <c r="U12" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="10">
+        <v>60</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="10">
+        <v>12</v>
+      </c>
+      <c r="U13" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>100205</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="7">
+        <v>60</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="6">
+        <v>6</v>
+      </c>
+      <c r="H14" s="6">
+        <v>6</v>
+      </c>
+      <c r="I14" s="14">
+        <v>4</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M14" s="6">
+        <v>4</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="O14" s="6">
+        <v>4</v>
+      </c>
+      <c r="P14" s="6">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="14">
+        <v>3</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="T14" s="7">
+        <v>12</v>
+      </c>
+      <c r="U14" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
+        <v>100405</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="7">
+        <v>60</v>
+      </c>
+      <c r="F15" s="12">
+        <v>9</v>
+      </c>
+      <c r="G15" s="6">
+        <v>6</v>
+      </c>
+      <c r="H15" s="14">
+        <v>6</v>
+      </c>
+      <c r="I15" s="14">
+        <v>4</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" s="14">
+        <v>12</v>
+      </c>
+      <c r="L15" s="7">
+        <v>12</v>
+      </c>
+      <c r="M15" s="14">
+        <v>5</v>
+      </c>
+      <c r="N15" s="14">
+        <v>6</v>
+      </c>
+      <c r="O15" s="14">
+        <v>3</v>
+      </c>
+      <c r="P15" s="14">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>3</v>
+      </c>
+      <c r="R15" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="S15" s="14">
+        <v>13</v>
+      </c>
+      <c r="T15" s="7">
+        <v>13</v>
+      </c>
+      <c r="U15" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
+        <v>100505</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="7">
+        <v>60</v>
+      </c>
+      <c r="F16" s="12">
+        <v>10</v>
+      </c>
+      <c r="G16" s="14">
+        <v>7</v>
+      </c>
+      <c r="H16" s="14">
+        <v>7</v>
+      </c>
+      <c r="I16" s="14">
+        <v>4</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K16" s="14">
+        <v>12</v>
+      </c>
+      <c r="L16" s="7">
+        <v>12</v>
+      </c>
+      <c r="M16" s="14">
+        <v>6</v>
+      </c>
+      <c r="N16" s="14">
+        <v>6</v>
+      </c>
+      <c r="O16" s="14">
+        <v>4</v>
+      </c>
+      <c r="P16" s="14">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="14">
+        <v>4</v>
+      </c>
+      <c r="R16" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="S16" s="14">
+        <v>13</v>
+      </c>
+      <c r="T16" s="7">
+        <v>12</v>
+      </c>
+      <c r="U16" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="10">
+        <v>60</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="10">
+        <v>12</v>
+      </c>
+      <c r="U17" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="7">
+        <v>200</v>
+      </c>
+      <c r="F18" s="12">
+        <v>9</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="6">
+        <v>5</v>
+      </c>
+      <c r="I18" s="14">
+        <v>5</v>
+      </c>
+      <c r="J18" s="14">
+        <v>6</v>
+      </c>
+      <c r="K18" s="14">
+        <v>7</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M18" s="14">
+        <v>6</v>
+      </c>
+      <c r="N18" s="14">
+        <v>5</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="P18" s="14">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="14">
+        <v>4</v>
+      </c>
+      <c r="R18" s="14">
+        <v>7</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="T18" s="7">
+        <v>5</v>
+      </c>
+      <c r="U18" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="7">
+        <v>200</v>
+      </c>
+      <c r="F19" s="12">
+        <v>10</v>
+      </c>
+      <c r="G19" s="6">
+        <v>8</v>
+      </c>
+      <c r="H19" s="14">
+        <v>7</v>
+      </c>
+      <c r="I19" s="14">
+        <v>6</v>
+      </c>
+      <c r="J19" s="14">
+        <v>6</v>
+      </c>
+      <c r="K19" s="14">
+        <v>8</v>
+      </c>
+      <c r="L19" s="7">
+        <v>5</v>
+      </c>
+      <c r="M19" s="14">
+        <v>6</v>
+      </c>
+      <c r="N19" s="14">
+        <v>5</v>
+      </c>
+      <c r="O19" s="14">
+        <v>5</v>
+      </c>
+      <c r="P19" s="14">
+        <v>7</v>
+      </c>
+      <c r="Q19" s="14">
+        <v>4</v>
+      </c>
+      <c r="R19" s="14">
+        <v>8</v>
+      </c>
+      <c r="S19" s="14">
+        <v>10</v>
+      </c>
+      <c r="T19" s="7">
+        <v>5</v>
+      </c>
+      <c r="U19" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="7">
+        <v>200</v>
+      </c>
+      <c r="F20" s="12">
+        <v>11</v>
+      </c>
+      <c r="G20" s="14">
+        <v>9</v>
+      </c>
+      <c r="H20" s="14">
+        <v>7</v>
+      </c>
+      <c r="I20" s="14">
+        <v>5</v>
+      </c>
+      <c r="J20" s="6">
+        <v>6</v>
+      </c>
+      <c r="K20" s="14">
+        <v>8</v>
+      </c>
+      <c r="L20" s="7">
+        <v>5</v>
+      </c>
+      <c r="M20" s="14">
+        <v>6</v>
+      </c>
+      <c r="N20" s="14">
+        <v>5</v>
+      </c>
+      <c r="O20" s="14">
+        <v>5</v>
+      </c>
+      <c r="P20" s="14">
+        <v>7</v>
+      </c>
+      <c r="Q20" s="14">
+        <v>4</v>
+      </c>
+      <c r="R20" s="14">
+        <v>7</v>
+      </c>
+      <c r="S20" s="14">
+        <v>11</v>
+      </c>
+      <c r="T20" s="7">
+        <v>6</v>
+      </c>
+      <c r="U20" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="7">
+        <v>200</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="10">
+        <v>6</v>
+      </c>
+      <c r="U21" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>100205</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="4">
+        <v>200</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="6">
+        <v>5</v>
+      </c>
+      <c r="H22" s="6">
+        <v>4</v>
+      </c>
+      <c r="I22" s="14">
+        <v>4</v>
+      </c>
+      <c r="J22" s="14">
+        <v>4</v>
+      </c>
+      <c r="K22" s="14">
+        <v>6</v>
+      </c>
+      <c r="L22" s="7">
+        <v>4</v>
+      </c>
+      <c r="M22" s="14">
+        <v>4</v>
+      </c>
+      <c r="N22" s="14">
+        <v>3</v>
+      </c>
+      <c r="O22" s="14">
+        <v>3</v>
+      </c>
+      <c r="P22" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="14">
+        <v>3</v>
+      </c>
+      <c r="R22" s="14">
+        <v>5</v>
+      </c>
+      <c r="S22" s="14">
+        <v>7</v>
+      </c>
+      <c r="T22" s="7">
+        <v>4</v>
+      </c>
+      <c r="U22" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A23" s="5">
+        <v>100405</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="7">
+        <v>200</v>
+      </c>
+      <c r="F23" s="12">
+        <v>7</v>
+      </c>
+      <c r="G23" s="6">
+        <v>6</v>
+      </c>
+      <c r="H23" s="14">
+        <v>5</v>
+      </c>
+      <c r="I23" s="14">
+        <v>4</v>
+      </c>
+      <c r="J23" s="14">
+        <v>5</v>
+      </c>
+      <c r="K23" s="14">
+        <v>6</v>
+      </c>
+      <c r="L23" s="7">
+        <v>4</v>
+      </c>
+      <c r="M23" s="14">
+        <v>5</v>
+      </c>
+      <c r="N23" s="14">
+        <v>4</v>
+      </c>
+      <c r="O23" s="14">
+        <v>3</v>
+      </c>
+      <c r="P23" s="14">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="14">
+        <v>3</v>
+      </c>
+      <c r="R23" s="14">
+        <v>6</v>
+      </c>
+      <c r="S23" s="14">
+        <v>8</v>
+      </c>
+      <c r="T23" s="7">
+        <v>5</v>
+      </c>
+      <c r="U23" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A24" s="5">
+        <v>100505</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="7">
+        <v>200</v>
+      </c>
+      <c r="F24" s="12">
+        <v>7</v>
+      </c>
+      <c r="G24" s="14">
+        <v>6</v>
+      </c>
+      <c r="H24" s="14">
+        <v>6</v>
+      </c>
+      <c r="I24" s="14">
+        <v>4</v>
+      </c>
+      <c r="J24" s="14">
+        <v>5</v>
+      </c>
+      <c r="K24" s="14">
+        <v>6</v>
+      </c>
+      <c r="L24" s="7">
+        <v>4</v>
+      </c>
+      <c r="M24" s="14">
+        <v>6</v>
+      </c>
+      <c r="N24" s="14">
+        <v>4</v>
+      </c>
+      <c r="O24" s="14">
+        <v>4</v>
+      </c>
+      <c r="P24" s="14">
+        <v>6</v>
+      </c>
+      <c r="Q24" s="14">
+        <v>3</v>
+      </c>
+      <c r="R24" s="14">
+        <v>5</v>
+      </c>
+      <c r="S24" s="14">
+        <v>8</v>
+      </c>
+      <c r="T24" s="7">
+        <v>5</v>
+      </c>
+      <c r="U24" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="10">
+        <v>200</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="10">
+        <v>4</v>
+      </c>
+      <c r="U25" s="16">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2 A3:A37 A38:A51 A87:A91 A97:A101" numberStoredAsText="1"/>
+    <ignoredError sqref="A2 A5 A9 A3 A4 A10:A25" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813114BA-5A05-4982-B1CD-D343B056E596}">
+  <dimension ref="A1:S9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.54296875" style="1" customWidth="1"/>
+    <col min="2" max="4" width="15.6328125" customWidth="1"/>
+    <col min="5" max="19" width="10.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="12">
+        <v>9</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="14">
+        <v>5</v>
+      </c>
+      <c r="H2" s="14">
+        <v>5</v>
+      </c>
+      <c r="I2" s="14">
+        <v>6</v>
+      </c>
+      <c r="J2" s="14">
+        <v>7</v>
+      </c>
+      <c r="K2" s="17">
+        <v>4</v>
+      </c>
+      <c r="L2" s="14">
+        <v>6</v>
+      </c>
+      <c r="M2" s="14">
+        <v>5</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" s="14">
+        <v>5</v>
+      </c>
+      <c r="P2" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>7</v>
+      </c>
+      <c r="R2" s="14">
+        <v>9</v>
+      </c>
+      <c r="S2" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="12">
+        <v>10</v>
+      </c>
+      <c r="F3" s="6">
+        <v>8</v>
+      </c>
+      <c r="G3" s="14">
+        <v>7</v>
+      </c>
+      <c r="H3" s="14">
+        <v>6</v>
+      </c>
+      <c r="I3" s="14">
+        <v>6</v>
+      </c>
+      <c r="J3" s="14">
+        <v>7</v>
+      </c>
+      <c r="K3" s="7">
+        <v>5</v>
+      </c>
+      <c r="L3" s="14">
+        <v>6</v>
+      </c>
+      <c r="M3" s="14">
+        <v>5</v>
+      </c>
+      <c r="N3" s="14">
+        <v>5</v>
+      </c>
+      <c r="O3" s="14">
+        <v>7</v>
+      </c>
+      <c r="P3" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>8</v>
+      </c>
+      <c r="R3" s="14">
+        <v>10</v>
+      </c>
+      <c r="S3" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="12">
+        <v>11</v>
+      </c>
+      <c r="F4" s="6">
+        <v>9</v>
+      </c>
+      <c r="G4" s="14">
+        <v>7</v>
+      </c>
+      <c r="H4" s="14">
+        <v>5</v>
+      </c>
+      <c r="I4" s="14">
+        <v>6</v>
+      </c>
+      <c r="J4" s="14">
+        <v>8</v>
+      </c>
+      <c r="K4" s="7">
+        <v>5</v>
+      </c>
+      <c r="L4" s="14">
+        <v>6</v>
+      </c>
+      <c r="M4" s="14">
+        <v>5</v>
+      </c>
+      <c r="N4" s="14">
+        <v>5</v>
+      </c>
+      <c r="O4" s="14">
+        <v>7</v>
+      </c>
+      <c r="P4" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>7</v>
+      </c>
+      <c r="R4" s="14">
+        <v>11</v>
+      </c>
+      <c r="S4" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="13">
+        <v>11</v>
+      </c>
+      <c r="F5" s="9">
+        <v>8</v>
+      </c>
+      <c r="G5" s="9">
+        <v>7</v>
+      </c>
+      <c r="H5" s="9">
+        <v>5</v>
+      </c>
+      <c r="I5" s="9">
+        <v>6</v>
+      </c>
+      <c r="J5" s="9">
+        <v>7</v>
+      </c>
+      <c r="K5" s="10">
+        <v>5</v>
+      </c>
+      <c r="L5" s="9">
+        <v>6</v>
+      </c>
+      <c r="M5" s="9">
+        <v>5</v>
+      </c>
+      <c r="N5" s="9">
+        <v>5</v>
+      </c>
+      <c r="O5" s="9">
+        <v>7</v>
+      </c>
+      <c r="P5" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>8</v>
+      </c>
+      <c r="R5" s="9">
+        <v>10</v>
+      </c>
+      <c r="S5" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>100205</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="14">
+        <v>5</v>
+      </c>
+      <c r="G6" s="14">
+        <v>4</v>
+      </c>
+      <c r="H6" s="6">
+        <v>4</v>
+      </c>
+      <c r="I6" s="14">
+        <v>4</v>
+      </c>
+      <c r="J6" s="14">
+        <v>5</v>
+      </c>
+      <c r="K6" s="7">
+        <v>4</v>
+      </c>
+      <c r="L6" s="14">
+        <v>4</v>
+      </c>
+      <c r="M6" s="14">
+        <v>3</v>
+      </c>
+      <c r="N6" s="14">
+        <v>3</v>
+      </c>
+      <c r="O6" s="14">
+        <v>4</v>
+      </c>
+      <c r="P6" s="14">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>5</v>
+      </c>
+      <c r="R6" s="14">
+        <v>7</v>
+      </c>
+      <c r="S6" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>100405</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="12">
+        <v>7</v>
+      </c>
+      <c r="F7" s="6">
+        <v>6</v>
+      </c>
+      <c r="G7" s="14">
+        <v>5</v>
+      </c>
+      <c r="H7" s="14">
+        <v>4</v>
+      </c>
+      <c r="I7" s="14">
+        <v>5</v>
+      </c>
+      <c r="J7" s="14">
+        <v>6</v>
+      </c>
+      <c r="K7" s="7">
+        <v>4</v>
+      </c>
+      <c r="L7" s="14">
+        <v>5</v>
+      </c>
+      <c r="M7" s="14">
+        <v>4</v>
+      </c>
+      <c r="N7" s="14">
+        <v>3</v>
+      </c>
+      <c r="O7" s="14">
+        <v>5</v>
+      </c>
+      <c r="P7" s="14">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>6</v>
+      </c>
+      <c r="R7" s="14">
+        <v>8</v>
+      </c>
+      <c r="S7" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>100505</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="12">
+        <v>7</v>
+      </c>
+      <c r="F8" s="14">
+        <v>6</v>
+      </c>
+      <c r="G8" s="14">
+        <v>6</v>
+      </c>
+      <c r="H8" s="14">
+        <v>4</v>
+      </c>
+      <c r="I8" s="14">
+        <v>5</v>
+      </c>
+      <c r="J8" s="14">
+        <v>6</v>
+      </c>
+      <c r="K8" s="7">
+        <v>4</v>
+      </c>
+      <c r="L8" s="14">
+        <v>6</v>
+      </c>
+      <c r="M8" s="14">
+        <v>4</v>
+      </c>
+      <c r="N8" s="14">
+        <v>4</v>
+      </c>
+      <c r="O8" s="14">
+        <v>6</v>
+      </c>
+      <c r="P8" s="14">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>5</v>
+      </c>
+      <c r="R8" s="14">
+        <v>8</v>
+      </c>
+      <c r="S8" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="13">
+        <v>8</v>
+      </c>
+      <c r="F9" s="9">
+        <v>6</v>
+      </c>
+      <c r="G9" s="9">
+        <v>5</v>
+      </c>
+      <c r="H9" s="9">
+        <v>4</v>
+      </c>
+      <c r="I9" s="9">
+        <v>5</v>
+      </c>
+      <c r="J9" s="9">
+        <v>5</v>
+      </c>
+      <c r="K9" s="10">
+        <v>4</v>
+      </c>
+      <c r="L9" s="9">
+        <v>4</v>
+      </c>
+      <c r="M9" s="9">
+        <v>4</v>
+      </c>
+      <c r="N9" s="9">
+        <v>4</v>
+      </c>
+      <c r="O9" s="9">
+        <v>5</v>
+      </c>
+      <c r="P9" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>5</v>
+      </c>
+      <c r="R9" s="9">
+        <v>7</v>
+      </c>
+      <c r="S9" s="10">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2:A9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completion of model runs and updated results
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C36D27-DEF4-4627-BC39-E0447BA5EE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426ABB23-171B-4578-9225-3D5DA3EC823C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{28F97023-1D5E-44FA-A19C-A9B15763E968}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{28F97023-1D5E-44FA-A19C-A9B15763E968}"/>
   </bookViews>
   <sheets>
     <sheet name="full_model_set" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="99">
   <si>
     <t>id</t>
   </si>
@@ -478,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -497,6 +497,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3897,10 +3901,10 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T12" sqref="T12"/>
+      <selection pane="bottomRight" activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4186,20 +4190,48 @@
       <c r="E5" s="10">
         <v>40</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
+      <c r="F5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="9">
+        <v>9</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="9">
+        <v>6</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="9">
+        <v>6</v>
+      </c>
+      <c r="N5" s="9">
+        <v>9</v>
+      </c>
+      <c r="O5" s="9">
+        <v>5</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>5</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="T5" s="9" t="s">
         <v>98</v>
       </c>
@@ -4418,20 +4450,48 @@
       <c r="E9" s="10">
         <v>40</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
+      <c r="F9" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="9">
+        <v>7</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" s="9">
+        <v>5</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="M9" s="9">
+        <v>5</v>
+      </c>
+      <c r="N9" s="9">
+        <v>9</v>
+      </c>
+      <c r="O9" s="9">
+        <v>5</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>4</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="T9" s="9" t="s">
         <v>98</v>
       </c>
@@ -4650,20 +4710,48 @@
       <c r="E13" s="10">
         <v>60</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
+      <c r="F13" s="13">
+        <v>13</v>
+      </c>
+      <c r="G13" s="9">
+        <v>8</v>
+      </c>
+      <c r="H13" s="9">
+        <v>8</v>
+      </c>
+      <c r="I13" s="9">
+        <v>6</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" s="9">
+        <v>13</v>
+      </c>
+      <c r="L13" s="10">
+        <v>12</v>
+      </c>
+      <c r="M13" s="9">
+        <v>6</v>
+      </c>
+      <c r="N13" s="9">
+        <v>7</v>
+      </c>
+      <c r="O13" s="9">
+        <v>5</v>
+      </c>
+      <c r="P13" s="9">
+        <v>8</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>5</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="S13" s="9">
+        <v>15</v>
+      </c>
       <c r="T13" s="10">
         <v>12</v>
       </c>
@@ -4882,20 +4970,48 @@
       <c r="E17" s="10">
         <v>60</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
+      <c r="F17" s="13">
+        <v>10</v>
+      </c>
+      <c r="G17" s="9">
+        <v>7</v>
+      </c>
+      <c r="H17" s="9">
+        <v>6</v>
+      </c>
+      <c r="I17" s="9">
+        <v>4</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" s="9">
+        <v>11</v>
+      </c>
+      <c r="L17" s="10">
+        <v>12</v>
+      </c>
+      <c r="M17" s="9">
+        <v>4</v>
+      </c>
+      <c r="N17" s="9">
+        <v>6</v>
+      </c>
+      <c r="O17" s="9">
+        <v>4</v>
+      </c>
+      <c r="P17" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>4</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="S17" s="9">
+        <v>13</v>
+      </c>
       <c r="T17" s="10">
         <v>12</v>
       </c>
@@ -4919,13 +5035,13 @@
       <c r="E18" s="7">
         <v>200</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="18">
         <v>9</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="14">
         <v>5</v>
       </c>
       <c r="I18" s="14">
@@ -4937,7 +5053,7 @@
       <c r="K18" s="14">
         <v>7</v>
       </c>
-      <c r="L18" s="7" t="s">
+      <c r="L18" s="17" t="s">
         <v>98</v>
       </c>
       <c r="M18" s="14">
@@ -4946,7 +5062,7 @@
       <c r="N18" s="14">
         <v>5</v>
       </c>
-      <c r="O18" s="6" t="s">
+      <c r="O18" s="14" t="s">
         <v>98</v>
       </c>
       <c r="P18" s="14">
@@ -4958,10 +5074,10 @@
       <c r="R18" s="14">
         <v>7</v>
       </c>
-      <c r="S18" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="T18" s="7">
+      <c r="S18" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="T18" s="17">
         <v>5</v>
       </c>
       <c r="U18" s="15">
@@ -4984,10 +5100,10 @@
       <c r="E19" s="7">
         <v>200</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="18">
         <v>10</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="14">
         <v>8</v>
       </c>
       <c r="H19" s="14">
@@ -5002,7 +5118,7 @@
       <c r="K19" s="14">
         <v>8</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="17">
         <v>5</v>
       </c>
       <c r="M19" s="14">
@@ -5026,7 +5142,7 @@
       <c r="S19" s="14">
         <v>10</v>
       </c>
-      <c r="T19" s="7">
+      <c r="T19" s="17">
         <v>5</v>
       </c>
       <c r="U19" s="15">
@@ -5049,7 +5165,7 @@
       <c r="E20" s="7">
         <v>200</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="18">
         <v>11</v>
       </c>
       <c r="G20" s="14">
@@ -5061,13 +5177,13 @@
       <c r="I20" s="14">
         <v>5</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="14">
         <v>6</v>
       </c>
       <c r="K20" s="14">
         <v>8</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="17">
         <v>5</v>
       </c>
       <c r="M20" s="14">
@@ -5091,7 +5207,7 @@
       <c r="S20" s="14">
         <v>11</v>
       </c>
-      <c r="T20" s="7">
+      <c r="T20" s="17">
         <v>6</v>
       </c>
       <c r="U20" s="15">
@@ -5114,21 +5230,49 @@
       <c r="E21" s="7">
         <v>200</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="10">
+      <c r="F21" s="19">
+        <v>11</v>
+      </c>
+      <c r="G21" s="20">
+        <v>8</v>
+      </c>
+      <c r="H21" s="20">
+        <v>7</v>
+      </c>
+      <c r="I21" s="20">
+        <v>5</v>
+      </c>
+      <c r="J21" s="20">
+        <v>6</v>
+      </c>
+      <c r="K21" s="20">
+        <v>7</v>
+      </c>
+      <c r="L21" s="21">
+        <v>5</v>
+      </c>
+      <c r="M21" s="20">
+        <v>6</v>
+      </c>
+      <c r="N21" s="20">
+        <v>5</v>
+      </c>
+      <c r="O21" s="20">
+        <v>5</v>
+      </c>
+      <c r="P21" s="20">
+        <v>7</v>
+      </c>
+      <c r="Q21" s="20">
+        <v>4</v>
+      </c>
+      <c r="R21" s="20">
+        <v>8</v>
+      </c>
+      <c r="S21" s="20">
+        <v>10</v>
+      </c>
+      <c r="T21" s="21">
         <v>6</v>
       </c>
       <c r="U21" s="16">
@@ -5151,13 +5295,13 @@
       <c r="E22" s="4">
         <v>200</v>
       </c>
-      <c r="F22" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="G22" s="6">
-        <v>5</v>
-      </c>
-      <c r="H22" s="6">
+      <c r="F22" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="14">
+        <v>5</v>
+      </c>
+      <c r="H22" s="14">
         <v>4</v>
       </c>
       <c r="I22" s="14">
@@ -5169,7 +5313,7 @@
       <c r="K22" s="14">
         <v>6</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="17">
         <v>4</v>
       </c>
       <c r="M22" s="14">
@@ -5193,7 +5337,7 @@
       <c r="S22" s="14">
         <v>7</v>
       </c>
-      <c r="T22" s="7">
+      <c r="T22" s="17">
         <v>4</v>
       </c>
       <c r="U22" s="15">
@@ -5216,10 +5360,10 @@
       <c r="E23" s="7">
         <v>200</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="18">
         <v>7</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="14">
         <v>6</v>
       </c>
       <c r="H23" s="14">
@@ -5234,7 +5378,7 @@
       <c r="K23" s="14">
         <v>6</v>
       </c>
-      <c r="L23" s="7">
+      <c r="L23" s="17">
         <v>4</v>
       </c>
       <c r="M23" s="14">
@@ -5258,7 +5402,7 @@
       <c r="S23" s="14">
         <v>8</v>
       </c>
-      <c r="T23" s="7">
+      <c r="T23" s="17">
         <v>5</v>
       </c>
       <c r="U23" s="15">
@@ -5281,7 +5425,7 @@
       <c r="E24" s="7">
         <v>200</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="18">
         <v>7</v>
       </c>
       <c r="G24" s="14">
@@ -5299,7 +5443,7 @@
       <c r="K24" s="14">
         <v>6</v>
       </c>
-      <c r="L24" s="7">
+      <c r="L24" s="17">
         <v>4</v>
       </c>
       <c r="M24" s="14">
@@ -5323,7 +5467,7 @@
       <c r="S24" s="14">
         <v>8</v>
       </c>
-      <c r="T24" s="7">
+      <c r="T24" s="17">
         <v>5</v>
       </c>
       <c r="U24" s="15">
@@ -5346,21 +5490,49 @@
       <c r="E25" s="10">
         <v>200</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="10">
+      <c r="F25" s="19">
+        <v>8</v>
+      </c>
+      <c r="G25" s="20">
+        <v>6</v>
+      </c>
+      <c r="H25" s="20">
+        <v>5</v>
+      </c>
+      <c r="I25" s="20">
+        <v>4</v>
+      </c>
+      <c r="J25" s="20">
+        <v>5</v>
+      </c>
+      <c r="K25" s="20">
+        <v>6</v>
+      </c>
+      <c r="L25" s="21">
+        <v>4</v>
+      </c>
+      <c r="M25" s="20">
+        <v>4</v>
+      </c>
+      <c r="N25" s="20">
+        <v>4</v>
+      </c>
+      <c r="O25" s="20">
+        <v>4</v>
+      </c>
+      <c r="P25" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="20">
+        <v>3</v>
+      </c>
+      <c r="R25" s="20">
+        <v>5</v>
+      </c>
+      <c r="S25" s="20">
+        <v>8</v>
+      </c>
+      <c r="T25" s="21">
         <v>4</v>
       </c>
       <c r="U25" s="16">

</xml_diff>

<commit_message>
1st round re-running models
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F1FF409-D31A-4094-BF5C-A1685AA4C859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05F6387-A5A7-4243-A1E8-D79A3E5DFC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_model_set" sheetId="4" r:id="rId1"/>
     <sheet name="reduced_model_set" sheetId="5" r:id="rId2"/>
-    <sheet name="reduced_model_set (2)" sheetId="6" r:id="rId3"/>
+    <sheet name="model_rerun_tracker" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="122">
   <si>
     <t>shift</t>
   </si>
@@ -390,6 +390,9 @@
   </si>
   <si>
     <t>t1005</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -405,12 +408,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -529,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -559,6 +568,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3774,7 +3787,7 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J7" sqref="J7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3866,25 +3879,25 @@
       <c r="E2" s="13">
         <v>40</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="14">
-        <v>8</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="16" t="s">
+      <c r="F2" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="28">
+        <v>8</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="29" t="s">
         <v>34</v>
       </c>
       <c r="M2" s="14">
@@ -3931,25 +3944,25 @@
       <c r="E3" s="13">
         <v>40</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="14">
-        <v>7</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="14">
-        <v>5</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="13" t="s">
+      <c r="F3" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="28">
+        <v>7</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="28">
+        <v>5</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="29" t="s">
         <v>34</v>
       </c>
       <c r="M3" s="14">
@@ -3996,25 +4009,25 @@
       <c r="E4" s="13">
         <v>40</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="14">
+      <c r="F4" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="28">
         <v>9</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="14">
-        <v>6</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="13" t="s">
+      <c r="H4" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="28">
+        <v>6</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="29" t="s">
         <v>34</v>
       </c>
       <c r="M4" s="14">
@@ -4061,7 +4074,7 @@
       <c r="E5" s="17">
         <v>40</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="30" t="s">
         <v>34</v>
       </c>
       <c r="G5" s="18">
@@ -4126,25 +4139,25 @@
       <c r="E6" s="13">
         <v>40</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="14">
-        <v>5</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="13" t="s">
+      <c r="F6" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="28">
+        <v>5</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="29" t="s">
         <v>34</v>
       </c>
       <c r="M6" s="14">
@@ -4191,25 +4204,25 @@
       <c r="E7" s="13">
         <v>40</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="14">
-        <v>6</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="14">
-        <v>4</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="13" t="s">
+      <c r="F7" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="28">
+        <v>4</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="29" t="s">
         <v>34</v>
       </c>
       <c r="M7" s="15">
@@ -5920,5 +5933,8 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2:A33" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
starting to create maps - issue with routes not showing up, possible API timeout errors?
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4513" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4522" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -10528,7 +10528,7 @@
   <dimension ref="A1:T481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10996,7 +10996,9 @@
       <c r="K10" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L10" s="31"/>
+      <c r="L10" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M10" s="31"/>
       <c r="N10" s="31"/>
       <c r="O10" s="32"/>
@@ -11350,7 +11352,9 @@
       <c r="K18" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L18" s="32"/>
+      <c r="L18" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M18" s="32"/>
       <c r="N18" s="32"/>
       <c r="O18" s="32"/>
@@ -11704,7 +11708,9 @@
       <c r="K26" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L26" s="32"/>
+      <c r="L26" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M26" s="32"/>
       <c r="N26" s="32"/>
       <c r="O26" s="31"/>
@@ -13178,7 +13184,9 @@
       <c r="J66" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="K66" s="32"/>
+      <c r="K66" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="L66" s="30" t="s">
         <v>34</v>
       </c>
@@ -13273,6 +13281,21 @@
       </c>
       <c r="G70" s="30" t="s">
         <v>271</v>
+      </c>
+      <c r="H70" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="I70" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J70" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="K70" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L70" s="30" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
model results for ideal region 1
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4522" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4544" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -2126,12 +2126,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -2250,7 +2256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2288,6 +2294,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6918,50 +6935,50 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="I1" s="36" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="I1" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="J2" s="36" t="s">
+      <c r="G2" s="47"/>
+      <c r="J2" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36" t="s">
+      <c r="M2" s="47"/>
+      <c r="N2" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="36"/>
+      <c r="O2" s="47"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -7193,50 +7210,50 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="I8" s="36" t="s">
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="I8" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36" t="s">
+      <c r="C9" s="47"/>
+      <c r="D9" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36" t="s">
+      <c r="E9" s="47"/>
+      <c r="F9" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="J9" s="36" t="s">
+      <c r="G9" s="47"/>
+      <c r="J9" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36" t="s">
+      <c r="K9" s="47"/>
+      <c r="L9" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36" t="s">
+      <c r="M9" s="47"/>
+      <c r="N9" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="O9" s="36"/>
+      <c r="O9" s="47"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -7468,50 +7485,50 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="I15" s="36" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="I15" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36" t="s">
+      <c r="C16" s="47"/>
+      <c r="D16" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36" t="s">
+      <c r="E16" s="47"/>
+      <c r="F16" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="J16" s="36" t="s">
+      <c r="G16" s="47"/>
+      <c r="J16" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36" t="s">
+      <c r="K16" s="47"/>
+      <c r="L16" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36" t="s">
+      <c r="M16" s="47"/>
+      <c r="N16" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="O16" s="36"/>
+      <c r="O16" s="47"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -7743,50 +7760,50 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="I22" s="36" t="s">
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="I22" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36" t="s">
+      <c r="C23" s="47"/>
+      <c r="D23" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36" t="s">
+      <c r="E23" s="47"/>
+      <c r="F23" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="36"/>
-      <c r="J23" s="36" t="s">
+      <c r="G23" s="47"/>
+      <c r="J23" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36" t="s">
+      <c r="K23" s="47"/>
+      <c r="L23" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36" t="s">
+      <c r="M23" s="47"/>
+      <c r="N23" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="O23" s="36"/>
+      <c r="O23" s="47"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -8019,50 +8036,50 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="I29" s="36" t="s">
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="I29" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="36"/>
-      <c r="O29" s="36"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36" t="s">
+      <c r="C30" s="47"/>
+      <c r="D30" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36" t="s">
+      <c r="E30" s="47"/>
+      <c r="F30" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="G30" s="36"/>
-      <c r="J30" s="36" t="s">
+      <c r="G30" s="47"/>
+      <c r="J30" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36" t="s">
+      <c r="K30" s="47"/>
+      <c r="L30" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="M30" s="36"/>
-      <c r="N30" s="36" t="s">
+      <c r="M30" s="47"/>
+      <c r="N30" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="O30" s="36"/>
+      <c r="O30" s="47"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -8295,50 +8312,50 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="I36" s="36" t="s">
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="I36" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="36"/>
-      <c r="O36" s="36"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="47"/>
+      <c r="O36" s="47"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36" t="s">
+      <c r="C37" s="47"/>
+      <c r="D37" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36" t="s">
+      <c r="E37" s="47"/>
+      <c r="F37" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="G37" s="36"/>
-      <c r="J37" s="36" t="s">
+      <c r="G37" s="47"/>
+      <c r="J37" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36" t="s">
+      <c r="K37" s="47"/>
+      <c r="L37" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="M37" s="36"/>
-      <c r="N37" s="36" t="s">
+      <c r="M37" s="47"/>
+      <c r="N37" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="O37" s="36"/>
+      <c r="O37" s="47"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -8571,50 +8588,50 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="I43" s="36" t="s">
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="I43" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="J43" s="36"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="36"/>
-      <c r="N43" s="36"/>
-      <c r="O43" s="36"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="47"/>
+      <c r="N43" s="47"/>
+      <c r="O43" s="47"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="36" t="s">
+      <c r="B44" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36" t="s">
+      <c r="C44" s="47"/>
+      <c r="D44" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36" t="s">
+      <c r="E44" s="47"/>
+      <c r="F44" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="G44" s="36"/>
-      <c r="J44" s="36" t="s">
+      <c r="G44" s="47"/>
+      <c r="J44" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K44" s="36"/>
-      <c r="L44" s="36" t="s">
+      <c r="K44" s="47"/>
+      <c r="L44" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="M44" s="36"/>
-      <c r="N44" s="36" t="s">
+      <c r="M44" s="47"/>
+      <c r="N44" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="O44" s="36"/>
+      <c r="O44" s="47"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -8848,41 +8865,41 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="I50" s="36" t="s">
+      <c r="A50" s="46"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="I50" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="J50" s="36"/>
-      <c r="K50" s="36"/>
-      <c r="L50" s="36"/>
-      <c r="M50" s="36"/>
-      <c r="N50" s="36"/>
-      <c r="O50" s="36"/>
+      <c r="J50" s="47"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="47"/>
+      <c r="M50" s="47"/>
+      <c r="N50" s="47"/>
+      <c r="O50" s="47"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="J51" s="36" t="s">
+      <c r="B51" s="47"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="47"/>
+      <c r="J51" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K51" s="36"/>
-      <c r="L51" s="36" t="s">
+      <c r="K51" s="47"/>
+      <c r="L51" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="M51" s="36"/>
-      <c r="N51" s="36" t="s">
+      <c r="M51" s="47"/>
+      <c r="N51" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="O51" s="36"/>
+      <c r="O51" s="47"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J52" t="s">
@@ -10527,8 +10544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10595,40 +10612,40 @@
       <c r="T1" s="34"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="E2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="39">
         <v>40</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="40" t="s">
         <v>204</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="41" t="s">
         <v>34</v>
       </c>
       <c r="M2" s="31"/>
@@ -10659,7 +10676,7 @@
       <c r="F3" s="13">
         <v>40</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="35" t="s">
         <v>205</v>
       </c>
       <c r="H3" s="32" t="s">
@@ -10705,7 +10722,7 @@
       <c r="F4" s="13">
         <v>40</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="35" t="s">
         <v>206</v>
       </c>
       <c r="H4" s="32" t="s">
@@ -10733,40 +10750,40 @@
       <c r="T4" s="31"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="13">
+      <c r="C5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="17">
         <v>40</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="32" t="s">
+      <c r="K5" s="37" t="s">
         <v>689</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="37" t="s">
         <v>34</v>
       </c>
       <c r="M5" s="31"/>
@@ -10779,40 +10796,40 @@
       <c r="T5" s="31"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="13">
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="39">
         <v>40</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="40" t="s">
         <v>208</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="32" t="s">
+      <c r="K6" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="L6" s="32" t="s">
+      <c r="L6" s="41" t="s">
         <v>34</v>
       </c>
       <c r="M6" s="31"/>
@@ -10843,7 +10860,7 @@
       <c r="F7" s="13">
         <v>40</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="35" t="s">
         <v>209</v>
       </c>
       <c r="H7" s="32" t="s">
@@ -10889,7 +10906,7 @@
       <c r="F8" s="13">
         <v>40</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="35" t="s">
         <v>210</v>
       </c>
       <c r="H8" s="32" t="s">
@@ -10917,40 +10934,40 @@
       <c r="T8" s="31"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="13">
+      <c r="C9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="17">
         <v>40</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="37" t="s">
         <v>689</v>
       </c>
-      <c r="L9" s="32" t="s">
+      <c r="L9" s="37" t="s">
         <v>34</v>
       </c>
       <c r="M9" s="31"/>
@@ -10963,40 +10980,40 @@
       <c r="T9" s="31"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="13">
+      <c r="E10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="39">
         <v>60</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="40" t="s">
         <v>212</v>
       </c>
-      <c r="H10" s="31">
+      <c r="H10" s="42">
         <v>11</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="41">
         <v>4580</v>
       </c>
-      <c r="J10" s="32">
-        <v>2506.64</v>
-      </c>
-      <c r="K10" s="32" t="s">
+      <c r="J10" s="41">
+        <v>2506.06</v>
+      </c>
+      <c r="K10" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="L10" s="32" t="s">
+      <c r="L10" s="41" t="s">
         <v>689</v>
       </c>
       <c r="M10" s="31"/>
@@ -11027,22 +11044,24 @@
       <c r="F11" s="13">
         <v>60</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="35" t="s">
         <v>213</v>
       </c>
       <c r="H11" s="32">
         <v>12</v>
       </c>
       <c r="I11" s="32">
-        <v>4535</v>
+        <v>4553</v>
       </c>
       <c r="J11" s="32">
-        <v>2561.44</v>
+        <v>2588.81</v>
       </c>
       <c r="K11" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L11" s="31"/>
+      <c r="L11" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M11" s="32"/>
       <c r="N11" s="32"/>
       <c r="O11" s="32"/>
@@ -11071,7 +11090,7 @@
       <c r="F12" s="13">
         <v>60</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="35" t="s">
         <v>214</v>
       </c>
       <c r="H12" s="32">
@@ -11086,7 +11105,9 @@
       <c r="K12" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L12" s="31"/>
+      <c r="L12" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M12" s="32"/>
       <c r="N12" s="32"/>
       <c r="O12" s="32"/>
@@ -11097,40 +11118,42 @@
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="13">
+      <c r="C13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="17">
         <v>60</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="37">
         <v>13</v>
       </c>
-      <c r="I13" s="32">
-        <v>4629</v>
-      </c>
-      <c r="J13" s="32">
-        <v>2601.96</v>
-      </c>
-      <c r="K13" s="32" t="s">
+      <c r="I13" s="37">
+        <v>4407</v>
+      </c>
+      <c r="J13" s="37">
+        <v>2430.5700000000002</v>
+      </c>
+      <c r="K13" s="37" t="s">
         <v>689</v>
       </c>
-      <c r="L13" s="31"/>
+      <c r="L13" s="36" t="s">
+        <v>689</v>
+      </c>
       <c r="M13" s="31"/>
       <c r="N13" s="31"/>
       <c r="O13" s="31"/>
@@ -11141,40 +11164,40 @@
       <c r="T13" s="31"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="13">
+      <c r="E14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="39">
         <v>60</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="H14" s="32" t="s">
+      <c r="H14" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="32" t="s">
+      <c r="I14" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="32" t="s">
+      <c r="K14" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="L14" s="32" t="s">
+      <c r="L14" s="41" t="s">
         <v>34</v>
       </c>
       <c r="M14" s="31"/>
@@ -11205,22 +11228,24 @@
       <c r="F15" s="13">
         <v>60</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="35" t="s">
         <v>217</v>
       </c>
       <c r="H15" s="32">
         <v>9</v>
       </c>
       <c r="I15" s="32">
-        <v>3952</v>
+        <v>3968</v>
       </c>
       <c r="J15" s="32">
-        <v>2105.7199999999998</v>
+        <v>2120.6799999999998</v>
       </c>
       <c r="K15" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L15" s="31"/>
+      <c r="L15" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M15" s="32"/>
       <c r="N15" s="32"/>
       <c r="O15" s="32"/>
@@ -11249,7 +11274,7 @@
       <c r="F16" s="13">
         <v>60</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="35" t="s">
         <v>218</v>
       </c>
       <c r="H16" s="32">
@@ -11264,7 +11289,9 @@
       <c r="K16" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L16" s="31"/>
+      <c r="L16" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M16" s="32"/>
       <c r="N16" s="32"/>
       <c r="O16" s="32"/>
@@ -11275,40 +11302,42 @@
       <c r="T16" s="31"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="13">
+      <c r="C17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="17">
         <v>60</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="37">
         <v>10</v>
       </c>
-      <c r="I17" s="32">
-        <v>4183</v>
-      </c>
-      <c r="J17" s="32">
-        <v>2247.3200000000002</v>
-      </c>
-      <c r="K17" s="32" t="s">
+      <c r="I17" s="37">
+        <v>4254</v>
+      </c>
+      <c r="J17" s="37">
+        <v>2321.21</v>
+      </c>
+      <c r="K17" s="37" t="s">
         <v>689</v>
       </c>
-      <c r="L17" s="31"/>
+      <c r="L17" s="36" t="s">
+        <v>689</v>
+      </c>
       <c r="M17" s="31"/>
       <c r="N17" s="31"/>
       <c r="O17" s="31"/>
@@ -11319,40 +11348,40 @@
       <c r="T17" s="31"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="39" t="s">
         <v>187</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="C18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="13">
+      <c r="E18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="39">
         <v>200</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="41">
         <v>9</v>
       </c>
-      <c r="I18" s="32">
+      <c r="I18" s="41">
         <v>4102</v>
       </c>
-      <c r="J18" s="32">
+      <c r="J18" s="41">
         <v>2177.8000000000002</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="K18" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="L18" s="32" t="s">
+      <c r="L18" s="41" t="s">
         <v>689</v>
       </c>
       <c r="M18" s="32"/>
@@ -11383,22 +11412,24 @@
       <c r="F19" s="13">
         <v>200</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="35" t="s">
         <v>221</v>
       </c>
       <c r="H19" s="32">
         <v>10</v>
       </c>
       <c r="I19" s="32">
-        <v>4117</v>
+        <v>4349</v>
       </c>
       <c r="J19" s="32">
-        <v>2203.42</v>
+        <v>2289.35</v>
       </c>
       <c r="K19" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L19" s="32"/>
+      <c r="L19" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M19" s="32"/>
       <c r="N19" s="32"/>
       <c r="O19" s="32"/>
@@ -11427,22 +11458,24 @@
       <c r="F20" s="13">
         <v>200</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="G20" s="35" t="s">
         <v>222</v>
       </c>
       <c r="H20" s="32">
         <v>11</v>
       </c>
       <c r="I20" s="32">
-        <v>4146</v>
+        <v>4137</v>
       </c>
       <c r="J20" s="32">
-        <v>2197.42</v>
+        <v>2197.91</v>
       </c>
       <c r="K20" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L20" s="32"/>
+      <c r="L20" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M20" s="32"/>
       <c r="N20" s="32"/>
       <c r="O20" s="32"/>
@@ -11453,40 +11486,42 @@
       <c r="T20" s="32"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="13">
+      <c r="C21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="17">
         <v>200</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="37">
         <v>11</v>
       </c>
-      <c r="I21" s="32">
-        <v>4345</v>
-      </c>
-      <c r="J21" s="32">
-        <v>2378.52</v>
-      </c>
-      <c r="K21" s="32" t="s">
+      <c r="I21" s="37">
+        <v>4296</v>
+      </c>
+      <c r="J21" s="37">
+        <v>2373.54</v>
+      </c>
+      <c r="K21" s="37" t="s">
         <v>689</v>
       </c>
-      <c r="L21" s="32"/>
+      <c r="L21" s="37" t="s">
+        <v>689</v>
+      </c>
       <c r="M21" s="32"/>
       <c r="N21" s="32"/>
       <c r="O21" s="32"/>
@@ -11497,40 +11532,40 @@
       <c r="T21" s="32"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="C22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="13">
+      <c r="E22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="39">
         <v>200</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="40" t="s">
         <v>224</v>
       </c>
-      <c r="H22" s="32" t="s">
+      <c r="H22" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="I22" s="32" t="s">
+      <c r="I22" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="J22" s="32" t="s">
+      <c r="J22" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="K22" s="32" t="s">
+      <c r="K22" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="L22" s="32" t="s">
+      <c r="L22" s="41" t="s">
         <v>34</v>
       </c>
       <c r="M22" s="32"/>
@@ -11561,22 +11596,24 @@
       <c r="F23" s="13">
         <v>200</v>
       </c>
-      <c r="G23" s="32" t="s">
+      <c r="G23" s="35" t="s">
         <v>225</v>
       </c>
       <c r="H23" s="32">
         <v>7</v>
       </c>
       <c r="I23" s="32">
-        <v>3546</v>
+        <v>3619</v>
       </c>
       <c r="J23" s="32">
-        <v>1767.57</v>
+        <v>1798.09</v>
       </c>
       <c r="K23" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L23" s="32"/>
+      <c r="L23" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M23" s="32"/>
       <c r="N23" s="32"/>
       <c r="O23" s="32"/>
@@ -11605,22 +11642,24 @@
       <c r="F24" s="13">
         <v>200</v>
       </c>
-      <c r="G24" s="32" t="s">
+      <c r="G24" s="35" t="s">
         <v>226</v>
       </c>
       <c r="H24" s="32">
         <v>7</v>
       </c>
       <c r="I24" s="32">
-        <v>3699</v>
+        <v>3660</v>
       </c>
       <c r="J24" s="32">
-        <v>1832.26</v>
+        <v>1832.91</v>
       </c>
       <c r="K24" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L24" s="32"/>
+      <c r="L24" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M24" s="32"/>
       <c r="N24" s="32"/>
       <c r="O24" s="32"/>
@@ -11631,40 +11670,42 @@
       <c r="T24" s="32"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="13">
+      <c r="C25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="17">
         <v>200</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G25" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="37">
         <v>8</v>
       </c>
-      <c r="I25" s="32">
-        <v>3945</v>
-      </c>
-      <c r="J25" s="32">
-        <v>2058.4299999999998</v>
-      </c>
-      <c r="K25" s="32" t="s">
+      <c r="I25" s="37">
+        <v>3948</v>
+      </c>
+      <c r="J25" s="37">
+        <v>2037.85</v>
+      </c>
+      <c r="K25" s="37" t="s">
         <v>689</v>
       </c>
-      <c r="L25" s="32"/>
+      <c r="L25" s="37" t="s">
+        <v>689</v>
+      </c>
       <c r="M25" s="32"/>
       <c r="N25" s="32"/>
       <c r="O25" s="32"/>
@@ -11675,40 +11716,40 @@
       <c r="T25" s="32"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="C26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="14">
+      <c r="E26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="43">
         <v>0</v>
       </c>
-      <c r="G26" s="32" t="s">
+      <c r="G26" s="40" t="s">
         <v>228</v>
       </c>
-      <c r="H26" s="32">
+      <c r="H26" s="41">
         <v>9</v>
       </c>
-      <c r="I26" s="32">
+      <c r="I26" s="41">
         <v>4102</v>
       </c>
-      <c r="J26" s="32">
+      <c r="J26" s="41">
         <v>2177.8000000000002</v>
       </c>
-      <c r="K26" s="32" t="s">
+      <c r="K26" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="L26" s="32" t="s">
+      <c r="L26" s="41" t="s">
         <v>689</v>
       </c>
       <c r="M26" s="32"/>
@@ -11739,22 +11780,24 @@
       <c r="F27" s="14">
         <v>0</v>
       </c>
-      <c r="G27" s="31" t="s">
+      <c r="G27" s="35" t="s">
         <v>229</v>
       </c>
       <c r="H27" s="32">
         <v>10</v>
       </c>
       <c r="I27" s="32">
-        <v>4117</v>
+        <v>4282</v>
       </c>
       <c r="J27" s="32">
-        <v>2203.42</v>
+        <v>2260.87</v>
       </c>
       <c r="K27" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L27" s="31"/>
+      <c r="L27" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M27" s="32"/>
       <c r="N27" s="32"/>
       <c r="O27" s="32"/>
@@ -11783,7 +11826,7 @@
       <c r="F28" s="14">
         <v>0</v>
       </c>
-      <c r="G28" s="31" t="s">
+      <c r="G28" s="35" t="s">
         <v>230</v>
       </c>
       <c r="H28" s="32">
@@ -11798,7 +11841,9 @@
       <c r="K28" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L28" s="31"/>
+      <c r="L28" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M28" s="32"/>
       <c r="N28" s="32"/>
       <c r="O28" s="32"/>
@@ -11809,40 +11854,42 @@
       <c r="T28" s="31"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="14">
+      <c r="C29" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="20">
         <v>0</v>
       </c>
-      <c r="G29" s="31" t="s">
+      <c r="G29" s="45" t="s">
         <v>231</v>
       </c>
-      <c r="H29" s="32">
+      <c r="H29" s="37">
         <v>11</v>
       </c>
-      <c r="I29" s="32">
-        <v>4345</v>
-      </c>
-      <c r="J29" s="32">
-        <v>2378.52</v>
-      </c>
-      <c r="K29" s="32" t="s">
+      <c r="I29" s="37">
+        <v>4323</v>
+      </c>
+      <c r="J29" s="37">
+        <v>2367.27</v>
+      </c>
+      <c r="K29" s="37" t="s">
         <v>689</v>
       </c>
-      <c r="L29" s="31"/>
+      <c r="L29" s="36" t="s">
+        <v>689</v>
+      </c>
       <c r="M29" s="31"/>
       <c r="N29" s="31"/>
       <c r="O29" s="31"/>
@@ -11853,40 +11900,40 @@
       <c r="T29" s="31"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="C30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="14">
+      <c r="E30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="43">
         <v>0</v>
       </c>
-      <c r="G30" s="32" t="s">
+      <c r="G30" s="40" t="s">
         <v>232</v>
       </c>
-      <c r="H30" s="32" t="s">
+      <c r="H30" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="32" t="s">
+      <c r="I30" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="J30" s="32" t="s">
+      <c r="J30" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="K30" s="32" t="s">
+      <c r="K30" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="L30" s="32" t="s">
+      <c r="L30" s="41" t="s">
         <v>34</v>
       </c>
       <c r="M30" s="32"/>
@@ -11917,7 +11964,7 @@
       <c r="F31" s="14">
         <v>0</v>
       </c>
-      <c r="G31" s="31" t="s">
+      <c r="G31" s="35" t="s">
         <v>233</v>
       </c>
       <c r="H31" s="32">
@@ -11932,7 +11979,9 @@
       <c r="K31" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L31" s="31"/>
+      <c r="L31" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M31" s="32"/>
       <c r="N31" s="32"/>
       <c r="O31" s="32"/>
@@ -11961,22 +12010,24 @@
       <c r="F32" s="14">
         <v>0</v>
       </c>
-      <c r="G32" s="32" t="s">
+      <c r="G32" s="35" t="s">
         <v>234</v>
       </c>
       <c r="H32" s="32">
         <v>7</v>
       </c>
       <c r="I32" s="32">
-        <v>3660</v>
+        <v>3688</v>
       </c>
       <c r="J32" s="32">
-        <v>1832.91</v>
+        <v>1832.05</v>
       </c>
       <c r="K32" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L32" s="31"/>
+      <c r="L32" s="32" t="s">
+        <v>689</v>
+      </c>
       <c r="M32" s="32"/>
       <c r="N32" s="32"/>
       <c r="O32" s="32"/>
@@ -11987,40 +12038,42 @@
       <c r="T32" s="31"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="14">
+      <c r="C33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="20">
         <v>0</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="45" t="s">
         <v>678</v>
       </c>
-      <c r="H33" s="32">
+      <c r="H33" s="37">
         <v>8</v>
       </c>
-      <c r="I33" s="32">
-        <v>3974</v>
-      </c>
-      <c r="J33" s="32">
-        <v>2061.06</v>
-      </c>
-      <c r="K33" s="32" t="s">
+      <c r="I33" s="37">
+        <v>3930</v>
+      </c>
+      <c r="J33" s="37">
+        <v>2026.88</v>
+      </c>
+      <c r="K33" s="37" t="s">
         <v>689</v>
       </c>
-      <c r="L33" s="31"/>
+      <c r="L33" s="36" t="s">
+        <v>689</v>
+      </c>
       <c r="M33" s="31"/>
       <c r="N33" s="31"/>
       <c r="O33" s="31"/>
@@ -12031,37 +12084,40 @@
       <c r="T33" s="31"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="6" t="s">
+      <c r="C34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F34" s="13">
+      <c r="E34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="39">
         <v>40</v>
       </c>
-      <c r="G34" s="30" t="s">
+      <c r="G34" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="H34" s="32">
+      <c r="H34" s="41">
         <v>10</v>
       </c>
-      <c r="I34" s="32">
+      <c r="I34" s="41">
         <v>3604</v>
       </c>
-      <c r="J34" s="32">
+      <c r="J34" s="41">
         <v>2084.15</v>
       </c>
-      <c r="K34" s="32" t="s">
+      <c r="K34" s="41" t="s">
+        <v>689</v>
+      </c>
+      <c r="L34" s="42" t="s">
         <v>689</v>
       </c>
     </row>
@@ -12084,7 +12140,7 @@
       <c r="F35" s="13">
         <v>40</v>
       </c>
-      <c r="G35" s="30" t="s">
+      <c r="G35" s="35" t="s">
         <v>237</v>
       </c>
       <c r="H35" s="32">
@@ -12097,6 +12153,9 @@
         <v>1955.08</v>
       </c>
       <c r="K35" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L35" s="32" t="s">
         <v>689</v>
       </c>
     </row>
@@ -12119,7 +12178,7 @@
       <c r="F36" s="13">
         <v>40</v>
       </c>
-      <c r="G36" s="30" t="s">
+      <c r="G36" s="35" t="s">
         <v>238</v>
       </c>
       <c r="H36" s="32">
@@ -12134,77 +12193,83 @@
       <c r="K36" s="32" t="s">
         <v>689</v>
       </c>
+      <c r="L36" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F37" s="13">
+      <c r="C37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="17">
         <v>40</v>
       </c>
-      <c r="G37" s="30" t="s">
+      <c r="G37" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="H37" s="32">
+      <c r="H37" s="37">
         <v>11</v>
       </c>
-      <c r="I37" s="32">
+      <c r="I37" s="37">
         <v>3429</v>
       </c>
-      <c r="J37" s="32">
+      <c r="J37" s="37">
         <v>2083.9699999999998</v>
       </c>
-      <c r="K37" s="32" t="s">
+      <c r="K37" s="37" t="s">
         <v>689</v>
       </c>
+      <c r="L37" s="36" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="6" t="s">
+      <c r="C38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F38" s="13">
+      <c r="E38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="39">
         <v>40</v>
       </c>
-      <c r="G38" s="30" t="s">
+      <c r="G38" s="42" t="s">
         <v>240</v>
       </c>
-      <c r="H38" s="30" t="s">
+      <c r="H38" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="I38" s="30" t="s">
+      <c r="I38" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="J38" s="30" t="s">
+      <c r="J38" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="K38" s="32" t="s">
+      <c r="K38" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="L38" s="30" t="s">
+      <c r="L38" s="42" t="s">
         <v>34</v>
       </c>
     </row>
@@ -12227,21 +12292,22 @@
       <c r="F39" s="13">
         <v>40</v>
       </c>
-      <c r="G39" s="30" t="s">
+      <c r="G39" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="H39" s="30">
+      <c r="H39" s="31">
         <v>10</v>
       </c>
-      <c r="I39" s="30">
+      <c r="I39" s="31">
         <v>3564</v>
       </c>
-      <c r="J39" s="30">
+      <c r="J39" s="31">
         <v>2023.52</v>
       </c>
       <c r="K39" s="32" t="s">
         <v>689</v>
       </c>
+      <c r="L39" s="31"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
@@ -12262,91 +12328,94 @@
       <c r="F40" s="13">
         <v>40</v>
       </c>
-      <c r="G40" s="30" t="s">
+      <c r="G40" s="31" t="s">
         <v>242</v>
       </c>
-      <c r="H40" s="30">
+      <c r="H40" s="31">
         <v>10</v>
       </c>
-      <c r="I40" s="30">
+      <c r="I40" s="31">
         <v>3247</v>
       </c>
-      <c r="J40" s="30">
+      <c r="J40" s="31">
         <v>1842.37</v>
       </c>
       <c r="K40" s="32" t="s">
         <v>689</v>
       </c>
+      <c r="L40" s="31"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F41" s="13">
+      <c r="C41" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="17">
         <v>40</v>
       </c>
-      <c r="G41" s="30" t="s">
+      <c r="G41" s="36" t="s">
         <v>243</v>
       </c>
-      <c r="H41" s="30">
+      <c r="H41" s="36">
         <v>10</v>
       </c>
-      <c r="I41" s="30">
+      <c r="I41" s="36">
         <v>3549</v>
       </c>
-      <c r="J41" s="30">
+      <c r="J41" s="36">
         <v>2032.15</v>
       </c>
-      <c r="K41" s="32" t="s">
+      <c r="K41" s="37" t="s">
         <v>689</v>
       </c>
+      <c r="L41" s="36"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="6" t="s">
+      <c r="C42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F42" s="13">
+      <c r="E42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="39">
         <v>60</v>
       </c>
-      <c r="G42" s="30" t="s">
+      <c r="G42" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="H42" s="30">
+      <c r="H42" s="42">
         <v>7</v>
       </c>
-      <c r="I42" s="30">
+      <c r="I42" s="42">
         <v>2904</v>
       </c>
-      <c r="J42" s="30">
+      <c r="J42" s="42">
         <v>1525.86</v>
       </c>
-      <c r="K42" s="32" t="s">
+      <c r="K42" s="41" t="s">
         <v>689</v>
       </c>
+      <c r="L42" s="42"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
@@ -12367,21 +12436,22 @@
       <c r="F43" s="13">
         <v>60</v>
       </c>
-      <c r="G43" s="30" t="s">
+      <c r="G43" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="H43" s="30">
+      <c r="H43" s="31">
         <v>8</v>
       </c>
-      <c r="I43" s="30">
+      <c r="I43" s="31">
         <v>3210</v>
       </c>
-      <c r="J43" s="30">
+      <c r="J43" s="31">
         <v>1752.01</v>
       </c>
       <c r="K43" s="32" t="s">
         <v>689</v>
       </c>
+      <c r="L43" s="31"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
@@ -12402,91 +12472,94 @@
       <c r="F44" s="13">
         <v>60</v>
       </c>
-      <c r="G44" s="30" t="s">
+      <c r="G44" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="H44" s="30">
+      <c r="H44" s="31">
         <v>9</v>
       </c>
-      <c r="I44" s="30">
+      <c r="I44" s="31">
         <v>3173</v>
       </c>
-      <c r="J44" s="30">
+      <c r="J44" s="31">
         <v>1690.28</v>
       </c>
       <c r="K44" s="32" t="s">
         <v>689</v>
       </c>
+      <c r="L44" s="31"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="13">
+      <c r="C45" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="17">
         <v>60</v>
       </c>
-      <c r="G45" s="30" t="s">
+      <c r="G45" s="36" t="s">
         <v>247</v>
       </c>
-      <c r="H45" s="30">
+      <c r="H45" s="36">
         <v>8</v>
       </c>
-      <c r="I45" s="30">
+      <c r="I45" s="36">
         <v>3154</v>
       </c>
-      <c r="J45" s="30">
+      <c r="J45" s="36">
         <v>1683.56</v>
       </c>
-      <c r="K45" s="32" t="s">
+      <c r="K45" s="37" t="s">
         <v>689</v>
       </c>
+      <c r="L45" s="36"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="6" t="s">
+      <c r="C46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F46" s="13">
+      <c r="E46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="39">
         <v>60</v>
       </c>
-      <c r="G46" s="30" t="s">
+      <c r="G46" s="42" t="s">
         <v>248</v>
       </c>
-      <c r="H46" s="30">
+      <c r="H46" s="42">
         <v>6</v>
       </c>
-      <c r="I46" s="30">
+      <c r="I46" s="42">
         <v>2977</v>
       </c>
-      <c r="J46" s="30">
+      <c r="J46" s="42">
         <v>1569.43</v>
       </c>
-      <c r="K46" s="32" t="s">
+      <c r="K46" s="41" t="s">
         <v>689</v>
       </c>
+      <c r="L46" s="42"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="s">
@@ -12507,21 +12580,22 @@
       <c r="F47" s="13">
         <v>60</v>
       </c>
-      <c r="G47" s="30" t="s">
+      <c r="G47" s="31" t="s">
         <v>249</v>
       </c>
-      <c r="H47" s="30">
+      <c r="H47" s="31">
         <v>6</v>
       </c>
-      <c r="I47" s="30">
+      <c r="I47" s="31">
         <v>2890</v>
       </c>
-      <c r="J47" s="30">
+      <c r="J47" s="31">
         <v>1501.44</v>
       </c>
       <c r="K47" s="32" t="s">
         <v>689</v>
       </c>
+      <c r="L47" s="31"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
@@ -12542,93 +12616,96 @@
       <c r="F48" s="13">
         <v>60</v>
       </c>
-      <c r="G48" s="30" t="s">
+      <c r="G48" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="H48" s="30">
+      <c r="H48" s="31">
         <v>7</v>
       </c>
-      <c r="I48" s="30">
+      <c r="I48" s="31">
         <v>3017</v>
       </c>
-      <c r="J48" s="30">
+      <c r="J48" s="31">
         <v>1594.69</v>
       </c>
       <c r="K48" s="32" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="29" t="s">
+      <c r="L48" s="31"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F49" s="13">
+      <c r="C49" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="17">
         <v>60</v>
       </c>
-      <c r="G49" s="30" t="s">
+      <c r="G49" s="36" t="s">
         <v>251</v>
       </c>
-      <c r="H49" s="30">
+      <c r="H49" s="36">
         <v>6</v>
       </c>
-      <c r="I49" s="30">
+      <c r="I49" s="36">
         <v>2846</v>
       </c>
-      <c r="J49" s="30">
+      <c r="J49" s="36">
         <v>1493.35</v>
       </c>
-      <c r="K49" s="32" t="s">
+      <c r="K49" s="37" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="L49" s="36"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="39" t="s">
         <v>187</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50" s="6" t="s">
+      <c r="C50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E50" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F50" s="13">
+      <c r="E50" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" s="39">
         <v>200</v>
       </c>
-      <c r="G50" s="30" t="s">
+      <c r="G50" s="42" t="s">
         <v>252</v>
       </c>
-      <c r="H50" s="30">
+      <c r="H50" s="42">
         <v>7</v>
       </c>
-      <c r="I50" s="30">
+      <c r="I50" s="42">
         <v>2809</v>
       </c>
-      <c r="J50" s="30">
+      <c r="J50" s="42">
         <v>1479.11</v>
       </c>
-      <c r="K50" s="32" t="s">
+      <c r="K50" s="41" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" s="42"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
         <v>19</v>
       </c>
@@ -12647,23 +12724,24 @@
       <c r="F51" s="13">
         <v>200</v>
       </c>
-      <c r="G51" s="30" t="s">
+      <c r="G51" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="H51" s="30">
+      <c r="H51" s="31">
         <v>7</v>
       </c>
-      <c r="I51" s="30">
+      <c r="I51" s="31">
         <v>2987</v>
       </c>
-      <c r="J51" s="30">
+      <c r="J51" s="31">
         <v>1552.52</v>
       </c>
       <c r="K51" s="32" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" s="31"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="29" t="s">
         <v>19</v>
       </c>
@@ -12682,93 +12760,96 @@
       <c r="F52" s="13">
         <v>200</v>
       </c>
-      <c r="G52" s="30" t="s">
+      <c r="G52" s="31" t="s">
         <v>254</v>
       </c>
-      <c r="H52" s="30">
+      <c r="H52" s="31">
         <v>8</v>
       </c>
-      <c r="I52" s="30">
+      <c r="I52" s="31">
         <v>3365</v>
       </c>
-      <c r="J52" s="30">
+      <c r="J52" s="31">
         <v>1835.07</v>
       </c>
       <c r="K52" s="32" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="29" t="s">
+      <c r="L52" s="31"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="C53" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F53" s="13">
+      <c r="C53" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F53" s="17">
         <v>200</v>
       </c>
-      <c r="G53" s="30" t="s">
+      <c r="G53" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="H53" s="30">
+      <c r="H53" s="36">
         <v>8</v>
       </c>
-      <c r="I53" s="30">
+      <c r="I53" s="36">
         <v>3195</v>
       </c>
-      <c r="J53" s="30">
+      <c r="J53" s="36">
         <v>1717.42</v>
       </c>
-      <c r="K53" s="32" t="s">
+      <c r="K53" s="37" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="29" t="s">
+      <c r="L53" s="36"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="C54" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" s="6" t="s">
+      <c r="C54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F54" s="13">
+      <c r="E54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F54" s="39">
         <v>200</v>
       </c>
-      <c r="G54" s="30" t="s">
+      <c r="G54" s="42" t="s">
         <v>256</v>
       </c>
-      <c r="H54" s="30">
+      <c r="H54" s="42">
         <v>5</v>
       </c>
-      <c r="I54" s="30">
+      <c r="I54" s="42">
         <v>2749</v>
       </c>
-      <c r="J54" s="30">
+      <c r="J54" s="42">
         <v>1410.65</v>
       </c>
-      <c r="K54" s="32" t="s">
+      <c r="K54" s="41" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54" s="42"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="29" t="s">
         <v>19</v>
       </c>
@@ -12787,23 +12868,24 @@
       <c r="F55" s="13">
         <v>200</v>
       </c>
-      <c r="G55" s="30" t="s">
+      <c r="G55" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="H55" s="30">
+      <c r="H55" s="31">
         <v>6</v>
       </c>
-      <c r="I55" s="30">
+      <c r="I55" s="31">
         <v>2875</v>
       </c>
-      <c r="J55" s="30">
+      <c r="J55" s="31">
         <v>1522.64</v>
       </c>
       <c r="K55" s="32" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55" s="31"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
         <v>19</v>
       </c>
@@ -12822,93 +12904,96 @@
       <c r="F56" s="13">
         <v>200</v>
       </c>
-      <c r="G56" s="30" t="s">
+      <c r="G56" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="H56" s="30">
+      <c r="H56" s="31">
         <v>6</v>
       </c>
-      <c r="I56" s="30">
+      <c r="I56" s="31">
         <v>2952</v>
       </c>
-      <c r="J56" s="30">
+      <c r="J56" s="31">
         <v>1558.32</v>
       </c>
       <c r="K56" s="32" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="29" t="s">
+      <c r="L56" s="31"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F57" s="13">
+      <c r="C57" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" s="17">
         <v>200</v>
       </c>
-      <c r="G57" s="30" t="s">
+      <c r="G57" s="36" t="s">
         <v>259</v>
       </c>
-      <c r="H57" s="30">
+      <c r="H57" s="36">
         <v>6</v>
       </c>
-      <c r="I57" s="30">
+      <c r="I57" s="36">
         <v>2871</v>
       </c>
-      <c r="J57" s="30">
+      <c r="J57" s="36">
         <v>1496.98</v>
       </c>
-      <c r="K57" s="32" t="s">
+      <c r="K57" s="37" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="29" t="s">
+      <c r="L57" s="36"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="C58" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D58" s="6" t="s">
+      <c r="C58" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F58" s="14">
+      <c r="E58" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F58" s="43">
         <v>0</v>
       </c>
-      <c r="G58" s="30" t="s">
+      <c r="G58" s="42" t="s">
         <v>260</v>
       </c>
-      <c r="H58" s="30">
+      <c r="H58" s="42">
         <v>7</v>
       </c>
-      <c r="I58" s="30">
+      <c r="I58" s="42">
         <v>2809</v>
       </c>
-      <c r="J58" s="30">
+      <c r="J58" s="42">
         <v>1479.11</v>
       </c>
-      <c r="K58" s="32" t="s">
+      <c r="K58" s="41" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58" s="42"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="29" t="s">
         <v>19</v>
       </c>
@@ -12927,23 +13012,24 @@
       <c r="F59" s="14">
         <v>0</v>
       </c>
-      <c r="G59" s="30" t="s">
+      <c r="G59" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="H59" s="30">
+      <c r="H59" s="31">
         <v>7</v>
       </c>
-      <c r="I59" s="30">
+      <c r="I59" s="31">
         <v>2987</v>
       </c>
-      <c r="J59" s="30">
+      <c r="J59" s="31">
         <v>1552.52</v>
       </c>
-      <c r="K59" s="30" t="s">
+      <c r="K59" s="31" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" s="31"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="29" t="s">
         <v>19</v>
       </c>
@@ -12962,93 +13048,96 @@
       <c r="F60" s="14">
         <v>0</v>
       </c>
-      <c r="G60" s="30" t="s">
+      <c r="G60" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="H60" s="30">
+      <c r="H60" s="31">
         <v>8</v>
       </c>
-      <c r="I60" s="30">
+      <c r="I60" s="31">
         <v>3365</v>
       </c>
-      <c r="J60" s="30">
+      <c r="J60" s="31">
         <v>1835.07</v>
       </c>
-      <c r="K60" s="30" t="s">
+      <c r="K60" s="31" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="s">
+      <c r="L60" s="31"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="C61" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F61" s="14">
+      <c r="C61" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" s="20">
         <v>0</v>
       </c>
-      <c r="G61" s="30" t="s">
+      <c r="G61" s="36" t="s">
         <v>263</v>
       </c>
-      <c r="H61" s="30">
+      <c r="H61" s="36">
         <v>8</v>
       </c>
-      <c r="I61" s="30">
+      <c r="I61" s="36">
         <v>3195</v>
       </c>
-      <c r="J61" s="30">
+      <c r="J61" s="36">
         <v>1717.42</v>
       </c>
-      <c r="K61" s="30" t="s">
+      <c r="K61" s="36" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="29" t="s">
+      <c r="L61" s="36"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="C62" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D62" s="6" t="s">
+      <c r="C62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F62" s="14">
+      <c r="E62" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F62" s="43">
         <v>0</v>
       </c>
-      <c r="G62" s="30" t="s">
+      <c r="G62" s="42" t="s">
         <v>264</v>
       </c>
-      <c r="H62" s="30">
+      <c r="H62" s="42">
         <v>5</v>
       </c>
-      <c r="I62" s="30">
+      <c r="I62" s="42">
         <v>2749</v>
       </c>
-      <c r="J62" s="30">
+      <c r="J62" s="42">
         <v>1410.65</v>
       </c>
-      <c r="K62" s="30" t="s">
+      <c r="K62" s="42" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62" s="42"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="29" t="s">
         <v>19</v>
       </c>
@@ -13067,23 +13156,24 @@
       <c r="F63" s="14">
         <v>0</v>
       </c>
-      <c r="G63" s="30" t="s">
+      <c r="G63" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="H63" s="30">
+      <c r="H63" s="31">
         <v>6</v>
       </c>
-      <c r="I63" s="30">
+      <c r="I63" s="31">
         <v>2875</v>
       </c>
-      <c r="J63" s="30">
+      <c r="J63" s="31">
         <v>1522.64</v>
       </c>
-      <c r="K63" s="30" t="s">
+      <c r="K63" s="31" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63" s="31"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="29" t="s">
         <v>19</v>
       </c>
@@ -13102,56 +13192,58 @@
       <c r="F64" s="14">
         <v>0</v>
       </c>
-      <c r="G64" s="30" t="s">
+      <c r="G64" s="31" t="s">
         <v>266</v>
       </c>
-      <c r="H64" s="30">
+      <c r="H64" s="31">
         <v>6</v>
       </c>
-      <c r="I64" s="30">
+      <c r="I64" s="31">
         <v>2952</v>
       </c>
-      <c r="J64" s="30">
+      <c r="J64" s="31">
         <v>1558.32</v>
       </c>
-      <c r="K64" s="30" t="s">
+      <c r="K64" s="31" t="s">
         <v>689</v>
       </c>
+      <c r="L64" s="31"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="29" t="s">
+      <c r="A65" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="C65" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F65" s="14">
+      <c r="C65" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F65" s="20">
         <v>0</v>
       </c>
-      <c r="G65" s="30" t="s">
+      <c r="G65" s="36" t="s">
         <v>235</v>
       </c>
-      <c r="H65" s="30">
+      <c r="H65" s="36">
         <v>6</v>
       </c>
-      <c r="I65" s="30">
+      <c r="I65" s="36">
         <v>2871</v>
       </c>
-      <c r="J65" s="30">
+      <c r="J65" s="36">
         <v>1496.98</v>
       </c>
-      <c r="K65" s="30" t="s">
+      <c r="K65" s="36" t="s">
         <v>689</v>
       </c>
+      <c r="L65" s="36"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="29" t="s">

</xml_diff>

<commit_message>
model results for ideal region 3
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4126" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4205" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -2123,18 +2123,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -2253,7 +2247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2283,17 +2277,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6894,50 +6885,50 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="I1" s="39" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="I1" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39" t="s">
+      <c r="E2" s="36"/>
+      <c r="F2" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="J2" s="39" t="s">
+      <c r="G2" s="36"/>
+      <c r="J2" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39" t="s">
+      <c r="K2" s="36"/>
+      <c r="L2" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39" t="s">
+      <c r="M2" s="36"/>
+      <c r="N2" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="39"/>
+      <c r="O2" s="36"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -7169,50 +7160,50 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="I8" s="39" t="s">
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="I8" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39" t="s">
+      <c r="E9" s="36"/>
+      <c r="F9" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="J9" s="39" t="s">
+      <c r="G9" s="36"/>
+      <c r="J9" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39" t="s">
+      <c r="K9" s="36"/>
+      <c r="L9" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39" t="s">
+      <c r="M9" s="36"/>
+      <c r="N9" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O9" s="39"/>
+      <c r="O9" s="36"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -7444,50 +7435,50 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="I15" s="39" t="s">
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="I15" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39" t="s">
+      <c r="E16" s="36"/>
+      <c r="F16" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="39"/>
-      <c r="J16" s="39" t="s">
+      <c r="G16" s="36"/>
+      <c r="J16" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39" t="s">
+      <c r="K16" s="36"/>
+      <c r="L16" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39" t="s">
+      <c r="M16" s="36"/>
+      <c r="N16" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O16" s="39"/>
+      <c r="O16" s="36"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -7719,50 +7710,50 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="I22" s="39" t="s">
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="I22" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39" t="s">
+      <c r="C23" s="36"/>
+      <c r="D23" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39" t="s">
+      <c r="E23" s="36"/>
+      <c r="F23" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="39"/>
-      <c r="J23" s="39" t="s">
+      <c r="G23" s="36"/>
+      <c r="J23" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39" t="s">
+      <c r="K23" s="36"/>
+      <c r="L23" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39" t="s">
+      <c r="M23" s="36"/>
+      <c r="N23" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O23" s="39"/>
+      <c r="O23" s="36"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -7995,50 +7986,50 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="I29" s="39" t="s">
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="I29" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39" t="s">
+      <c r="C30" s="36"/>
+      <c r="D30" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39" t="s">
+      <c r="E30" s="36"/>
+      <c r="F30" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G30" s="39"/>
-      <c r="J30" s="39" t="s">
+      <c r="G30" s="36"/>
+      <c r="J30" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39" t="s">
+      <c r="K30" s="36"/>
+      <c r="L30" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39" t="s">
+      <c r="M30" s="36"/>
+      <c r="N30" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O30" s="39"/>
+      <c r="O30" s="36"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -8271,50 +8262,50 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="I36" s="39" t="s">
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="I36" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39"/>
-      <c r="O36" s="39"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39" t="s">
+      <c r="C37" s="36"/>
+      <c r="D37" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39" t="s">
+      <c r="E37" s="36"/>
+      <c r="F37" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G37" s="39"/>
-      <c r="J37" s="39" t="s">
+      <c r="G37" s="36"/>
+      <c r="J37" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39" t="s">
+      <c r="K37" s="36"/>
+      <c r="L37" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M37" s="39"/>
-      <c r="N37" s="39" t="s">
+      <c r="M37" s="36"/>
+      <c r="N37" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O37" s="39"/>
+      <c r="O37" s="36"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -8547,50 +8538,50 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="39"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="I43" s="39" t="s">
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="I43" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="39"/>
-      <c r="O43" s="39"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="36"/>
+      <c r="M43" s="36"/>
+      <c r="N43" s="36"/>
+      <c r="O43" s="36"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39" t="s">
+      <c r="C44" s="36"/>
+      <c r="D44" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39" t="s">
+      <c r="E44" s="36"/>
+      <c r="F44" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G44" s="39"/>
-      <c r="J44" s="39" t="s">
+      <c r="G44" s="36"/>
+      <c r="J44" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39" t="s">
+      <c r="K44" s="36"/>
+      <c r="L44" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39" t="s">
+      <c r="M44" s="36"/>
+      <c r="N44" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O44" s="39"/>
+      <c r="O44" s="36"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -8824,41 +8815,41 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="38"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="I50" s="39" t="s">
+      <c r="A50" s="35"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="I50" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="J50" s="39"/>
-      <c r="K50" s="39"/>
-      <c r="L50" s="39"/>
-      <c r="M50" s="39"/>
-      <c r="N50" s="39"/>
-      <c r="O50" s="39"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="36"/>
+      <c r="L50" s="36"/>
+      <c r="M50" s="36"/>
+      <c r="N50" s="36"/>
+      <c r="O50" s="36"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="39"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
-      <c r="J51" s="39" t="s">
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="36"/>
+      <c r="J51" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K51" s="39"/>
-      <c r="L51" s="39" t="s">
+      <c r="K51" s="36"/>
+      <c r="L51" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M51" s="39"/>
-      <c r="N51" s="39" t="s">
+      <c r="M51" s="36"/>
+      <c r="N51" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O51" s="39"/>
+      <c r="O51" s="36"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J52" t="s">
@@ -10503,8 +10494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H159" sqref="H159"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10574,7 +10565,7 @@
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>171</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -10586,25 +10577,25 @@
       <c r="E2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="30">
         <v>40</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="31" t="s">
         <v>34</v>
       </c>
       <c r="M2" s="23"/>
@@ -10635,7 +10626,7 @@
       <c r="F3" s="12">
         <v>40</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="24" t="s">
         <v>205</v>
       </c>
       <c r="H3" s="24" t="s">
@@ -10681,7 +10672,7 @@
       <c r="F4" s="12">
         <v>40</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="24" t="s">
         <v>206</v>
       </c>
       <c r="H4" s="24" t="s">
@@ -10727,22 +10718,22 @@
       <c r="F5" s="14">
         <v>40</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L5" s="29" t="s">
+      <c r="L5" s="28" t="s">
         <v>34</v>
       </c>
       <c r="M5" s="23"/>
@@ -10758,7 +10749,7 @@
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>175</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -10770,25 +10761,25 @@
       <c r="E6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="30">
         <v>40</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="K6" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="31" t="s">
         <v>34</v>
       </c>
       <c r="M6" s="23"/>
@@ -10819,7 +10810,7 @@
       <c r="F7" s="12">
         <v>40</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="24" t="s">
         <v>209</v>
       </c>
       <c r="H7" s="24" t="s">
@@ -10865,7 +10856,7 @@
       <c r="F8" s="12">
         <v>40</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="24" t="s">
         <v>210</v>
       </c>
       <c r="H8" s="24" t="s">
@@ -10911,22 +10902,22 @@
       <c r="F9" s="14">
         <v>40</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="29" t="s">
+      <c r="I9" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L9" s="29" t="s">
+      <c r="L9" s="28" t="s">
         <v>34</v>
       </c>
       <c r="M9" s="23"/>
@@ -10942,7 +10933,7 @@
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>179</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -10954,25 +10945,25 @@
       <c r="E10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="30">
         <v>60</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="H10" s="34">
+      <c r="H10" s="32">
         <v>11</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="31">
         <v>4580</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J10" s="31">
         <v>2506.06</v>
       </c>
-      <c r="K10" s="33" t="s">
+      <c r="K10" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="L10" s="31" t="s">
         <v>689</v>
       </c>
       <c r="M10" s="23"/>
@@ -11003,7 +10994,7 @@
       <c r="F11" s="12">
         <v>60</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="24" t="s">
         <v>213</v>
       </c>
       <c r="H11" s="24">
@@ -11049,7 +11040,7 @@
       <c r="F12" s="12">
         <v>60</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="24" t="s">
         <v>214</v>
       </c>
       <c r="H12" s="24">
@@ -11095,22 +11086,22 @@
       <c r="F13" s="14">
         <v>60</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="28">
         <v>13</v>
       </c>
-      <c r="I13" s="29">
+      <c r="I13" s="28">
         <v>4407</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="28">
         <v>2430.5700000000002</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L13" s="28" t="s">
+      <c r="L13" s="27" t="s">
         <v>689</v>
       </c>
       <c r="M13" s="23"/>
@@ -11126,7 +11117,7 @@
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="30" t="s">
         <v>183</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -11138,25 +11129,25 @@
       <c r="E14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="30">
         <v>60</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="33" t="s">
+      <c r="I14" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="33" t="s">
+      <c r="J14" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="33" t="s">
+      <c r="K14" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L14" s="33" t="s">
+      <c r="L14" s="31" t="s">
         <v>34</v>
       </c>
       <c r="M14" s="23"/>
@@ -11187,7 +11178,7 @@
       <c r="F15" s="12">
         <v>60</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="24" t="s">
         <v>217</v>
       </c>
       <c r="H15" s="24">
@@ -11233,7 +11224,7 @@
       <c r="F16" s="12">
         <v>60</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="24" t="s">
         <v>218</v>
       </c>
       <c r="H16" s="24">
@@ -11279,22 +11270,22 @@
       <c r="F17" s="14">
         <v>60</v>
       </c>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H17" s="28">
         <v>10</v>
       </c>
-      <c r="I17" s="29">
+      <c r="I17" s="28">
         <v>4254</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="28">
         <v>2321.21</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L17" s="28" t="s">
+      <c r="L17" s="27" t="s">
         <v>689</v>
       </c>
       <c r="M17" s="23"/>
@@ -11310,7 +11301,7 @@
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="30" t="s">
         <v>187</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -11322,25 +11313,25 @@
       <c r="E18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="30">
         <v>200</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="H18" s="33">
+      <c r="H18" s="31">
         <v>9</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="31">
         <v>4102</v>
       </c>
-      <c r="J18" s="33">
+      <c r="J18" s="31">
         <v>2177.8000000000002</v>
       </c>
-      <c r="K18" s="33" t="s">
+      <c r="K18" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L18" s="33" t="s">
+      <c r="L18" s="31" t="s">
         <v>689</v>
       </c>
       <c r="M18" s="24"/>
@@ -11371,7 +11362,7 @@
       <c r="F19" s="12">
         <v>200</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="24" t="s">
         <v>221</v>
       </c>
       <c r="H19" s="24">
@@ -11417,7 +11408,7 @@
       <c r="F20" s="12">
         <v>200</v>
       </c>
-      <c r="G20" s="27" t="s">
+      <c r="G20" s="24" t="s">
         <v>222</v>
       </c>
       <c r="H20" s="24">
@@ -11463,22 +11454,22 @@
       <c r="F21" s="14">
         <v>200</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="H21" s="29">
+      <c r="H21" s="28">
         <v>11</v>
       </c>
-      <c r="I21" s="29">
+      <c r="I21" s="28">
         <v>4296</v>
       </c>
-      <c r="J21" s="29">
+      <c r="J21" s="28">
         <v>2373.54</v>
       </c>
-      <c r="K21" s="29" t="s">
+      <c r="K21" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L21" s="29" t="s">
+      <c r="L21" s="28" t="s">
         <v>689</v>
       </c>
       <c r="M21" s="24"/>
@@ -11494,7 +11485,7 @@
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="30" t="s">
         <v>191</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -11506,25 +11497,25 @@
       <c r="E22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="30">
         <v>200</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="H22" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I22" s="33" t="s">
+      <c r="I22" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="J22" s="33" t="s">
+      <c r="J22" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="K22" s="33" t="s">
+      <c r="K22" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L22" s="33" t="s">
+      <c r="L22" s="31" t="s">
         <v>34</v>
       </c>
       <c r="M22" s="24"/>
@@ -11555,7 +11546,7 @@
       <c r="F23" s="12">
         <v>200</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="G23" s="24" t="s">
         <v>225</v>
       </c>
       <c r="H23" s="24">
@@ -11601,7 +11592,7 @@
       <c r="F24" s="12">
         <v>200</v>
       </c>
-      <c r="G24" s="27" t="s">
+      <c r="G24" s="24" t="s">
         <v>226</v>
       </c>
       <c r="H24" s="24">
@@ -11647,22 +11638,22 @@
       <c r="F25" s="14">
         <v>200</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="H25" s="29">
+      <c r="H25" s="28">
         <v>8</v>
       </c>
-      <c r="I25" s="29">
+      <c r="I25" s="28">
         <v>3948</v>
       </c>
-      <c r="J25" s="29">
+      <c r="J25" s="28">
         <v>2037.85</v>
       </c>
-      <c r="K25" s="29" t="s">
+      <c r="K25" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L25" s="29" t="s">
+      <c r="L25" s="28" t="s">
         <v>689</v>
       </c>
       <c r="M25" s="24"/>
@@ -11678,7 +11669,7 @@
       <c r="A26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="30" t="s">
         <v>195</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -11690,25 +11681,25 @@
       <c r="E26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="35">
+      <c r="F26" s="33">
         <v>0</v>
       </c>
-      <c r="G26" s="32" t="s">
+      <c r="G26" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="H26" s="33">
+      <c r="H26" s="31">
         <v>9</v>
       </c>
-      <c r="I26" s="33">
+      <c r="I26" s="31">
         <v>4102</v>
       </c>
-      <c r="J26" s="33">
+      <c r="J26" s="31">
         <v>2177.8000000000002</v>
       </c>
-      <c r="K26" s="33" t="s">
+      <c r="K26" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L26" s="33" t="s">
+      <c r="L26" s="31" t="s">
         <v>689</v>
       </c>
       <c r="M26" s="24"/>
@@ -11739,7 +11730,7 @@
       <c r="F27" s="13">
         <v>0</v>
       </c>
-      <c r="G27" s="27" t="s">
+      <c r="G27" s="24" t="s">
         <v>229</v>
       </c>
       <c r="H27" s="24">
@@ -11785,7 +11776,7 @@
       <c r="F28" s="13">
         <v>0</v>
       </c>
-      <c r="G28" s="27" t="s">
+      <c r="G28" s="24" t="s">
         <v>230</v>
       </c>
       <c r="H28" s="24">
@@ -11831,22 +11822,22 @@
       <c r="F29" s="15">
         <v>0</v>
       </c>
-      <c r="G29" s="37" t="s">
+      <c r="G29" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="H29" s="29">
+      <c r="H29" s="28">
         <v>11</v>
       </c>
-      <c r="I29" s="29">
+      <c r="I29" s="28">
         <v>4323</v>
       </c>
-      <c r="J29" s="29">
+      <c r="J29" s="28">
         <v>2367.27</v>
       </c>
-      <c r="K29" s="29" t="s">
+      <c r="K29" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L29" s="28" t="s">
+      <c r="L29" s="27" t="s">
         <v>689</v>
       </c>
       <c r="M29" s="23"/>
@@ -11862,7 +11853,7 @@
       <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="30" t="s">
         <v>199</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -11874,25 +11865,25 @@
       <c r="E30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="35">
+      <c r="F30" s="33">
         <v>0</v>
       </c>
-      <c r="G30" s="32" t="s">
+      <c r="G30" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="H30" s="33" t="s">
+      <c r="H30" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="33" t="s">
+      <c r="I30" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="J30" s="33" t="s">
+      <c r="J30" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="K30" s="33" t="s">
+      <c r="K30" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L30" s="33" t="s">
+      <c r="L30" s="31" t="s">
         <v>34</v>
       </c>
       <c r="M30" s="24"/>
@@ -11923,7 +11914,7 @@
       <c r="F31" s="13">
         <v>0</v>
       </c>
-      <c r="G31" s="27" t="s">
+      <c r="G31" s="24" t="s">
         <v>233</v>
       </c>
       <c r="H31" s="24">
@@ -11969,7 +11960,7 @@
       <c r="F32" s="13">
         <v>0</v>
       </c>
-      <c r="G32" s="27" t="s">
+      <c r="G32" s="24" t="s">
         <v>234</v>
       </c>
       <c r="H32" s="24">
@@ -12015,22 +12006,22 @@
       <c r="F33" s="15">
         <v>0</v>
       </c>
-      <c r="G33" s="37" t="s">
+      <c r="G33" s="28" t="s">
         <v>678</v>
       </c>
-      <c r="H33" s="29">
+      <c r="H33" s="28">
         <v>8</v>
       </c>
-      <c r="I33" s="29">
+      <c r="I33" s="28">
         <v>3930</v>
       </c>
-      <c r="J33" s="29">
+      <c r="J33" s="28">
         <v>2026.88</v>
       </c>
-      <c r="K33" s="29" t="s">
+      <c r="K33" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L33" s="28" t="s">
+      <c r="L33" s="27" t="s">
         <v>689</v>
       </c>
       <c r="M33" s="23"/>
@@ -12043,10 +12034,10 @@
       <c r="T33" s="23"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="30" t="s">
         <v>171</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -12058,25 +12049,25 @@
       <c r="E34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="31">
+      <c r="F34" s="30">
         <v>40</v>
       </c>
-      <c r="G34" s="32" t="s">
+      <c r="G34" s="31" t="s">
         <v>236</v>
       </c>
-      <c r="H34" s="33">
+      <c r="H34" s="31">
         <v>10</v>
       </c>
-      <c r="I34" s="33">
+      <c r="I34" s="31">
         <v>3604</v>
       </c>
-      <c r="J34" s="33">
+      <c r="J34" s="31">
         <v>2084.15</v>
       </c>
-      <c r="K34" s="33" t="s">
+      <c r="K34" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L34" s="34" t="s">
+      <c r="L34" s="32" t="s">
         <v>689</v>
       </c>
     </row>
@@ -12099,7 +12090,7 @@
       <c r="F35" s="12">
         <v>40</v>
       </c>
-      <c r="G35" s="27" t="s">
+      <c r="G35" s="24" t="s">
         <v>237</v>
       </c>
       <c r="H35" s="24">
@@ -12137,7 +12128,7 @@
       <c r="F36" s="12">
         <v>40</v>
       </c>
-      <c r="G36" s="27" t="s">
+      <c r="G36" s="24" t="s">
         <v>238</v>
       </c>
       <c r="H36" s="24">
@@ -12157,7 +12148,7 @@
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -12175,30 +12166,30 @@
       <c r="F37" s="14">
         <v>40</v>
       </c>
-      <c r="G37" s="37" t="s">
+      <c r="G37" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="H37" s="29">
+      <c r="H37" s="28">
         <v>11</v>
       </c>
-      <c r="I37" s="29">
+      <c r="I37" s="28">
         <v>3429</v>
       </c>
-      <c r="J37" s="29">
+      <c r="J37" s="28">
         <v>2083.9699999999998</v>
       </c>
-      <c r="K37" s="29" t="s">
+      <c r="K37" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L37" s="28" t="s">
+      <c r="L37" s="27" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="30" t="s">
         <v>175</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -12210,25 +12201,25 @@
       <c r="E38" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="31">
+      <c r="F38" s="30">
         <v>40</v>
       </c>
-      <c r="G38" s="32" t="s">
+      <c r="G38" s="31" t="s">
         <v>240</v>
       </c>
-      <c r="H38" s="34" t="s">
+      <c r="H38" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="I38" s="34" t="s">
+      <c r="I38" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="J38" s="34" t="s">
+      <c r="J38" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="K38" s="33" t="s">
+      <c r="K38" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L38" s="34" t="s">
+      <c r="L38" s="32" t="s">
         <v>34</v>
       </c>
     </row>
@@ -12251,7 +12242,7 @@
       <c r="F39" s="12">
         <v>40</v>
       </c>
-      <c r="G39" s="27" t="s">
+      <c r="G39" s="24" t="s">
         <v>241</v>
       </c>
       <c r="H39" s="23">
@@ -12289,7 +12280,7 @@
       <c r="F40" s="12">
         <v>40</v>
       </c>
-      <c r="G40" s="27" t="s">
+      <c r="G40" s="24" t="s">
         <v>242</v>
       </c>
       <c r="H40" s="23">
@@ -12309,7 +12300,7 @@
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="14" t="s">
@@ -12327,30 +12318,30 @@
       <c r="F41" s="14">
         <v>40</v>
       </c>
-      <c r="G41" s="37" t="s">
+      <c r="G41" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="H41" s="28">
+      <c r="H41" s="27">
         <v>10</v>
       </c>
-      <c r="I41" s="28">
+      <c r="I41" s="27">
         <v>3549</v>
       </c>
-      <c r="J41" s="28">
+      <c r="J41" s="27">
         <v>2032.15</v>
       </c>
-      <c r="K41" s="29" t="s">
+      <c r="K41" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L41" s="28" t="s">
+      <c r="L41" s="27" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="30" t="s">
         <v>179</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -12362,25 +12353,25 @@
       <c r="E42" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="31">
+      <c r="F42" s="30">
         <v>60</v>
       </c>
-      <c r="G42" s="32" t="s">
+      <c r="G42" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="H42" s="34">
+      <c r="H42" s="32">
         <v>7</v>
       </c>
-      <c r="I42" s="34">
+      <c r="I42" s="32">
         <v>2904</v>
       </c>
-      <c r="J42" s="34">
+      <c r="J42" s="32">
         <v>1525.86</v>
       </c>
-      <c r="K42" s="33" t="s">
+      <c r="K42" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L42" s="34" t="s">
+      <c r="L42" s="32" t="s">
         <v>689</v>
       </c>
     </row>
@@ -12403,7 +12394,7 @@
       <c r="F43" s="12">
         <v>60</v>
       </c>
-      <c r="G43" s="27" t="s">
+      <c r="G43" s="24" t="s">
         <v>245</v>
       </c>
       <c r="H43" s="23">
@@ -12441,7 +12432,7 @@
       <c r="F44" s="12">
         <v>60</v>
       </c>
-      <c r="G44" s="27" t="s">
+      <c r="G44" s="24" t="s">
         <v>246</v>
       </c>
       <c r="H44" s="23">
@@ -12461,7 +12452,7 @@
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="14" t="s">
@@ -12479,30 +12470,30 @@
       <c r="F45" s="14">
         <v>60</v>
       </c>
-      <c r="G45" s="37" t="s">
+      <c r="G45" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="H45" s="28">
+      <c r="H45" s="27">
         <v>8</v>
       </c>
-      <c r="I45" s="28">
+      <c r="I45" s="27">
         <v>3154</v>
       </c>
-      <c r="J45" s="28">
+      <c r="J45" s="27">
         <v>1683.56</v>
       </c>
-      <c r="K45" s="29" t="s">
+      <c r="K45" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L45" s="28" t="s">
+      <c r="L45" s="27" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="30" t="s">
         <v>183</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -12514,25 +12505,25 @@
       <c r="E46" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="31">
+      <c r="F46" s="30">
         <v>60</v>
       </c>
-      <c r="G46" s="32" t="s">
+      <c r="G46" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="H46" s="34">
+      <c r="H46" s="32">
         <v>6</v>
       </c>
-      <c r="I46" s="34">
+      <c r="I46" s="32">
         <v>2977</v>
       </c>
-      <c r="J46" s="34">
+      <c r="J46" s="32">
         <v>1569.43</v>
       </c>
-      <c r="K46" s="33" t="s">
+      <c r="K46" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L46" s="34" t="s">
+      <c r="L46" s="32" t="s">
         <v>689</v>
       </c>
     </row>
@@ -12555,7 +12546,7 @@
       <c r="F47" s="12">
         <v>60</v>
       </c>
-      <c r="G47" s="27" t="s">
+      <c r="G47" s="24" t="s">
         <v>249</v>
       </c>
       <c r="H47" s="23">
@@ -12593,7 +12584,7 @@
       <c r="F48" s="12">
         <v>60</v>
       </c>
-      <c r="G48" s="27" t="s">
+      <c r="G48" s="24" t="s">
         <v>250</v>
       </c>
       <c r="H48" s="23">
@@ -12613,7 +12604,7 @@
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="14" t="s">
@@ -12631,30 +12622,30 @@
       <c r="F49" s="14">
         <v>60</v>
       </c>
-      <c r="G49" s="37" t="s">
+      <c r="G49" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="H49" s="28">
+      <c r="H49" s="27">
         <v>6</v>
       </c>
-      <c r="I49" s="28">
+      <c r="I49" s="27">
         <v>2846</v>
       </c>
-      <c r="J49" s="28">
+      <c r="J49" s="27">
         <v>1493.35</v>
       </c>
-      <c r="K49" s="29" t="s">
+      <c r="K49" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L49" s="28" t="s">
+      <c r="L49" s="27" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="30" t="s">
         <v>187</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -12666,25 +12657,25 @@
       <c r="E50" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F50" s="31">
+      <c r="F50" s="30">
         <v>200</v>
       </c>
-      <c r="G50" s="32" t="s">
+      <c r="G50" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="H50" s="34">
+      <c r="H50" s="32">
         <v>7</v>
       </c>
-      <c r="I50" s="34">
+      <c r="I50" s="32">
         <v>2809</v>
       </c>
-      <c r="J50" s="34">
+      <c r="J50" s="32">
         <v>1479.11</v>
       </c>
-      <c r="K50" s="33" t="s">
+      <c r="K50" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L50" s="34" t="s">
+      <c r="L50" s="32" t="s">
         <v>689</v>
       </c>
     </row>
@@ -12707,7 +12698,7 @@
       <c r="F51" s="12">
         <v>200</v>
       </c>
-      <c r="G51" s="27" t="s">
+      <c r="G51" s="24" t="s">
         <v>253</v>
       </c>
       <c r="H51" s="23">
@@ -12745,7 +12736,7 @@
       <c r="F52" s="12">
         <v>200</v>
       </c>
-      <c r="G52" s="27" t="s">
+      <c r="G52" s="24" t="s">
         <v>254</v>
       </c>
       <c r="H52" s="23">
@@ -12765,7 +12756,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="14" t="s">
@@ -12783,30 +12774,30 @@
       <c r="F53" s="14">
         <v>200</v>
       </c>
-      <c r="G53" s="37" t="s">
+      <c r="G53" s="28" t="s">
         <v>255</v>
       </c>
-      <c r="H53" s="28">
+      <c r="H53" s="27">
         <v>8</v>
       </c>
-      <c r="I53" s="28">
+      <c r="I53" s="27">
         <v>3195</v>
       </c>
-      <c r="J53" s="28">
+      <c r="J53" s="27">
         <v>1717.42</v>
       </c>
-      <c r="K53" s="29" t="s">
+      <c r="K53" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L53" s="28" t="s">
+      <c r="L53" s="27" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="36" t="s">
+      <c r="A54" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="31" t="s">
+      <c r="B54" s="30" t="s">
         <v>191</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -12818,25 +12809,25 @@
       <c r="E54" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F54" s="31">
+      <c r="F54" s="30">
         <v>200</v>
       </c>
-      <c r="G54" s="32" t="s">
+      <c r="G54" s="31" t="s">
         <v>256</v>
       </c>
-      <c r="H54" s="34">
+      <c r="H54" s="32">
         <v>5</v>
       </c>
-      <c r="I54" s="34">
+      <c r="I54" s="32">
         <v>2749</v>
       </c>
-      <c r="J54" s="34">
+      <c r="J54" s="32">
         <v>1410.65</v>
       </c>
-      <c r="K54" s="33" t="s">
+      <c r="K54" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L54" s="34" t="s">
+      <c r="L54" s="32" t="s">
         <v>689</v>
       </c>
     </row>
@@ -12859,7 +12850,7 @@
       <c r="F55" s="12">
         <v>200</v>
       </c>
-      <c r="G55" s="27" t="s">
+      <c r="G55" s="24" t="s">
         <v>257</v>
       </c>
       <c r="H55" s="23">
@@ -12897,7 +12888,7 @@
       <c r="F56" s="12">
         <v>200</v>
       </c>
-      <c r="G56" s="27" t="s">
+      <c r="G56" s="24" t="s">
         <v>258</v>
       </c>
       <c r="H56" s="23">
@@ -12917,7 +12908,7 @@
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+      <c r="A57" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B57" s="14" t="s">
@@ -12935,30 +12926,30 @@
       <c r="F57" s="14">
         <v>200</v>
       </c>
-      <c r="G57" s="37" t="s">
+      <c r="G57" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="H57" s="28">
+      <c r="H57" s="27">
         <v>6</v>
       </c>
-      <c r="I57" s="28">
+      <c r="I57" s="27">
         <v>2871</v>
       </c>
-      <c r="J57" s="28">
+      <c r="J57" s="27">
         <v>1496.98</v>
       </c>
-      <c r="K57" s="29" t="s">
+      <c r="K57" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="L57" s="28" t="s">
+      <c r="L57" s="27" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="36" t="s">
+      <c r="A58" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="30" t="s">
         <v>195</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -12970,25 +12961,25 @@
       <c r="E58" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F58" s="35">
+      <c r="F58" s="33">
         <v>0</v>
       </c>
-      <c r="G58" s="32" t="s">
+      <c r="G58" s="31" t="s">
         <v>260</v>
       </c>
-      <c r="H58" s="34">
+      <c r="H58" s="32">
         <v>7</v>
       </c>
-      <c r="I58" s="34">
+      <c r="I58" s="32">
         <v>2809</v>
       </c>
-      <c r="J58" s="34">
+      <c r="J58" s="32">
         <v>1479.11</v>
       </c>
-      <c r="K58" s="33" t="s">
+      <c r="K58" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L58" s="34" t="s">
+      <c r="L58" s="32" t="s">
         <v>689</v>
       </c>
     </row>
@@ -13011,7 +13002,7 @@
       <c r="F59" s="13">
         <v>0</v>
       </c>
-      <c r="G59" s="27" t="s">
+      <c r="G59" s="24" t="s">
         <v>261</v>
       </c>
       <c r="H59" s="23">
@@ -13049,7 +13040,7 @@
       <c r="F60" s="13">
         <v>0</v>
       </c>
-      <c r="G60" s="27" t="s">
+      <c r="G60" s="24" t="s">
         <v>262</v>
       </c>
       <c r="H60" s="23">
@@ -13069,7 +13060,7 @@
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+      <c r="A61" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B61" s="14" t="s">
@@ -13087,30 +13078,30 @@
       <c r="F61" s="15">
         <v>0</v>
       </c>
-      <c r="G61" s="37" t="s">
+      <c r="G61" s="28" t="s">
         <v>263</v>
       </c>
-      <c r="H61" s="28">
+      <c r="H61" s="27">
         <v>8</v>
       </c>
-      <c r="I61" s="28">
+      <c r="I61" s="27">
         <v>3195</v>
       </c>
-      <c r="J61" s="28">
+      <c r="J61" s="27">
         <v>1717.42</v>
       </c>
-      <c r="K61" s="28" t="s">
+      <c r="K61" s="27" t="s">
         <v>689</v>
       </c>
-      <c r="L61" s="28" t="s">
+      <c r="L61" s="27" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="36" t="s">
+      <c r="A62" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B62" s="31" t="s">
+      <c r="B62" s="30" t="s">
         <v>199</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -13122,25 +13113,25 @@
       <c r="E62" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F62" s="35">
+      <c r="F62" s="33">
         <v>0</v>
       </c>
-      <c r="G62" s="32" t="s">
+      <c r="G62" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="H62" s="34">
+      <c r="H62" s="32">
         <v>5</v>
       </c>
-      <c r="I62" s="34">
+      <c r="I62" s="32">
         <v>2749</v>
       </c>
-      <c r="J62" s="34">
+      <c r="J62" s="32">
         <v>1410.65</v>
       </c>
-      <c r="K62" s="34" t="s">
+      <c r="K62" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="L62" s="34" t="s">
+      <c r="L62" s="32" t="s">
         <v>689</v>
       </c>
     </row>
@@ -13163,7 +13154,7 @@
       <c r="F63" s="13">
         <v>0</v>
       </c>
-      <c r="G63" s="27" t="s">
+      <c r="G63" s="24" t="s">
         <v>265</v>
       </c>
       <c r="H63" s="23">
@@ -13201,7 +13192,7 @@
       <c r="F64" s="13">
         <v>0</v>
       </c>
-      <c r="G64" s="27" t="s">
+      <c r="G64" s="24" t="s">
         <v>266</v>
       </c>
       <c r="H64" s="23">
@@ -13221,7 +13212,7 @@
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="s">
+      <c r="A65" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B65" s="14" t="s">
@@ -13242,25 +13233,27 @@
       <c r="G65" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="H65" s="28">
+      <c r="H65" s="27">
         <v>6</v>
       </c>
-      <c r="I65" s="28">
+      <c r="I65" s="27">
         <v>2871</v>
       </c>
-      <c r="J65" s="28">
+      <c r="J65" s="27">
         <v>1496.98</v>
       </c>
-      <c r="K65" s="28" t="s">
+      <c r="K65" s="27" t="s">
         <v>689</v>
       </c>
-      <c r="L65" s="28"/>
+      <c r="L65" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="36" t="s">
+      <c r="A66" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="31" t="s">
+      <c r="B66" s="30" t="s">
         <v>171</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -13272,25 +13265,25 @@
       <c r="E66" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F66" s="31">
+      <c r="F66" s="30">
         <v>40</v>
       </c>
-      <c r="G66" s="34" t="s">
+      <c r="G66" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="H66" s="34" t="s">
+      <c r="H66" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="I66" s="34" t="s">
+      <c r="I66" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="J66" s="34" t="s">
+      <c r="J66" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="K66" s="33" t="s">
+      <c r="K66" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L66" s="34" t="s">
+      <c r="L66" s="32" t="s">
         <v>34</v>
       </c>
     </row>
@@ -13316,11 +13309,21 @@
       <c r="G67" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="H67" s="23"/>
-      <c r="I67" s="23"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="23"/>
+      <c r="H67" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I67" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J67" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K67" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L67" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
@@ -13344,14 +13347,24 @@
       <c r="G68" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="H68" s="23"/>
-      <c r="I68" s="23"/>
-      <c r="J68" s="23"/>
-      <c r="K68" s="23"/>
-      <c r="L68" s="23"/>
+      <c r="H68" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I68" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J68" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K68" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L68" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="30" t="s">
+      <c r="A69" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B69" s="14" t="s">
@@ -13369,20 +13382,30 @@
       <c r="F69" s="14">
         <v>40</v>
       </c>
-      <c r="G69" s="28" t="s">
+      <c r="G69" s="27" t="s">
         <v>270</v>
       </c>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
+      <c r="H69" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I69" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J69" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K69" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L69" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="36" t="s">
+      <c r="A70" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B70" s="31" t="s">
+      <c r="B70" s="30" t="s">
         <v>175</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -13394,25 +13417,25 @@
       <c r="E70" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F70" s="31">
+      <c r="F70" s="30">
         <v>40</v>
       </c>
-      <c r="G70" s="34" t="s">
+      <c r="G70" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="H70" s="34" t="s">
+      <c r="H70" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="I70" s="34" t="s">
+      <c r="I70" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="J70" s="34" t="s">
+      <c r="J70" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="K70" s="33" t="s">
+      <c r="K70" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="L70" s="34" t="s">
+      <c r="L70" s="32" t="s">
         <v>34</v>
       </c>
     </row>
@@ -13438,11 +13461,21 @@
       <c r="G71" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="H71" s="23"/>
-      <c r="I71" s="23"/>
-      <c r="J71" s="23"/>
-      <c r="K71" s="23"/>
-      <c r="L71" s="23"/>
+      <c r="H71" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I71" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J71" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K71" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L71" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
@@ -13466,14 +13499,24 @@
       <c r="G72" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="H72" s="23"/>
-      <c r="I72" s="23"/>
-      <c r="J72" s="23"/>
-      <c r="K72" s="23"/>
-      <c r="L72" s="23"/>
+      <c r="H72" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I72" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J72" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K72" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L72" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="30" t="s">
+      <c r="A73" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B73" s="14" t="s">
@@ -13491,20 +13534,30 @@
       <c r="F73" s="14">
         <v>40</v>
       </c>
-      <c r="G73" s="28" t="s">
+      <c r="G73" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="H73" s="28"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="28"/>
-      <c r="K73" s="28"/>
-      <c r="L73" s="28"/>
+      <c r="H73" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I73" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J73" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K73" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L73" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="36" t="s">
+      <c r="A74" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B74" s="31" t="s">
+      <c r="B74" s="30" t="s">
         <v>179</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -13516,17 +13569,27 @@
       <c r="E74" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F74" s="31">
+      <c r="F74" s="30">
         <v>60</v>
       </c>
-      <c r="G74" s="34" t="s">
+      <c r="G74" s="32" t="s">
         <v>275</v>
       </c>
-      <c r="H74" s="34"/>
-      <c r="I74" s="34"/>
-      <c r="J74" s="34"/>
-      <c r="K74" s="34"/>
-      <c r="L74" s="34"/>
+      <c r="H74" s="32">
+        <v>7</v>
+      </c>
+      <c r="I74" s="32">
+        <v>2329</v>
+      </c>
+      <c r="J74" s="32">
+        <v>1126.8599999999999</v>
+      </c>
+      <c r="K74" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L74" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="21" t="s">
@@ -13550,11 +13613,21 @@
       <c r="G75" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="H75" s="23"/>
-      <c r="I75" s="23"/>
-      <c r="J75" s="23"/>
-      <c r="K75" s="23"/>
-      <c r="L75" s="23"/>
+      <c r="H75" s="23">
+        <v>8</v>
+      </c>
+      <c r="I75" s="23">
+        <v>2695</v>
+      </c>
+      <c r="J75" s="24">
+        <v>1519.24</v>
+      </c>
+      <c r="K75" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L75" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
@@ -13578,14 +13651,24 @@
       <c r="G76" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="H76" s="23"/>
-      <c r="I76" s="23"/>
-      <c r="J76" s="23"/>
-      <c r="K76" s="23"/>
-      <c r="L76" s="23"/>
+      <c r="H76" s="23">
+        <v>8</v>
+      </c>
+      <c r="I76" s="23">
+        <v>2912</v>
+      </c>
+      <c r="J76" s="24">
+        <v>1558.6</v>
+      </c>
+      <c r="K76" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L76" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="30" t="s">
+      <c r="A77" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B77" s="14" t="s">
@@ -13603,20 +13686,30 @@
       <c r="F77" s="14">
         <v>60</v>
       </c>
-      <c r="G77" s="28" t="s">
+      <c r="G77" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="H77" s="28"/>
-      <c r="I77" s="28"/>
-      <c r="J77" s="28"/>
-      <c r="K77" s="28"/>
-      <c r="L77" s="28"/>
+      <c r="H77" s="27">
+        <v>8</v>
+      </c>
+      <c r="I77" s="27">
+        <v>2658</v>
+      </c>
+      <c r="J77" s="27">
+        <v>1465.3</v>
+      </c>
+      <c r="K77" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L77" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="36" t="s">
+      <c r="A78" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B78" s="31" t="s">
+      <c r="B78" s="30" t="s">
         <v>183</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -13628,17 +13721,27 @@
       <c r="E78" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F78" s="31">
+      <c r="F78" s="30">
         <v>60</v>
       </c>
-      <c r="G78" s="34" t="s">
+      <c r="G78" s="32" t="s">
         <v>279</v>
       </c>
-      <c r="H78" s="34"/>
-      <c r="I78" s="34"/>
-      <c r="J78" s="34"/>
-      <c r="K78" s="34"/>
-      <c r="L78" s="34"/>
+      <c r="H78" s="32">
+        <v>6</v>
+      </c>
+      <c r="I78" s="32">
+        <v>2537</v>
+      </c>
+      <c r="J78" s="32">
+        <v>1305.26</v>
+      </c>
+      <c r="K78" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L78" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="21" t="s">
@@ -13662,11 +13765,21 @@
       <c r="G79" s="23" t="s">
         <v>280</v>
       </c>
-      <c r="H79" s="23"/>
-      <c r="I79" s="23"/>
-      <c r="J79" s="23"/>
-      <c r="K79" s="23"/>
-      <c r="L79" s="23"/>
+      <c r="H79" s="24">
+        <v>6</v>
+      </c>
+      <c r="I79" s="24">
+        <v>2674</v>
+      </c>
+      <c r="J79" s="24">
+        <v>1343.06</v>
+      </c>
+      <c r="K79" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L79" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="21" t="s">
@@ -13690,14 +13803,24 @@
       <c r="G80" s="23" t="s">
         <v>281</v>
       </c>
-      <c r="H80" s="23"/>
-      <c r="I80" s="23"/>
-      <c r="J80" s="23"/>
-      <c r="K80" s="23"/>
-      <c r="L80" s="23"/>
+      <c r="H80" s="24">
+        <v>7</v>
+      </c>
+      <c r="I80" s="24">
+        <v>2631</v>
+      </c>
+      <c r="J80" s="24">
+        <v>1367.83</v>
+      </c>
+      <c r="K80" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L80" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" s="30" t="s">
+      <c r="A81" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B81" s="14" t="s">
@@ -13715,20 +13838,30 @@
       <c r="F81" s="14">
         <v>60</v>
       </c>
-      <c r="G81" s="28" t="s">
+      <c r="G81" s="27" t="s">
         <v>282</v>
       </c>
-      <c r="H81" s="28"/>
-      <c r="I81" s="28"/>
-      <c r="J81" s="28"/>
-      <c r="K81" s="28"/>
-      <c r="L81" s="28"/>
+      <c r="H81" s="27">
+        <v>6</v>
+      </c>
+      <c r="I81" s="27">
+        <v>2726</v>
+      </c>
+      <c r="J81" s="27">
+        <v>1396.91</v>
+      </c>
+      <c r="K81" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L81" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" s="36" t="s">
+      <c r="A82" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B82" s="31" t="s">
+      <c r="B82" s="30" t="s">
         <v>187</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -13740,17 +13873,27 @@
       <c r="E82" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F82" s="31">
+      <c r="F82" s="30">
         <v>200</v>
       </c>
-      <c r="G82" s="34" t="s">
+      <c r="G82" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="H82" s="34"/>
-      <c r="I82" s="34"/>
-      <c r="J82" s="34"/>
-      <c r="K82" s="34"/>
-      <c r="L82" s="34"/>
+      <c r="H82" s="32">
+        <v>5</v>
+      </c>
+      <c r="I82" s="32">
+        <v>2327</v>
+      </c>
+      <c r="J82" s="32">
+        <v>1104.1500000000001</v>
+      </c>
+      <c r="K82" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L82" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="21" t="s">
@@ -13774,11 +13917,21 @@
       <c r="G83" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="H83" s="23"/>
-      <c r="I83" s="23"/>
-      <c r="J83" s="23"/>
-      <c r="K83" s="23"/>
-      <c r="L83" s="23"/>
+      <c r="H83" s="24">
+        <v>7</v>
+      </c>
+      <c r="I83" s="24">
+        <v>2605</v>
+      </c>
+      <c r="J83" s="24">
+        <v>1350.11</v>
+      </c>
+      <c r="K83" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L83" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="21" t="s">
@@ -13802,14 +13955,24 @@
       <c r="G84" s="23" t="s">
         <v>285</v>
       </c>
-      <c r="H84" s="23"/>
-      <c r="I84" s="23"/>
-      <c r="J84" s="23"/>
-      <c r="K84" s="23"/>
-      <c r="L84" s="23"/>
+      <c r="H84" s="24">
+        <v>7</v>
+      </c>
+      <c r="I84" s="24">
+        <v>2534</v>
+      </c>
+      <c r="J84" s="24">
+        <v>1304.95</v>
+      </c>
+      <c r="K84" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L84" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="30" t="s">
+      <c r="A85" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B85" s="14" t="s">
@@ -13827,20 +13990,30 @@
       <c r="F85" s="14">
         <v>200</v>
       </c>
-      <c r="G85" s="28" t="s">
+      <c r="G85" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="H85" s="28"/>
-      <c r="I85" s="28"/>
-      <c r="J85" s="28"/>
-      <c r="K85" s="28"/>
-      <c r="L85" s="28"/>
+      <c r="H85" s="27">
+        <v>7</v>
+      </c>
+      <c r="I85" s="27">
+        <v>2736</v>
+      </c>
+      <c r="J85" s="27">
+        <v>1412.54</v>
+      </c>
+      <c r="K85" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L85" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="36" t="s">
+      <c r="A86" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B86" s="31" t="s">
+      <c r="B86" s="30" t="s">
         <v>191</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -13852,17 +14025,27 @@
       <c r="E86" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F86" s="31">
+      <c r="F86" s="30">
         <v>200</v>
       </c>
-      <c r="G86" s="34" t="s">
+      <c r="G86" s="32" t="s">
         <v>287</v>
       </c>
-      <c r="H86" s="34"/>
-      <c r="I86" s="34"/>
-      <c r="J86" s="34"/>
-      <c r="K86" s="34"/>
-      <c r="L86" s="34"/>
+      <c r="H86" s="32">
+        <v>4</v>
+      </c>
+      <c r="I86" s="32">
+        <v>2135</v>
+      </c>
+      <c r="J86" s="32">
+        <v>985.32</v>
+      </c>
+      <c r="K86" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L86" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="21" t="s">
@@ -13886,11 +14069,21 @@
       <c r="G87" s="23" t="s">
         <v>288</v>
       </c>
-      <c r="H87" s="23"/>
-      <c r="I87" s="23"/>
-      <c r="J87" s="23"/>
-      <c r="K87" s="23"/>
-      <c r="L87" s="23"/>
+      <c r="H87" s="24">
+        <v>5</v>
+      </c>
+      <c r="I87" s="24">
+        <v>2325</v>
+      </c>
+      <c r="J87" s="24">
+        <v>1127.8699999999999</v>
+      </c>
+      <c r="K87" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L87" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="21" t="s">
@@ -13914,14 +14107,24 @@
       <c r="G88" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="H88" s="23"/>
-      <c r="I88" s="23"/>
-      <c r="J88" s="23"/>
-      <c r="K88" s="23"/>
-      <c r="L88" s="23"/>
+      <c r="H88" s="24">
+        <v>6</v>
+      </c>
+      <c r="I88" s="24">
+        <v>2561</v>
+      </c>
+      <c r="J88" s="24">
+        <v>1283.95</v>
+      </c>
+      <c r="K88" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L88" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="30" t="s">
+      <c r="A89" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B89" s="14" t="s">
@@ -13939,20 +14142,30 @@
       <c r="F89" s="14">
         <v>200</v>
       </c>
-      <c r="G89" s="28" t="s">
+      <c r="G89" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="H89" s="28"/>
-      <c r="I89" s="28"/>
-      <c r="J89" s="28"/>
-      <c r="K89" s="28"/>
-      <c r="L89" s="28"/>
+      <c r="H89" s="27">
+        <v>5</v>
+      </c>
+      <c r="I89" s="27">
+        <v>2360</v>
+      </c>
+      <c r="J89" s="27">
+        <v>1138.05</v>
+      </c>
+      <c r="K89" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L89" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="36" t="s">
+      <c r="A90" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B90" s="31" t="s">
+      <c r="B90" s="30" t="s">
         <v>195</v>
       </c>
       <c r="C90" s="3" t="s">
@@ -13964,17 +14177,27 @@
       <c r="E90" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F90" s="35">
+      <c r="F90" s="33">
         <v>0</v>
       </c>
-      <c r="G90" s="34" t="s">
+      <c r="G90" s="32" t="s">
         <v>291</v>
       </c>
-      <c r="H90" s="34"/>
-      <c r="I90" s="34"/>
-      <c r="J90" s="34"/>
-      <c r="K90" s="34"/>
-      <c r="L90" s="34"/>
+      <c r="H90" s="32">
+        <v>5</v>
+      </c>
+      <c r="I90" s="32">
+        <v>2327</v>
+      </c>
+      <c r="J90" s="32">
+        <v>1104.1500000000001</v>
+      </c>
+      <c r="K90" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L90" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="21" t="s">
@@ -13998,11 +14221,21 @@
       <c r="G91" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="H91" s="23"/>
-      <c r="I91" s="23"/>
-      <c r="J91" s="23"/>
-      <c r="K91" s="23"/>
-      <c r="L91" s="23"/>
+      <c r="H91" s="24">
+        <v>7</v>
+      </c>
+      <c r="I91" s="24">
+        <v>2582</v>
+      </c>
+      <c r="J91" s="24">
+        <v>1341.12</v>
+      </c>
+      <c r="K91" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L91" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="21" t="s">
@@ -14026,14 +14259,24 @@
       <c r="G92" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="H92" s="23"/>
-      <c r="I92" s="23"/>
-      <c r="J92" s="23"/>
-      <c r="K92" s="23"/>
-      <c r="L92" s="23"/>
+      <c r="H92" s="24">
+        <v>7</v>
+      </c>
+      <c r="I92" s="24">
+        <v>2534</v>
+      </c>
+      <c r="J92" s="24">
+        <v>1304.95</v>
+      </c>
+      <c r="K92" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L92" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A93" s="30" t="s">
+      <c r="A93" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B93" s="14" t="s">
@@ -14051,20 +14294,30 @@
       <c r="F93" s="15">
         <v>0</v>
       </c>
-      <c r="G93" s="28" t="s">
+      <c r="G93" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="H93" s="28"/>
-      <c r="I93" s="28"/>
-      <c r="J93" s="28"/>
-      <c r="K93" s="28"/>
-      <c r="L93" s="28"/>
+      <c r="H93" s="27">
+        <v>7</v>
+      </c>
+      <c r="I93" s="27">
+        <v>2736</v>
+      </c>
+      <c r="J93" s="27">
+        <v>1412.54</v>
+      </c>
+      <c r="K93" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L93" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A94" s="36" t="s">
+      <c r="A94" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B94" s="31" t="s">
+      <c r="B94" s="30" t="s">
         <v>199</v>
       </c>
       <c r="C94" s="3" t="s">
@@ -14076,17 +14329,27 @@
       <c r="E94" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F94" s="35">
+      <c r="F94" s="33">
         <v>0</v>
       </c>
-      <c r="G94" s="34" t="s">
+      <c r="G94" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="H94" s="34"/>
-      <c r="I94" s="34"/>
-      <c r="J94" s="34"/>
-      <c r="K94" s="34"/>
-      <c r="L94" s="34"/>
+      <c r="H94" s="32">
+        <v>4</v>
+      </c>
+      <c r="I94" s="32">
+        <v>2135</v>
+      </c>
+      <c r="J94" s="32">
+        <v>985.32</v>
+      </c>
+      <c r="K94" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L94" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="21" t="s">
@@ -14110,11 +14373,21 @@
       <c r="G95" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="H95" s="23"/>
-      <c r="I95" s="23"/>
-      <c r="J95" s="23"/>
-      <c r="K95" s="23"/>
-      <c r="L95" s="23"/>
+      <c r="H95" s="24">
+        <v>5</v>
+      </c>
+      <c r="I95" s="24">
+        <v>2325</v>
+      </c>
+      <c r="J95" s="24">
+        <v>1127.8699999999999</v>
+      </c>
+      <c r="K95" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L95" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="21" t="s">
@@ -14138,14 +14411,24 @@
       <c r="G96" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="H96" s="23"/>
-      <c r="I96" s="23"/>
-      <c r="J96" s="23"/>
-      <c r="K96" s="23"/>
-      <c r="L96" s="23"/>
+      <c r="H96" s="24">
+        <v>6</v>
+      </c>
+      <c r="I96" s="24">
+        <v>2561</v>
+      </c>
+      <c r="J96" s="24">
+        <v>1283.95</v>
+      </c>
+      <c r="K96" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L96" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A97" s="30" t="s">
+      <c r="A97" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B97" s="14" t="s">
@@ -14163,20 +14446,30 @@
       <c r="F97" s="15">
         <v>0</v>
       </c>
-      <c r="G97" s="28" t="s">
+      <c r="G97" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="H97" s="28"/>
-      <c r="I97" s="28"/>
-      <c r="J97" s="28"/>
-      <c r="K97" s="28"/>
-      <c r="L97" s="28"/>
+      <c r="H97" s="27">
+        <v>5</v>
+      </c>
+      <c r="I97" s="27">
+        <v>2288</v>
+      </c>
+      <c r="J97" s="27">
+        <v>1089.8399999999999</v>
+      </c>
+      <c r="K97" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L97" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A98" s="36" t="s">
+      <c r="A98" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B98" s="31" t="s">
+      <c r="B98" s="30" t="s">
         <v>171</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -14188,17 +14481,17 @@
       <c r="E98" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F98" s="31">
+      <c r="F98" s="30">
         <v>40</v>
       </c>
-      <c r="G98" s="34" t="s">
+      <c r="G98" s="32" t="s">
         <v>330</v>
       </c>
-      <c r="H98" s="34"/>
-      <c r="I98" s="34"/>
-      <c r="J98" s="34"/>
-      <c r="K98" s="34"/>
-      <c r="L98" s="34"/>
+      <c r="H98" s="32"/>
+      <c r="I98" s="32"/>
+      <c r="J98" s="32"/>
+      <c r="K98" s="32"/>
+      <c r="L98" s="32"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="21" t="s">
@@ -14257,7 +14550,7 @@
       <c r="L100" s="23"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A101" s="30" t="s">
+      <c r="A101" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B101" s="14" t="s">
@@ -14275,20 +14568,20 @@
       <c r="F101" s="14">
         <v>40</v>
       </c>
-      <c r="G101" s="28" t="s">
+      <c r="G101" s="27" t="s">
         <v>301</v>
       </c>
-      <c r="H101" s="28"/>
-      <c r="I101" s="28"/>
-      <c r="J101" s="28"/>
-      <c r="K101" s="28"/>
-      <c r="L101" s="28"/>
+      <c r="H101" s="27"/>
+      <c r="I101" s="27"/>
+      <c r="J101" s="27"/>
+      <c r="K101" s="27"/>
+      <c r="L101" s="27"/>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A102" s="36" t="s">
+      <c r="A102" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B102" s="31" t="s">
+      <c r="B102" s="30" t="s">
         <v>175</v>
       </c>
       <c r="C102" s="3" t="s">
@@ -14300,17 +14593,17 @@
       <c r="E102" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F102" s="31">
+      <c r="F102" s="30">
         <v>40</v>
       </c>
-      <c r="G102" s="34" t="s">
+      <c r="G102" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="H102" s="34"/>
-      <c r="I102" s="34"/>
-      <c r="J102" s="34"/>
-      <c r="K102" s="34"/>
-      <c r="L102" s="34"/>
+      <c r="H102" s="32"/>
+      <c r="I102" s="32"/>
+      <c r="J102" s="32"/>
+      <c r="K102" s="32"/>
+      <c r="L102" s="32"/>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="21" t="s">
@@ -14369,7 +14662,7 @@
       <c r="L104" s="23"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A105" s="30" t="s">
+      <c r="A105" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B105" s="14" t="s">
@@ -14387,20 +14680,20 @@
       <c r="F105" s="14">
         <v>40</v>
       </c>
-      <c r="G105" s="28" t="s">
+      <c r="G105" s="27" t="s">
         <v>305</v>
       </c>
-      <c r="H105" s="28"/>
-      <c r="I105" s="28"/>
-      <c r="J105" s="28"/>
-      <c r="K105" s="28"/>
-      <c r="L105" s="28"/>
+      <c r="H105" s="27"/>
+      <c r="I105" s="27"/>
+      <c r="J105" s="27"/>
+      <c r="K105" s="27"/>
+      <c r="L105" s="27"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A106" s="36" t="s">
+      <c r="A106" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B106" s="31" t="s">
+      <c r="B106" s="30" t="s">
         <v>179</v>
       </c>
       <c r="C106" s="3" t="s">
@@ -14412,17 +14705,17 @@
       <c r="E106" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F106" s="31">
+      <c r="F106" s="30">
         <v>60</v>
       </c>
-      <c r="G106" s="34" t="s">
+      <c r="G106" s="32" t="s">
         <v>306</v>
       </c>
-      <c r="H106" s="34"/>
-      <c r="I106" s="34"/>
-      <c r="J106" s="34"/>
-      <c r="K106" s="34"/>
-      <c r="L106" s="34"/>
+      <c r="H106" s="32"/>
+      <c r="I106" s="32"/>
+      <c r="J106" s="32"/>
+      <c r="K106" s="32"/>
+      <c r="L106" s="32"/>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="21" t="s">
@@ -14481,7 +14774,7 @@
       <c r="L108" s="23"/>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A109" s="30" t="s">
+      <c r="A109" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B109" s="14" t="s">
@@ -14499,20 +14792,20 @@
       <c r="F109" s="14">
         <v>60</v>
       </c>
-      <c r="G109" s="28" t="s">
+      <c r="G109" s="27" t="s">
         <v>309</v>
       </c>
-      <c r="H109" s="28"/>
-      <c r="I109" s="28"/>
-      <c r="J109" s="28"/>
-      <c r="K109" s="28"/>
-      <c r="L109" s="28"/>
+      <c r="H109" s="27"/>
+      <c r="I109" s="27"/>
+      <c r="J109" s="27"/>
+      <c r="K109" s="27"/>
+      <c r="L109" s="27"/>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A110" s="36" t="s">
+      <c r="A110" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B110" s="31" t="s">
+      <c r="B110" s="30" t="s">
         <v>183</v>
       </c>
       <c r="C110" s="3" t="s">
@@ -14524,17 +14817,17 @@
       <c r="E110" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F110" s="31">
+      <c r="F110" s="30">
         <v>60</v>
       </c>
-      <c r="G110" s="34" t="s">
+      <c r="G110" s="32" t="s">
         <v>310</v>
       </c>
-      <c r="H110" s="34"/>
-      <c r="I110" s="34"/>
-      <c r="J110" s="34"/>
-      <c r="K110" s="34"/>
-      <c r="L110" s="34"/>
+      <c r="H110" s="32"/>
+      <c r="I110" s="32"/>
+      <c r="J110" s="32"/>
+      <c r="K110" s="32"/>
+      <c r="L110" s="32"/>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="21" t="s">
@@ -14593,7 +14886,7 @@
       <c r="L112" s="23"/>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A113" s="30" t="s">
+      <c r="A113" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B113" s="14" t="s">
@@ -14611,20 +14904,20 @@
       <c r="F113" s="14">
         <v>60</v>
       </c>
-      <c r="G113" s="28" t="s">
+      <c r="G113" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="H113" s="28"/>
-      <c r="I113" s="28"/>
-      <c r="J113" s="28"/>
-      <c r="K113" s="28"/>
-      <c r="L113" s="28"/>
+      <c r="H113" s="27"/>
+      <c r="I113" s="27"/>
+      <c r="J113" s="27"/>
+      <c r="K113" s="27"/>
+      <c r="L113" s="27"/>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" s="36" t="s">
+      <c r="A114" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B114" s="31" t="s">
+      <c r="B114" s="30" t="s">
         <v>187</v>
       </c>
       <c r="C114" s="3" t="s">
@@ -14636,17 +14929,17 @@
       <c r="E114" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F114" s="31">
+      <c r="F114" s="30">
         <v>200</v>
       </c>
-      <c r="G114" s="34" t="s">
+      <c r="G114" s="32" t="s">
         <v>314</v>
       </c>
-      <c r="H114" s="34"/>
-      <c r="I114" s="34"/>
-      <c r="J114" s="34"/>
-      <c r="K114" s="34"/>
-      <c r="L114" s="34"/>
+      <c r="H114" s="32"/>
+      <c r="I114" s="32"/>
+      <c r="J114" s="32"/>
+      <c r="K114" s="32"/>
+      <c r="L114" s="32"/>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="21" t="s">
@@ -14705,7 +14998,7 @@
       <c r="L116" s="23"/>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A117" s="30" t="s">
+      <c r="A117" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B117" s="14" t="s">
@@ -14723,20 +15016,20 @@
       <c r="F117" s="14">
         <v>200</v>
       </c>
-      <c r="G117" s="28" t="s">
+      <c r="G117" s="27" t="s">
         <v>317</v>
       </c>
-      <c r="H117" s="28"/>
-      <c r="I117" s="28"/>
-      <c r="J117" s="28"/>
-      <c r="K117" s="28"/>
-      <c r="L117" s="28"/>
+      <c r="H117" s="27"/>
+      <c r="I117" s="27"/>
+      <c r="J117" s="27"/>
+      <c r="K117" s="27"/>
+      <c r="L117" s="27"/>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A118" s="36" t="s">
+      <c r="A118" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B118" s="31" t="s">
+      <c r="B118" s="30" t="s">
         <v>191</v>
       </c>
       <c r="C118" s="3" t="s">
@@ -14748,17 +15041,17 @@
       <c r="E118" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F118" s="31">
+      <c r="F118" s="30">
         <v>200</v>
       </c>
-      <c r="G118" s="34" t="s">
+      <c r="G118" s="32" t="s">
         <v>318</v>
       </c>
-      <c r="H118" s="34"/>
-      <c r="I118" s="34"/>
-      <c r="J118" s="34"/>
-      <c r="K118" s="34"/>
-      <c r="L118" s="34"/>
+      <c r="H118" s="32"/>
+      <c r="I118" s="32"/>
+      <c r="J118" s="32"/>
+      <c r="K118" s="32"/>
+      <c r="L118" s="32"/>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="21" t="s">
@@ -14817,7 +15110,7 @@
       <c r="L120" s="23"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A121" s="30" t="s">
+      <c r="A121" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B121" s="14" t="s">
@@ -14835,20 +15128,20 @@
       <c r="F121" s="14">
         <v>200</v>
       </c>
-      <c r="G121" s="28" t="s">
+      <c r="G121" s="27" t="s">
         <v>321</v>
       </c>
-      <c r="H121" s="28"/>
-      <c r="I121" s="28"/>
-      <c r="J121" s="28"/>
-      <c r="K121" s="28"/>
-      <c r="L121" s="28"/>
+      <c r="H121" s="27"/>
+      <c r="I121" s="27"/>
+      <c r="J121" s="27"/>
+      <c r="K121" s="27"/>
+      <c r="L121" s="27"/>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A122" s="36" t="s">
+      <c r="A122" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B122" s="31" t="s">
+      <c r="B122" s="30" t="s">
         <v>195</v>
       </c>
       <c r="C122" s="3" t="s">
@@ -14860,17 +15153,17 @@
       <c r="E122" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F122" s="35">
+      <c r="F122" s="33">
         <v>0</v>
       </c>
-      <c r="G122" s="34" t="s">
+      <c r="G122" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="H122" s="34"/>
-      <c r="I122" s="34"/>
-      <c r="J122" s="34"/>
-      <c r="K122" s="34"/>
-      <c r="L122" s="34"/>
+      <c r="H122" s="32"/>
+      <c r="I122" s="32"/>
+      <c r="J122" s="32"/>
+      <c r="K122" s="32"/>
+      <c r="L122" s="32"/>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="21" t="s">
@@ -14929,7 +15222,7 @@
       <c r="L124" s="23"/>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A125" s="30" t="s">
+      <c r="A125" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B125" s="14" t="s">
@@ -14947,20 +15240,20 @@
       <c r="F125" s="15">
         <v>0</v>
       </c>
-      <c r="G125" s="28" t="s">
+      <c r="G125" s="27" t="s">
         <v>325</v>
       </c>
-      <c r="H125" s="28"/>
-      <c r="I125" s="28"/>
-      <c r="J125" s="28"/>
-      <c r="K125" s="28"/>
-      <c r="L125" s="28"/>
+      <c r="H125" s="27"/>
+      <c r="I125" s="27"/>
+      <c r="J125" s="27"/>
+      <c r="K125" s="27"/>
+      <c r="L125" s="27"/>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A126" s="36" t="s">
+      <c r="A126" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B126" s="31" t="s">
+      <c r="B126" s="30" t="s">
         <v>199</v>
       </c>
       <c r="C126" s="3" t="s">
@@ -14972,17 +15265,17 @@
       <c r="E126" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F126" s="35">
+      <c r="F126" s="33">
         <v>0</v>
       </c>
-      <c r="G126" s="34" t="s">
+      <c r="G126" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="H126" s="34"/>
-      <c r="I126" s="34"/>
-      <c r="J126" s="34"/>
-      <c r="K126" s="34"/>
-      <c r="L126" s="34"/>
+      <c r="H126" s="32"/>
+      <c r="I126" s="32"/>
+      <c r="J126" s="32"/>
+      <c r="K126" s="32"/>
+      <c r="L126" s="32"/>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="21" t="s">
@@ -15041,7 +15334,7 @@
       <c r="L128" s="23"/>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A129" s="30" t="s">
+      <c r="A129" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B129" s="14" t="s">
@@ -15059,20 +15352,20 @@
       <c r="F129" s="15">
         <v>0</v>
       </c>
-      <c r="G129" s="28" t="s">
+      <c r="G129" s="27" t="s">
         <v>329</v>
       </c>
-      <c r="H129" s="28"/>
-      <c r="I129" s="28"/>
-      <c r="J129" s="28"/>
-      <c r="K129" s="28"/>
-      <c r="L129" s="28"/>
+      <c r="H129" s="27"/>
+      <c r="I129" s="27"/>
+      <c r="J129" s="27"/>
+      <c r="K129" s="27"/>
+      <c r="L129" s="27"/>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A130" s="36" t="s">
+      <c r="A130" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B130" s="31" t="s">
+      <c r="B130" s="30" t="s">
         <v>171</v>
       </c>
       <c r="C130" s="3" t="s">
@@ -15084,17 +15377,17 @@
       <c r="E130" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F130" s="31">
+      <c r="F130" s="30">
         <v>40</v>
       </c>
-      <c r="G130" s="34" t="s">
+      <c r="G130" s="32" t="s">
         <v>361</v>
       </c>
-      <c r="H130" s="34"/>
-      <c r="I130" s="34"/>
-      <c r="J130" s="34"/>
-      <c r="K130" s="34"/>
-      <c r="L130" s="34"/>
+      <c r="H130" s="32"/>
+      <c r="I130" s="32"/>
+      <c r="J130" s="32"/>
+      <c r="K130" s="32"/>
+      <c r="L130" s="32"/>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="21" t="s">
@@ -15153,7 +15446,7 @@
       <c r="L132" s="23"/>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A133" s="30" t="s">
+      <c r="A133" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B133" s="14" t="s">
@@ -15171,20 +15464,20 @@
       <c r="F133" s="14">
         <v>40</v>
       </c>
-      <c r="G133" s="28" t="s">
+      <c r="G133" s="27" t="s">
         <v>332</v>
       </c>
-      <c r="H133" s="28"/>
-      <c r="I133" s="28"/>
-      <c r="J133" s="28"/>
-      <c r="K133" s="28"/>
-      <c r="L133" s="28"/>
+      <c r="H133" s="27"/>
+      <c r="I133" s="27"/>
+      <c r="J133" s="27"/>
+      <c r="K133" s="27"/>
+      <c r="L133" s="27"/>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A134" s="36" t="s">
+      <c r="A134" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B134" s="31" t="s">
+      <c r="B134" s="30" t="s">
         <v>175</v>
       </c>
       <c r="C134" s="3" t="s">
@@ -15196,17 +15489,17 @@
       <c r="E134" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F134" s="31">
+      <c r="F134" s="30">
         <v>40</v>
       </c>
-      <c r="G134" s="34" t="s">
+      <c r="G134" s="32" t="s">
         <v>333</v>
       </c>
-      <c r="H134" s="34"/>
-      <c r="I134" s="34"/>
-      <c r="J134" s="34"/>
-      <c r="K134" s="34"/>
-      <c r="L134" s="34"/>
+      <c r="H134" s="32"/>
+      <c r="I134" s="32"/>
+      <c r="J134" s="32"/>
+      <c r="K134" s="32"/>
+      <c r="L134" s="32"/>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="21" t="s">
@@ -15265,7 +15558,7 @@
       <c r="L136" s="23"/>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A137" s="30" t="s">
+      <c r="A137" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B137" s="14" t="s">
@@ -15283,20 +15576,20 @@
       <c r="F137" s="14">
         <v>40</v>
       </c>
-      <c r="G137" s="28" t="s">
+      <c r="G137" s="27" t="s">
         <v>336</v>
       </c>
-      <c r="H137" s="28"/>
-      <c r="I137" s="28"/>
-      <c r="J137" s="28"/>
-      <c r="K137" s="28"/>
-      <c r="L137" s="28"/>
+      <c r="H137" s="27"/>
+      <c r="I137" s="27"/>
+      <c r="J137" s="27"/>
+      <c r="K137" s="27"/>
+      <c r="L137" s="27"/>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A138" s="36" t="s">
+      <c r="A138" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B138" s="31" t="s">
+      <c r="B138" s="30" t="s">
         <v>179</v>
       </c>
       <c r="C138" s="3" t="s">
@@ -15308,17 +15601,17 @@
       <c r="E138" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F138" s="31">
+      <c r="F138" s="30">
         <v>60</v>
       </c>
-      <c r="G138" s="34" t="s">
+      <c r="G138" s="32" t="s">
         <v>337</v>
       </c>
-      <c r="H138" s="34"/>
-      <c r="I138" s="34"/>
-      <c r="J138" s="34"/>
-      <c r="K138" s="34"/>
-      <c r="L138" s="34"/>
+      <c r="H138" s="32"/>
+      <c r="I138" s="32"/>
+      <c r="J138" s="32"/>
+      <c r="K138" s="32"/>
+      <c r="L138" s="32"/>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="21" t="s">
@@ -15377,7 +15670,7 @@
       <c r="L140" s="23"/>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A141" s="30" t="s">
+      <c r="A141" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B141" s="14" t="s">
@@ -15395,20 +15688,20 @@
       <c r="F141" s="14">
         <v>60</v>
       </c>
-      <c r="G141" s="28" t="s">
+      <c r="G141" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="H141" s="28"/>
-      <c r="I141" s="28"/>
-      <c r="J141" s="28"/>
-      <c r="K141" s="28"/>
-      <c r="L141" s="28"/>
+      <c r="H141" s="27"/>
+      <c r="I141" s="27"/>
+      <c r="J141" s="27"/>
+      <c r="K141" s="27"/>
+      <c r="L141" s="27"/>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A142" s="36" t="s">
+      <c r="A142" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B142" s="31" t="s">
+      <c r="B142" s="30" t="s">
         <v>183</v>
       </c>
       <c r="C142" s="3" t="s">
@@ -15420,17 +15713,17 @@
       <c r="E142" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F142" s="31">
+      <c r="F142" s="30">
         <v>60</v>
       </c>
-      <c r="G142" s="34" t="s">
+      <c r="G142" s="32" t="s">
         <v>341</v>
       </c>
-      <c r="H142" s="34"/>
-      <c r="I142" s="34"/>
-      <c r="J142" s="34"/>
-      <c r="K142" s="34"/>
-      <c r="L142" s="34"/>
+      <c r="H142" s="32"/>
+      <c r="I142" s="32"/>
+      <c r="J142" s="32"/>
+      <c r="K142" s="32"/>
+      <c r="L142" s="32"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="21" t="s">
@@ -15489,7 +15782,7 @@
       <c r="L144" s="23"/>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A145" s="30" t="s">
+      <c r="A145" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B145" s="14" t="s">
@@ -15507,20 +15800,20 @@
       <c r="F145" s="14">
         <v>60</v>
       </c>
-      <c r="G145" s="28" t="s">
+      <c r="G145" s="27" t="s">
         <v>344</v>
       </c>
-      <c r="H145" s="28"/>
-      <c r="I145" s="28"/>
-      <c r="J145" s="28"/>
-      <c r="K145" s="28"/>
-      <c r="L145" s="28"/>
+      <c r="H145" s="27"/>
+      <c r="I145" s="27"/>
+      <c r="J145" s="27"/>
+      <c r="K145" s="27"/>
+      <c r="L145" s="27"/>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A146" s="36" t="s">
+      <c r="A146" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B146" s="31" t="s">
+      <c r="B146" s="30" t="s">
         <v>187</v>
       </c>
       <c r="C146" s="3" t="s">
@@ -15532,17 +15825,17 @@
       <c r="E146" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F146" s="31">
+      <c r="F146" s="30">
         <v>200</v>
       </c>
-      <c r="G146" s="34" t="s">
+      <c r="G146" s="32" t="s">
         <v>345</v>
       </c>
-      <c r="H146" s="34"/>
-      <c r="I146" s="34"/>
-      <c r="J146" s="34"/>
-      <c r="K146" s="34"/>
-      <c r="L146" s="34"/>
+      <c r="H146" s="32"/>
+      <c r="I146" s="32"/>
+      <c r="J146" s="32"/>
+      <c r="K146" s="32"/>
+      <c r="L146" s="32"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="21" t="s">
@@ -15601,7 +15894,7 @@
       <c r="L148" s="23"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A149" s="30" t="s">
+      <c r="A149" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B149" s="14" t="s">
@@ -15619,20 +15912,20 @@
       <c r="F149" s="14">
         <v>200</v>
       </c>
-      <c r="G149" s="28" t="s">
+      <c r="G149" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="H149" s="28"/>
-      <c r="I149" s="28"/>
-      <c r="J149" s="28"/>
-      <c r="K149" s="28"/>
-      <c r="L149" s="28"/>
+      <c r="H149" s="27"/>
+      <c r="I149" s="27"/>
+      <c r="J149" s="27"/>
+      <c r="K149" s="27"/>
+      <c r="L149" s="27"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A150" s="36" t="s">
+      <c r="A150" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B150" s="31" t="s">
+      <c r="B150" s="30" t="s">
         <v>191</v>
       </c>
       <c r="C150" s="3" t="s">
@@ -15644,17 +15937,17 @@
       <c r="E150" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F150" s="31">
+      <c r="F150" s="30">
         <v>200</v>
       </c>
-      <c r="G150" s="34" t="s">
+      <c r="G150" s="32" t="s">
         <v>349</v>
       </c>
-      <c r="H150" s="34"/>
-      <c r="I150" s="34"/>
-      <c r="J150" s="34"/>
-      <c r="K150" s="34"/>
-      <c r="L150" s="34"/>
+      <c r="H150" s="32"/>
+      <c r="I150" s="32"/>
+      <c r="J150" s="32"/>
+      <c r="K150" s="32"/>
+      <c r="L150" s="32"/>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="21" t="s">
@@ -15713,7 +16006,7 @@
       <c r="L152" s="23"/>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A153" s="30" t="s">
+      <c r="A153" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B153" s="14" t="s">
@@ -15731,20 +16024,20 @@
       <c r="F153" s="14">
         <v>200</v>
       </c>
-      <c r="G153" s="28" t="s">
+      <c r="G153" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="H153" s="28"/>
-      <c r="I153" s="28"/>
-      <c r="J153" s="28"/>
-      <c r="K153" s="28"/>
-      <c r="L153" s="28"/>
+      <c r="H153" s="27"/>
+      <c r="I153" s="27"/>
+      <c r="J153" s="27"/>
+      <c r="K153" s="27"/>
+      <c r="L153" s="27"/>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A154" s="36" t="s">
+      <c r="A154" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B154" s="31" t="s">
+      <c r="B154" s="30" t="s">
         <v>195</v>
       </c>
       <c r="C154" s="3" t="s">
@@ -15756,17 +16049,17 @@
       <c r="E154" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F154" s="35">
+      <c r="F154" s="33">
         <v>0</v>
       </c>
-      <c r="G154" s="34" t="s">
+      <c r="G154" s="32" t="s">
         <v>353</v>
       </c>
-      <c r="H154" s="34"/>
-      <c r="I154" s="34"/>
-      <c r="J154" s="34"/>
-      <c r="K154" s="34"/>
-      <c r="L154" s="34"/>
+      <c r="H154" s="32"/>
+      <c r="I154" s="32"/>
+      <c r="J154" s="32"/>
+      <c r="K154" s="32"/>
+      <c r="L154" s="32"/>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="21" t="s">
@@ -15825,7 +16118,7 @@
       <c r="L156" s="23"/>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A157" s="30" t="s">
+      <c r="A157" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B157" s="14" t="s">
@@ -15843,20 +16136,20 @@
       <c r="F157" s="15">
         <v>0</v>
       </c>
-      <c r="G157" s="28" t="s">
+      <c r="G157" s="27" t="s">
         <v>356</v>
       </c>
-      <c r="H157" s="28"/>
-      <c r="I157" s="28"/>
-      <c r="J157" s="28"/>
-      <c r="K157" s="28"/>
-      <c r="L157" s="28"/>
+      <c r="H157" s="27"/>
+      <c r="I157" s="27"/>
+      <c r="J157" s="27"/>
+      <c r="K157" s="27"/>
+      <c r="L157" s="27"/>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A158" s="36" t="s">
+      <c r="A158" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B158" s="31" t="s">
+      <c r="B158" s="30" t="s">
         <v>199</v>
       </c>
       <c r="C158" s="3" t="s">
@@ -15868,17 +16161,17 @@
       <c r="E158" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F158" s="35">
+      <c r="F158" s="33">
         <v>0</v>
       </c>
-      <c r="G158" s="34" t="s">
+      <c r="G158" s="32" t="s">
         <v>357</v>
       </c>
-      <c r="H158" s="34"/>
-      <c r="I158" s="34"/>
-      <c r="J158" s="34"/>
-      <c r="K158" s="34"/>
-      <c r="L158" s="34"/>
+      <c r="H158" s="32"/>
+      <c r="I158" s="32"/>
+      <c r="J158" s="32"/>
+      <c r="K158" s="32"/>
+      <c r="L158" s="32"/>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="21" t="s">
@@ -15937,7 +16230,7 @@
       <c r="L160" s="23"/>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A161" s="30" t="s">
+      <c r="A161" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B161" s="14" t="s">
@@ -15955,14 +16248,14 @@
       <c r="F161" s="15">
         <v>0</v>
       </c>
-      <c r="G161" s="28" t="s">
+      <c r="G161" s="27" t="s">
         <v>360</v>
       </c>
-      <c r="H161" s="28"/>
-      <c r="I161" s="28"/>
-      <c r="J161" s="28"/>
-      <c r="K161" s="28"/>
-      <c r="L161" s="28"/>
+      <c r="H161" s="27"/>
+      <c r="I161" s="27"/>
+      <c r="J161" s="27"/>
+      <c r="K161" s="27"/>
+      <c r="L161" s="27"/>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="21" t="s">

</xml_diff>

<commit_message>
ideal region 4 results
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A091B007-5D4D-48C9-85A5-7CEE10C4B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BC81BF-094A-4EE4-8BD2-88E0CBEAD37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="870" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="870" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="full_model_set" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4205" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4272" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -2286,10 +2286,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4675,11 +4675,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6328,7 +6328,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6886,50 +6886,50 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="I1" s="35" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="I1" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="36"/>
+      <c r="F2" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="G2" s="36"/>
+      <c r="J2" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35" t="s">
+      <c r="K2" s="36"/>
+      <c r="L2" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="M2" s="36"/>
+      <c r="N2" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="35"/>
+      <c r="O2" s="36"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -7161,50 +7161,50 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="I8" s="35" t="s">
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="I8" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35" t="s">
+      <c r="E9" s="36"/>
+      <c r="F9" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="J9" s="35" t="s">
+      <c r="G9" s="36"/>
+      <c r="J9" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35" t="s">
+      <c r="K9" s="36"/>
+      <c r="L9" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35" t="s">
+      <c r="M9" s="36"/>
+      <c r="N9" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O9" s="35"/>
+      <c r="O9" s="36"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
@@ -7436,50 +7436,50 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="I15" s="35" t="s">
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="I15" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35" t="s">
+      <c r="E16" s="36"/>
+      <c r="F16" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="35"/>
-      <c r="J16" s="35" t="s">
+      <c r="G16" s="36"/>
+      <c r="J16" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35" t="s">
+      <c r="K16" s="36"/>
+      <c r="L16" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35" t="s">
+      <c r="M16" s="36"/>
+      <c r="N16" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O16" s="35"/>
+      <c r="O16" s="36"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
@@ -7711,50 +7711,50 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="I22" s="35" t="s">
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="I22" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35" t="s">
+      <c r="C23" s="36"/>
+      <c r="D23" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35" t="s">
+      <c r="E23" s="36"/>
+      <c r="F23" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="35"/>
-      <c r="J23" s="35" t="s">
+      <c r="G23" s="36"/>
+      <c r="J23" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35" t="s">
+      <c r="K23" s="36"/>
+      <c r="L23" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35" t="s">
+      <c r="M23" s="36"/>
+      <c r="N23" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O23" s="35"/>
+      <c r="O23" s="36"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
@@ -7987,50 +7987,50 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="I29" s="35" t="s">
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="I29" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="35"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35" t="s">
+      <c r="C30" s="36"/>
+      <c r="D30" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35" t="s">
+      <c r="E30" s="36"/>
+      <c r="F30" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G30" s="35"/>
-      <c r="J30" s="35" t="s">
+      <c r="G30" s="36"/>
+      <c r="J30" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K30" s="35"/>
-      <c r="L30" s="35" t="s">
+      <c r="K30" s="36"/>
+      <c r="L30" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M30" s="35"/>
-      <c r="N30" s="35" t="s">
+      <c r="M30" s="36"/>
+      <c r="N30" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O30" s="35"/>
+      <c r="O30" s="36"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
@@ -8263,50 +8263,50 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="I36" s="35" t="s">
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="I36" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="J36" s="35"/>
-      <c r="K36" s="35"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="35"/>
-      <c r="N36" s="35"/>
-      <c r="O36" s="35"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35" t="s">
+      <c r="C37" s="36"/>
+      <c r="D37" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35" t="s">
+      <c r="E37" s="36"/>
+      <c r="F37" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G37" s="35"/>
-      <c r="J37" s="35" t="s">
+      <c r="G37" s="36"/>
+      <c r="J37" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K37" s="35"/>
-      <c r="L37" s="35" t="s">
+      <c r="K37" s="36"/>
+      <c r="L37" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M37" s="35"/>
-      <c r="N37" s="35" t="s">
+      <c r="M37" s="36"/>
+      <c r="N37" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O37" s="35"/>
+      <c r="O37" s="36"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
@@ -8539,50 +8539,50 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="I43" s="35" t="s">
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="I43" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="J43" s="35"/>
-      <c r="K43" s="35"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35"/>
-      <c r="O43" s="35"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="36"/>
+      <c r="M43" s="36"/>
+      <c r="N43" s="36"/>
+      <c r="O43" s="36"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35" t="s">
+      <c r="C44" s="36"/>
+      <c r="D44" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35" t="s">
+      <c r="E44" s="36"/>
+      <c r="F44" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G44" s="35"/>
-      <c r="J44" s="35" t="s">
+      <c r="G44" s="36"/>
+      <c r="J44" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K44" s="35"/>
-      <c r="L44" s="35" t="s">
+      <c r="K44" s="36"/>
+      <c r="L44" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M44" s="35"/>
-      <c r="N44" s="35" t="s">
+      <c r="M44" s="36"/>
+      <c r="N44" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O44" s="35"/>
+      <c r="O44" s="36"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
@@ -8816,41 +8816,41 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="I50" s="35" t="s">
+      <c r="A50" s="35"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="I50" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="J50" s="35"/>
-      <c r="K50" s="35"/>
-      <c r="L50" s="35"/>
-      <c r="M50" s="35"/>
-      <c r="N50" s="35"/>
-      <c r="O50" s="35"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="36"/>
+      <c r="L50" s="36"/>
+      <c r="M50" s="36"/>
+      <c r="N50" s="36"/>
+      <c r="O50" s="36"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B51" s="35"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="35"/>
-      <c r="J51" s="35" t="s">
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="36"/>
+      <c r="J51" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K51" s="35"/>
-      <c r="L51" s="35" t="s">
+      <c r="K51" s="36"/>
+      <c r="L51" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="M51" s="35"/>
-      <c r="N51" s="35" t="s">
+      <c r="M51" s="36"/>
+      <c r="N51" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="O51" s="35"/>
+      <c r="O51" s="36"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J52" t="s">
@@ -8981,6 +8981,62 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="I8:O8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="I15:O15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="I22:O22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="I29:O29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="I36:O36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="I43:O43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="N44:O44"/>
     <mergeCell ref="A50:F50"/>
     <mergeCell ref="I50:O50"/>
     <mergeCell ref="B51:C51"/>
@@ -8989,62 +9045,6 @@
     <mergeCell ref="J51:K51"/>
     <mergeCell ref="L51:M51"/>
     <mergeCell ref="N51:O51"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="I43:O43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="I36:O36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="I29:O29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="I22:O22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="I15:O15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="I8:O8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="L32:L35">
     <cfRule type="colorScale" priority="60">
@@ -10495,8 +10495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView tabSelected="1" topLeftCell="B124" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H130" sqref="H130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14488,11 +14488,21 @@
       <c r="G98" s="32" t="s">
         <v>330</v>
       </c>
-      <c r="H98" s="32"/>
-      <c r="I98" s="32"/>
-      <c r="J98" s="32"/>
-      <c r="K98" s="32"/>
-      <c r="L98" s="32"/>
+      <c r="H98" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I98" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J98" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K98" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L98" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="21" t="s">
@@ -14516,11 +14526,21 @@
       <c r="G99" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="H99" s="23"/>
-      <c r="I99" s="23"/>
-      <c r="J99" s="23"/>
-      <c r="K99" s="23"/>
-      <c r="L99" s="23"/>
+      <c r="H99" s="24">
+        <v>6</v>
+      </c>
+      <c r="I99" s="24">
+        <v>1953</v>
+      </c>
+      <c r="J99" s="24">
+        <v>1011.56</v>
+      </c>
+      <c r="K99" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L99" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="21" t="s">
@@ -14544,11 +14564,21 @@
       <c r="G100" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="H100" s="23"/>
-      <c r="I100" s="23"/>
-      <c r="J100" s="23"/>
-      <c r="K100" s="23"/>
-      <c r="L100" s="23"/>
+      <c r="H100" s="24">
+        <v>6</v>
+      </c>
+      <c r="I100" s="24">
+        <v>1980</v>
+      </c>
+      <c r="J100" s="24">
+        <v>1039.4000000000001</v>
+      </c>
+      <c r="K100" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L100" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="29" t="s">
@@ -14572,11 +14602,21 @@
       <c r="G101" s="27" t="s">
         <v>301</v>
       </c>
-      <c r="H101" s="27"/>
-      <c r="I101" s="27"/>
-      <c r="J101" s="27"/>
-      <c r="K101" s="27"/>
-      <c r="L101" s="27"/>
+      <c r="H101" s="27">
+        <v>6</v>
+      </c>
+      <c r="I101" s="27">
+        <v>1946</v>
+      </c>
+      <c r="J101" s="27">
+        <v>997.49</v>
+      </c>
+      <c r="K101" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L101" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="34" t="s">
@@ -14600,11 +14640,21 @@
       <c r="G102" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="H102" s="32"/>
-      <c r="I102" s="32"/>
-      <c r="J102" s="32"/>
-      <c r="K102" s="32"/>
-      <c r="L102" s="32"/>
+      <c r="H102" s="32">
+        <v>5</v>
+      </c>
+      <c r="I102" s="32">
+        <v>2228</v>
+      </c>
+      <c r="J102" s="32">
+        <v>1104.3900000000001</v>
+      </c>
+      <c r="K102" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L102" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="21" t="s">
@@ -14628,11 +14678,21 @@
       <c r="G103" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="H103" s="23"/>
-      <c r="I103" s="23"/>
-      <c r="J103" s="23"/>
-      <c r="K103" s="23"/>
-      <c r="L103" s="23"/>
+      <c r="H103" s="24">
+        <v>5</v>
+      </c>
+      <c r="I103" s="24">
+        <v>1916</v>
+      </c>
+      <c r="J103" s="24">
+        <v>811.71</v>
+      </c>
+      <c r="K103" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L103" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="21" t="s">
@@ -14656,11 +14716,21 @@
       <c r="G104" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="H104" s="23"/>
-      <c r="I104" s="23"/>
-      <c r="J104" s="23"/>
-      <c r="K104" s="23"/>
-      <c r="L104" s="23"/>
+      <c r="H104" s="24">
+        <v>6</v>
+      </c>
+      <c r="I104" s="24">
+        <v>2023</v>
+      </c>
+      <c r="J104" s="24">
+        <v>1048.6199999999999</v>
+      </c>
+      <c r="K104" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L104" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" s="29" t="s">
@@ -14684,11 +14754,21 @@
       <c r="G105" s="27" t="s">
         <v>305</v>
       </c>
-      <c r="H105" s="27"/>
-      <c r="I105" s="27"/>
-      <c r="J105" s="27"/>
-      <c r="K105" s="27"/>
-      <c r="L105" s="27"/>
+      <c r="H105" s="27">
+        <v>5</v>
+      </c>
+      <c r="I105" s="27">
+        <v>2249</v>
+      </c>
+      <c r="J105" s="27">
+        <v>1105.3900000000001</v>
+      </c>
+      <c r="K105" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L105" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" s="34" t="s">
@@ -14712,11 +14792,21 @@
       <c r="G106" s="32" t="s">
         <v>306</v>
       </c>
-      <c r="H106" s="32"/>
-      <c r="I106" s="32"/>
-      <c r="J106" s="32"/>
-      <c r="K106" s="32"/>
-      <c r="L106" s="32"/>
+      <c r="H106" s="32">
+        <v>5</v>
+      </c>
+      <c r="I106" s="32">
+        <v>2024</v>
+      </c>
+      <c r="J106" s="32">
+        <v>946.12</v>
+      </c>
+      <c r="K106" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L106" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" s="21" t="s">
@@ -14740,11 +14830,21 @@
       <c r="G107" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="H107" s="23"/>
-      <c r="I107" s="23"/>
-      <c r="J107" s="23"/>
-      <c r="K107" s="23"/>
-      <c r="L107" s="23"/>
+      <c r="H107" s="24">
+        <v>6</v>
+      </c>
+      <c r="I107" s="24">
+        <v>1942</v>
+      </c>
+      <c r="J107" s="24">
+        <v>999.83</v>
+      </c>
+      <c r="K107" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L107" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" s="21" t="s">
@@ -14768,11 +14868,21 @@
       <c r="G108" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="H108" s="23"/>
-      <c r="I108" s="23"/>
-      <c r="J108" s="23"/>
-      <c r="K108" s="23"/>
-      <c r="L108" s="23"/>
+      <c r="H108" s="24">
+        <v>6</v>
+      </c>
+      <c r="I108" s="24">
+        <v>1973</v>
+      </c>
+      <c r="J108" s="24">
+        <v>1027.52</v>
+      </c>
+      <c r="K108" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L108" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" s="29" t="s">
@@ -14796,11 +14906,21 @@
       <c r="G109" s="27" t="s">
         <v>309</v>
       </c>
-      <c r="H109" s="27"/>
-      <c r="I109" s="27"/>
-      <c r="J109" s="27"/>
-      <c r="K109" s="27"/>
-      <c r="L109" s="27"/>
+      <c r="H109" s="27">
+        <v>6</v>
+      </c>
+      <c r="I109" s="27">
+        <v>1962</v>
+      </c>
+      <c r="J109" s="27">
+        <v>1002.87</v>
+      </c>
+      <c r="K109" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L109" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" s="34" t="s">
@@ -14824,11 +14944,21 @@
       <c r="G110" s="32" t="s">
         <v>310</v>
       </c>
-      <c r="H110" s="32"/>
-      <c r="I110" s="32"/>
-      <c r="J110" s="32"/>
-      <c r="K110" s="32"/>
-      <c r="L110" s="32"/>
+      <c r="H110" s="32">
+        <v>4</v>
+      </c>
+      <c r="I110" s="32">
+        <v>1934</v>
+      </c>
+      <c r="J110" s="32">
+        <v>903.18</v>
+      </c>
+      <c r="K110" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L110" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" s="21" t="s">
@@ -14852,11 +14982,21 @@
       <c r="G111" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="H111" s="23"/>
-      <c r="I111" s="23"/>
-      <c r="J111" s="23"/>
-      <c r="K111" s="23"/>
-      <c r="L111" s="23"/>
+      <c r="H111" s="24">
+        <v>4</v>
+      </c>
+      <c r="I111" s="24">
+        <v>1891</v>
+      </c>
+      <c r="J111" s="24">
+        <v>868.49</v>
+      </c>
+      <c r="K111" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L111" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" s="21" t="s">
@@ -14880,11 +15020,21 @@
       <c r="G112" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="H112" s="23"/>
-      <c r="I112" s="23"/>
-      <c r="J112" s="23"/>
-      <c r="K112" s="23"/>
-      <c r="L112" s="23"/>
+      <c r="H112" s="24">
+        <v>4</v>
+      </c>
+      <c r="I112" s="24">
+        <v>2110</v>
+      </c>
+      <c r="J112" s="24">
+        <v>1023.16</v>
+      </c>
+      <c r="K112" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L112" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" s="29" t="s">
@@ -14908,11 +15058,21 @@
       <c r="G113" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="H113" s="27"/>
-      <c r="I113" s="27"/>
-      <c r="J113" s="27"/>
-      <c r="K113" s="27"/>
-      <c r="L113" s="27"/>
+      <c r="H113" s="27">
+        <v>4</v>
+      </c>
+      <c r="I113" s="27">
+        <v>1935</v>
+      </c>
+      <c r="J113" s="27">
+        <v>900.72</v>
+      </c>
+      <c r="K113" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L113" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="34" t="s">
@@ -14936,11 +15096,21 @@
       <c r="G114" s="32" t="s">
         <v>314</v>
       </c>
-      <c r="H114" s="32"/>
-      <c r="I114" s="32"/>
-      <c r="J114" s="32"/>
-      <c r="K114" s="32"/>
-      <c r="L114" s="32"/>
+      <c r="H114" s="32">
+        <v>5</v>
+      </c>
+      <c r="I114" s="32">
+        <v>1982</v>
+      </c>
+      <c r="J114" s="32">
+        <v>941.06</v>
+      </c>
+      <c r="K114" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L114" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" s="21" t="s">
@@ -14964,11 +15134,21 @@
       <c r="G115" s="23" t="s">
         <v>315</v>
       </c>
-      <c r="H115" s="23"/>
-      <c r="I115" s="23"/>
-      <c r="J115" s="23"/>
-      <c r="K115" s="23"/>
-      <c r="L115" s="23"/>
+      <c r="H115" s="24">
+        <v>6</v>
+      </c>
+      <c r="I115" s="24">
+        <v>1942</v>
+      </c>
+      <c r="J115" s="24">
+        <v>999.83</v>
+      </c>
+      <c r="K115" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L115" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" s="21" t="s">
@@ -14992,11 +15172,21 @@
       <c r="G116" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="H116" s="23"/>
-      <c r="I116" s="23"/>
-      <c r="J116" s="23"/>
-      <c r="K116" s="23"/>
-      <c r="L116" s="23"/>
+      <c r="H116" s="24">
+        <v>5</v>
+      </c>
+      <c r="I116" s="24">
+        <v>2000</v>
+      </c>
+      <c r="J116" s="24">
+        <v>929.49</v>
+      </c>
+      <c r="K116" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L116" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="29" t="s">
@@ -15020,11 +15210,21 @@
       <c r="G117" s="27" t="s">
         <v>317</v>
       </c>
-      <c r="H117" s="27"/>
-      <c r="I117" s="27"/>
-      <c r="J117" s="27"/>
-      <c r="K117" s="27"/>
-      <c r="L117" s="27"/>
+      <c r="H117" s="27">
+        <v>5</v>
+      </c>
+      <c r="I117" s="27">
+        <v>2012</v>
+      </c>
+      <c r="J117" s="27">
+        <v>959.92</v>
+      </c>
+      <c r="K117" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L117" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="34" t="s">
@@ -15048,11 +15248,21 @@
       <c r="G118" s="32" t="s">
         <v>318</v>
       </c>
-      <c r="H118" s="32"/>
-      <c r="I118" s="32"/>
-      <c r="J118" s="32"/>
-      <c r="K118" s="32"/>
-      <c r="L118" s="32"/>
+      <c r="H118" s="32">
+        <v>4</v>
+      </c>
+      <c r="I118" s="32">
+        <v>1916</v>
+      </c>
+      <c r="J118" s="32">
+        <v>881.17</v>
+      </c>
+      <c r="K118" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L118" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="21" t="s">
@@ -15076,11 +15286,21 @@
       <c r="G119" s="23" t="s">
         <v>319</v>
       </c>
-      <c r="H119" s="23"/>
-      <c r="I119" s="23"/>
-      <c r="J119" s="23"/>
-      <c r="K119" s="23"/>
-      <c r="L119" s="23"/>
+      <c r="H119" s="24">
+        <v>4</v>
+      </c>
+      <c r="I119" s="24">
+        <v>1935</v>
+      </c>
+      <c r="J119" s="24">
+        <v>882.19</v>
+      </c>
+      <c r="K119" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L119" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" s="21" t="s">
@@ -15104,11 +15324,21 @@
       <c r="G120" s="23" t="s">
         <v>320</v>
       </c>
-      <c r="H120" s="23"/>
-      <c r="I120" s="23"/>
-      <c r="J120" s="23"/>
-      <c r="K120" s="23"/>
-      <c r="L120" s="23"/>
+      <c r="H120" s="24">
+        <v>4</v>
+      </c>
+      <c r="I120" s="24">
+        <v>1995</v>
+      </c>
+      <c r="J120" s="24">
+        <v>972.51</v>
+      </c>
+      <c r="K120" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L120" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" s="29" t="s">
@@ -15132,11 +15362,21 @@
       <c r="G121" s="27" t="s">
         <v>321</v>
       </c>
-      <c r="H121" s="27"/>
-      <c r="I121" s="27"/>
-      <c r="J121" s="27"/>
-      <c r="K121" s="27"/>
-      <c r="L121" s="27"/>
+      <c r="H121" s="27">
+        <v>4</v>
+      </c>
+      <c r="I121" s="27">
+        <v>2040</v>
+      </c>
+      <c r="J121" s="27">
+        <v>951.6</v>
+      </c>
+      <c r="K121" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L121" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" s="34" t="s">
@@ -15160,11 +15400,21 @@
       <c r="G122" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="H122" s="32"/>
-      <c r="I122" s="32"/>
-      <c r="J122" s="32"/>
-      <c r="K122" s="32"/>
-      <c r="L122" s="32"/>
+      <c r="H122" s="32">
+        <v>5</v>
+      </c>
+      <c r="I122" s="32">
+        <v>1982</v>
+      </c>
+      <c r="J122" s="32">
+        <v>941.06</v>
+      </c>
+      <c r="K122" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L122" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" s="21" t="s">
@@ -15188,11 +15438,21 @@
       <c r="G123" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="H123" s="23"/>
-      <c r="I123" s="23"/>
-      <c r="J123" s="23"/>
-      <c r="K123" s="23"/>
-      <c r="L123" s="23"/>
+      <c r="H123" s="24">
+        <v>6</v>
+      </c>
+      <c r="I123" s="24">
+        <v>1942</v>
+      </c>
+      <c r="J123" s="24">
+        <v>999.83</v>
+      </c>
+      <c r="K123" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L123" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" s="21" t="s">
@@ -15216,11 +15476,21 @@
       <c r="G124" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="H124" s="23"/>
-      <c r="I124" s="23"/>
-      <c r="J124" s="23"/>
-      <c r="K124" s="23"/>
-      <c r="L124" s="23"/>
+      <c r="H124" s="24">
+        <v>5</v>
+      </c>
+      <c r="I124" s="24">
+        <v>2000</v>
+      </c>
+      <c r="J124" s="24">
+        <v>929.49</v>
+      </c>
+      <c r="K124" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L124" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" s="29" t="s">
@@ -15244,11 +15514,21 @@
       <c r="G125" s="27" t="s">
         <v>325</v>
       </c>
-      <c r="H125" s="27"/>
-      <c r="I125" s="27"/>
-      <c r="J125" s="27"/>
-      <c r="K125" s="27"/>
-      <c r="L125" s="27"/>
+      <c r="H125" s="27">
+        <v>5</v>
+      </c>
+      <c r="I125" s="27">
+        <v>2012</v>
+      </c>
+      <c r="J125" s="27">
+        <v>959.92</v>
+      </c>
+      <c r="K125" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L125" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="34" t="s">
@@ -15272,11 +15552,21 @@
       <c r="G126" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="H126" s="32"/>
-      <c r="I126" s="32"/>
-      <c r="J126" s="32"/>
-      <c r="K126" s="32"/>
-      <c r="L126" s="32"/>
+      <c r="H126" s="32">
+        <v>4</v>
+      </c>
+      <c r="I126" s="32">
+        <v>1916</v>
+      </c>
+      <c r="J126" s="32">
+        <v>881.17</v>
+      </c>
+      <c r="K126" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L126" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" s="21" t="s">
@@ -15300,11 +15590,21 @@
       <c r="G127" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="H127" s="23"/>
-      <c r="I127" s="23"/>
-      <c r="J127" s="23"/>
-      <c r="K127" s="23"/>
-      <c r="L127" s="23"/>
+      <c r="H127" s="24">
+        <v>4</v>
+      </c>
+      <c r="I127" s="24">
+        <v>1935</v>
+      </c>
+      <c r="J127" s="24">
+        <v>882.19</v>
+      </c>
+      <c r="K127" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L127" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" s="21" t="s">
@@ -15328,11 +15628,21 @@
       <c r="G128" s="23" t="s">
         <v>328</v>
       </c>
-      <c r="H128" s="23"/>
-      <c r="I128" s="23"/>
-      <c r="J128" s="23"/>
-      <c r="K128" s="23"/>
-      <c r="L128" s="23"/>
+      <c r="H128" s="24">
+        <v>4</v>
+      </c>
+      <c r="I128" s="24">
+        <v>1995</v>
+      </c>
+      <c r="J128" s="24">
+        <v>972.51</v>
+      </c>
+      <c r="K128" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L128" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A129" s="29" t="s">
@@ -15356,11 +15666,21 @@
       <c r="G129" s="27" t="s">
         <v>329</v>
       </c>
-      <c r="H129" s="27"/>
-      <c r="I129" s="27"/>
-      <c r="J129" s="27"/>
-      <c r="K129" s="27"/>
-      <c r="L129" s="27"/>
+      <c r="H129" s="27">
+        <v>4</v>
+      </c>
+      <c r="I129" s="27">
+        <v>2040</v>
+      </c>
+      <c r="J129" s="27">
+        <v>951.6</v>
+      </c>
+      <c r="K129" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L129" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A130" s="34" t="s">

</xml_diff>

<commit_message>
ideal region 5 results
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BC81BF-094A-4EE4-8BD2-88E0CBEAD37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586EE4AF-AAB3-4410-A7A8-BC7E66BDCB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="870" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4272" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4384" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -4676,10 +4676,10 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6328,7 +6328,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10495,8 +10495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B124" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H130" sqref="H130"/>
+    <sheetView tabSelected="1" topLeftCell="C145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H162" sqref="H162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15704,11 +15704,21 @@
       <c r="G130" s="32" t="s">
         <v>361</v>
       </c>
-      <c r="H130" s="32"/>
-      <c r="I130" s="32"/>
-      <c r="J130" s="32"/>
-      <c r="K130" s="32"/>
-      <c r="L130" s="32"/>
+      <c r="H130" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I130" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J130" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="K130" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L130" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A131" s="21" t="s">
@@ -15732,11 +15742,21 @@
       <c r="G131" s="23" t="s">
         <v>362</v>
       </c>
-      <c r="H131" s="23"/>
-      <c r="I131" s="23"/>
-      <c r="J131" s="23"/>
-      <c r="K131" s="23"/>
-      <c r="L131" s="23"/>
+      <c r="H131" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I131" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J131" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K131" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L131" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A132" s="21" t="s">
@@ -15760,11 +15780,21 @@
       <c r="G132" s="23" t="s">
         <v>331</v>
       </c>
-      <c r="H132" s="23"/>
-      <c r="I132" s="23"/>
-      <c r="J132" s="23"/>
-      <c r="K132" s="23"/>
-      <c r="L132" s="23"/>
+      <c r="H132" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I132" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J132" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K132" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L132" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A133" s="29" t="s">
@@ -15788,11 +15818,21 @@
       <c r="G133" s="27" t="s">
         <v>332</v>
       </c>
-      <c r="H133" s="27"/>
-      <c r="I133" s="27"/>
-      <c r="J133" s="27"/>
-      <c r="K133" s="27"/>
-      <c r="L133" s="27"/>
+      <c r="H133" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I133" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J133" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K133" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L133" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A134" s="34" t="s">
@@ -15816,11 +15856,21 @@
       <c r="G134" s="32" t="s">
         <v>333</v>
       </c>
-      <c r="H134" s="32"/>
-      <c r="I134" s="32"/>
-      <c r="J134" s="32"/>
-      <c r="K134" s="32"/>
-      <c r="L134" s="32"/>
+      <c r="H134" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I134" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J134" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="K134" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L134" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A135" s="21" t="s">
@@ -15844,11 +15894,21 @@
       <c r="G135" s="23" t="s">
         <v>334</v>
       </c>
-      <c r="H135" s="23"/>
-      <c r="I135" s="23"/>
-      <c r="J135" s="23"/>
-      <c r="K135" s="23"/>
-      <c r="L135" s="23"/>
+      <c r="H135" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I135" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J135" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K135" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L135" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" s="21" t="s">
@@ -15872,11 +15932,21 @@
       <c r="G136" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="H136" s="23"/>
-      <c r="I136" s="23"/>
-      <c r="J136" s="23"/>
-      <c r="K136" s="23"/>
-      <c r="L136" s="23"/>
+      <c r="H136" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I136" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J136" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K136" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L136" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A137" s="29" t="s">
@@ -15900,11 +15970,21 @@
       <c r="G137" s="27" t="s">
         <v>336</v>
       </c>
-      <c r="H137" s="27"/>
-      <c r="I137" s="27"/>
-      <c r="J137" s="27"/>
-      <c r="K137" s="27"/>
-      <c r="L137" s="27"/>
+      <c r="H137" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I137" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J137" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K137" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L137" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A138" s="34" t="s">
@@ -15928,11 +16008,21 @@
       <c r="G138" s="32" t="s">
         <v>337</v>
       </c>
-      <c r="H138" s="32"/>
-      <c r="I138" s="32"/>
-      <c r="J138" s="32"/>
-      <c r="K138" s="32"/>
-      <c r="L138" s="32"/>
+      <c r="H138" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I138" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J138" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="K138" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L138" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A139" s="21" t="s">
@@ -15956,11 +16046,21 @@
       <c r="G139" s="23" t="s">
         <v>338</v>
       </c>
-      <c r="H139" s="23"/>
-      <c r="I139" s="23"/>
-      <c r="J139" s="23"/>
-      <c r="K139" s="23"/>
-      <c r="L139" s="23"/>
+      <c r="H139" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I139" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J139" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K139" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L139" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" s="21" t="s">
@@ -15984,11 +16084,21 @@
       <c r="G140" s="23" t="s">
         <v>339</v>
       </c>
-      <c r="H140" s="23"/>
-      <c r="I140" s="23"/>
-      <c r="J140" s="23"/>
-      <c r="K140" s="23"/>
-      <c r="L140" s="23"/>
+      <c r="H140" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I140" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J140" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K140" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L140" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A141" s="29" t="s">
@@ -16012,11 +16122,21 @@
       <c r="G141" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="H141" s="27"/>
-      <c r="I141" s="27"/>
-      <c r="J141" s="27"/>
-      <c r="K141" s="27"/>
-      <c r="L141" s="27"/>
+      <c r="H141" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I141" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J141" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K141" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L141" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A142" s="34" t="s">
@@ -16040,11 +16160,21 @@
       <c r="G142" s="32" t="s">
         <v>341</v>
       </c>
-      <c r="H142" s="32"/>
-      <c r="I142" s="32"/>
-      <c r="J142" s="32"/>
-      <c r="K142" s="32"/>
-      <c r="L142" s="32"/>
+      <c r="H142" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I142" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J142" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="K142" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L142" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A143" s="21" t="s">
@@ -16068,11 +16198,21 @@
       <c r="G143" s="23" t="s">
         <v>342</v>
       </c>
-      <c r="H143" s="23"/>
-      <c r="I143" s="23"/>
-      <c r="J143" s="23"/>
-      <c r="K143" s="23"/>
-      <c r="L143" s="23"/>
+      <c r="H143" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I143" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J143" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K143" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L143" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A144" s="21" t="s">
@@ -16096,11 +16236,21 @@
       <c r="G144" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="H144" s="23"/>
-      <c r="I144" s="23"/>
-      <c r="J144" s="23"/>
-      <c r="K144" s="23"/>
-      <c r="L144" s="23"/>
+      <c r="H144" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I144" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J144" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K144" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L144" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A145" s="29" t="s">
@@ -16124,11 +16274,21 @@
       <c r="G145" s="27" t="s">
         <v>344</v>
       </c>
-      <c r="H145" s="27"/>
-      <c r="I145" s="27"/>
-      <c r="J145" s="27"/>
-      <c r="K145" s="27"/>
-      <c r="L145" s="27"/>
+      <c r="H145" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I145" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J145" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K145" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L145" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A146" s="34" t="s">
@@ -16152,11 +16312,21 @@
       <c r="G146" s="32" t="s">
         <v>345</v>
       </c>
-      <c r="H146" s="32"/>
-      <c r="I146" s="32"/>
-      <c r="J146" s="32"/>
-      <c r="K146" s="32"/>
-      <c r="L146" s="32"/>
+      <c r="H146" s="32">
+        <v>6</v>
+      </c>
+      <c r="I146" s="32">
+        <v>2471</v>
+      </c>
+      <c r="J146" s="32">
+        <v>1087.55</v>
+      </c>
+      <c r="K146" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L146" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A147" s="21" t="s">
@@ -16180,11 +16350,21 @@
       <c r="G147" s="23" t="s">
         <v>346</v>
       </c>
-      <c r="H147" s="23"/>
-      <c r="I147" s="23"/>
-      <c r="J147" s="23"/>
-      <c r="K147" s="23"/>
-      <c r="L147" s="23"/>
+      <c r="H147" s="23">
+        <v>6</v>
+      </c>
+      <c r="I147" s="23">
+        <v>2580</v>
+      </c>
+      <c r="J147" s="24">
+        <v>1120.95</v>
+      </c>
+      <c r="K147" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L147" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" s="21" t="s">
@@ -16208,11 +16388,21 @@
       <c r="G148" s="23" t="s">
         <v>347</v>
       </c>
-      <c r="H148" s="23"/>
-      <c r="I148" s="23"/>
-      <c r="J148" s="23"/>
-      <c r="K148" s="23"/>
-      <c r="L148" s="23"/>
+      <c r="H148" s="23">
+        <v>6</v>
+      </c>
+      <c r="I148" s="23">
+        <v>2506</v>
+      </c>
+      <c r="J148" s="24">
+        <v>1088.67</v>
+      </c>
+      <c r="K148" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L148" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A149" s="29" t="s">
@@ -16236,11 +16426,21 @@
       <c r="G149" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="H149" s="27"/>
-      <c r="I149" s="27"/>
-      <c r="J149" s="27"/>
-      <c r="K149" s="27"/>
-      <c r="L149" s="27"/>
+      <c r="H149" s="27">
+        <v>6</v>
+      </c>
+      <c r="I149" s="27">
+        <v>2534</v>
+      </c>
+      <c r="J149" s="27">
+        <v>1113.17</v>
+      </c>
+      <c r="K149" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L149" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" s="34" t="s">
@@ -16264,11 +16464,21 @@
       <c r="G150" s="32" t="s">
         <v>349</v>
       </c>
-      <c r="H150" s="32"/>
-      <c r="I150" s="32"/>
-      <c r="J150" s="32"/>
-      <c r="K150" s="32"/>
-      <c r="L150" s="32"/>
+      <c r="H150" s="32">
+        <v>4</v>
+      </c>
+      <c r="I150" s="32">
+        <v>2353</v>
+      </c>
+      <c r="J150" s="32">
+        <v>1007.94</v>
+      </c>
+      <c r="K150" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L150" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A151" s="21" t="s">
@@ -16292,11 +16502,21 @@
       <c r="G151" s="23" t="s">
         <v>350</v>
       </c>
-      <c r="H151" s="23"/>
-      <c r="I151" s="23"/>
-      <c r="J151" s="23"/>
-      <c r="K151" s="23"/>
-      <c r="L151" s="23"/>
+      <c r="H151" s="24">
+        <v>5</v>
+      </c>
+      <c r="I151" s="24">
+        <v>2434</v>
+      </c>
+      <c r="J151" s="24">
+        <v>1009.44</v>
+      </c>
+      <c r="K151" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L151" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" s="21" t="s">
@@ -16320,11 +16540,21 @@
       <c r="G152" s="23" t="s">
         <v>351</v>
       </c>
-      <c r="H152" s="23"/>
-      <c r="I152" s="23"/>
-      <c r="J152" s="23"/>
-      <c r="K152" s="23"/>
-      <c r="L152" s="23"/>
+      <c r="H152" s="24">
+        <v>5</v>
+      </c>
+      <c r="I152" s="24">
+        <v>2547</v>
+      </c>
+      <c r="J152" s="24">
+        <v>1150.0899999999999</v>
+      </c>
+      <c r="K152" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L152" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A153" s="29" t="s">
@@ -16348,11 +16578,21 @@
       <c r="G153" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="H153" s="27"/>
-      <c r="I153" s="27"/>
-      <c r="J153" s="27"/>
-      <c r="K153" s="27"/>
-      <c r="L153" s="27"/>
+      <c r="H153" s="27">
+        <v>5</v>
+      </c>
+      <c r="I153" s="27">
+        <v>2562</v>
+      </c>
+      <c r="J153" s="27">
+        <v>1156.81</v>
+      </c>
+      <c r="K153" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L153" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" s="34" t="s">
@@ -16376,11 +16616,21 @@
       <c r="G154" s="32" t="s">
         <v>353</v>
       </c>
-      <c r="H154" s="32"/>
-      <c r="I154" s="32"/>
-      <c r="J154" s="32"/>
-      <c r="K154" s="32"/>
-      <c r="L154" s="32"/>
+      <c r="H154" s="32">
+        <v>6</v>
+      </c>
+      <c r="I154" s="32">
+        <v>2471</v>
+      </c>
+      <c r="J154" s="32">
+        <v>1087.55</v>
+      </c>
+      <c r="K154" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L154" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A155" s="21" t="s">
@@ -16404,11 +16654,21 @@
       <c r="G155" s="23" t="s">
         <v>354</v>
       </c>
-      <c r="H155" s="23"/>
-      <c r="I155" s="23"/>
-      <c r="J155" s="23"/>
-      <c r="K155" s="23"/>
-      <c r="L155" s="23"/>
+      <c r="H155" s="24">
+        <v>6</v>
+      </c>
+      <c r="I155" s="24">
+        <v>2551</v>
+      </c>
+      <c r="J155" s="24">
+        <v>1121.22</v>
+      </c>
+      <c r="K155" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L155" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" s="21" t="s">
@@ -16432,11 +16692,21 @@
       <c r="G156" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="H156" s="23"/>
-      <c r="I156" s="23"/>
-      <c r="J156" s="23"/>
-      <c r="K156" s="23"/>
-      <c r="L156" s="23"/>
+      <c r="H156" s="24">
+        <v>6</v>
+      </c>
+      <c r="I156" s="24">
+        <v>2506</v>
+      </c>
+      <c r="J156" s="24">
+        <v>1088.67</v>
+      </c>
+      <c r="K156" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L156" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A157" s="29" t="s">
@@ -16460,11 +16730,21 @@
       <c r="G157" s="27" t="s">
         <v>356</v>
       </c>
-      <c r="H157" s="27"/>
-      <c r="I157" s="27"/>
-      <c r="J157" s="27"/>
-      <c r="K157" s="27"/>
-      <c r="L157" s="27"/>
+      <c r="H157" s="27">
+        <v>6</v>
+      </c>
+      <c r="I157" s="27">
+        <v>2526</v>
+      </c>
+      <c r="J157" s="27">
+        <v>1108.9100000000001</v>
+      </c>
+      <c r="K157" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L157" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" s="34" t="s">
@@ -16488,11 +16768,21 @@
       <c r="G158" s="32" t="s">
         <v>357</v>
       </c>
-      <c r="H158" s="32"/>
-      <c r="I158" s="32"/>
-      <c r="J158" s="32"/>
-      <c r="K158" s="32"/>
-      <c r="L158" s="32"/>
+      <c r="H158" s="32">
+        <v>4</v>
+      </c>
+      <c r="I158" s="32">
+        <v>2353</v>
+      </c>
+      <c r="J158" s="32">
+        <v>1007.94</v>
+      </c>
+      <c r="K158" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L158" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A159" s="21" t="s">
@@ -16516,11 +16806,21 @@
       <c r="G159" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="H159" s="23"/>
-      <c r="I159" s="23"/>
-      <c r="J159" s="23"/>
-      <c r="K159" s="23"/>
-      <c r="L159" s="23"/>
+      <c r="H159" s="24">
+        <v>5</v>
+      </c>
+      <c r="I159" s="24">
+        <v>2434</v>
+      </c>
+      <c r="J159" s="24">
+        <v>1009.34</v>
+      </c>
+      <c r="K159" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L159" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" s="21" t="s">
@@ -16544,11 +16844,21 @@
       <c r="G160" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="H160" s="23"/>
-      <c r="I160" s="23"/>
-      <c r="J160" s="23"/>
-      <c r="K160" s="23"/>
-      <c r="L160" s="23"/>
+      <c r="H160" s="24">
+        <v>5</v>
+      </c>
+      <c r="I160" s="24">
+        <v>2451</v>
+      </c>
+      <c r="J160" s="24">
+        <v>1068.5999999999999</v>
+      </c>
+      <c r="K160" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L160" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A161" s="29" t="s">
@@ -16572,11 +16882,21 @@
       <c r="G161" s="27" t="s">
         <v>360</v>
       </c>
-      <c r="H161" s="27"/>
-      <c r="I161" s="27"/>
-      <c r="J161" s="27"/>
-      <c r="K161" s="27"/>
-      <c r="L161" s="27"/>
+      <c r="H161" s="27">
+        <v>5</v>
+      </c>
+      <c r="I161" s="27">
+        <v>2530</v>
+      </c>
+      <c r="J161" s="27">
+        <v>1131.48</v>
+      </c>
+      <c r="K161" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L161" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A162" s="21" t="s">

</xml_diff>

<commit_message>
ideal region 7 results
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FE7B06-46F6-46F3-9539-0817ADF3D987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B24AC37-5631-47D8-A866-09CCB1E3636A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="870" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4478" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4575" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -4682,10 +4682,10 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10501,8 +10501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C181" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H195" sqref="H195"/>
+    <sheetView tabSelected="1" topLeftCell="C206" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H226" sqref="H226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17844,7 +17844,7 @@
       <c r="I186" s="32">
         <v>2947</v>
       </c>
-      <c r="J186" s="32">
+      <c r="J186" s="40">
         <v>1214.71</v>
       </c>
       <c r="K186" s="32" t="s">
@@ -17958,7 +17958,7 @@
       <c r="I189" s="27">
         <v>3026</v>
       </c>
-      <c r="J189" s="27">
+      <c r="J189" s="42">
         <v>1278.57</v>
       </c>
       <c r="K189" s="27" t="s">
@@ -17996,7 +17996,7 @@
       <c r="I190" s="32">
         <v>2835</v>
       </c>
-      <c r="J190" s="32">
+      <c r="J190" s="40">
         <v>1162.78</v>
       </c>
       <c r="K190" s="32" t="s">
@@ -18034,7 +18034,7 @@
       <c r="I191" s="24">
         <v>2971</v>
       </c>
-      <c r="J191" s="24">
+      <c r="J191" s="38">
         <v>1232.73</v>
       </c>
       <c r="K191" s="24" t="s">
@@ -18072,7 +18072,7 @@
       <c r="I192" s="24">
         <v>3088</v>
       </c>
-      <c r="J192" s="24">
+      <c r="J192" s="38">
         <v>1289.8599999999999</v>
       </c>
       <c r="K192" s="24" t="s">
@@ -18110,7 +18110,7 @@
       <c r="I193" s="27">
         <v>2741</v>
       </c>
-      <c r="J193" s="27">
+      <c r="J193" s="42">
         <v>1069.1300000000001</v>
       </c>
       <c r="K193" s="27" t="s">
@@ -18142,11 +18142,21 @@
       <c r="G194" s="32" t="s">
         <v>679</v>
       </c>
-      <c r="H194" s="32"/>
-      <c r="I194" s="32"/>
-      <c r="J194" s="32"/>
-      <c r="K194" s="32"/>
-      <c r="L194" s="32"/>
+      <c r="H194" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I194" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J194" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="K194" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L194" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A195" s="21" t="s">
@@ -18170,11 +18180,21 @@
       <c r="G195" s="23" t="s">
         <v>680</v>
       </c>
-      <c r="H195" s="23"/>
-      <c r="I195" s="23"/>
-      <c r="J195" s="23"/>
-      <c r="K195" s="23"/>
-      <c r="L195" s="23"/>
+      <c r="H195" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I195" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J195" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K195" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L195" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" s="21" t="s">
@@ -18198,11 +18218,21 @@
       <c r="G196" s="23" t="s">
         <v>681</v>
       </c>
-      <c r="H196" s="23"/>
-      <c r="I196" s="23"/>
-      <c r="J196" s="23"/>
-      <c r="K196" s="23"/>
-      <c r="L196" s="23"/>
+      <c r="H196" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I196" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J196" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K196" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L196" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A197" s="21" t="s">
@@ -18226,11 +18256,21 @@
       <c r="G197" s="27" t="s">
         <v>682</v>
       </c>
-      <c r="H197" s="27"/>
-      <c r="I197" s="27"/>
-      <c r="J197" s="27"/>
-      <c r="K197" s="27"/>
-      <c r="L197" s="27"/>
+      <c r="H197" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I197" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J197" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K197" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L197" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" s="21" t="s">
@@ -18254,11 +18294,21 @@
       <c r="G198" s="32" t="s">
         <v>395</v>
       </c>
-      <c r="H198" s="32"/>
-      <c r="I198" s="32"/>
-      <c r="J198" s="32"/>
-      <c r="K198" s="32"/>
-      <c r="L198" s="32"/>
+      <c r="H198" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I198" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J198" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="K198" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L198" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A199" s="21" t="s">
@@ -18282,11 +18332,21 @@
       <c r="G199" s="23" t="s">
         <v>396</v>
       </c>
-      <c r="H199" s="23"/>
-      <c r="I199" s="23"/>
-      <c r="J199" s="23"/>
-      <c r="K199" s="23"/>
-      <c r="L199" s="23"/>
+      <c r="H199" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I199" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J199" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K199" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L199" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" s="21" t="s">
@@ -18310,11 +18370,21 @@
       <c r="G200" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="H200" s="23"/>
-      <c r="I200" s="23"/>
-      <c r="J200" s="23"/>
-      <c r="K200" s="23"/>
-      <c r="L200" s="23"/>
+      <c r="H200" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I200" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J200" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K200" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L200" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A201" s="21" t="s">
@@ -18338,11 +18408,21 @@
       <c r="G201" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="H201" s="27"/>
-      <c r="I201" s="27"/>
-      <c r="J201" s="27"/>
-      <c r="K201" s="27"/>
-      <c r="L201" s="27"/>
+      <c r="H201" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I201" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J201" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K201" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L201" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" s="21" t="s">
@@ -18366,11 +18446,21 @@
       <c r="G202" s="32" t="s">
         <v>399</v>
       </c>
-      <c r="H202" s="32"/>
-      <c r="I202" s="32"/>
-      <c r="J202" s="32"/>
-      <c r="K202" s="32"/>
-      <c r="L202" s="32"/>
+      <c r="H202" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I202" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J202" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="K202" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L202" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A203" s="21" t="s">
@@ -18394,11 +18484,21 @@
       <c r="G203" s="23" t="s">
         <v>400</v>
       </c>
-      <c r="H203" s="23"/>
-      <c r="I203" s="23"/>
-      <c r="J203" s="23"/>
-      <c r="K203" s="23"/>
-      <c r="L203" s="23"/>
+      <c r="H203" s="23">
+        <v>12</v>
+      </c>
+      <c r="I203" s="23">
+        <v>2393</v>
+      </c>
+      <c r="J203" s="38">
+        <v>1102.03</v>
+      </c>
+      <c r="K203" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L203" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A204" s="21" t="s">
@@ -18422,11 +18522,21 @@
       <c r="G204" s="23" t="s">
         <v>401</v>
       </c>
-      <c r="H204" s="23"/>
-      <c r="I204" s="23"/>
-      <c r="J204" s="23"/>
-      <c r="K204" s="23"/>
-      <c r="L204" s="23"/>
+      <c r="H204" s="23">
+        <v>12</v>
+      </c>
+      <c r="I204" s="23">
+        <v>2355</v>
+      </c>
+      <c r="J204" s="38">
+        <v>1088.9100000000001</v>
+      </c>
+      <c r="K204" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L204" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A205" s="21" t="s">
@@ -18450,11 +18560,21 @@
       <c r="G205" s="27" t="s">
         <v>402</v>
       </c>
-      <c r="H205" s="27"/>
-      <c r="I205" s="27"/>
-      <c r="J205" s="27"/>
-      <c r="K205" s="27"/>
-      <c r="L205" s="27"/>
+      <c r="H205" s="27">
+        <v>12</v>
+      </c>
+      <c r="I205" s="27">
+        <v>2352</v>
+      </c>
+      <c r="J205" s="42">
+        <v>1067.8399999999999</v>
+      </c>
+      <c r="K205" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L205" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A206" s="21" t="s">
@@ -18478,11 +18598,21 @@
       <c r="G206" s="32" t="s">
         <v>403</v>
       </c>
-      <c r="H206" s="32"/>
-      <c r="I206" s="32"/>
-      <c r="J206" s="32"/>
-      <c r="K206" s="32"/>
-      <c r="L206" s="32"/>
+      <c r="H206" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I206" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J206" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="K206" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L206" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A207" s="21" t="s">
@@ -18506,11 +18636,21 @@
       <c r="G207" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="H207" s="23"/>
-      <c r="I207" s="23"/>
-      <c r="J207" s="23"/>
-      <c r="K207" s="23"/>
-      <c r="L207" s="23"/>
+      <c r="H207" s="23">
+        <v>12</v>
+      </c>
+      <c r="I207" s="23">
+        <v>2393</v>
+      </c>
+      <c r="J207" s="38">
+        <v>1102.03</v>
+      </c>
+      <c r="K207" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L207" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A208" s="21" t="s">
@@ -18534,11 +18674,21 @@
       <c r="G208" s="23" t="s">
         <v>405</v>
       </c>
-      <c r="H208" s="23"/>
-      <c r="I208" s="23"/>
-      <c r="J208" s="23"/>
-      <c r="K208" s="23"/>
-      <c r="L208" s="23"/>
+      <c r="H208" s="23">
+        <v>12</v>
+      </c>
+      <c r="I208" s="23">
+        <v>2355</v>
+      </c>
+      <c r="J208" s="38">
+        <v>1088.9100000000001</v>
+      </c>
+      <c r="K208" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L208" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A209" s="21" t="s">
@@ -18562,11 +18712,21 @@
       <c r="G209" s="27" t="s">
         <v>406</v>
       </c>
-      <c r="H209" s="27"/>
-      <c r="I209" s="27"/>
-      <c r="J209" s="27"/>
-      <c r="K209" s="27"/>
-      <c r="L209" s="27"/>
+      <c r="H209" s="27">
+        <v>12</v>
+      </c>
+      <c r="I209" s="27">
+        <v>2352</v>
+      </c>
+      <c r="J209" s="42">
+        <v>1067.8399999999999</v>
+      </c>
+      <c r="K209" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L209" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A210" s="21" t="s">
@@ -18590,11 +18750,21 @@
       <c r="G210" s="32" t="s">
         <v>407</v>
       </c>
-      <c r="H210" s="32"/>
-      <c r="I210" s="32"/>
-      <c r="J210" s="32"/>
-      <c r="K210" s="32"/>
-      <c r="L210" s="32"/>
+      <c r="H210" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I210" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J210" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="K210" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L210" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A211" s="21" t="s">
@@ -18618,11 +18788,21 @@
       <c r="G211" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="H211" s="23"/>
-      <c r="I211" s="23"/>
-      <c r="J211" s="23"/>
-      <c r="K211" s="23"/>
-      <c r="L211" s="23"/>
+      <c r="H211" s="24">
+        <v>5</v>
+      </c>
+      <c r="I211" s="24">
+        <v>1993</v>
+      </c>
+      <c r="J211" s="38">
+        <v>736.03</v>
+      </c>
+      <c r="K211" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L211" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A212" s="21" t="s">
@@ -18646,11 +18826,21 @@
       <c r="G212" s="23" t="s">
         <v>409</v>
       </c>
-      <c r="H212" s="23"/>
-      <c r="I212" s="23"/>
-      <c r="J212" s="23"/>
-      <c r="K212" s="23"/>
-      <c r="L212" s="23"/>
+      <c r="H212" s="24">
+        <v>5</v>
+      </c>
+      <c r="I212" s="24">
+        <v>1917</v>
+      </c>
+      <c r="J212" s="38">
+        <v>659.01</v>
+      </c>
+      <c r="K212" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L212" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A213" s="21" t="s">
@@ -18674,11 +18864,21 @@
       <c r="G213" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="H213" s="27"/>
-      <c r="I213" s="27"/>
-      <c r="J213" s="27"/>
-      <c r="K213" s="27"/>
-      <c r="L213" s="27"/>
+      <c r="H213" s="27">
+        <v>5</v>
+      </c>
+      <c r="I213" s="27">
+        <v>2015</v>
+      </c>
+      <c r="J213" s="42">
+        <v>726.21</v>
+      </c>
+      <c r="K213" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L213" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A214" s="21" t="s">
@@ -18702,11 +18902,21 @@
       <c r="G214" s="32" t="s">
         <v>411</v>
       </c>
-      <c r="H214" s="32"/>
-      <c r="I214" s="32"/>
-      <c r="J214" s="32"/>
-      <c r="K214" s="32"/>
-      <c r="L214" s="32"/>
+      <c r="H214" s="32">
+        <v>4</v>
+      </c>
+      <c r="I214" s="32">
+        <v>1894</v>
+      </c>
+      <c r="J214" s="40">
+        <v>655.47</v>
+      </c>
+      <c r="K214" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L214" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A215" s="21" t="s">
@@ -18730,11 +18940,21 @@
       <c r="G215" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="H215" s="23"/>
-      <c r="I215" s="23"/>
-      <c r="J215" s="23"/>
-      <c r="K215" s="23"/>
-      <c r="L215" s="23"/>
+      <c r="H215" s="24">
+        <v>4</v>
+      </c>
+      <c r="I215" s="24">
+        <v>1916</v>
+      </c>
+      <c r="J215" s="38">
+        <v>646.29999999999995</v>
+      </c>
+      <c r="K215" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L215" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A216" s="21" t="s">
@@ -18758,11 +18978,21 @@
       <c r="G216" s="23" t="s">
         <v>413</v>
       </c>
-      <c r="H216" s="23"/>
-      <c r="I216" s="23"/>
-      <c r="J216" s="23"/>
-      <c r="K216" s="23"/>
-      <c r="L216" s="23"/>
+      <c r="H216" s="24">
+        <v>4</v>
+      </c>
+      <c r="I216" s="24">
+        <v>1916</v>
+      </c>
+      <c r="J216" s="41">
+        <v>685.69</v>
+      </c>
+      <c r="K216" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L216" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A217" s="21" t="s">
@@ -18786,11 +19016,21 @@
       <c r="G217" s="27" t="s">
         <v>414</v>
       </c>
-      <c r="H217" s="27"/>
-      <c r="I217" s="27"/>
-      <c r="J217" s="27"/>
-      <c r="K217" s="27"/>
-      <c r="L217" s="27"/>
+      <c r="H217" s="27">
+        <v>4</v>
+      </c>
+      <c r="I217" s="27">
+        <v>1931</v>
+      </c>
+      <c r="J217" s="42">
+        <v>678.42</v>
+      </c>
+      <c r="K217" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L217" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A218" s="21" t="s">
@@ -18814,11 +19054,21 @@
       <c r="G218" s="32" t="s">
         <v>415</v>
       </c>
-      <c r="H218" s="32"/>
-      <c r="I218" s="32"/>
-      <c r="J218" s="32"/>
-      <c r="K218" s="32"/>
-      <c r="L218" s="32"/>
+      <c r="H218" s="32">
+        <v>4</v>
+      </c>
+      <c r="I218" s="32">
+        <v>1884</v>
+      </c>
+      <c r="J218" s="40">
+        <v>626.70000000000005</v>
+      </c>
+      <c r="K218" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L218" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A219" s="21" t="s">
@@ -18842,11 +19092,21 @@
       <c r="G219" s="23" t="s">
         <v>416</v>
       </c>
-      <c r="H219" s="23"/>
-      <c r="I219" s="23"/>
-      <c r="J219" s="23"/>
-      <c r="K219" s="23"/>
-      <c r="L219" s="23"/>
+      <c r="H219" s="24">
+        <v>5</v>
+      </c>
+      <c r="I219" s="24">
+        <v>1980</v>
+      </c>
+      <c r="J219" s="41">
+        <v>697.12</v>
+      </c>
+      <c r="K219" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L219" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A220" s="21" t="s">
@@ -18870,11 +19130,21 @@
       <c r="G220" s="23" t="s">
         <v>417</v>
       </c>
-      <c r="H220" s="23"/>
-      <c r="I220" s="23"/>
-      <c r="J220" s="23"/>
-      <c r="K220" s="23"/>
-      <c r="L220" s="23"/>
+      <c r="H220" s="24">
+        <v>5</v>
+      </c>
+      <c r="I220" s="24">
+        <v>1975</v>
+      </c>
+      <c r="J220" s="41">
+        <v>708.27</v>
+      </c>
+      <c r="K220" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L220" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A221" s="21" t="s">
@@ -18898,11 +19168,21 @@
       <c r="G221" s="27" t="s">
         <v>418</v>
       </c>
-      <c r="H221" s="27"/>
-      <c r="I221" s="27"/>
-      <c r="J221" s="27"/>
-      <c r="K221" s="27"/>
-      <c r="L221" s="27"/>
+      <c r="H221" s="27">
+        <v>5</v>
+      </c>
+      <c r="I221" s="27">
+        <v>2003</v>
+      </c>
+      <c r="J221" s="42">
+        <v>708.46</v>
+      </c>
+      <c r="K221" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L221" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A222" s="21" t="s">
@@ -18926,11 +19206,21 @@
       <c r="G222" s="32" t="s">
         <v>419</v>
       </c>
-      <c r="H222" s="32"/>
-      <c r="I222" s="32"/>
-      <c r="J222" s="32"/>
-      <c r="K222" s="32"/>
-      <c r="L222" s="32"/>
+      <c r="H222" s="32">
+        <v>4</v>
+      </c>
+      <c r="I222" s="32">
+        <v>1861</v>
+      </c>
+      <c r="J222" s="40">
+        <v>626.24</v>
+      </c>
+      <c r="K222" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L222" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A223" s="21" t="s">
@@ -18954,11 +19244,21 @@
       <c r="G223" s="23" t="s">
         <v>420</v>
       </c>
-      <c r="H223" s="23"/>
-      <c r="I223" s="23"/>
-      <c r="J223" s="23"/>
-      <c r="K223" s="23"/>
-      <c r="L223" s="23"/>
+      <c r="H223" s="24">
+        <v>4</v>
+      </c>
+      <c r="I223" s="24">
+        <v>1898</v>
+      </c>
+      <c r="J223" s="41">
+        <v>660.32</v>
+      </c>
+      <c r="K223" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L223" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A224" s="21" t="s">
@@ -18982,11 +19282,21 @@
       <c r="G224" s="23" t="s">
         <v>421</v>
       </c>
-      <c r="H224" s="23"/>
-      <c r="I224" s="23"/>
-      <c r="J224" s="23"/>
-      <c r="K224" s="23"/>
-      <c r="L224" s="23"/>
+      <c r="H224" s="24">
+        <v>4</v>
+      </c>
+      <c r="I224" s="24">
+        <v>1803</v>
+      </c>
+      <c r="J224" s="41">
+        <v>589.07000000000005</v>
+      </c>
+      <c r="K224" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L224" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A225" s="21" t="s">
@@ -19010,11 +19320,21 @@
       <c r="G225" s="27" t="s">
         <v>422</v>
       </c>
-      <c r="H225" s="27"/>
-      <c r="I225" s="27"/>
-      <c r="J225" s="27"/>
-      <c r="K225" s="27"/>
-      <c r="L225" s="27"/>
+      <c r="H225" s="27">
+        <v>4</v>
+      </c>
+      <c r="I225" s="27">
+        <v>1938</v>
+      </c>
+      <c r="J225" s="42">
+        <v>674.69</v>
+      </c>
+      <c r="K225" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L225" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A226" s="21" t="s">
@@ -19040,7 +19360,7 @@
       </c>
       <c r="H226" s="32"/>
       <c r="I226" s="32"/>
-      <c r="J226" s="32"/>
+      <c r="J226" s="40"/>
       <c r="K226" s="32"/>
       <c r="L226" s="32"/>
     </row>
@@ -19068,7 +19388,7 @@
       </c>
       <c r="H227" s="23"/>
       <c r="I227" s="23"/>
-      <c r="J227" s="23"/>
+      <c r="J227" s="41"/>
       <c r="K227" s="23"/>
       <c r="L227" s="23"/>
     </row>
@@ -19096,7 +19416,7 @@
       </c>
       <c r="H228" s="23"/>
       <c r="I228" s="23"/>
-      <c r="J228" s="23"/>
+      <c r="J228" s="41"/>
       <c r="K228" s="23"/>
       <c r="L228" s="23"/>
     </row>
@@ -19124,7 +19444,7 @@
       </c>
       <c r="H229" s="27"/>
       <c r="I229" s="27"/>
-      <c r="J229" s="27"/>
+      <c r="J229" s="42"/>
       <c r="K229" s="27"/>
       <c r="L229" s="27"/>
     </row>
@@ -19152,7 +19472,7 @@
       </c>
       <c r="H230" s="32"/>
       <c r="I230" s="32"/>
-      <c r="J230" s="32"/>
+      <c r="J230" s="40"/>
       <c r="K230" s="32"/>
       <c r="L230" s="32"/>
     </row>
@@ -19180,7 +19500,7 @@
       </c>
       <c r="H231" s="23"/>
       <c r="I231" s="23"/>
-      <c r="J231" s="23"/>
+      <c r="J231" s="41"/>
       <c r="K231" s="23"/>
       <c r="L231" s="23"/>
     </row>
@@ -19208,7 +19528,7 @@
       </c>
       <c r="H232" s="23"/>
       <c r="I232" s="23"/>
-      <c r="J232" s="23"/>
+      <c r="J232" s="41"/>
       <c r="K232" s="23"/>
       <c r="L232" s="23"/>
     </row>
@@ -19236,7 +19556,7 @@
       </c>
       <c r="H233" s="27"/>
       <c r="I233" s="27"/>
-      <c r="J233" s="27"/>
+      <c r="J233" s="42"/>
       <c r="K233" s="27"/>
       <c r="L233" s="27"/>
     </row>
@@ -19264,7 +19584,7 @@
       </c>
       <c r="H234" s="32"/>
       <c r="I234" s="32"/>
-      <c r="J234" s="32"/>
+      <c r="J234" s="40"/>
       <c r="K234" s="32"/>
       <c r="L234" s="32"/>
     </row>
@@ -19292,7 +19612,7 @@
       </c>
       <c r="H235" s="23"/>
       <c r="I235" s="23"/>
-      <c r="J235" s="23"/>
+      <c r="J235" s="41"/>
       <c r="K235" s="23"/>
       <c r="L235" s="23"/>
     </row>
@@ -19320,7 +19640,7 @@
       </c>
       <c r="H236" s="23"/>
       <c r="I236" s="23"/>
-      <c r="J236" s="23"/>
+      <c r="J236" s="41"/>
       <c r="K236" s="23"/>
       <c r="L236" s="23"/>
     </row>
@@ -19348,7 +19668,7 @@
       </c>
       <c r="H237" s="27"/>
       <c r="I237" s="27"/>
-      <c r="J237" s="27"/>
+      <c r="J237" s="42"/>
       <c r="K237" s="27"/>
       <c r="L237" s="27"/>
     </row>
@@ -19376,7 +19696,7 @@
       </c>
       <c r="H238" s="32"/>
       <c r="I238" s="32"/>
-      <c r="J238" s="32"/>
+      <c r="J238" s="40"/>
       <c r="K238" s="32"/>
       <c r="L238" s="32"/>
     </row>
@@ -19404,7 +19724,7 @@
       </c>
       <c r="H239" s="23"/>
       <c r="I239" s="23"/>
-      <c r="J239" s="23"/>
+      <c r="J239" s="41"/>
       <c r="K239" s="23"/>
       <c r="L239" s="23"/>
     </row>
@@ -19432,7 +19752,7 @@
       </c>
       <c r="H240" s="23"/>
       <c r="I240" s="23"/>
-      <c r="J240" s="23"/>
+      <c r="J240" s="41"/>
       <c r="K240" s="23"/>
       <c r="L240" s="23"/>
     </row>
@@ -19460,7 +19780,7 @@
       </c>
       <c r="H241" s="27"/>
       <c r="I241" s="27"/>
-      <c r="J241" s="27"/>
+      <c r="J241" s="42"/>
       <c r="K241" s="27"/>
       <c r="L241" s="27"/>
     </row>
@@ -19488,7 +19808,7 @@
       </c>
       <c r="H242" s="32"/>
       <c r="I242" s="32"/>
-      <c r="J242" s="32"/>
+      <c r="J242" s="40"/>
       <c r="K242" s="32"/>
       <c r="L242" s="32"/>
     </row>
@@ -19516,7 +19836,7 @@
       </c>
       <c r="H243" s="23"/>
       <c r="I243" s="23"/>
-      <c r="J243" s="23"/>
+      <c r="J243" s="41"/>
       <c r="K243" s="23"/>
       <c r="L243" s="23"/>
     </row>
@@ -19544,7 +19864,7 @@
       </c>
       <c r="H244" s="23"/>
       <c r="I244" s="23"/>
-      <c r="J244" s="23"/>
+      <c r="J244" s="41"/>
       <c r="K244" s="23"/>
       <c r="L244" s="23"/>
     </row>
@@ -19572,7 +19892,7 @@
       </c>
       <c r="H245" s="27"/>
       <c r="I245" s="27"/>
-      <c r="J245" s="27"/>
+      <c r="J245" s="42"/>
       <c r="K245" s="27"/>
       <c r="L245" s="27"/>
     </row>
@@ -19600,7 +19920,7 @@
       </c>
       <c r="H246" s="32"/>
       <c r="I246" s="32"/>
-      <c r="J246" s="32"/>
+      <c r="J246" s="40"/>
       <c r="K246" s="32"/>
       <c r="L246" s="32"/>
     </row>
@@ -19628,7 +19948,7 @@
       </c>
       <c r="H247" s="23"/>
       <c r="I247" s="23"/>
-      <c r="J247" s="23"/>
+      <c r="J247" s="41"/>
       <c r="K247" s="23"/>
       <c r="L247" s="23"/>
     </row>
@@ -19656,7 +19976,7 @@
       </c>
       <c r="H248" s="23"/>
       <c r="I248" s="23"/>
-      <c r="J248" s="23"/>
+      <c r="J248" s="41"/>
       <c r="K248" s="23"/>
       <c r="L248" s="23"/>
     </row>
@@ -19684,7 +20004,7 @@
       </c>
       <c r="H249" s="27"/>
       <c r="I249" s="27"/>
-      <c r="J249" s="27"/>
+      <c r="J249" s="42"/>
       <c r="K249" s="27"/>
       <c r="L249" s="27"/>
     </row>
@@ -19712,7 +20032,7 @@
       </c>
       <c r="H250" s="32"/>
       <c r="I250" s="32"/>
-      <c r="J250" s="32"/>
+      <c r="J250" s="40"/>
       <c r="K250" s="32"/>
       <c r="L250" s="32"/>
     </row>
@@ -19740,7 +20060,7 @@
       </c>
       <c r="H251" s="23"/>
       <c r="I251" s="23"/>
-      <c r="J251" s="23"/>
+      <c r="J251" s="41"/>
       <c r="K251" s="23"/>
       <c r="L251" s="23"/>
     </row>
@@ -19768,7 +20088,7 @@
       </c>
       <c r="H252" s="23"/>
       <c r="I252" s="23"/>
-      <c r="J252" s="23"/>
+      <c r="J252" s="41"/>
       <c r="K252" s="23"/>
       <c r="L252" s="23"/>
     </row>
@@ -19796,7 +20116,7 @@
       </c>
       <c r="H253" s="27"/>
       <c r="I253" s="27"/>
-      <c r="J253" s="27"/>
+      <c r="J253" s="42"/>
       <c r="K253" s="27"/>
       <c r="L253" s="27"/>
     </row>
@@ -19824,7 +20144,7 @@
       </c>
       <c r="H254" s="32"/>
       <c r="I254" s="32"/>
-      <c r="J254" s="32"/>
+      <c r="J254" s="40"/>
       <c r="K254" s="32"/>
       <c r="L254" s="32"/>
     </row>
@@ -19852,7 +20172,7 @@
       </c>
       <c r="H255" s="23"/>
       <c r="I255" s="23"/>
-      <c r="J255" s="23"/>
+      <c r="J255" s="41"/>
       <c r="K255" s="23"/>
       <c r="L255" s="23"/>
     </row>
@@ -19880,7 +20200,7 @@
       </c>
       <c r="H256" s="23"/>
       <c r="I256" s="23"/>
-      <c r="J256" s="23"/>
+      <c r="J256" s="41"/>
       <c r="K256" s="23"/>
       <c r="L256" s="23"/>
     </row>
@@ -19908,7 +20228,7 @@
       </c>
       <c r="H257" s="27"/>
       <c r="I257" s="27"/>
-      <c r="J257" s="27"/>
+      <c r="J257" s="42"/>
       <c r="K257" s="27"/>
       <c r="L257" s="27"/>
     </row>
@@ -19936,7 +20256,7 @@
       </c>
       <c r="H258" s="32"/>
       <c r="I258" s="32"/>
-      <c r="J258" s="32"/>
+      <c r="J258" s="40"/>
       <c r="K258" s="32"/>
       <c r="L258" s="32"/>
     </row>
@@ -19964,7 +20284,7 @@
       </c>
       <c r="H259" s="23"/>
       <c r="I259" s="23"/>
-      <c r="J259" s="23"/>
+      <c r="J259" s="41"/>
       <c r="K259" s="23"/>
       <c r="L259" s="23"/>
     </row>
@@ -19992,7 +20312,7 @@
       </c>
       <c r="H260" s="23"/>
       <c r="I260" s="23"/>
-      <c r="J260" s="23"/>
+      <c r="J260" s="41"/>
       <c r="K260" s="23"/>
       <c r="L260" s="23"/>
     </row>
@@ -20020,7 +20340,7 @@
       </c>
       <c r="H261" s="27"/>
       <c r="I261" s="27"/>
-      <c r="J261" s="27"/>
+      <c r="J261" s="42"/>
       <c r="K261" s="27"/>
       <c r="L261" s="27"/>
     </row>
@@ -20048,7 +20368,7 @@
       </c>
       <c r="H262" s="32"/>
       <c r="I262" s="32"/>
-      <c r="J262" s="32"/>
+      <c r="J262" s="40"/>
       <c r="K262" s="32"/>
       <c r="L262" s="32"/>
     </row>
@@ -20076,7 +20396,7 @@
       </c>
       <c r="H263" s="23"/>
       <c r="I263" s="23"/>
-      <c r="J263" s="23"/>
+      <c r="J263" s="41"/>
       <c r="K263" s="23"/>
       <c r="L263" s="23"/>
     </row>
@@ -20104,7 +20424,7 @@
       </c>
       <c r="H264" s="23"/>
       <c r="I264" s="23"/>
-      <c r="J264" s="23"/>
+      <c r="J264" s="41"/>
       <c r="K264" s="23"/>
       <c r="L264" s="23"/>
     </row>
@@ -20132,7 +20452,7 @@
       </c>
       <c r="H265" s="27"/>
       <c r="I265" s="27"/>
-      <c r="J265" s="27"/>
+      <c r="J265" s="42"/>
       <c r="K265" s="27"/>
       <c r="L265" s="27"/>
     </row>
@@ -20160,7 +20480,7 @@
       </c>
       <c r="H266" s="32"/>
       <c r="I266" s="32"/>
-      <c r="J266" s="32"/>
+      <c r="J266" s="40"/>
       <c r="K266" s="32"/>
       <c r="L266" s="32"/>
     </row>
@@ -20188,7 +20508,7 @@
       </c>
       <c r="H267" s="23"/>
       <c r="I267" s="23"/>
-      <c r="J267" s="23"/>
+      <c r="J267" s="41"/>
       <c r="K267" s="23"/>
       <c r="L267" s="23"/>
     </row>
@@ -20216,7 +20536,7 @@
       </c>
       <c r="H268" s="23"/>
       <c r="I268" s="23"/>
-      <c r="J268" s="23"/>
+      <c r="J268" s="41"/>
       <c r="K268" s="23"/>
       <c r="L268" s="23"/>
     </row>
@@ -20244,7 +20564,7 @@
       </c>
       <c r="H269" s="27"/>
       <c r="I269" s="27"/>
-      <c r="J269" s="27"/>
+      <c r="J269" s="42"/>
       <c r="K269" s="27"/>
       <c r="L269" s="27"/>
     </row>
@@ -20272,7 +20592,7 @@
       </c>
       <c r="H270" s="32"/>
       <c r="I270" s="32"/>
-      <c r="J270" s="32"/>
+      <c r="J270" s="40"/>
       <c r="K270" s="32"/>
       <c r="L270" s="32"/>
     </row>
@@ -20300,7 +20620,7 @@
       </c>
       <c r="H271" s="23"/>
       <c r="I271" s="23"/>
-      <c r="J271" s="23"/>
+      <c r="J271" s="41"/>
       <c r="K271" s="23"/>
       <c r="L271" s="23"/>
     </row>
@@ -20328,7 +20648,7 @@
       </c>
       <c r="H272" s="23"/>
       <c r="I272" s="23"/>
-      <c r="J272" s="23"/>
+      <c r="J272" s="41"/>
       <c r="K272" s="23"/>
       <c r="L272" s="23"/>
     </row>
@@ -20356,7 +20676,7 @@
       </c>
       <c r="H273" s="27"/>
       <c r="I273" s="27"/>
-      <c r="J273" s="27"/>
+      <c r="J273" s="42"/>
       <c r="K273" s="27"/>
       <c r="L273" s="27"/>
     </row>
@@ -20384,7 +20704,7 @@
       </c>
       <c r="H274" s="32"/>
       <c r="I274" s="32"/>
-      <c r="J274" s="32"/>
+      <c r="J274" s="40"/>
       <c r="K274" s="32"/>
       <c r="L274" s="32"/>
     </row>
@@ -20412,7 +20732,7 @@
       </c>
       <c r="H275" s="23"/>
       <c r="I275" s="23"/>
-      <c r="J275" s="23"/>
+      <c r="J275" s="41"/>
       <c r="K275" s="23"/>
       <c r="L275" s="23"/>
     </row>
@@ -20440,7 +20760,7 @@
       </c>
       <c r="H276" s="23"/>
       <c r="I276" s="23"/>
-      <c r="J276" s="23"/>
+      <c r="J276" s="41"/>
       <c r="K276" s="23"/>
       <c r="L276" s="23"/>
     </row>
@@ -20468,7 +20788,7 @@
       </c>
       <c r="H277" s="27"/>
       <c r="I277" s="27"/>
-      <c r="J277" s="27"/>
+      <c r="J277" s="42"/>
       <c r="K277" s="27"/>
       <c r="L277" s="27"/>
     </row>
@@ -20496,7 +20816,7 @@
       </c>
       <c r="H278" s="32"/>
       <c r="I278" s="32"/>
-      <c r="J278" s="32"/>
+      <c r="J278" s="40"/>
       <c r="K278" s="32"/>
       <c r="L278" s="32"/>
     </row>
@@ -20524,7 +20844,7 @@
       </c>
       <c r="H279" s="23"/>
       <c r="I279" s="23"/>
-      <c r="J279" s="23"/>
+      <c r="J279" s="41"/>
       <c r="K279" s="23"/>
       <c r="L279" s="23"/>
     </row>
@@ -20552,7 +20872,7 @@
       </c>
       <c r="H280" s="23"/>
       <c r="I280" s="23"/>
-      <c r="J280" s="23"/>
+      <c r="J280" s="41"/>
       <c r="K280" s="23"/>
       <c r="L280" s="23"/>
     </row>
@@ -20580,7 +20900,7 @@
       </c>
       <c r="H281" s="27"/>
       <c r="I281" s="27"/>
-      <c r="J281" s="27"/>
+      <c r="J281" s="42"/>
       <c r="K281" s="27"/>
       <c r="L281" s="27"/>
     </row>
@@ -20608,7 +20928,7 @@
       </c>
       <c r="H282" s="32"/>
       <c r="I282" s="32"/>
-      <c r="J282" s="32"/>
+      <c r="J282" s="40"/>
       <c r="K282" s="32"/>
       <c r="L282" s="32"/>
     </row>
@@ -20636,7 +20956,7 @@
       </c>
       <c r="H283" s="23"/>
       <c r="I283" s="23"/>
-      <c r="J283" s="23"/>
+      <c r="J283" s="41"/>
       <c r="K283" s="23"/>
       <c r="L283" s="23"/>
     </row>
@@ -20664,7 +20984,7 @@
       </c>
       <c r="H284" s="23"/>
       <c r="I284" s="23"/>
-      <c r="J284" s="23"/>
+      <c r="J284" s="41"/>
       <c r="K284" s="23"/>
       <c r="L284" s="23"/>
     </row>
@@ -20692,7 +21012,7 @@
       </c>
       <c r="H285" s="27"/>
       <c r="I285" s="27"/>
-      <c r="J285" s="27"/>
+      <c r="J285" s="42"/>
       <c r="K285" s="27"/>
       <c r="L285" s="27"/>
     </row>
@@ -20720,7 +21040,7 @@
       </c>
       <c r="H286" s="32"/>
       <c r="I286" s="32"/>
-      <c r="J286" s="32"/>
+      <c r="J286" s="40"/>
       <c r="K286" s="32"/>
       <c r="L286" s="32"/>
     </row>
@@ -20748,7 +21068,7 @@
       </c>
       <c r="H287" s="23"/>
       <c r="I287" s="23"/>
-      <c r="J287" s="23"/>
+      <c r="J287" s="41"/>
       <c r="K287" s="23"/>
       <c r="L287" s="23"/>
     </row>
@@ -20776,7 +21096,7 @@
       </c>
       <c r="H288" s="23"/>
       <c r="I288" s="23"/>
-      <c r="J288" s="23"/>
+      <c r="J288" s="41"/>
       <c r="K288" s="23"/>
       <c r="L288" s="23"/>
     </row>
@@ -20804,7 +21124,7 @@
       </c>
       <c r="H289" s="27"/>
       <c r="I289" s="27"/>
-      <c r="J289" s="27"/>
+      <c r="J289" s="42"/>
       <c r="K289" s="27"/>
       <c r="L289" s="27"/>
     </row>
@@ -20832,7 +21152,7 @@
       </c>
       <c r="H290" s="32"/>
       <c r="I290" s="32"/>
-      <c r="J290" s="32"/>
+      <c r="J290" s="40"/>
       <c r="K290" s="32"/>
       <c r="L290" s="32"/>
     </row>
@@ -20860,7 +21180,7 @@
       </c>
       <c r="H291" s="23"/>
       <c r="I291" s="23"/>
-      <c r="J291" s="23"/>
+      <c r="J291" s="41"/>
       <c r="K291" s="23"/>
       <c r="L291" s="23"/>
     </row>
@@ -20888,7 +21208,7 @@
       </c>
       <c r="H292" s="23"/>
       <c r="I292" s="23"/>
-      <c r="J292" s="23"/>
+      <c r="J292" s="41"/>
       <c r="K292" s="23"/>
       <c r="L292" s="23"/>
     </row>
@@ -20916,7 +21236,7 @@
       </c>
       <c r="H293" s="27"/>
       <c r="I293" s="27"/>
-      <c r="J293" s="27"/>
+      <c r="J293" s="42"/>
       <c r="K293" s="27"/>
       <c r="L293" s="27"/>
     </row>
@@ -20944,7 +21264,7 @@
       </c>
       <c r="H294" s="32"/>
       <c r="I294" s="32"/>
-      <c r="J294" s="32"/>
+      <c r="J294" s="40"/>
       <c r="K294" s="32"/>
       <c r="L294" s="32"/>
     </row>
@@ -20972,7 +21292,7 @@
       </c>
       <c r="H295" s="23"/>
       <c r="I295" s="23"/>
-      <c r="J295" s="23"/>
+      <c r="J295" s="41"/>
       <c r="K295" s="23"/>
       <c r="L295" s="23"/>
     </row>
@@ -21000,7 +21320,7 @@
       </c>
       <c r="H296" s="23"/>
       <c r="I296" s="23"/>
-      <c r="J296" s="23"/>
+      <c r="J296" s="41"/>
       <c r="K296" s="23"/>
       <c r="L296" s="23"/>
     </row>
@@ -21028,7 +21348,7 @@
       </c>
       <c r="H297" s="27"/>
       <c r="I297" s="27"/>
-      <c r="J297" s="27"/>
+      <c r="J297" s="42"/>
       <c r="K297" s="27"/>
       <c r="L297" s="27"/>
     </row>
@@ -21056,7 +21376,7 @@
       </c>
       <c r="H298" s="32"/>
       <c r="I298" s="32"/>
-      <c r="J298" s="32"/>
+      <c r="J298" s="40"/>
       <c r="K298" s="32"/>
       <c r="L298" s="32"/>
     </row>
@@ -21084,7 +21404,7 @@
       </c>
       <c r="H299" s="23"/>
       <c r="I299" s="23"/>
-      <c r="J299" s="23"/>
+      <c r="J299" s="41"/>
       <c r="K299" s="23"/>
       <c r="L299" s="23"/>
     </row>
@@ -21112,7 +21432,7 @@
       </c>
       <c r="H300" s="23"/>
       <c r="I300" s="23"/>
-      <c r="J300" s="23"/>
+      <c r="J300" s="41"/>
       <c r="K300" s="23"/>
       <c r="L300" s="23"/>
     </row>
@@ -21140,7 +21460,7 @@
       </c>
       <c r="H301" s="27"/>
       <c r="I301" s="27"/>
-      <c r="J301" s="27"/>
+      <c r="J301" s="42"/>
       <c r="K301" s="27"/>
       <c r="L301" s="27"/>
     </row>
@@ -21168,7 +21488,7 @@
       </c>
       <c r="H302" s="32"/>
       <c r="I302" s="32"/>
-      <c r="J302" s="32"/>
+      <c r="J302" s="40"/>
       <c r="K302" s="32"/>
       <c r="L302" s="32"/>
     </row>
@@ -21196,7 +21516,7 @@
       </c>
       <c r="H303" s="23"/>
       <c r="I303" s="23"/>
-      <c r="J303" s="23"/>
+      <c r="J303" s="41"/>
       <c r="K303" s="23"/>
       <c r="L303" s="23"/>
     </row>
@@ -21224,7 +21544,7 @@
       </c>
       <c r="H304" s="23"/>
       <c r="I304" s="23"/>
-      <c r="J304" s="23"/>
+      <c r="J304" s="41"/>
       <c r="K304" s="23"/>
       <c r="L304" s="23"/>
     </row>
@@ -21252,7 +21572,7 @@
       </c>
       <c r="H305" s="27"/>
       <c r="I305" s="27"/>
-      <c r="J305" s="27"/>
+      <c r="J305" s="42"/>
       <c r="K305" s="27"/>
       <c r="L305" s="27"/>
     </row>
@@ -21280,7 +21600,7 @@
       </c>
       <c r="H306" s="32"/>
       <c r="I306" s="32"/>
-      <c r="J306" s="32"/>
+      <c r="J306" s="40"/>
       <c r="K306" s="32"/>
       <c r="L306" s="32"/>
     </row>
@@ -21308,7 +21628,7 @@
       </c>
       <c r="H307" s="23"/>
       <c r="I307" s="23"/>
-      <c r="J307" s="23"/>
+      <c r="J307" s="41"/>
       <c r="K307" s="23"/>
       <c r="L307" s="23"/>
     </row>
@@ -21336,7 +21656,7 @@
       </c>
       <c r="H308" s="23"/>
       <c r="I308" s="23"/>
-      <c r="J308" s="23"/>
+      <c r="J308" s="41"/>
       <c r="K308" s="23"/>
       <c r="L308" s="23"/>
     </row>
@@ -21364,7 +21684,7 @@
       </c>
       <c r="H309" s="27"/>
       <c r="I309" s="27"/>
-      <c r="J309" s="27"/>
+      <c r="J309" s="42"/>
       <c r="K309" s="27"/>
       <c r="L309" s="27"/>
     </row>
@@ -21392,7 +21712,7 @@
       </c>
       <c r="H310" s="32"/>
       <c r="I310" s="32"/>
-      <c r="J310" s="32"/>
+      <c r="J310" s="40"/>
       <c r="K310" s="32"/>
       <c r="L310" s="32"/>
     </row>
@@ -21420,7 +21740,7 @@
       </c>
       <c r="H311" s="23"/>
       <c r="I311" s="23"/>
-      <c r="J311" s="23"/>
+      <c r="J311" s="41"/>
       <c r="K311" s="23"/>
       <c r="L311" s="23"/>
     </row>
@@ -21448,7 +21768,7 @@
       </c>
       <c r="H312" s="23"/>
       <c r="I312" s="23"/>
-      <c r="J312" s="23"/>
+      <c r="J312" s="41"/>
       <c r="K312" s="23"/>
       <c r="L312" s="23"/>
     </row>
@@ -21476,7 +21796,7 @@
       </c>
       <c r="H313" s="27"/>
       <c r="I313" s="27"/>
-      <c r="J313" s="27"/>
+      <c r="J313" s="42"/>
       <c r="K313" s="27"/>
       <c r="L313" s="27"/>
     </row>
@@ -21504,7 +21824,7 @@
       </c>
       <c r="H314" s="32"/>
       <c r="I314" s="32"/>
-      <c r="J314" s="32"/>
+      <c r="J314" s="40"/>
       <c r="K314" s="32"/>
       <c r="L314" s="32"/>
     </row>
@@ -21532,7 +21852,7 @@
       </c>
       <c r="H315" s="23"/>
       <c r="I315" s="23"/>
-      <c r="J315" s="23"/>
+      <c r="J315" s="41"/>
       <c r="K315" s="23"/>
       <c r="L315" s="23"/>
     </row>
@@ -21560,7 +21880,7 @@
       </c>
       <c r="H316" s="23"/>
       <c r="I316" s="23"/>
-      <c r="J316" s="23"/>
+      <c r="J316" s="41"/>
       <c r="K316" s="23"/>
       <c r="L316" s="23"/>
     </row>
@@ -21588,7 +21908,7 @@
       </c>
       <c r="H317" s="27"/>
       <c r="I317" s="27"/>
-      <c r="J317" s="27"/>
+      <c r="J317" s="42"/>
       <c r="K317" s="27"/>
       <c r="L317" s="27"/>
     </row>
@@ -21616,7 +21936,7 @@
       </c>
       <c r="H318" s="32"/>
       <c r="I318" s="32"/>
-      <c r="J318" s="32"/>
+      <c r="J318" s="40"/>
       <c r="K318" s="32"/>
       <c r="L318" s="32"/>
     </row>
@@ -21644,7 +21964,7 @@
       </c>
       <c r="H319" s="23"/>
       <c r="I319" s="23"/>
-      <c r="J319" s="23"/>
+      <c r="J319" s="41"/>
       <c r="K319" s="23"/>
       <c r="L319" s="23"/>
     </row>
@@ -21672,7 +21992,7 @@
       </c>
       <c r="H320" s="23"/>
       <c r="I320" s="23"/>
-      <c r="J320" s="23"/>
+      <c r="J320" s="41"/>
       <c r="K320" s="23"/>
       <c r="L320" s="23"/>
     </row>
@@ -21700,7 +22020,7 @@
       </c>
       <c r="H321" s="27"/>
       <c r="I321" s="27"/>
-      <c r="J321" s="27"/>
+      <c r="J321" s="42"/>
       <c r="K321" s="27"/>
       <c r="L321" s="27"/>
     </row>
@@ -21728,7 +22048,7 @@
       </c>
       <c r="H322" s="32"/>
       <c r="I322" s="32"/>
-      <c r="J322" s="32"/>
+      <c r="J322" s="40"/>
       <c r="K322" s="32"/>
       <c r="L322" s="32"/>
     </row>
@@ -21756,7 +22076,7 @@
       </c>
       <c r="H323" s="23"/>
       <c r="I323" s="23"/>
-      <c r="J323" s="23"/>
+      <c r="J323" s="41"/>
       <c r="K323" s="23"/>
       <c r="L323" s="23"/>
     </row>
@@ -21784,7 +22104,7 @@
       </c>
       <c r="H324" s="23"/>
       <c r="I324" s="23"/>
-      <c r="J324" s="23"/>
+      <c r="J324" s="41"/>
       <c r="K324" s="23"/>
       <c r="L324" s="23"/>
     </row>
@@ -21812,7 +22132,7 @@
       </c>
       <c r="H325" s="27"/>
       <c r="I325" s="27"/>
-      <c r="J325" s="27"/>
+      <c r="J325" s="42"/>
       <c r="K325" s="27"/>
       <c r="L325" s="27"/>
     </row>
@@ -21840,7 +22160,7 @@
       </c>
       <c r="H326" s="32"/>
       <c r="I326" s="32"/>
-      <c r="J326" s="32"/>
+      <c r="J326" s="40"/>
       <c r="K326" s="32"/>
       <c r="L326" s="32"/>
     </row>
@@ -21868,7 +22188,7 @@
       </c>
       <c r="H327" s="23"/>
       <c r="I327" s="23"/>
-      <c r="J327" s="23"/>
+      <c r="J327" s="41"/>
       <c r="K327" s="23"/>
       <c r="L327" s="23"/>
     </row>
@@ -21896,7 +22216,7 @@
       </c>
       <c r="H328" s="23"/>
       <c r="I328" s="23"/>
-      <c r="J328" s="23"/>
+      <c r="J328" s="41"/>
       <c r="K328" s="23"/>
       <c r="L328" s="23"/>
     </row>
@@ -21924,7 +22244,7 @@
       </c>
       <c r="H329" s="27"/>
       <c r="I329" s="27"/>
-      <c r="J329" s="27"/>
+      <c r="J329" s="42"/>
       <c r="K329" s="27"/>
       <c r="L329" s="27"/>
     </row>
@@ -21952,7 +22272,7 @@
       </c>
       <c r="H330" s="32"/>
       <c r="I330" s="32"/>
-      <c r="J330" s="32"/>
+      <c r="J330" s="40"/>
       <c r="K330" s="32"/>
       <c r="L330" s="32"/>
     </row>
@@ -21980,7 +22300,7 @@
       </c>
       <c r="H331" s="23"/>
       <c r="I331" s="23"/>
-      <c r="J331" s="23"/>
+      <c r="J331" s="41"/>
       <c r="K331" s="23"/>
       <c r="L331" s="23"/>
     </row>
@@ -22008,7 +22328,7 @@
       </c>
       <c r="H332" s="23"/>
       <c r="I332" s="23"/>
-      <c r="J332" s="23"/>
+      <c r="J332" s="41"/>
       <c r="K332" s="23"/>
       <c r="L332" s="23"/>
     </row>
@@ -22036,7 +22356,7 @@
       </c>
       <c r="H333" s="27"/>
       <c r="I333" s="27"/>
-      <c r="J333" s="27"/>
+      <c r="J333" s="42"/>
       <c r="K333" s="27"/>
       <c r="L333" s="27"/>
     </row>
@@ -22064,7 +22384,7 @@
       </c>
       <c r="H334" s="32"/>
       <c r="I334" s="32"/>
-      <c r="J334" s="32"/>
+      <c r="J334" s="40"/>
       <c r="K334" s="32"/>
       <c r="L334" s="32"/>
     </row>
@@ -22092,7 +22412,7 @@
       </c>
       <c r="H335" s="23"/>
       <c r="I335" s="23"/>
-      <c r="J335" s="23"/>
+      <c r="J335" s="41"/>
       <c r="K335" s="23"/>
       <c r="L335" s="23"/>
     </row>
@@ -22120,7 +22440,7 @@
       </c>
       <c r="H336" s="23"/>
       <c r="I336" s="23"/>
-      <c r="J336" s="23"/>
+      <c r="J336" s="41"/>
       <c r="K336" s="23"/>
       <c r="L336" s="23"/>
     </row>
@@ -22148,7 +22468,7 @@
       </c>
       <c r="H337" s="27"/>
       <c r="I337" s="27"/>
-      <c r="J337" s="27"/>
+      <c r="J337" s="42"/>
       <c r="K337" s="27"/>
       <c r="L337" s="27"/>
     </row>
@@ -22176,7 +22496,7 @@
       </c>
       <c r="H338" s="32"/>
       <c r="I338" s="32"/>
-      <c r="J338" s="32"/>
+      <c r="J338" s="40"/>
       <c r="K338" s="32"/>
       <c r="L338" s="32"/>
     </row>
@@ -22204,7 +22524,7 @@
       </c>
       <c r="H339" s="23"/>
       <c r="I339" s="23"/>
-      <c r="J339" s="23"/>
+      <c r="J339" s="41"/>
       <c r="K339" s="23"/>
       <c r="L339" s="23"/>
     </row>
@@ -22232,7 +22552,7 @@
       </c>
       <c r="H340" s="23"/>
       <c r="I340" s="23"/>
-      <c r="J340" s="23"/>
+      <c r="J340" s="41"/>
       <c r="K340" s="23"/>
       <c r="L340" s="23"/>
     </row>
@@ -22260,7 +22580,7 @@
       </c>
       <c r="H341" s="27"/>
       <c r="I341" s="27"/>
-      <c r="J341" s="27"/>
+      <c r="J341" s="42"/>
       <c r="K341" s="27"/>
       <c r="L341" s="27"/>
     </row>
@@ -22288,7 +22608,7 @@
       </c>
       <c r="H342" s="32"/>
       <c r="I342" s="32"/>
-      <c r="J342" s="32"/>
+      <c r="J342" s="40"/>
       <c r="K342" s="32"/>
       <c r="L342" s="32"/>
     </row>
@@ -22316,7 +22636,7 @@
       </c>
       <c r="H343" s="23"/>
       <c r="I343" s="23"/>
-      <c r="J343" s="23"/>
+      <c r="J343" s="41"/>
       <c r="K343" s="23"/>
       <c r="L343" s="23"/>
     </row>
@@ -22344,7 +22664,7 @@
       </c>
       <c r="H344" s="23"/>
       <c r="I344" s="23"/>
-      <c r="J344" s="23"/>
+      <c r="J344" s="41"/>
       <c r="K344" s="23"/>
       <c r="L344" s="23"/>
     </row>
@@ -22372,7 +22692,7 @@
       </c>
       <c r="H345" s="27"/>
       <c r="I345" s="27"/>
-      <c r="J345" s="27"/>
+      <c r="J345" s="42"/>
       <c r="K345" s="27"/>
       <c r="L345" s="27"/>
     </row>
@@ -22400,7 +22720,7 @@
       </c>
       <c r="H346" s="32"/>
       <c r="I346" s="32"/>
-      <c r="J346" s="32"/>
+      <c r="J346" s="40"/>
       <c r="K346" s="32"/>
       <c r="L346" s="32"/>
     </row>
@@ -22428,7 +22748,7 @@
       </c>
       <c r="H347" s="23"/>
       <c r="I347" s="23"/>
-      <c r="J347" s="23"/>
+      <c r="J347" s="41"/>
       <c r="K347" s="23"/>
       <c r="L347" s="23"/>
     </row>
@@ -22456,7 +22776,7 @@
       </c>
       <c r="H348" s="23"/>
       <c r="I348" s="23"/>
-      <c r="J348" s="23"/>
+      <c r="J348" s="41"/>
       <c r="K348" s="23"/>
       <c r="L348" s="23"/>
     </row>
@@ -22484,7 +22804,7 @@
       </c>
       <c r="H349" s="27"/>
       <c r="I349" s="27"/>
-      <c r="J349" s="27"/>
+      <c r="J349" s="42"/>
       <c r="K349" s="27"/>
       <c r="L349" s="27"/>
     </row>
@@ -22512,7 +22832,7 @@
       </c>
       <c r="H350" s="32"/>
       <c r="I350" s="32"/>
-      <c r="J350" s="32"/>
+      <c r="J350" s="40"/>
       <c r="K350" s="32"/>
       <c r="L350" s="32"/>
     </row>
@@ -22540,7 +22860,7 @@
       </c>
       <c r="H351" s="23"/>
       <c r="I351" s="23"/>
-      <c r="J351" s="23"/>
+      <c r="J351" s="41"/>
       <c r="K351" s="23"/>
       <c r="L351" s="23"/>
     </row>
@@ -22568,7 +22888,7 @@
       </c>
       <c r="H352" s="23"/>
       <c r="I352" s="23"/>
-      <c r="J352" s="23"/>
+      <c r="J352" s="41"/>
       <c r="K352" s="23"/>
       <c r="L352" s="23"/>
     </row>
@@ -22596,7 +22916,7 @@
       </c>
       <c r="H353" s="27"/>
       <c r="I353" s="27"/>
-      <c r="J353" s="27"/>
+      <c r="J353" s="42"/>
       <c r="K353" s="27"/>
       <c r="L353" s="27"/>
     </row>
@@ -22624,7 +22944,7 @@
       </c>
       <c r="H354" s="32"/>
       <c r="I354" s="32"/>
-      <c r="J354" s="32"/>
+      <c r="J354" s="40"/>
       <c r="K354" s="32"/>
       <c r="L354" s="32"/>
     </row>
@@ -22652,7 +22972,7 @@
       </c>
       <c r="H355" s="23"/>
       <c r="I355" s="23"/>
-      <c r="J355" s="23"/>
+      <c r="J355" s="41"/>
       <c r="K355" s="23"/>
       <c r="L355" s="23"/>
     </row>
@@ -22680,7 +23000,7 @@
       </c>
       <c r="H356" s="23"/>
       <c r="I356" s="23"/>
-      <c r="J356" s="23"/>
+      <c r="J356" s="41"/>
       <c r="K356" s="23"/>
       <c r="L356" s="23"/>
     </row>
@@ -22708,7 +23028,7 @@
       </c>
       <c r="H357" s="27"/>
       <c r="I357" s="27"/>
-      <c r="J357" s="27"/>
+      <c r="J357" s="42"/>
       <c r="K357" s="27"/>
       <c r="L357" s="27"/>
     </row>
@@ -22736,7 +23056,7 @@
       </c>
       <c r="H358" s="32"/>
       <c r="I358" s="32"/>
-      <c r="J358" s="32"/>
+      <c r="J358" s="40"/>
       <c r="K358" s="32"/>
       <c r="L358" s="32"/>
     </row>
@@ -22764,7 +23084,7 @@
       </c>
       <c r="H359" s="23"/>
       <c r="I359" s="23"/>
-      <c r="J359" s="23"/>
+      <c r="J359" s="41"/>
       <c r="K359" s="23"/>
       <c r="L359" s="23"/>
     </row>
@@ -22792,7 +23112,7 @@
       </c>
       <c r="H360" s="23"/>
       <c r="I360" s="23"/>
-      <c r="J360" s="23"/>
+      <c r="J360" s="41"/>
       <c r="K360" s="23"/>
       <c r="L360" s="23"/>
     </row>
@@ -22820,7 +23140,7 @@
       </c>
       <c r="H361" s="27"/>
       <c r="I361" s="27"/>
-      <c r="J361" s="27"/>
+      <c r="J361" s="42"/>
       <c r="K361" s="27"/>
       <c r="L361" s="27"/>
     </row>
@@ -22848,7 +23168,7 @@
       </c>
       <c r="H362" s="32"/>
       <c r="I362" s="32"/>
-      <c r="J362" s="32"/>
+      <c r="J362" s="40"/>
       <c r="K362" s="32"/>
       <c r="L362" s="32"/>
     </row>
@@ -22876,7 +23196,7 @@
       </c>
       <c r="H363" s="23"/>
       <c r="I363" s="23"/>
-      <c r="J363" s="23"/>
+      <c r="J363" s="41"/>
       <c r="K363" s="23"/>
       <c r="L363" s="23"/>
     </row>
@@ -22904,7 +23224,7 @@
       </c>
       <c r="H364" s="23"/>
       <c r="I364" s="23"/>
-      <c r="J364" s="23"/>
+      <c r="J364" s="41"/>
       <c r="K364" s="23"/>
       <c r="L364" s="23"/>
     </row>
@@ -22932,7 +23252,7 @@
       </c>
       <c r="H365" s="27"/>
       <c r="I365" s="27"/>
-      <c r="J365" s="27"/>
+      <c r="J365" s="42"/>
       <c r="K365" s="27"/>
       <c r="L365" s="27"/>
     </row>
@@ -22960,7 +23280,7 @@
       </c>
       <c r="H366" s="32"/>
       <c r="I366" s="32"/>
-      <c r="J366" s="32"/>
+      <c r="J366" s="40"/>
       <c r="K366" s="32"/>
       <c r="L366" s="32"/>
     </row>
@@ -22988,7 +23308,7 @@
       </c>
       <c r="H367" s="23"/>
       <c r="I367" s="23"/>
-      <c r="J367" s="23"/>
+      <c r="J367" s="41"/>
       <c r="K367" s="23"/>
       <c r="L367" s="23"/>
     </row>
@@ -23016,7 +23336,7 @@
       </c>
       <c r="H368" s="23"/>
       <c r="I368" s="23"/>
-      <c r="J368" s="23"/>
+      <c r="J368" s="41"/>
       <c r="K368" s="23"/>
       <c r="L368" s="23"/>
     </row>
@@ -23044,7 +23364,7 @@
       </c>
       <c r="H369" s="27"/>
       <c r="I369" s="27"/>
-      <c r="J369" s="27"/>
+      <c r="J369" s="42"/>
       <c r="K369" s="27"/>
       <c r="L369" s="27"/>
     </row>
@@ -23072,7 +23392,7 @@
       </c>
       <c r="H370" s="32"/>
       <c r="I370" s="32"/>
-      <c r="J370" s="32"/>
+      <c r="J370" s="40"/>
       <c r="K370" s="32"/>
       <c r="L370" s="32"/>
     </row>
@@ -23100,7 +23420,7 @@
       </c>
       <c r="H371" s="23"/>
       <c r="I371" s="23"/>
-      <c r="J371" s="23"/>
+      <c r="J371" s="41"/>
       <c r="K371" s="23"/>
       <c r="L371" s="23"/>
     </row>
@@ -23128,7 +23448,7 @@
       </c>
       <c r="H372" s="23"/>
       <c r="I372" s="23"/>
-      <c r="J372" s="23"/>
+      <c r="J372" s="41"/>
       <c r="K372" s="23"/>
       <c r="L372" s="23"/>
     </row>
@@ -23156,7 +23476,7 @@
       </c>
       <c r="H373" s="27"/>
       <c r="I373" s="27"/>
-      <c r="J373" s="27"/>
+      <c r="J373" s="42"/>
       <c r="K373" s="27"/>
       <c r="L373" s="27"/>
     </row>
@@ -23184,7 +23504,7 @@
       </c>
       <c r="H374" s="32"/>
       <c r="I374" s="32"/>
-      <c r="J374" s="32"/>
+      <c r="J374" s="40"/>
       <c r="K374" s="32"/>
       <c r="L374" s="32"/>
     </row>
@@ -23212,7 +23532,7 @@
       </c>
       <c r="H375" s="23"/>
       <c r="I375" s="23"/>
-      <c r="J375" s="23"/>
+      <c r="J375" s="41"/>
       <c r="K375" s="23"/>
       <c r="L375" s="23"/>
     </row>
@@ -23240,7 +23560,7 @@
       </c>
       <c r="H376" s="23"/>
       <c r="I376" s="23"/>
-      <c r="J376" s="23"/>
+      <c r="J376" s="41"/>
       <c r="K376" s="23"/>
       <c r="L376" s="23"/>
     </row>
@@ -23268,7 +23588,7 @@
       </c>
       <c r="H377" s="27"/>
       <c r="I377" s="27"/>
-      <c r="J377" s="27"/>
+      <c r="J377" s="42"/>
       <c r="K377" s="27"/>
       <c r="L377" s="27"/>
     </row>
@@ -23296,7 +23616,7 @@
       </c>
       <c r="H378" s="32"/>
       <c r="I378" s="32"/>
-      <c r="J378" s="32"/>
+      <c r="J378" s="40"/>
       <c r="K378" s="32"/>
       <c r="L378" s="32"/>
     </row>
@@ -23324,7 +23644,7 @@
       </c>
       <c r="H379" s="23"/>
       <c r="I379" s="23"/>
-      <c r="J379" s="23"/>
+      <c r="J379" s="41"/>
       <c r="K379" s="23"/>
       <c r="L379" s="23"/>
     </row>
@@ -23352,7 +23672,7 @@
       </c>
       <c r="H380" s="23"/>
       <c r="I380" s="23"/>
-      <c r="J380" s="23"/>
+      <c r="J380" s="41"/>
       <c r="K380" s="23"/>
       <c r="L380" s="23"/>
     </row>
@@ -23380,7 +23700,7 @@
       </c>
       <c r="H381" s="27"/>
       <c r="I381" s="27"/>
-      <c r="J381" s="27"/>
+      <c r="J381" s="42"/>
       <c r="K381" s="27"/>
       <c r="L381" s="27"/>
     </row>
@@ -23408,7 +23728,7 @@
       </c>
       <c r="H382" s="32"/>
       <c r="I382" s="32"/>
-      <c r="J382" s="32"/>
+      <c r="J382" s="40"/>
       <c r="K382" s="32"/>
       <c r="L382" s="32"/>
     </row>
@@ -23436,7 +23756,7 @@
       </c>
       <c r="H383" s="23"/>
       <c r="I383" s="23"/>
-      <c r="J383" s="23"/>
+      <c r="J383" s="41"/>
       <c r="K383" s="23"/>
       <c r="L383" s="23"/>
     </row>
@@ -23464,7 +23784,7 @@
       </c>
       <c r="H384" s="23"/>
       <c r="I384" s="23"/>
-      <c r="J384" s="23"/>
+      <c r="J384" s="41"/>
       <c r="K384" s="23"/>
       <c r="L384" s="23"/>
     </row>
@@ -23492,7 +23812,7 @@
       </c>
       <c r="H385" s="27"/>
       <c r="I385" s="27"/>
-      <c r="J385" s="27"/>
+      <c r="J385" s="42"/>
       <c r="K385" s="27"/>
       <c r="L385" s="27"/>
     </row>
@@ -23520,7 +23840,7 @@
       </c>
       <c r="H386" s="32"/>
       <c r="I386" s="32"/>
-      <c r="J386" s="32"/>
+      <c r="J386" s="40"/>
       <c r="K386" s="32"/>
       <c r="L386" s="32"/>
     </row>
@@ -23548,7 +23868,7 @@
       </c>
       <c r="H387" s="23"/>
       <c r="I387" s="23"/>
-      <c r="J387" s="23"/>
+      <c r="J387" s="41"/>
       <c r="K387" s="23"/>
       <c r="L387" s="23"/>
     </row>
@@ -23576,7 +23896,7 @@
       </c>
       <c r="H388" s="23"/>
       <c r="I388" s="23"/>
-      <c r="J388" s="23"/>
+      <c r="J388" s="41"/>
       <c r="K388" s="23"/>
       <c r="L388" s="23"/>
     </row>
@@ -23604,7 +23924,7 @@
       </c>
       <c r="H389" s="27"/>
       <c r="I389" s="27"/>
-      <c r="J389" s="27"/>
+      <c r="J389" s="42"/>
       <c r="K389" s="27"/>
       <c r="L389" s="27"/>
     </row>
@@ -23632,7 +23952,7 @@
       </c>
       <c r="H390" s="32"/>
       <c r="I390" s="32"/>
-      <c r="J390" s="32"/>
+      <c r="J390" s="40"/>
       <c r="K390" s="32"/>
       <c r="L390" s="32"/>
     </row>
@@ -23660,7 +23980,7 @@
       </c>
       <c r="H391" s="23"/>
       <c r="I391" s="23"/>
-      <c r="J391" s="23"/>
+      <c r="J391" s="41"/>
       <c r="K391" s="23"/>
       <c r="L391" s="23"/>
     </row>
@@ -23688,7 +24008,7 @@
       </c>
       <c r="H392" s="23"/>
       <c r="I392" s="23"/>
-      <c r="J392" s="23"/>
+      <c r="J392" s="41"/>
       <c r="K392" s="23"/>
       <c r="L392" s="23"/>
     </row>
@@ -23716,7 +24036,7 @@
       </c>
       <c r="H393" s="27"/>
       <c r="I393" s="27"/>
-      <c r="J393" s="27"/>
+      <c r="J393" s="42"/>
       <c r="K393" s="27"/>
       <c r="L393" s="27"/>
     </row>
@@ -23744,7 +24064,7 @@
       </c>
       <c r="H394" s="32"/>
       <c r="I394" s="32"/>
-      <c r="J394" s="32"/>
+      <c r="J394" s="40"/>
       <c r="K394" s="32"/>
       <c r="L394" s="32"/>
     </row>
@@ -23772,7 +24092,7 @@
       </c>
       <c r="H395" s="23"/>
       <c r="I395" s="23"/>
-      <c r="J395" s="23"/>
+      <c r="J395" s="41"/>
       <c r="K395" s="23"/>
       <c r="L395" s="23"/>
     </row>
@@ -23800,7 +24120,7 @@
       </c>
       <c r="H396" s="23"/>
       <c r="I396" s="23"/>
-      <c r="J396" s="23"/>
+      <c r="J396" s="41"/>
       <c r="K396" s="23"/>
       <c r="L396" s="23"/>
     </row>
@@ -23828,7 +24148,7 @@
       </c>
       <c r="H397" s="27"/>
       <c r="I397" s="27"/>
-      <c r="J397" s="27"/>
+      <c r="J397" s="42"/>
       <c r="K397" s="27"/>
       <c r="L397" s="27"/>
     </row>
@@ -23856,7 +24176,7 @@
       </c>
       <c r="H398" s="32"/>
       <c r="I398" s="32"/>
-      <c r="J398" s="32"/>
+      <c r="J398" s="40"/>
       <c r="K398" s="32"/>
       <c r="L398" s="32"/>
     </row>
@@ -23884,7 +24204,7 @@
       </c>
       <c r="H399" s="23"/>
       <c r="I399" s="23"/>
-      <c r="J399" s="23"/>
+      <c r="J399" s="41"/>
       <c r="K399" s="23"/>
       <c r="L399" s="23"/>
     </row>
@@ -23912,7 +24232,7 @@
       </c>
       <c r="H400" s="23"/>
       <c r="I400" s="23"/>
-      <c r="J400" s="23"/>
+      <c r="J400" s="41"/>
       <c r="K400" s="23"/>
       <c r="L400" s="23"/>
     </row>
@@ -23940,7 +24260,7 @@
       </c>
       <c r="H401" s="27"/>
       <c r="I401" s="27"/>
-      <c r="J401" s="27"/>
+      <c r="J401" s="42"/>
       <c r="K401" s="27"/>
       <c r="L401" s="27"/>
     </row>
@@ -23968,7 +24288,7 @@
       </c>
       <c r="H402" s="32"/>
       <c r="I402" s="32"/>
-      <c r="J402" s="32"/>
+      <c r="J402" s="40"/>
       <c r="K402" s="32"/>
       <c r="L402" s="32"/>
     </row>
@@ -23996,7 +24316,7 @@
       </c>
       <c r="H403" s="23"/>
       <c r="I403" s="23"/>
-      <c r="J403" s="23"/>
+      <c r="J403" s="41"/>
       <c r="K403" s="23"/>
       <c r="L403" s="23"/>
     </row>
@@ -24024,7 +24344,7 @@
       </c>
       <c r="H404" s="23"/>
       <c r="I404" s="23"/>
-      <c r="J404" s="23"/>
+      <c r="J404" s="41"/>
       <c r="K404" s="23"/>
       <c r="L404" s="23"/>
     </row>
@@ -24052,7 +24372,7 @@
       </c>
       <c r="H405" s="27"/>
       <c r="I405" s="27"/>
-      <c r="J405" s="27"/>
+      <c r="J405" s="42"/>
       <c r="K405" s="27"/>
       <c r="L405" s="27"/>
     </row>
@@ -24080,7 +24400,7 @@
       </c>
       <c r="H406" s="32"/>
       <c r="I406" s="32"/>
-      <c r="J406" s="32"/>
+      <c r="J406" s="40"/>
       <c r="K406" s="32"/>
       <c r="L406" s="32"/>
     </row>
@@ -24108,7 +24428,7 @@
       </c>
       <c r="H407" s="23"/>
       <c r="I407" s="23"/>
-      <c r="J407" s="23"/>
+      <c r="J407" s="41"/>
       <c r="K407" s="23"/>
       <c r="L407" s="23"/>
     </row>
@@ -24136,7 +24456,7 @@
       </c>
       <c r="H408" s="23"/>
       <c r="I408" s="23"/>
-      <c r="J408" s="23"/>
+      <c r="J408" s="41"/>
       <c r="K408" s="23"/>
       <c r="L408" s="23"/>
     </row>
@@ -24164,7 +24484,7 @@
       </c>
       <c r="H409" s="27"/>
       <c r="I409" s="27"/>
-      <c r="J409" s="27"/>
+      <c r="J409" s="42"/>
       <c r="K409" s="27"/>
       <c r="L409" s="27"/>
     </row>
@@ -24192,7 +24512,7 @@
       </c>
       <c r="H410" s="32"/>
       <c r="I410" s="32"/>
-      <c r="J410" s="32"/>
+      <c r="J410" s="40"/>
       <c r="K410" s="32"/>
       <c r="L410" s="32"/>
     </row>
@@ -24220,7 +24540,7 @@
       </c>
       <c r="H411" s="23"/>
       <c r="I411" s="23"/>
-      <c r="J411" s="23"/>
+      <c r="J411" s="41"/>
       <c r="K411" s="23"/>
       <c r="L411" s="23"/>
     </row>
@@ -24248,7 +24568,7 @@
       </c>
       <c r="H412" s="23"/>
       <c r="I412" s="23"/>
-      <c r="J412" s="23"/>
+      <c r="J412" s="41"/>
       <c r="K412" s="23"/>
       <c r="L412" s="23"/>
     </row>
@@ -24276,7 +24596,7 @@
       </c>
       <c r="H413" s="27"/>
       <c r="I413" s="27"/>
-      <c r="J413" s="27"/>
+      <c r="J413" s="42"/>
       <c r="K413" s="27"/>
       <c r="L413" s="27"/>
     </row>
@@ -24304,7 +24624,7 @@
       </c>
       <c r="H414" s="32"/>
       <c r="I414" s="32"/>
-      <c r="J414" s="32"/>
+      <c r="J414" s="40"/>
       <c r="K414" s="32"/>
       <c r="L414" s="32"/>
     </row>
@@ -24332,7 +24652,7 @@
       </c>
       <c r="H415" s="23"/>
       <c r="I415" s="23"/>
-      <c r="J415" s="23"/>
+      <c r="J415" s="41"/>
       <c r="K415" s="23"/>
       <c r="L415" s="23"/>
     </row>
@@ -24360,7 +24680,7 @@
       </c>
       <c r="H416" s="23"/>
       <c r="I416" s="23"/>
-      <c r="J416" s="23"/>
+      <c r="J416" s="41"/>
       <c r="K416" s="23"/>
       <c r="L416" s="23"/>
     </row>
@@ -24388,7 +24708,7 @@
       </c>
       <c r="H417" s="27"/>
       <c r="I417" s="27"/>
-      <c r="J417" s="27"/>
+      <c r="J417" s="42"/>
       <c r="K417" s="27"/>
       <c r="L417" s="27"/>
     </row>
@@ -24416,7 +24736,7 @@
       </c>
       <c r="H418" s="32"/>
       <c r="I418" s="32"/>
-      <c r="J418" s="32"/>
+      <c r="J418" s="40"/>
       <c r="K418" s="32"/>
       <c r="L418" s="32"/>
     </row>
@@ -24444,7 +24764,7 @@
       </c>
       <c r="H419" s="23"/>
       <c r="I419" s="23"/>
-      <c r="J419" s="23"/>
+      <c r="J419" s="41"/>
       <c r="K419" s="23"/>
       <c r="L419" s="23"/>
     </row>
@@ -24472,7 +24792,7 @@
       </c>
       <c r="H420" s="23"/>
       <c r="I420" s="23"/>
-      <c r="J420" s="23"/>
+      <c r="J420" s="41"/>
       <c r="K420" s="23"/>
       <c r="L420" s="23"/>
     </row>
@@ -24500,7 +24820,7 @@
       </c>
       <c r="H421" s="27"/>
       <c r="I421" s="27"/>
-      <c r="J421" s="27"/>
+      <c r="J421" s="42"/>
       <c r="K421" s="27"/>
       <c r="L421" s="27"/>
     </row>
@@ -24528,7 +24848,7 @@
       </c>
       <c r="H422" s="32"/>
       <c r="I422" s="32"/>
-      <c r="J422" s="32"/>
+      <c r="J422" s="40"/>
       <c r="K422" s="32"/>
       <c r="L422" s="32"/>
     </row>
@@ -24556,7 +24876,7 @@
       </c>
       <c r="H423" s="23"/>
       <c r="I423" s="23"/>
-      <c r="J423" s="23"/>
+      <c r="J423" s="41"/>
       <c r="K423" s="23"/>
       <c r="L423" s="23"/>
     </row>
@@ -24584,7 +24904,7 @@
       </c>
       <c r="H424" s="23"/>
       <c r="I424" s="23"/>
-      <c r="J424" s="23"/>
+      <c r="J424" s="41"/>
       <c r="K424" s="23"/>
       <c r="L424" s="23"/>
     </row>
@@ -24612,7 +24932,7 @@
       </c>
       <c r="H425" s="27"/>
       <c r="I425" s="27"/>
-      <c r="J425" s="27"/>
+      <c r="J425" s="42"/>
       <c r="K425" s="27"/>
       <c r="L425" s="27"/>
     </row>
@@ -24640,7 +24960,7 @@
       </c>
       <c r="H426" s="32"/>
       <c r="I426" s="32"/>
-      <c r="J426" s="32"/>
+      <c r="J426" s="40"/>
       <c r="K426" s="32"/>
       <c r="L426" s="32"/>
     </row>
@@ -24668,7 +24988,7 @@
       </c>
       <c r="H427" s="23"/>
       <c r="I427" s="23"/>
-      <c r="J427" s="23"/>
+      <c r="J427" s="41"/>
       <c r="K427" s="23"/>
       <c r="L427" s="23"/>
     </row>
@@ -24696,7 +25016,7 @@
       </c>
       <c r="H428" s="23"/>
       <c r="I428" s="23"/>
-      <c r="J428" s="23"/>
+      <c r="J428" s="41"/>
       <c r="K428" s="23"/>
       <c r="L428" s="23"/>
     </row>
@@ -24724,7 +25044,7 @@
       </c>
       <c r="H429" s="27"/>
       <c r="I429" s="27"/>
-      <c r="J429" s="27"/>
+      <c r="J429" s="42"/>
       <c r="K429" s="27"/>
       <c r="L429" s="27"/>
     </row>
@@ -24752,7 +25072,7 @@
       </c>
       <c r="H430" s="32"/>
       <c r="I430" s="32"/>
-      <c r="J430" s="32"/>
+      <c r="J430" s="40"/>
       <c r="K430" s="32"/>
       <c r="L430" s="32"/>
     </row>
@@ -24780,7 +25100,7 @@
       </c>
       <c r="H431" s="23"/>
       <c r="I431" s="23"/>
-      <c r="J431" s="23"/>
+      <c r="J431" s="41"/>
       <c r="K431" s="23"/>
       <c r="L431" s="23"/>
     </row>
@@ -24808,7 +25128,7 @@
       </c>
       <c r="H432" s="23"/>
       <c r="I432" s="23"/>
-      <c r="J432" s="23"/>
+      <c r="J432" s="41"/>
       <c r="K432" s="23"/>
       <c r="L432" s="23"/>
     </row>
@@ -24836,7 +25156,7 @@
       </c>
       <c r="H433" s="27"/>
       <c r="I433" s="27"/>
-      <c r="J433" s="27"/>
+      <c r="J433" s="42"/>
       <c r="K433" s="27"/>
       <c r="L433" s="27"/>
     </row>
@@ -24864,7 +25184,7 @@
       </c>
       <c r="H434" s="32"/>
       <c r="I434" s="32"/>
-      <c r="J434" s="32"/>
+      <c r="J434" s="40"/>
       <c r="K434" s="32"/>
       <c r="L434" s="32"/>
     </row>
@@ -24892,7 +25212,7 @@
       </c>
       <c r="H435" s="23"/>
       <c r="I435" s="23"/>
-      <c r="J435" s="23"/>
+      <c r="J435" s="41"/>
       <c r="K435" s="23"/>
       <c r="L435" s="23"/>
     </row>
@@ -24920,7 +25240,7 @@
       </c>
       <c r="H436" s="23"/>
       <c r="I436" s="23"/>
-      <c r="J436" s="23"/>
+      <c r="J436" s="41"/>
       <c r="K436" s="23"/>
       <c r="L436" s="23"/>
     </row>
@@ -24948,7 +25268,7 @@
       </c>
       <c r="H437" s="27"/>
       <c r="I437" s="27"/>
-      <c r="J437" s="27"/>
+      <c r="J437" s="42"/>
       <c r="K437" s="27"/>
       <c r="L437" s="27"/>
     </row>
@@ -24976,7 +25296,7 @@
       </c>
       <c r="H438" s="32"/>
       <c r="I438" s="32"/>
-      <c r="J438" s="32"/>
+      <c r="J438" s="40"/>
       <c r="K438" s="32"/>
       <c r="L438" s="32"/>
     </row>
@@ -25004,7 +25324,7 @@
       </c>
       <c r="H439" s="23"/>
       <c r="I439" s="23"/>
-      <c r="J439" s="23"/>
+      <c r="J439" s="41"/>
       <c r="K439" s="23"/>
       <c r="L439" s="23"/>
     </row>
@@ -25032,7 +25352,7 @@
       </c>
       <c r="H440" s="23"/>
       <c r="I440" s="23"/>
-      <c r="J440" s="23"/>
+      <c r="J440" s="41"/>
       <c r="K440" s="23"/>
       <c r="L440" s="23"/>
     </row>
@@ -25060,7 +25380,7 @@
       </c>
       <c r="H441" s="27"/>
       <c r="I441" s="27"/>
-      <c r="J441" s="27"/>
+      <c r="J441" s="42"/>
       <c r="K441" s="27"/>
       <c r="L441" s="27"/>
     </row>
@@ -25088,7 +25408,7 @@
       </c>
       <c r="H442" s="32"/>
       <c r="I442" s="32"/>
-      <c r="J442" s="32"/>
+      <c r="J442" s="40"/>
       <c r="K442" s="32"/>
       <c r="L442" s="32"/>
     </row>
@@ -25116,7 +25436,7 @@
       </c>
       <c r="H443" s="23"/>
       <c r="I443" s="23"/>
-      <c r="J443" s="23"/>
+      <c r="J443" s="41"/>
       <c r="K443" s="23"/>
       <c r="L443" s="23"/>
     </row>
@@ -25144,7 +25464,7 @@
       </c>
       <c r="H444" s="23"/>
       <c r="I444" s="23"/>
-      <c r="J444" s="23"/>
+      <c r="J444" s="41"/>
       <c r="K444" s="23"/>
       <c r="L444" s="23"/>
     </row>
@@ -25172,7 +25492,7 @@
       </c>
       <c r="H445" s="27"/>
       <c r="I445" s="27"/>
-      <c r="J445" s="27"/>
+      <c r="J445" s="42"/>
       <c r="K445" s="27"/>
       <c r="L445" s="27"/>
     </row>
@@ -25200,7 +25520,7 @@
       </c>
       <c r="H446" s="32"/>
       <c r="I446" s="32"/>
-      <c r="J446" s="32"/>
+      <c r="J446" s="40"/>
       <c r="K446" s="32"/>
       <c r="L446" s="32"/>
     </row>
@@ -25228,7 +25548,7 @@
       </c>
       <c r="H447" s="23"/>
       <c r="I447" s="23"/>
-      <c r="J447" s="23"/>
+      <c r="J447" s="41"/>
       <c r="K447" s="23"/>
       <c r="L447" s="23"/>
     </row>
@@ -25256,7 +25576,7 @@
       </c>
       <c r="H448" s="23"/>
       <c r="I448" s="23"/>
-      <c r="J448" s="23"/>
+      <c r="J448" s="41"/>
       <c r="K448" s="23"/>
       <c r="L448" s="23"/>
     </row>
@@ -25284,7 +25604,7 @@
       </c>
       <c r="H449" s="27"/>
       <c r="I449" s="27"/>
-      <c r="J449" s="27"/>
+      <c r="J449" s="42"/>
       <c r="K449" s="27"/>
       <c r="L449" s="27"/>
     </row>
@@ -25312,7 +25632,7 @@
       </c>
       <c r="H450" s="32"/>
       <c r="I450" s="32"/>
-      <c r="J450" s="32"/>
+      <c r="J450" s="40"/>
       <c r="K450" s="32"/>
       <c r="L450" s="32"/>
     </row>
@@ -25340,7 +25660,7 @@
       </c>
       <c r="H451" s="23"/>
       <c r="I451" s="23"/>
-      <c r="J451" s="23"/>
+      <c r="J451" s="41"/>
       <c r="K451" s="23"/>
       <c r="L451" s="23"/>
     </row>
@@ -25368,7 +25688,7 @@
       </c>
       <c r="H452" s="23"/>
       <c r="I452" s="23"/>
-      <c r="J452" s="23"/>
+      <c r="J452" s="41"/>
       <c r="K452" s="23"/>
       <c r="L452" s="23"/>
     </row>
@@ -25396,7 +25716,7 @@
       </c>
       <c r="H453" s="27"/>
       <c r="I453" s="27"/>
-      <c r="J453" s="27"/>
+      <c r="J453" s="42"/>
       <c r="K453" s="27"/>
       <c r="L453" s="27"/>
     </row>
@@ -25424,7 +25744,7 @@
       </c>
       <c r="H454" s="32"/>
       <c r="I454" s="32"/>
-      <c r="J454" s="32"/>
+      <c r="J454" s="40"/>
       <c r="K454" s="32"/>
       <c r="L454" s="32"/>
     </row>
@@ -25452,7 +25772,7 @@
       </c>
       <c r="H455" s="23"/>
       <c r="I455" s="23"/>
-      <c r="J455" s="23"/>
+      <c r="J455" s="41"/>
       <c r="K455" s="23"/>
       <c r="L455" s="23"/>
     </row>
@@ -25480,7 +25800,7 @@
       </c>
       <c r="H456" s="23"/>
       <c r="I456" s="23"/>
-      <c r="J456" s="23"/>
+      <c r="J456" s="41"/>
       <c r="K456" s="23"/>
       <c r="L456" s="23"/>
     </row>
@@ -25508,7 +25828,7 @@
       </c>
       <c r="H457" s="27"/>
       <c r="I457" s="27"/>
-      <c r="J457" s="27"/>
+      <c r="J457" s="42"/>
       <c r="K457" s="27"/>
       <c r="L457" s="27"/>
     </row>
@@ -25536,7 +25856,7 @@
       </c>
       <c r="H458" s="32"/>
       <c r="I458" s="32"/>
-      <c r="J458" s="32"/>
+      <c r="J458" s="40"/>
       <c r="K458" s="32"/>
       <c r="L458" s="32"/>
     </row>
@@ -25564,7 +25884,7 @@
       </c>
       <c r="H459" s="23"/>
       <c r="I459" s="23"/>
-      <c r="J459" s="23"/>
+      <c r="J459" s="41"/>
       <c r="K459" s="23"/>
       <c r="L459" s="23"/>
     </row>
@@ -25592,7 +25912,7 @@
       </c>
       <c r="H460" s="23"/>
       <c r="I460" s="23"/>
-      <c r="J460" s="23"/>
+      <c r="J460" s="41"/>
       <c r="K460" s="23"/>
       <c r="L460" s="23"/>
     </row>
@@ -25620,7 +25940,7 @@
       </c>
       <c r="H461" s="27"/>
       <c r="I461" s="27"/>
-      <c r="J461" s="27"/>
+      <c r="J461" s="42"/>
       <c r="K461" s="27"/>
       <c r="L461" s="27"/>
     </row>
@@ -25648,7 +25968,7 @@
       </c>
       <c r="H462" s="32"/>
       <c r="I462" s="32"/>
-      <c r="J462" s="32"/>
+      <c r="J462" s="40"/>
       <c r="K462" s="32"/>
       <c r="L462" s="32"/>
     </row>
@@ -25676,7 +25996,7 @@
       </c>
       <c r="H463" s="23"/>
       <c r="I463" s="23"/>
-      <c r="J463" s="23"/>
+      <c r="J463" s="41"/>
       <c r="K463" s="23"/>
       <c r="L463" s="23"/>
     </row>
@@ -25704,7 +26024,7 @@
       </c>
       <c r="H464" s="23"/>
       <c r="I464" s="23"/>
-      <c r="J464" s="23"/>
+      <c r="J464" s="41"/>
       <c r="K464" s="23"/>
       <c r="L464" s="23"/>
     </row>
@@ -25732,7 +26052,7 @@
       </c>
       <c r="H465" s="27"/>
       <c r="I465" s="27"/>
-      <c r="J465" s="27"/>
+      <c r="J465" s="42"/>
       <c r="K465" s="27"/>
       <c r="L465" s="27"/>
     </row>
@@ -25760,7 +26080,7 @@
       </c>
       <c r="H466" s="32"/>
       <c r="I466" s="32"/>
-      <c r="J466" s="32"/>
+      <c r="J466" s="40"/>
       <c r="K466" s="32"/>
       <c r="L466" s="32"/>
     </row>
@@ -25788,7 +26108,7 @@
       </c>
       <c r="H467" s="23"/>
       <c r="I467" s="23"/>
-      <c r="J467" s="23"/>
+      <c r="J467" s="41"/>
       <c r="K467" s="23"/>
       <c r="L467" s="23"/>
     </row>
@@ -25816,7 +26136,7 @@
       </c>
       <c r="H468" s="23"/>
       <c r="I468" s="23"/>
-      <c r="J468" s="23"/>
+      <c r="J468" s="41"/>
       <c r="K468" s="23"/>
       <c r="L468" s="23"/>
     </row>
@@ -25844,7 +26164,7 @@
       </c>
       <c r="H469" s="27"/>
       <c r="I469" s="27"/>
-      <c r="J469" s="27"/>
+      <c r="J469" s="42"/>
       <c r="K469" s="27"/>
       <c r="L469" s="27"/>
     </row>
@@ -25872,7 +26192,7 @@
       </c>
       <c r="H470" s="32"/>
       <c r="I470" s="32"/>
-      <c r="J470" s="32"/>
+      <c r="J470" s="40"/>
       <c r="K470" s="32"/>
       <c r="L470" s="32"/>
     </row>
@@ -25900,7 +26220,7 @@
       </c>
       <c r="H471" s="23"/>
       <c r="I471" s="23"/>
-      <c r="J471" s="23"/>
+      <c r="J471" s="41"/>
       <c r="K471" s="23"/>
       <c r="L471" s="23"/>
     </row>
@@ -25928,7 +26248,7 @@
       </c>
       <c r="H472" s="23"/>
       <c r="I472" s="23"/>
-      <c r="J472" s="23"/>
+      <c r="J472" s="41"/>
       <c r="K472" s="23"/>
       <c r="L472" s="23"/>
     </row>
@@ -25956,7 +26276,7 @@
       </c>
       <c r="H473" s="27"/>
       <c r="I473" s="27"/>
-      <c r="J473" s="27"/>
+      <c r="J473" s="42"/>
       <c r="K473" s="27"/>
       <c r="L473" s="27"/>
     </row>
@@ -25984,7 +26304,7 @@
       </c>
       <c r="H474" s="32"/>
       <c r="I474" s="32"/>
-      <c r="J474" s="32"/>
+      <c r="J474" s="40"/>
       <c r="K474" s="32"/>
       <c r="L474" s="32"/>
     </row>
@@ -26012,7 +26332,7 @@
       </c>
       <c r="H475" s="23"/>
       <c r="I475" s="23"/>
-      <c r="J475" s="23"/>
+      <c r="J475" s="41"/>
       <c r="K475" s="23"/>
       <c r="L475" s="23"/>
     </row>
@@ -26040,7 +26360,7 @@
       </c>
       <c r="H476" s="23"/>
       <c r="I476" s="23"/>
-      <c r="J476" s="23"/>
+      <c r="J476" s="41"/>
       <c r="K476" s="23"/>
       <c r="L476" s="23"/>
     </row>
@@ -26068,7 +26388,7 @@
       </c>
       <c r="H477" s="27"/>
       <c r="I477" s="27"/>
-      <c r="J477" s="27"/>
+      <c r="J477" s="42"/>
       <c r="K477" s="27"/>
       <c r="L477" s="27"/>
     </row>
@@ -26096,7 +26416,7 @@
       </c>
       <c r="H478" s="32"/>
       <c r="I478" s="32"/>
-      <c r="J478" s="32"/>
+      <c r="J478" s="40"/>
       <c r="K478" s="32"/>
       <c r="L478" s="32"/>
     </row>
@@ -26124,7 +26444,7 @@
       </c>
       <c r="H479" s="23"/>
       <c r="I479" s="23"/>
-      <c r="J479" s="23"/>
+      <c r="J479" s="41"/>
       <c r="K479" s="23"/>
       <c r="L479" s="23"/>
     </row>
@@ -26152,7 +26472,7 @@
       </c>
       <c r="H480" s="23"/>
       <c r="I480" s="23"/>
-      <c r="J480" s="23"/>
+      <c r="J480" s="41"/>
       <c r="K480" s="23"/>
       <c r="L480" s="23"/>
     </row>
@@ -26180,7 +26500,7 @@
       </c>
       <c r="H481" s="27"/>
       <c r="I481" s="27"/>
-      <c r="J481" s="27"/>
+      <c r="J481" s="42"/>
       <c r="K481" s="27"/>
       <c r="L481" s="27"/>
     </row>

</xml_diff>

<commit_message>
starter region 1 results
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B24AC37-5631-47D8-A866-09CCB1E3636A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A959418B-FCA5-4266-B0F7-13455D2ABAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="870" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4575" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4639" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -4685,7 +4685,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6334,7 +6334,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10501,8 +10501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C206" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H226" sqref="H226"/>
+    <sheetView tabSelected="1" topLeftCell="C237" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H254" sqref="H254:L257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19358,11 +19358,21 @@
       <c r="G226" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="H226" s="32"/>
-      <c r="I226" s="32"/>
-      <c r="J226" s="40"/>
-      <c r="K226" s="32"/>
-      <c r="L226" s="32"/>
+      <c r="H226" s="32">
+        <v>6</v>
+      </c>
+      <c r="I226" s="32">
+        <v>2586</v>
+      </c>
+      <c r="J226" s="40">
+        <v>1335.41</v>
+      </c>
+      <c r="K226" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L226" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A227" s="21" t="s">
@@ -19386,11 +19396,21 @@
       <c r="G227" s="23" t="s">
         <v>424</v>
       </c>
-      <c r="H227" s="23"/>
-      <c r="I227" s="23"/>
-      <c r="J227" s="41"/>
-      <c r="K227" s="23"/>
-      <c r="L227" s="23"/>
+      <c r="H227" s="24">
+        <v>6</v>
+      </c>
+      <c r="I227" s="24">
+        <v>2612</v>
+      </c>
+      <c r="J227" s="41">
+        <v>1360.19</v>
+      </c>
+      <c r="K227" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L227" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A228" s="21" t="s">
@@ -19414,11 +19434,21 @@
       <c r="G228" s="23" t="s">
         <v>425</v>
       </c>
-      <c r="H228" s="23"/>
-      <c r="I228" s="23"/>
-      <c r="J228" s="41"/>
-      <c r="K228" s="23"/>
-      <c r="L228" s="23"/>
+      <c r="H228" s="24">
+        <v>6</v>
+      </c>
+      <c r="I228" s="24">
+        <v>2613</v>
+      </c>
+      <c r="J228" s="41">
+        <v>1362.96</v>
+      </c>
+      <c r="K228" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L228" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A229" s="21" t="s">
@@ -19442,11 +19472,21 @@
       <c r="G229" s="27" t="s">
         <v>426</v>
       </c>
-      <c r="H229" s="27"/>
-      <c r="I229" s="27"/>
-      <c r="J229" s="42"/>
-      <c r="K229" s="27"/>
-      <c r="L229" s="27"/>
+      <c r="H229" s="27">
+        <v>6</v>
+      </c>
+      <c r="I229" s="27">
+        <v>2478</v>
+      </c>
+      <c r="J229" s="42">
+        <v>1279.94</v>
+      </c>
+      <c r="K229" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L229" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A230" s="21" t="s">
@@ -19470,11 +19510,21 @@
       <c r="G230" s="32" t="s">
         <v>427</v>
       </c>
-      <c r="H230" s="32"/>
-      <c r="I230" s="32"/>
-      <c r="J230" s="40"/>
-      <c r="K230" s="32"/>
-      <c r="L230" s="32"/>
+      <c r="H230" s="32">
+        <v>4</v>
+      </c>
+      <c r="I230" s="32">
+        <v>2128</v>
+      </c>
+      <c r="J230" s="40">
+        <v>1051.06</v>
+      </c>
+      <c r="K230" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L230" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A231" s="21" t="s">
@@ -19498,11 +19548,21 @@
       <c r="G231" s="23" t="s">
         <v>428</v>
       </c>
-      <c r="H231" s="23"/>
-      <c r="I231" s="23"/>
-      <c r="J231" s="41"/>
-      <c r="K231" s="23"/>
-      <c r="L231" s="23"/>
+      <c r="H231" s="24">
+        <v>5</v>
+      </c>
+      <c r="I231" s="24">
+        <v>2284</v>
+      </c>
+      <c r="J231" s="41">
+        <v>1169.03</v>
+      </c>
+      <c r="K231" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L231" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A232" s="21" t="s">
@@ -19526,11 +19586,21 @@
       <c r="G232" s="23" t="s">
         <v>429</v>
       </c>
-      <c r="H232" s="23"/>
-      <c r="I232" s="23"/>
-      <c r="J232" s="41"/>
-      <c r="K232" s="23"/>
-      <c r="L232" s="23"/>
+      <c r="H232" s="24">
+        <v>5</v>
+      </c>
+      <c r="I232" s="24">
+        <v>2341</v>
+      </c>
+      <c r="J232" s="41">
+        <v>1202.45</v>
+      </c>
+      <c r="K232" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L232" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A233" s="21" t="s">
@@ -19554,11 +19624,21 @@
       <c r="G233" s="27" t="s">
         <v>430</v>
       </c>
-      <c r="H233" s="27"/>
-      <c r="I233" s="27"/>
-      <c r="J233" s="42"/>
-      <c r="K233" s="27"/>
-      <c r="L233" s="27"/>
+      <c r="H233" s="27">
+        <v>5</v>
+      </c>
+      <c r="I233" s="27">
+        <v>2329</v>
+      </c>
+      <c r="J233" s="42">
+        <v>1182.8599999999999</v>
+      </c>
+      <c r="K233" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L233" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A234" s="21" t="s">
@@ -19582,11 +19662,21 @@
       <c r="G234" s="32" t="s">
         <v>431</v>
       </c>
-      <c r="H234" s="32"/>
-      <c r="I234" s="32"/>
-      <c r="J234" s="40"/>
-      <c r="K234" s="32"/>
-      <c r="L234" s="32"/>
+      <c r="H234" s="32">
+        <v>6</v>
+      </c>
+      <c r="I234" s="32">
+        <v>2586</v>
+      </c>
+      <c r="J234" s="40">
+        <v>1335.41</v>
+      </c>
+      <c r="K234" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L234" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A235" s="21" t="s">
@@ -19610,11 +19700,21 @@
       <c r="G235" s="23" t="s">
         <v>432</v>
       </c>
-      <c r="H235" s="23"/>
-      <c r="I235" s="23"/>
-      <c r="J235" s="41"/>
-      <c r="K235" s="23"/>
-      <c r="L235" s="23"/>
+      <c r="H235" s="24">
+        <v>6</v>
+      </c>
+      <c r="I235" s="24">
+        <v>2612</v>
+      </c>
+      <c r="J235" s="41">
+        <v>1360.19</v>
+      </c>
+      <c r="K235" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L235" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A236" s="21" t="s">
@@ -19638,11 +19738,21 @@
       <c r="G236" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="H236" s="23"/>
-      <c r="I236" s="23"/>
-      <c r="J236" s="41"/>
-      <c r="K236" s="23"/>
-      <c r="L236" s="23"/>
+      <c r="H236" s="24">
+        <v>6</v>
+      </c>
+      <c r="I236" s="24">
+        <v>2613</v>
+      </c>
+      <c r="J236" s="41">
+        <v>1362.96</v>
+      </c>
+      <c r="K236" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L236" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A237" s="21" t="s">
@@ -19666,11 +19776,21 @@
       <c r="G237" s="27" t="s">
         <v>434</v>
       </c>
-      <c r="H237" s="27"/>
-      <c r="I237" s="27"/>
-      <c r="J237" s="42"/>
-      <c r="K237" s="27"/>
-      <c r="L237" s="27"/>
+      <c r="H237" s="27">
+        <v>6</v>
+      </c>
+      <c r="I237" s="27">
+        <v>2478</v>
+      </c>
+      <c r="J237" s="42">
+        <v>1279.94</v>
+      </c>
+      <c r="K237" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L237" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A238" s="21" t="s">
@@ -19694,11 +19814,21 @@
       <c r="G238" s="32" t="s">
         <v>435</v>
       </c>
-      <c r="H238" s="32"/>
-      <c r="I238" s="32"/>
-      <c r="J238" s="40"/>
-      <c r="K238" s="32"/>
-      <c r="L238" s="32"/>
+      <c r="H238" s="32">
+        <v>4</v>
+      </c>
+      <c r="I238" s="32">
+        <v>2135</v>
+      </c>
+      <c r="J238" s="40">
+        <v>1063.6600000000001</v>
+      </c>
+      <c r="K238" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L238" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A239" s="21" t="s">
@@ -19722,11 +19852,21 @@
       <c r="G239" s="23" t="s">
         <v>436</v>
       </c>
-      <c r="H239" s="23"/>
-      <c r="I239" s="23"/>
-      <c r="J239" s="41"/>
-      <c r="K239" s="23"/>
-      <c r="L239" s="23"/>
+      <c r="H239" s="24">
+        <v>5</v>
+      </c>
+      <c r="I239" s="24">
+        <v>2284</v>
+      </c>
+      <c r="J239" s="41">
+        <v>1169.03</v>
+      </c>
+      <c r="K239" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L239" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A240" s="21" t="s">
@@ -19750,11 +19890,21 @@
       <c r="G240" s="23" t="s">
         <v>437</v>
       </c>
-      <c r="H240" s="23"/>
-      <c r="I240" s="23"/>
-      <c r="J240" s="41"/>
-      <c r="K240" s="23"/>
-      <c r="L240" s="23"/>
+      <c r="H240" s="24">
+        <v>6</v>
+      </c>
+      <c r="I240" s="24">
+        <v>2558</v>
+      </c>
+      <c r="J240" s="41">
+        <v>1327.72</v>
+      </c>
+      <c r="K240" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L240" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A241" s="21" t="s">
@@ -19778,11 +19928,21 @@
       <c r="G241" s="27" t="s">
         <v>438</v>
       </c>
-      <c r="H241" s="27"/>
-      <c r="I241" s="27"/>
-      <c r="J241" s="42"/>
-      <c r="K241" s="27"/>
-      <c r="L241" s="27"/>
+      <c r="H241" s="27">
+        <v>4</v>
+      </c>
+      <c r="I241" s="27">
+        <v>2218</v>
+      </c>
+      <c r="J241" s="42">
+        <v>1143.44</v>
+      </c>
+      <c r="K241" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L241" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A242" s="21" t="s">
@@ -19806,11 +19966,21 @@
       <c r="G242" s="32" t="s">
         <v>439</v>
       </c>
-      <c r="H242" s="32"/>
-      <c r="I242" s="32"/>
-      <c r="J242" s="40"/>
-      <c r="K242" s="32"/>
-      <c r="L242" s="32"/>
+      <c r="H242" s="32">
+        <v>6</v>
+      </c>
+      <c r="I242" s="32">
+        <v>2586</v>
+      </c>
+      <c r="J242" s="40">
+        <v>1335.41</v>
+      </c>
+      <c r="K242" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L242" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A243" s="21" t="s">
@@ -19834,11 +20004,21 @@
       <c r="G243" s="23" t="s">
         <v>440</v>
       </c>
-      <c r="H243" s="23"/>
-      <c r="I243" s="23"/>
-      <c r="J243" s="41"/>
-      <c r="K243" s="23"/>
-      <c r="L243" s="23"/>
+      <c r="H243" s="24">
+        <v>6</v>
+      </c>
+      <c r="I243" s="24">
+        <v>2612</v>
+      </c>
+      <c r="J243" s="41">
+        <v>1360.19</v>
+      </c>
+      <c r="K243" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L243" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A244" s="21" t="s">
@@ -19862,11 +20042,21 @@
       <c r="G244" s="23" t="s">
         <v>441</v>
       </c>
-      <c r="H244" s="23"/>
-      <c r="I244" s="23"/>
-      <c r="J244" s="41"/>
-      <c r="K244" s="23"/>
-      <c r="L244" s="23"/>
+      <c r="H244" s="24">
+        <v>6</v>
+      </c>
+      <c r="I244" s="24">
+        <v>2613</v>
+      </c>
+      <c r="J244" s="41">
+        <v>1362.96</v>
+      </c>
+      <c r="K244" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L244" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A245" s="21" t="s">
@@ -19890,11 +20080,21 @@
       <c r="G245" s="27" t="s">
         <v>442</v>
       </c>
-      <c r="H245" s="27"/>
-      <c r="I245" s="27"/>
-      <c r="J245" s="42"/>
-      <c r="K245" s="27"/>
-      <c r="L245" s="27"/>
+      <c r="H245" s="27">
+        <v>6</v>
+      </c>
+      <c r="I245" s="27">
+        <v>2478</v>
+      </c>
+      <c r="J245" s="42">
+        <v>1279.94</v>
+      </c>
+      <c r="K245" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L245" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A246" s="21" t="s">
@@ -19918,11 +20118,21 @@
       <c r="G246" s="32" t="s">
         <v>443</v>
       </c>
-      <c r="H246" s="32"/>
-      <c r="I246" s="32"/>
-      <c r="J246" s="40"/>
-      <c r="K246" s="32"/>
-      <c r="L246" s="32"/>
+      <c r="H246" s="32">
+        <v>4</v>
+      </c>
+      <c r="I246" s="32">
+        <v>2135</v>
+      </c>
+      <c r="J246" s="40">
+        <v>1063.6600000000001</v>
+      </c>
+      <c r="K246" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L246" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A247" s="21" t="s">
@@ -19946,11 +20156,21 @@
       <c r="G247" s="23" t="s">
         <v>444</v>
       </c>
-      <c r="H247" s="23"/>
-      <c r="I247" s="23"/>
-      <c r="J247" s="41"/>
-      <c r="K247" s="23"/>
-      <c r="L247" s="23"/>
+      <c r="H247" s="24">
+        <v>5</v>
+      </c>
+      <c r="I247" s="24">
+        <v>2284</v>
+      </c>
+      <c r="J247" s="41">
+        <v>1169.03</v>
+      </c>
+      <c r="K247" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L247" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A248" s="21" t="s">
@@ -19974,11 +20194,21 @@
       <c r="G248" s="23" t="s">
         <v>445</v>
       </c>
-      <c r="H248" s="23"/>
-      <c r="I248" s="23"/>
-      <c r="J248" s="41"/>
-      <c r="K248" s="23"/>
-      <c r="L248" s="23"/>
+      <c r="H248" s="24">
+        <v>6</v>
+      </c>
+      <c r="I248" s="24">
+        <v>2558</v>
+      </c>
+      <c r="J248" s="41">
+        <v>1327.72</v>
+      </c>
+      <c r="K248" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L248" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A249" s="21" t="s">
@@ -20002,11 +20232,21 @@
       <c r="G249" s="27" t="s">
         <v>446</v>
       </c>
-      <c r="H249" s="27"/>
-      <c r="I249" s="27"/>
-      <c r="J249" s="42"/>
-      <c r="K249" s="27"/>
-      <c r="L249" s="27"/>
+      <c r="H249" s="27">
+        <v>4</v>
+      </c>
+      <c r="I249" s="27">
+        <v>2218</v>
+      </c>
+      <c r="J249" s="42">
+        <v>1143.44</v>
+      </c>
+      <c r="K249" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L249" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A250" s="21" t="s">
@@ -20030,11 +20270,21 @@
       <c r="G250" s="32" t="s">
         <v>447</v>
       </c>
-      <c r="H250" s="32"/>
-      <c r="I250" s="32"/>
-      <c r="J250" s="40"/>
-      <c r="K250" s="32"/>
-      <c r="L250" s="32"/>
+      <c r="H250" s="32">
+        <v>6</v>
+      </c>
+      <c r="I250" s="32">
+        <v>2586</v>
+      </c>
+      <c r="J250" s="40">
+        <v>1335.41</v>
+      </c>
+      <c r="K250" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L250" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A251" s="21" t="s">
@@ -20058,11 +20308,21 @@
       <c r="G251" s="23" t="s">
         <v>448</v>
       </c>
-      <c r="H251" s="23"/>
-      <c r="I251" s="23"/>
-      <c r="J251" s="41"/>
-      <c r="K251" s="23"/>
-      <c r="L251" s="23"/>
+      <c r="H251" s="24">
+        <v>6</v>
+      </c>
+      <c r="I251" s="24">
+        <v>2612</v>
+      </c>
+      <c r="J251" s="41">
+        <v>1360.19</v>
+      </c>
+      <c r="K251" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L251" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A252" s="21" t="s">
@@ -20086,11 +20346,21 @@
       <c r="G252" s="23" t="s">
         <v>449</v>
       </c>
-      <c r="H252" s="23"/>
-      <c r="I252" s="23"/>
-      <c r="J252" s="41"/>
-      <c r="K252" s="23"/>
-      <c r="L252" s="23"/>
+      <c r="H252" s="24">
+        <v>6</v>
+      </c>
+      <c r="I252" s="24">
+        <v>2613</v>
+      </c>
+      <c r="J252" s="41">
+        <v>1362.96</v>
+      </c>
+      <c r="K252" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L252" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A253" s="21" t="s">
@@ -20114,11 +20384,21 @@
       <c r="G253" s="27" t="s">
         <v>450</v>
       </c>
-      <c r="H253" s="27"/>
-      <c r="I253" s="27"/>
-      <c r="J253" s="42"/>
-      <c r="K253" s="27"/>
-      <c r="L253" s="27"/>
+      <c r="H253" s="27">
+        <v>6</v>
+      </c>
+      <c r="I253" s="27">
+        <v>2478</v>
+      </c>
+      <c r="J253" s="42">
+        <v>1279.94</v>
+      </c>
+      <c r="K253" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L253" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A254" s="21" t="s">
@@ -20142,11 +20422,21 @@
       <c r="G254" s="32" t="s">
         <v>451</v>
       </c>
-      <c r="H254" s="32"/>
-      <c r="I254" s="32"/>
-      <c r="J254" s="40"/>
-      <c r="K254" s="32"/>
-      <c r="L254" s="32"/>
+      <c r="H254" s="32">
+        <v>4</v>
+      </c>
+      <c r="I254" s="32">
+        <v>2135</v>
+      </c>
+      <c r="J254" s="40">
+        <v>1063.6600000000001</v>
+      </c>
+      <c r="K254" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L254" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A255" s="21" t="s">
@@ -20170,11 +20460,21 @@
       <c r="G255" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="H255" s="23"/>
-      <c r="I255" s="23"/>
-      <c r="J255" s="41"/>
-      <c r="K255" s="23"/>
-      <c r="L255" s="23"/>
+      <c r="H255" s="24">
+        <v>5</v>
+      </c>
+      <c r="I255" s="24">
+        <v>2284</v>
+      </c>
+      <c r="J255" s="41">
+        <v>1169.03</v>
+      </c>
+      <c r="K255" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L255" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A256" s="21" t="s">
@@ -20198,11 +20498,21 @@
       <c r="G256" s="23" t="s">
         <v>453</v>
       </c>
-      <c r="H256" s="23"/>
-      <c r="I256" s="23"/>
-      <c r="J256" s="41"/>
-      <c r="K256" s="23"/>
-      <c r="L256" s="23"/>
+      <c r="H256" s="24">
+        <v>6</v>
+      </c>
+      <c r="I256" s="24">
+        <v>2558</v>
+      </c>
+      <c r="J256" s="41">
+        <v>1327.72</v>
+      </c>
+      <c r="K256" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L256" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A257" s="21" t="s">
@@ -20226,11 +20536,21 @@
       <c r="G257" s="27" t="s">
         <v>454</v>
       </c>
-      <c r="H257" s="27"/>
-      <c r="I257" s="27"/>
-      <c r="J257" s="42"/>
-      <c r="K257" s="27"/>
-      <c r="L257" s="27"/>
+      <c r="H257" s="27">
+        <v>4</v>
+      </c>
+      <c r="I257" s="27">
+        <v>2218</v>
+      </c>
+      <c r="J257" s="42">
+        <v>1143.44</v>
+      </c>
+      <c r="K257" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L257" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A258" s="21" t="s">

</xml_diff>

<commit_message>
starter region 3 results
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3297D5E6-C5C3-471A-B338-2A38CCD1F5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E27BAB0-19FC-48D6-B532-0B12D0F6F989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="870" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4715" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4782" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -4685,7 +4685,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10501,8 +10501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C255" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H290" sqref="H290"/>
+    <sheetView tabSelected="1" topLeftCell="C303" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H322" sqref="H322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21790,11 +21790,21 @@
       <c r="G290" s="32" t="s">
         <v>518</v>
       </c>
-      <c r="H290" s="32"/>
-      <c r="I290" s="32"/>
-      <c r="J290" s="38"/>
-      <c r="K290" s="32"/>
-      <c r="L290" s="32"/>
+      <c r="H290" s="32">
+        <v>6</v>
+      </c>
+      <c r="I290" s="32">
+        <v>1881</v>
+      </c>
+      <c r="J290" s="38">
+        <v>1129.44</v>
+      </c>
+      <c r="K290" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L290" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A291" s="21" t="s">
@@ -21818,11 +21828,21 @@
       <c r="G291" s="23" t="s">
         <v>487</v>
       </c>
-      <c r="H291" s="23"/>
-      <c r="I291" s="23"/>
-      <c r="J291" s="39"/>
-      <c r="K291" s="23"/>
-      <c r="L291" s="23"/>
+      <c r="H291" s="24">
+        <v>6</v>
+      </c>
+      <c r="I291" s="24">
+        <v>1913</v>
+      </c>
+      <c r="J291" s="39">
+        <v>1123.0899999999999</v>
+      </c>
+      <c r="K291" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L291" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A292" s="21" t="s">
@@ -21846,11 +21866,21 @@
       <c r="G292" s="23" t="s">
         <v>488</v>
       </c>
-      <c r="H292" s="23"/>
-      <c r="I292" s="23"/>
-      <c r="J292" s="39"/>
-      <c r="K292" s="23"/>
-      <c r="L292" s="23"/>
+      <c r="H292" s="24">
+        <v>7</v>
+      </c>
+      <c r="I292" s="24">
+        <v>2066</v>
+      </c>
+      <c r="J292" s="39">
+        <v>1286.08</v>
+      </c>
+      <c r="K292" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L292" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A293" s="21" t="s">
@@ -21874,11 +21904,21 @@
       <c r="G293" s="27" t="s">
         <v>489</v>
       </c>
-      <c r="H293" s="27"/>
-      <c r="I293" s="27"/>
-      <c r="J293" s="40"/>
-      <c r="K293" s="27"/>
-      <c r="L293" s="27"/>
+      <c r="H293" s="27">
+        <v>7</v>
+      </c>
+      <c r="I293" s="27">
+        <v>2050</v>
+      </c>
+      <c r="J293" s="40">
+        <v>1232.3599999999999</v>
+      </c>
+      <c r="K293" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L293" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A294" s="21" t="s">
@@ -21902,11 +21942,21 @@
       <c r="G294" s="32" t="s">
         <v>490</v>
       </c>
-      <c r="H294" s="32"/>
-      <c r="I294" s="32"/>
-      <c r="J294" s="38"/>
-      <c r="K294" s="32"/>
-      <c r="L294" s="32"/>
+      <c r="H294" s="32">
+        <v>6</v>
+      </c>
+      <c r="I294" s="32">
+        <v>1833</v>
+      </c>
+      <c r="J294" s="38">
+        <v>1077.54</v>
+      </c>
+      <c r="K294" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L294" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A295" s="21" t="s">
@@ -21930,11 +21980,21 @@
       <c r="G295" s="23" t="s">
         <v>491</v>
       </c>
-      <c r="H295" s="23"/>
-      <c r="I295" s="23"/>
-      <c r="J295" s="39"/>
-      <c r="K295" s="23"/>
-      <c r="L295" s="23"/>
+      <c r="H295" s="24">
+        <v>6</v>
+      </c>
+      <c r="I295" s="24">
+        <v>1890</v>
+      </c>
+      <c r="J295" s="39">
+        <v>1132.07</v>
+      </c>
+      <c r="K295" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L295" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A296" s="21" t="s">
@@ -21958,11 +22018,21 @@
       <c r="G296" s="23" t="s">
         <v>492</v>
       </c>
-      <c r="H296" s="23"/>
-      <c r="I296" s="23"/>
-      <c r="J296" s="39"/>
-      <c r="K296" s="23"/>
-      <c r="L296" s="23"/>
+      <c r="H296" s="24">
+        <v>6</v>
+      </c>
+      <c r="I296" s="24">
+        <v>1972</v>
+      </c>
+      <c r="J296" s="39">
+        <v>1169.22</v>
+      </c>
+      <c r="K296" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L296" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A297" s="21" t="s">
@@ -21986,11 +22056,21 @@
       <c r="G297" s="27" t="s">
         <v>493</v>
       </c>
-      <c r="H297" s="27"/>
-      <c r="I297" s="27"/>
-      <c r="J297" s="40"/>
-      <c r="K297" s="27"/>
-      <c r="L297" s="27"/>
+      <c r="H297" s="27">
+        <v>6</v>
+      </c>
+      <c r="I297" s="27">
+        <v>2153</v>
+      </c>
+      <c r="J297" s="40">
+        <v>1282.1099999999999</v>
+      </c>
+      <c r="K297" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L297" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A298" s="21" t="s">
@@ -22014,11 +22094,21 @@
       <c r="G298" s="32" t="s">
         <v>494</v>
       </c>
-      <c r="H298" s="32"/>
-      <c r="I298" s="32"/>
-      <c r="J298" s="38"/>
-      <c r="K298" s="32"/>
-      <c r="L298" s="32"/>
+      <c r="H298" s="32">
+        <v>4</v>
+      </c>
+      <c r="I298" s="32">
+        <v>1745</v>
+      </c>
+      <c r="J298" s="38">
+        <v>933.51</v>
+      </c>
+      <c r="K298" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L298" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A299" s="21" t="s">
@@ -22042,11 +22132,21 @@
       <c r="G299" s="23" t="s">
         <v>495</v>
       </c>
-      <c r="H299" s="23"/>
-      <c r="I299" s="23"/>
-      <c r="J299" s="39"/>
-      <c r="K299" s="23"/>
-      <c r="L299" s="23"/>
+      <c r="H299" s="24">
+        <v>5</v>
+      </c>
+      <c r="I299" s="24">
+        <v>1690</v>
+      </c>
+      <c r="J299" s="39">
+        <v>961.8</v>
+      </c>
+      <c r="K299" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L299" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A300" s="21" t="s">
@@ -22070,11 +22170,21 @@
       <c r="G300" s="23" t="s">
         <v>496</v>
       </c>
-      <c r="H300" s="23"/>
-      <c r="I300" s="23"/>
-      <c r="J300" s="39"/>
-      <c r="K300" s="23"/>
-      <c r="L300" s="23"/>
+      <c r="H300" s="24">
+        <v>5</v>
+      </c>
+      <c r="I300" s="24">
+        <v>1719</v>
+      </c>
+      <c r="J300" s="39">
+        <v>990.43</v>
+      </c>
+      <c r="K300" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L300" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A301" s="21" t="s">
@@ -22098,11 +22208,21 @@
       <c r="G301" s="27" t="s">
         <v>497</v>
       </c>
-      <c r="H301" s="27"/>
-      <c r="I301" s="27"/>
-      <c r="J301" s="40"/>
-      <c r="K301" s="27"/>
-      <c r="L301" s="27"/>
+      <c r="H301" s="27">
+        <v>5</v>
+      </c>
+      <c r="I301" s="27">
+        <v>1740</v>
+      </c>
+      <c r="J301" s="40">
+        <v>996.49</v>
+      </c>
+      <c r="K301" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L301" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="302" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A302" s="21" t="s">
@@ -22126,11 +22246,21 @@
       <c r="G302" s="32" t="s">
         <v>498</v>
       </c>
-      <c r="H302" s="32"/>
-      <c r="I302" s="32"/>
-      <c r="J302" s="38"/>
-      <c r="K302" s="32"/>
-      <c r="L302" s="32"/>
+      <c r="H302" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I302" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J302" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K302" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L302" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="303" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A303" s="21" t="s">
@@ -22154,11 +22284,21 @@
       <c r="G303" s="23" t="s">
         <v>499</v>
       </c>
-      <c r="H303" s="23"/>
-      <c r="I303" s="23"/>
-      <c r="J303" s="39"/>
-      <c r="K303" s="23"/>
-      <c r="L303" s="23"/>
+      <c r="H303" s="24">
+        <v>4</v>
+      </c>
+      <c r="I303" s="24">
+        <v>1710</v>
+      </c>
+      <c r="J303" s="39">
+        <v>882.42</v>
+      </c>
+      <c r="K303" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L303" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="304" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A304" s="21" t="s">
@@ -22182,11 +22322,21 @@
       <c r="G304" s="23" t="s">
         <v>500</v>
       </c>
-      <c r="H304" s="23"/>
-      <c r="I304" s="23"/>
-      <c r="J304" s="39"/>
-      <c r="K304" s="23"/>
-      <c r="L304" s="23"/>
+      <c r="H304" s="24">
+        <v>4</v>
+      </c>
+      <c r="I304" s="24">
+        <v>1639</v>
+      </c>
+      <c r="J304" s="39">
+        <v>849.76</v>
+      </c>
+      <c r="K304" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L304" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="305" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A305" s="21" t="s">
@@ -22210,11 +22360,21 @@
       <c r="G305" s="27" t="s">
         <v>501</v>
       </c>
-      <c r="H305" s="27"/>
-      <c r="I305" s="27"/>
-      <c r="J305" s="40"/>
-      <c r="K305" s="27"/>
-      <c r="L305" s="27"/>
+      <c r="H305" s="27">
+        <v>4</v>
+      </c>
+      <c r="I305" s="27">
+        <v>1627</v>
+      </c>
+      <c r="J305" s="40">
+        <v>838.37</v>
+      </c>
+      <c r="K305" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L305" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="306" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A306" s="21" t="s">
@@ -22238,11 +22398,21 @@
       <c r="G306" s="32" t="s">
         <v>502</v>
       </c>
-      <c r="H306" s="32"/>
-      <c r="I306" s="32"/>
-      <c r="J306" s="38"/>
-      <c r="K306" s="32"/>
-      <c r="L306" s="32"/>
+      <c r="H306" s="32">
+        <v>4</v>
+      </c>
+      <c r="I306" s="32">
+        <v>1753</v>
+      </c>
+      <c r="J306" s="38">
+        <v>927.56</v>
+      </c>
+      <c r="K306" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L306" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="307" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A307" s="21" t="s">
@@ -22266,11 +22436,21 @@
       <c r="G307" s="23" t="s">
         <v>503</v>
       </c>
-      <c r="H307" s="23"/>
-      <c r="I307" s="23"/>
-      <c r="J307" s="39"/>
-      <c r="K307" s="23"/>
-      <c r="L307" s="23"/>
+      <c r="H307" s="24">
+        <v>5</v>
+      </c>
+      <c r="I307" s="24">
+        <v>1715</v>
+      </c>
+      <c r="J307" s="39">
+        <v>994.53</v>
+      </c>
+      <c r="K307" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L307" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A308" s="21" t="s">
@@ -22294,11 +22474,21 @@
       <c r="G308" s="23" t="s">
         <v>504</v>
       </c>
-      <c r="H308" s="23"/>
-      <c r="I308" s="23"/>
-      <c r="J308" s="39"/>
-      <c r="K308" s="23"/>
-      <c r="L308" s="23"/>
+      <c r="H308" s="24">
+        <v>5</v>
+      </c>
+      <c r="I308" s="24">
+        <v>1730</v>
+      </c>
+      <c r="J308" s="39">
+        <v>936.48</v>
+      </c>
+      <c r="K308" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L308" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="309" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A309" s="21" t="s">
@@ -22322,11 +22512,21 @@
       <c r="G309" s="27" t="s">
         <v>505</v>
       </c>
-      <c r="H309" s="27"/>
-      <c r="I309" s="27"/>
-      <c r="J309" s="40"/>
-      <c r="K309" s="27"/>
-      <c r="L309" s="27"/>
+      <c r="H309" s="27">
+        <v>4</v>
+      </c>
+      <c r="I309" s="27">
+        <v>1723</v>
+      </c>
+      <c r="J309" s="40">
+        <v>890.2</v>
+      </c>
+      <c r="K309" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L309" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A310" s="21" t="s">
@@ -22350,11 +22550,21 @@
       <c r="G310" s="32" t="s">
         <v>506</v>
       </c>
-      <c r="H310" s="32"/>
-      <c r="I310" s="32"/>
-      <c r="J310" s="38"/>
-      <c r="K310" s="32"/>
-      <c r="L310" s="32"/>
+      <c r="H310" s="32">
+        <v>3</v>
+      </c>
+      <c r="I310" s="32">
+        <v>1550</v>
+      </c>
+      <c r="J310" s="38">
+        <v>789.86</v>
+      </c>
+      <c r="K310" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L310" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="311" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A311" s="21" t="s">
@@ -22378,11 +22588,21 @@
       <c r="G311" s="23" t="s">
         <v>507</v>
       </c>
-      <c r="H311" s="23"/>
-      <c r="I311" s="23"/>
-      <c r="J311" s="39"/>
-      <c r="K311" s="23"/>
-      <c r="L311" s="23"/>
+      <c r="H311" s="24">
+        <v>3</v>
+      </c>
+      <c r="I311" s="24">
+        <v>1483</v>
+      </c>
+      <c r="J311" s="39">
+        <v>744.89</v>
+      </c>
+      <c r="K311" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L311" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="312" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A312" s="21" t="s">
@@ -22406,11 +22626,21 @@
       <c r="G312" s="23" t="s">
         <v>508</v>
       </c>
-      <c r="H312" s="23"/>
-      <c r="I312" s="23"/>
-      <c r="J312" s="39"/>
-      <c r="K312" s="23"/>
-      <c r="L312" s="23"/>
+      <c r="H312" s="24">
+        <v>3</v>
+      </c>
+      <c r="I312" s="24">
+        <v>1627</v>
+      </c>
+      <c r="J312" s="39">
+        <v>840.1</v>
+      </c>
+      <c r="K312" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L312" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="313" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A313" s="21" t="s">
@@ -22434,11 +22664,21 @@
       <c r="G313" s="27" t="s">
         <v>509</v>
       </c>
-      <c r="H313" s="27"/>
-      <c r="I313" s="27"/>
-      <c r="J313" s="40"/>
-      <c r="K313" s="27"/>
-      <c r="L313" s="27"/>
+      <c r="H313" s="27">
+        <v>4</v>
+      </c>
+      <c r="I313" s="27">
+        <v>1725</v>
+      </c>
+      <c r="J313" s="40">
+        <v>892.99</v>
+      </c>
+      <c r="K313" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L313" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="314" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A314" s="21" t="s">
@@ -22462,11 +22702,21 @@
       <c r="G314" s="32" t="s">
         <v>510</v>
       </c>
-      <c r="H314" s="32"/>
-      <c r="I314" s="32"/>
-      <c r="J314" s="38"/>
-      <c r="K314" s="32"/>
-      <c r="L314" s="32"/>
+      <c r="H314" s="32">
+        <v>4</v>
+      </c>
+      <c r="I314" s="32">
+        <v>1753</v>
+      </c>
+      <c r="J314" s="38">
+        <v>927.56</v>
+      </c>
+      <c r="K314" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L314" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="315" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A315" s="21" t="s">
@@ -22490,11 +22740,21 @@
       <c r="G315" s="23" t="s">
         <v>511</v>
       </c>
-      <c r="H315" s="23"/>
-      <c r="I315" s="23"/>
-      <c r="J315" s="39"/>
-      <c r="K315" s="23"/>
-      <c r="L315" s="23"/>
+      <c r="H315" s="24">
+        <v>5</v>
+      </c>
+      <c r="I315" s="24">
+        <v>1715</v>
+      </c>
+      <c r="J315" s="39">
+        <v>994.53</v>
+      </c>
+      <c r="K315" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L315" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="316" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A316" s="21" t="s">
@@ -22518,11 +22778,21 @@
       <c r="G316" s="23" t="s">
         <v>512</v>
       </c>
-      <c r="H316" s="23"/>
-      <c r="I316" s="23"/>
-      <c r="J316" s="39"/>
-      <c r="K316" s="23"/>
-      <c r="L316" s="23"/>
+      <c r="H316" s="24">
+        <v>5</v>
+      </c>
+      <c r="I316" s="24">
+        <v>1730</v>
+      </c>
+      <c r="J316" s="39">
+        <v>936.48</v>
+      </c>
+      <c r="K316" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L316" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="317" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A317" s="21" t="s">
@@ -22546,11 +22816,21 @@
       <c r="G317" s="27" t="s">
         <v>513</v>
       </c>
-      <c r="H317" s="27"/>
-      <c r="I317" s="27"/>
-      <c r="J317" s="40"/>
-      <c r="K317" s="27"/>
-      <c r="L317" s="27"/>
+      <c r="H317" s="27">
+        <v>4</v>
+      </c>
+      <c r="I317" s="27">
+        <v>1723</v>
+      </c>
+      <c r="J317" s="40">
+        <v>890.2</v>
+      </c>
+      <c r="K317" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L317" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="318" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A318" s="21" t="s">
@@ -22574,11 +22854,21 @@
       <c r="G318" s="32" t="s">
         <v>514</v>
       </c>
-      <c r="H318" s="32"/>
-      <c r="I318" s="32"/>
-      <c r="J318" s="38"/>
-      <c r="K318" s="32"/>
-      <c r="L318" s="32"/>
+      <c r="H318" s="32">
+        <v>3</v>
+      </c>
+      <c r="I318" s="32">
+        <v>1550</v>
+      </c>
+      <c r="J318" s="38">
+        <v>789.86</v>
+      </c>
+      <c r="K318" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L318" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="319" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A319" s="21" t="s">
@@ -22602,11 +22892,21 @@
       <c r="G319" s="23" t="s">
         <v>515</v>
       </c>
-      <c r="H319" s="23"/>
-      <c r="I319" s="23"/>
-      <c r="J319" s="39"/>
-      <c r="K319" s="23"/>
-      <c r="L319" s="23"/>
+      <c r="H319" s="24">
+        <v>3</v>
+      </c>
+      <c r="I319" s="24">
+        <v>1483</v>
+      </c>
+      <c r="J319" s="39">
+        <v>744.89</v>
+      </c>
+      <c r="K319" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L319" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="320" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A320" s="21" t="s">
@@ -22630,11 +22930,21 @@
       <c r="G320" s="23" t="s">
         <v>516</v>
       </c>
-      <c r="H320" s="23"/>
-      <c r="I320" s="23"/>
-      <c r="J320" s="39"/>
-      <c r="K320" s="23"/>
-      <c r="L320" s="23"/>
+      <c r="H320" s="24">
+        <v>3</v>
+      </c>
+      <c r="I320" s="24">
+        <v>1627</v>
+      </c>
+      <c r="J320" s="39">
+        <v>840.1</v>
+      </c>
+      <c r="K320" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L320" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="321" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A321" s="21" t="s">
@@ -22658,11 +22968,21 @@
       <c r="G321" s="27" t="s">
         <v>517</v>
       </c>
-      <c r="H321" s="27"/>
-      <c r="I321" s="27"/>
-      <c r="J321" s="40"/>
-      <c r="K321" s="27"/>
-      <c r="L321" s="27"/>
+      <c r="H321" s="27">
+        <v>4</v>
+      </c>
+      <c r="I321" s="27">
+        <v>1725</v>
+      </c>
+      <c r="J321" s="40">
+        <v>892.99</v>
+      </c>
+      <c r="K321" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L321" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="322" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A322" s="21" t="s">

</xml_diff>

<commit_message>
starter region 4 results
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E27BAB0-19FC-48D6-B532-0B12D0F6F989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3393BB53-1F80-40B3-9FEA-896E30FB45C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="870" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="870" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="full_model_set" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4782" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4870" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -10501,8 +10501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C303" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H322" sqref="H322"/>
+    <sheetView tabSelected="1" topLeftCell="C339" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H354" sqref="H354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23006,11 +23006,21 @@
       <c r="G322" s="32" t="s">
         <v>549</v>
       </c>
-      <c r="H322" s="32"/>
-      <c r="I322" s="32"/>
-      <c r="J322" s="38"/>
-      <c r="K322" s="32"/>
-      <c r="L322" s="32"/>
+      <c r="H322" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I322" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J322" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K322" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L322" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="323" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A323" s="21" t="s">
@@ -23034,11 +23044,21 @@
       <c r="G323" s="23" t="s">
         <v>550</v>
       </c>
-      <c r="H323" s="23"/>
-      <c r="I323" s="23"/>
-      <c r="J323" s="39"/>
-      <c r="K323" s="23"/>
-      <c r="L323" s="23"/>
+      <c r="H323" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I323" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J323" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K323" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L323" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="324" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A324" s="21" t="s">
@@ -23062,11 +23082,21 @@
       <c r="G324" s="23" t="s">
         <v>519</v>
       </c>
-      <c r="H324" s="23"/>
-      <c r="I324" s="23"/>
-      <c r="J324" s="39"/>
-      <c r="K324" s="23"/>
-      <c r="L324" s="23"/>
+      <c r="H324" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I324" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J324" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K324" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L324" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="325" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A325" s="21" t="s">
@@ -23090,11 +23120,21 @@
       <c r="G325" s="27" t="s">
         <v>520</v>
       </c>
-      <c r="H325" s="27"/>
-      <c r="I325" s="27"/>
-      <c r="J325" s="40"/>
-      <c r="K325" s="27"/>
-      <c r="L325" s="27"/>
+      <c r="H325" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I325" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J325" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K325" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L325" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="326" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A326" s="21" t="s">
@@ -23118,11 +23158,21 @@
       <c r="G326" s="32" t="s">
         <v>521</v>
       </c>
-      <c r="H326" s="32"/>
-      <c r="I326" s="32"/>
-      <c r="J326" s="38"/>
-      <c r="K326" s="32"/>
-      <c r="L326" s="32"/>
+      <c r="H326" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I326" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J326" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K326" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L326" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="327" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A327" s="21" t="s">
@@ -23146,11 +23196,21 @@
       <c r="G327" s="23" t="s">
         <v>522</v>
       </c>
-      <c r="H327" s="23"/>
-      <c r="I327" s="23"/>
-      <c r="J327" s="39"/>
-      <c r="K327" s="23"/>
-      <c r="L327" s="23"/>
+      <c r="H327" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I327" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J327" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K327" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L327" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="328" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A328" s="21" t="s">
@@ -23174,11 +23234,21 @@
       <c r="G328" s="23" t="s">
         <v>523</v>
       </c>
-      <c r="H328" s="23"/>
-      <c r="I328" s="23"/>
-      <c r="J328" s="39"/>
-      <c r="K328" s="23"/>
-      <c r="L328" s="23"/>
+      <c r="H328" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I328" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J328" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K328" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L328" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="329" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A329" s="21" t="s">
@@ -23202,11 +23272,21 @@
       <c r="G329" s="27" t="s">
         <v>524</v>
       </c>
-      <c r="H329" s="27"/>
-      <c r="I329" s="27"/>
-      <c r="J329" s="40"/>
-      <c r="K329" s="27"/>
-      <c r="L329" s="27"/>
+      <c r="H329" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I329" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J329" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K329" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L329" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="330" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A330" s="21" t="s">
@@ -23230,11 +23310,21 @@
       <c r="G330" s="32" t="s">
         <v>525</v>
       </c>
-      <c r="H330" s="32"/>
-      <c r="I330" s="32"/>
-      <c r="J330" s="38"/>
-      <c r="K330" s="32"/>
-      <c r="L330" s="32"/>
+      <c r="H330" s="32">
+        <v>7</v>
+      </c>
+      <c r="I330" s="32">
+        <v>2329</v>
+      </c>
+      <c r="J330" s="38">
+        <v>1126.8599999999999</v>
+      </c>
+      <c r="K330" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L330" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="331" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A331" s="21" t="s">
@@ -23258,11 +23348,21 @@
       <c r="G331" s="23" t="s">
         <v>526</v>
       </c>
-      <c r="H331" s="23"/>
-      <c r="I331" s="23"/>
-      <c r="J331" s="39"/>
-      <c r="K331" s="23"/>
-      <c r="L331" s="23"/>
+      <c r="H331" s="23">
+        <v>8</v>
+      </c>
+      <c r="I331" s="23">
+        <v>2695</v>
+      </c>
+      <c r="J331" s="39">
+        <v>1519.24</v>
+      </c>
+      <c r="K331" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L331" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="332" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A332" s="21" t="s">
@@ -23286,11 +23386,21 @@
       <c r="G332" s="23" t="s">
         <v>527</v>
       </c>
-      <c r="H332" s="23"/>
-      <c r="I332" s="23"/>
-      <c r="J332" s="39"/>
-      <c r="K332" s="23"/>
-      <c r="L332" s="23"/>
+      <c r="H332" s="23">
+        <v>8</v>
+      </c>
+      <c r="I332" s="23">
+        <v>2912</v>
+      </c>
+      <c r="J332" s="39">
+        <v>1558.6</v>
+      </c>
+      <c r="K332" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L332" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="333" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A333" s="21" t="s">
@@ -23314,11 +23424,21 @@
       <c r="G333" s="27" t="s">
         <v>528</v>
       </c>
-      <c r="H333" s="27"/>
-      <c r="I333" s="27"/>
-      <c r="J333" s="40"/>
-      <c r="K333" s="27"/>
-      <c r="L333" s="27"/>
+      <c r="H333" s="27">
+        <v>8</v>
+      </c>
+      <c r="I333" s="27">
+        <v>2658</v>
+      </c>
+      <c r="J333" s="40">
+        <v>1465.3</v>
+      </c>
+      <c r="K333" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L333" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="334" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A334" s="21" t="s">
@@ -23342,11 +23462,21 @@
       <c r="G334" s="32" t="s">
         <v>529</v>
       </c>
-      <c r="H334" s="32"/>
-      <c r="I334" s="32"/>
-      <c r="J334" s="38"/>
-      <c r="K334" s="32"/>
-      <c r="L334" s="32"/>
+      <c r="H334" s="32">
+        <v>6</v>
+      </c>
+      <c r="I334" s="32">
+        <v>2537</v>
+      </c>
+      <c r="J334" s="38">
+        <v>1305.26</v>
+      </c>
+      <c r="K334" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L334" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="335" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A335" s="21" t="s">
@@ -23370,11 +23500,21 @@
       <c r="G335" s="23" t="s">
         <v>530</v>
       </c>
-      <c r="H335" s="23"/>
-      <c r="I335" s="23"/>
-      <c r="J335" s="39"/>
-      <c r="K335" s="23"/>
-      <c r="L335" s="23"/>
+      <c r="H335" s="24">
+        <v>6</v>
+      </c>
+      <c r="I335" s="24">
+        <v>2674</v>
+      </c>
+      <c r="J335" s="39">
+        <v>1343.06</v>
+      </c>
+      <c r="K335" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L335" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="336" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A336" s="21" t="s">
@@ -23398,11 +23538,21 @@
       <c r="G336" s="23" t="s">
         <v>531</v>
       </c>
-      <c r="H336" s="23"/>
-      <c r="I336" s="23"/>
-      <c r="J336" s="39"/>
-      <c r="K336" s="23"/>
-      <c r="L336" s="23"/>
+      <c r="H336" s="24">
+        <v>7</v>
+      </c>
+      <c r="I336" s="24">
+        <v>2631</v>
+      </c>
+      <c r="J336" s="39">
+        <v>1367.83</v>
+      </c>
+      <c r="K336" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L336" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="337" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A337" s="21" t="s">
@@ -23426,11 +23576,21 @@
       <c r="G337" s="27" t="s">
         <v>532</v>
       </c>
-      <c r="H337" s="27"/>
-      <c r="I337" s="27"/>
-      <c r="J337" s="40"/>
-      <c r="K337" s="27"/>
-      <c r="L337" s="27"/>
+      <c r="H337" s="27">
+        <v>6</v>
+      </c>
+      <c r="I337" s="27">
+        <v>2726</v>
+      </c>
+      <c r="J337" s="40">
+        <v>1396.91</v>
+      </c>
+      <c r="K337" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L337" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="338" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A338" s="21" t="s">
@@ -23454,11 +23614,21 @@
       <c r="G338" s="32" t="s">
         <v>533</v>
       </c>
-      <c r="H338" s="32"/>
-      <c r="I338" s="32"/>
-      <c r="J338" s="38"/>
-      <c r="K338" s="32"/>
-      <c r="L338" s="32"/>
+      <c r="H338" s="32">
+        <v>5</v>
+      </c>
+      <c r="I338" s="32">
+        <v>2327</v>
+      </c>
+      <c r="J338" s="38">
+        <v>1104.1500000000001</v>
+      </c>
+      <c r="K338" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L338" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="339" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A339" s="21" t="s">
@@ -23482,11 +23652,21 @@
       <c r="G339" s="23" t="s">
         <v>534</v>
       </c>
-      <c r="H339" s="23"/>
-      <c r="I339" s="23"/>
-      <c r="J339" s="39"/>
-      <c r="K339" s="23"/>
-      <c r="L339" s="23"/>
+      <c r="H339" s="24">
+        <v>7</v>
+      </c>
+      <c r="I339" s="24">
+        <v>2594</v>
+      </c>
+      <c r="J339" s="39">
+        <v>1350.12</v>
+      </c>
+      <c r="K339" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L339" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="340" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A340" s="21" t="s">
@@ -23510,11 +23690,21 @@
       <c r="G340" s="23" t="s">
         <v>535</v>
       </c>
-      <c r="H340" s="23"/>
-      <c r="I340" s="23"/>
-      <c r="J340" s="39"/>
-      <c r="K340" s="23"/>
-      <c r="L340" s="23"/>
+      <c r="H340" s="24">
+        <v>7</v>
+      </c>
+      <c r="I340" s="24">
+        <v>2534</v>
+      </c>
+      <c r="J340" s="39">
+        <v>1304.95</v>
+      </c>
+      <c r="K340" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L340" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="341" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A341" s="21" t="s">
@@ -23538,11 +23728,21 @@
       <c r="G341" s="27" t="s">
         <v>536</v>
       </c>
-      <c r="H341" s="27"/>
-      <c r="I341" s="27"/>
-      <c r="J341" s="40"/>
-      <c r="K341" s="27"/>
-      <c r="L341" s="27"/>
+      <c r="H341" s="27">
+        <v>7</v>
+      </c>
+      <c r="I341" s="27">
+        <v>2736</v>
+      </c>
+      <c r="J341" s="40">
+        <v>1412.54</v>
+      </c>
+      <c r="K341" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L341" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="342" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A342" s="21" t="s">
@@ -23566,11 +23766,21 @@
       <c r="G342" s="32" t="s">
         <v>537</v>
       </c>
-      <c r="H342" s="32"/>
-      <c r="I342" s="32"/>
-      <c r="J342" s="38"/>
-      <c r="K342" s="32"/>
-      <c r="L342" s="32"/>
+      <c r="H342" s="32">
+        <v>4</v>
+      </c>
+      <c r="I342" s="32">
+        <v>2135</v>
+      </c>
+      <c r="J342" s="38">
+        <v>985.32</v>
+      </c>
+      <c r="K342" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L342" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="343" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A343" s="21" t="s">
@@ -23594,11 +23804,21 @@
       <c r="G343" s="23" t="s">
         <v>538</v>
       </c>
-      <c r="H343" s="23"/>
-      <c r="I343" s="23"/>
-      <c r="J343" s="39"/>
-      <c r="K343" s="23"/>
-      <c r="L343" s="23"/>
+      <c r="H343" s="24">
+        <v>5</v>
+      </c>
+      <c r="I343" s="24">
+        <v>2325</v>
+      </c>
+      <c r="J343" s="39">
+        <v>1127.8699999999999</v>
+      </c>
+      <c r="K343" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L343" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="344" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A344" s="21" t="s">
@@ -23622,11 +23842,21 @@
       <c r="G344" s="23" t="s">
         <v>539</v>
       </c>
-      <c r="H344" s="23"/>
-      <c r="I344" s="23"/>
-      <c r="J344" s="39"/>
-      <c r="K344" s="23"/>
-      <c r="L344" s="23"/>
+      <c r="H344" s="24">
+        <v>6</v>
+      </c>
+      <c r="I344" s="24">
+        <v>2561</v>
+      </c>
+      <c r="J344" s="39">
+        <v>1283.95</v>
+      </c>
+      <c r="K344" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L344" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="345" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A345" s="21" t="s">
@@ -23650,11 +23880,21 @@
       <c r="G345" s="27" t="s">
         <v>540</v>
       </c>
-      <c r="H345" s="27"/>
-      <c r="I345" s="27"/>
-      <c r="J345" s="40"/>
-      <c r="K345" s="27"/>
-      <c r="L345" s="27"/>
+      <c r="H345" s="27">
+        <v>5</v>
+      </c>
+      <c r="I345" s="27">
+        <v>2298</v>
+      </c>
+      <c r="J345" s="40">
+        <v>1102.31</v>
+      </c>
+      <c r="K345" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L345" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="346" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A346" s="21" t="s">
@@ -23678,11 +23918,21 @@
       <c r="G346" s="32" t="s">
         <v>541</v>
       </c>
-      <c r="H346" s="32"/>
-      <c r="I346" s="32"/>
-      <c r="J346" s="38"/>
-      <c r="K346" s="32"/>
-      <c r="L346" s="32"/>
+      <c r="H346" s="32">
+        <v>5</v>
+      </c>
+      <c r="I346" s="32">
+        <v>2327</v>
+      </c>
+      <c r="J346" s="38">
+        <v>1104.1500000000001</v>
+      </c>
+      <c r="K346" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L346" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="347" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A347" s="21" t="s">
@@ -23706,11 +23956,21 @@
       <c r="G347" s="23" t="s">
         <v>542</v>
       </c>
-      <c r="H347" s="23"/>
-      <c r="I347" s="23"/>
-      <c r="J347" s="39"/>
-      <c r="K347" s="23"/>
-      <c r="L347" s="23"/>
+      <c r="H347" s="24">
+        <v>7</v>
+      </c>
+      <c r="I347" s="24">
+        <v>2582</v>
+      </c>
+      <c r="J347" s="39">
+        <v>1341.42</v>
+      </c>
+      <c r="K347" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L347" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="348" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A348" s="21" t="s">
@@ -23734,11 +23994,21 @@
       <c r="G348" s="23" t="s">
         <v>543</v>
       </c>
-      <c r="H348" s="23"/>
-      <c r="I348" s="23"/>
-      <c r="J348" s="39"/>
-      <c r="K348" s="23"/>
-      <c r="L348" s="23"/>
+      <c r="H348" s="24">
+        <v>7</v>
+      </c>
+      <c r="I348" s="24">
+        <v>2534</v>
+      </c>
+      <c r="J348" s="39">
+        <v>1304.95</v>
+      </c>
+      <c r="K348" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L348" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="349" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A349" s="21" t="s">
@@ -23762,11 +24032,21 @@
       <c r="G349" s="27" t="s">
         <v>544</v>
       </c>
-      <c r="H349" s="27"/>
-      <c r="I349" s="27"/>
-      <c r="J349" s="40"/>
-      <c r="K349" s="27"/>
-      <c r="L349" s="27"/>
+      <c r="H349" s="27">
+        <v>7</v>
+      </c>
+      <c r="I349" s="27">
+        <v>2736</v>
+      </c>
+      <c r="J349" s="40">
+        <v>1412.54</v>
+      </c>
+      <c r="K349" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L349" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="350" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A350" s="21" t="s">
@@ -23790,11 +24070,21 @@
       <c r="G350" s="32" t="s">
         <v>545</v>
       </c>
-      <c r="H350" s="32"/>
-      <c r="I350" s="32"/>
-      <c r="J350" s="38"/>
-      <c r="K350" s="32"/>
-      <c r="L350" s="32"/>
+      <c r="H350" s="32">
+        <v>4</v>
+      </c>
+      <c r="I350" s="32">
+        <v>2135</v>
+      </c>
+      <c r="J350" s="38">
+        <v>985.32</v>
+      </c>
+      <c r="K350" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L350" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="351" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A351" s="21" t="s">
@@ -23818,11 +24108,21 @@
       <c r="G351" s="23" t="s">
         <v>546</v>
       </c>
-      <c r="H351" s="23"/>
-      <c r="I351" s="23"/>
-      <c r="J351" s="39"/>
-      <c r="K351" s="23"/>
-      <c r="L351" s="23"/>
+      <c r="H351" s="24">
+        <v>5</v>
+      </c>
+      <c r="I351" s="24">
+        <v>2325</v>
+      </c>
+      <c r="J351" s="39">
+        <v>1127.8699999999999</v>
+      </c>
+      <c r="K351" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L351" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="352" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A352" s="21" t="s">
@@ -23846,11 +24146,21 @@
       <c r="G352" s="23" t="s">
         <v>547</v>
       </c>
-      <c r="H352" s="23"/>
-      <c r="I352" s="23"/>
-      <c r="J352" s="39"/>
-      <c r="K352" s="23"/>
-      <c r="L352" s="23"/>
+      <c r="H352" s="24">
+        <v>6</v>
+      </c>
+      <c r="I352" s="24">
+        <v>2561</v>
+      </c>
+      <c r="J352" s="39">
+        <v>1283.95</v>
+      </c>
+      <c r="K352" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L352" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="353" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A353" s="21" t="s">
@@ -23874,11 +24184,21 @@
       <c r="G353" s="27" t="s">
         <v>548</v>
       </c>
-      <c r="H353" s="27"/>
-      <c r="I353" s="27"/>
-      <c r="J353" s="40"/>
-      <c r="K353" s="27"/>
-      <c r="L353" s="27"/>
+      <c r="H353" s="27">
+        <v>5</v>
+      </c>
+      <c r="I353" s="27">
+        <v>2360</v>
+      </c>
+      <c r="J353" s="40">
+        <v>1138.05</v>
+      </c>
+      <c r="K353" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L353" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="354" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A354" s="21" t="s">

</xml_diff>

<commit_message>
starter region 6 results
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4934" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5046" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -4684,7 +4684,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6333,7 +6333,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10500,8 +10500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C349" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H362" sqref="H362"/>
+    <sheetView tabSelected="1" topLeftCell="C390" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H418" sqref="H418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25437,11 +25437,21 @@
       <c r="G386" s="32" t="s">
         <v>611</v>
       </c>
-      <c r="H386" s="32"/>
-      <c r="I386" s="32"/>
-      <c r="J386" s="38"/>
-      <c r="K386" s="32"/>
-      <c r="L386" s="32"/>
+      <c r="H386" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I386" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J386" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K386" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L386" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="387" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A387" s="21" t="s">
@@ -25465,11 +25475,21 @@
       <c r="G387" s="23" t="s">
         <v>612</v>
       </c>
-      <c r="H387" s="23"/>
-      <c r="I387" s="23"/>
-      <c r="J387" s="39"/>
-      <c r="K387" s="23"/>
-      <c r="L387" s="23"/>
+      <c r="H387" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I387" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J387" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K387" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L387" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="388" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A388" s="21" t="s">
@@ -25493,11 +25513,21 @@
       <c r="G388" s="23" t="s">
         <v>613</v>
       </c>
-      <c r="H388" s="23"/>
-      <c r="I388" s="23"/>
-      <c r="J388" s="39"/>
-      <c r="K388" s="23"/>
-      <c r="L388" s="23"/>
+      <c r="H388" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I388" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J388" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K388" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L388" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="389" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A389" s="21" t="s">
@@ -25521,11 +25551,21 @@
       <c r="G389" s="27" t="s">
         <v>614</v>
       </c>
-      <c r="H389" s="27"/>
-      <c r="I389" s="27"/>
-      <c r="J389" s="40"/>
-      <c r="K389" s="27"/>
-      <c r="L389" s="27"/>
+      <c r="H389" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I389" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J389" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K389" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L389" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="390" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A390" s="21" t="s">
@@ -25549,11 +25589,21 @@
       <c r="G390" s="32" t="s">
         <v>583</v>
       </c>
-      <c r="H390" s="32"/>
-      <c r="I390" s="32"/>
-      <c r="J390" s="38"/>
-      <c r="K390" s="32"/>
-      <c r="L390" s="32"/>
+      <c r="H390" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I390" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J390" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K390" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L390" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="391" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A391" s="21" t="s">
@@ -25577,11 +25627,21 @@
       <c r="G391" s="23" t="s">
         <v>584</v>
       </c>
-      <c r="H391" s="23"/>
-      <c r="I391" s="23"/>
-      <c r="J391" s="39"/>
-      <c r="K391" s="23"/>
-      <c r="L391" s="23"/>
+      <c r="H391" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I391" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J391" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K391" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L391" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="392" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A392" s="21" t="s">
@@ -25605,11 +25665,21 @@
       <c r="G392" s="23" t="s">
         <v>585</v>
       </c>
-      <c r="H392" s="23"/>
-      <c r="I392" s="23"/>
-      <c r="J392" s="39"/>
-      <c r="K392" s="23"/>
-      <c r="L392" s="23"/>
+      <c r="H392" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I392" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J392" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K392" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L392" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="393" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A393" s="21" t="s">
@@ -25633,11 +25703,21 @@
       <c r="G393" s="27" t="s">
         <v>586</v>
       </c>
-      <c r="H393" s="27"/>
-      <c r="I393" s="27"/>
-      <c r="J393" s="40"/>
-      <c r="K393" s="27"/>
-      <c r="L393" s="27"/>
+      <c r="H393" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I393" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J393" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K393" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L393" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="394" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A394" s="21" t="s">
@@ -25661,11 +25741,21 @@
       <c r="G394" s="32" t="s">
         <v>587</v>
       </c>
-      <c r="H394" s="32"/>
-      <c r="I394" s="32"/>
-      <c r="J394" s="38"/>
-      <c r="K394" s="32"/>
-      <c r="L394" s="32"/>
+      <c r="H394" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I394" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J394" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K394" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L394" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="395" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A395" s="21" t="s">
@@ -25689,11 +25779,21 @@
       <c r="G395" s="23" t="s">
         <v>588</v>
       </c>
-      <c r="H395" s="23"/>
-      <c r="I395" s="23"/>
-      <c r="J395" s="39"/>
-      <c r="K395" s="23"/>
-      <c r="L395" s="23"/>
+      <c r="H395" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I395" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J395" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K395" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L395" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="396" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A396" s="21" t="s">
@@ -25717,11 +25817,21 @@
       <c r="G396" s="23" t="s">
         <v>589</v>
       </c>
-      <c r="H396" s="23"/>
-      <c r="I396" s="23"/>
-      <c r="J396" s="39"/>
-      <c r="K396" s="23"/>
-      <c r="L396" s="23"/>
+      <c r="H396" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I396" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J396" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K396" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L396" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="397" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A397" s="21" t="s">
@@ -25745,11 +25855,21 @@
       <c r="G397" s="27" t="s">
         <v>590</v>
       </c>
-      <c r="H397" s="27"/>
-      <c r="I397" s="27"/>
-      <c r="J397" s="40"/>
-      <c r="K397" s="27"/>
-      <c r="L397" s="27"/>
+      <c r="H397" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I397" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J397" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K397" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L397" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="398" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A398" s="21" t="s">
@@ -25773,11 +25893,21 @@
       <c r="G398" s="32" t="s">
         <v>591</v>
       </c>
-      <c r="H398" s="32"/>
-      <c r="I398" s="32"/>
-      <c r="J398" s="38"/>
-      <c r="K398" s="32"/>
-      <c r="L398" s="32"/>
+      <c r="H398" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I398" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J398" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K398" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L398" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="399" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A399" s="21" t="s">
@@ -25801,11 +25931,21 @@
       <c r="G399" s="23" t="s">
         <v>592</v>
       </c>
-      <c r="H399" s="23"/>
-      <c r="I399" s="23"/>
-      <c r="J399" s="39"/>
-      <c r="K399" s="23"/>
-      <c r="L399" s="23"/>
+      <c r="H399" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I399" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J399" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K399" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L399" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="400" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A400" s="21" t="s">
@@ -25829,11 +25969,21 @@
       <c r="G400" s="23" t="s">
         <v>593</v>
       </c>
-      <c r="H400" s="23"/>
-      <c r="I400" s="23"/>
-      <c r="J400" s="39"/>
-      <c r="K400" s="23"/>
-      <c r="L400" s="23"/>
+      <c r="H400" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I400" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J400" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K400" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L400" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="401" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A401" s="21" t="s">
@@ -25857,11 +26007,21 @@
       <c r="G401" s="27" t="s">
         <v>594</v>
       </c>
-      <c r="H401" s="27"/>
-      <c r="I401" s="27"/>
-      <c r="J401" s="40"/>
-      <c r="K401" s="27"/>
-      <c r="L401" s="27"/>
+      <c r="H401" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I401" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J401" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K401" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L401" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="402" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A402" s="21" t="s">
@@ -25885,11 +26045,21 @@
       <c r="G402" s="32" t="s">
         <v>595</v>
       </c>
-      <c r="H402" s="32"/>
-      <c r="I402" s="32"/>
-      <c r="J402" s="38"/>
-      <c r="K402" s="32"/>
-      <c r="L402" s="32"/>
+      <c r="H402" s="32">
+        <v>6</v>
+      </c>
+      <c r="I402" s="32">
+        <v>2673</v>
+      </c>
+      <c r="J402" s="38">
+        <v>1220.53</v>
+      </c>
+      <c r="K402" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L402" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="403" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A403" s="21" t="s">
@@ -25913,11 +26083,21 @@
       <c r="G403" s="23" t="s">
         <v>596</v>
       </c>
-      <c r="H403" s="23"/>
-      <c r="I403" s="23"/>
-      <c r="J403" s="39"/>
-      <c r="K403" s="23"/>
-      <c r="L403" s="23"/>
+      <c r="H403" s="23">
+        <v>7</v>
+      </c>
+      <c r="I403" s="23">
+        <v>2955</v>
+      </c>
+      <c r="J403" s="39">
+        <v>1405.63</v>
+      </c>
+      <c r="K403" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L403" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="404" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A404" s="21" t="s">
@@ -25941,11 +26121,21 @@
       <c r="G404" s="23" t="s">
         <v>597</v>
       </c>
-      <c r="H404" s="23"/>
-      <c r="I404" s="23"/>
-      <c r="J404" s="39"/>
-      <c r="K404" s="23"/>
-      <c r="L404" s="23"/>
+      <c r="H404" s="23">
+        <v>7</v>
+      </c>
+      <c r="I404" s="23">
+        <v>2719</v>
+      </c>
+      <c r="J404" s="39">
+        <v>1252.6600000000001</v>
+      </c>
+      <c r="K404" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L404" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="405" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A405" s="21" t="s">
@@ -25969,11 +26159,21 @@
       <c r="G405" s="27" t="s">
         <v>598</v>
       </c>
-      <c r="H405" s="27"/>
-      <c r="I405" s="27"/>
-      <c r="J405" s="40"/>
-      <c r="K405" s="27"/>
-      <c r="L405" s="27"/>
+      <c r="H405" s="27">
+        <v>7</v>
+      </c>
+      <c r="I405" s="27">
+        <v>2751</v>
+      </c>
+      <c r="J405" s="40">
+        <v>1262.0899999999999</v>
+      </c>
+      <c r="K405" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L405" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="406" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A406" s="21" t="s">
@@ -25997,11 +26197,21 @@
       <c r="G406" s="32" t="s">
         <v>599</v>
       </c>
-      <c r="H406" s="32"/>
-      <c r="I406" s="32"/>
-      <c r="J406" s="38"/>
-      <c r="K406" s="32"/>
-      <c r="L406" s="32"/>
+      <c r="H406" s="32">
+        <v>5</v>
+      </c>
+      <c r="I406" s="32">
+        <v>2566</v>
+      </c>
+      <c r="J406" s="38">
+        <v>1136.72</v>
+      </c>
+      <c r="K406" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L406" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="407" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A407" s="21" t="s">
@@ -26025,11 +26235,21 @@
       <c r="G407" s="23" t="s">
         <v>600</v>
       </c>
-      <c r="H407" s="23"/>
-      <c r="I407" s="23"/>
-      <c r="J407" s="39"/>
-      <c r="K407" s="23"/>
-      <c r="L407" s="23"/>
+      <c r="H407" s="24">
+        <v>6</v>
+      </c>
+      <c r="I407" s="24">
+        <v>2856</v>
+      </c>
+      <c r="J407" s="39">
+        <v>1315.37</v>
+      </c>
+      <c r="K407" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L407" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="408" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A408" s="21" t="s">
@@ -26053,11 +26273,21 @@
       <c r="G408" s="23" t="s">
         <v>601</v>
       </c>
-      <c r="H408" s="23"/>
-      <c r="I408" s="23"/>
-      <c r="J408" s="39"/>
-      <c r="K408" s="23"/>
-      <c r="L408" s="23"/>
+      <c r="H408" s="24">
+        <v>5</v>
+      </c>
+      <c r="I408" s="24">
+        <v>2574</v>
+      </c>
+      <c r="J408" s="39">
+        <v>1151.22</v>
+      </c>
+      <c r="K408" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L408" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="409" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A409" s="21" t="s">
@@ -26081,11 +26311,21 @@
       <c r="G409" s="27" t="s">
         <v>602</v>
       </c>
-      <c r="H409" s="27"/>
-      <c r="I409" s="27"/>
-      <c r="J409" s="40"/>
-      <c r="K409" s="27"/>
-      <c r="L409" s="27"/>
+      <c r="H409" s="27">
+        <v>5</v>
+      </c>
+      <c r="I409" s="27">
+        <v>2470</v>
+      </c>
+      <c r="J409" s="40">
+        <v>1094.18</v>
+      </c>
+      <c r="K409" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L409" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="410" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A410" s="21" t="s">
@@ -26109,11 +26349,21 @@
       <c r="G410" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="H410" s="32"/>
-      <c r="I410" s="32"/>
-      <c r="J410" s="38"/>
-      <c r="K410" s="32"/>
-      <c r="L410" s="32"/>
+      <c r="H410" s="32">
+        <v>6</v>
+      </c>
+      <c r="I410" s="32">
+        <v>2594</v>
+      </c>
+      <c r="J410" s="38">
+        <v>1195.67</v>
+      </c>
+      <c r="K410" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L410" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="411" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A411" s="21" t="s">
@@ -26137,11 +26387,21 @@
       <c r="G411" s="23" t="s">
         <v>604</v>
       </c>
-      <c r="H411" s="23"/>
-      <c r="I411" s="23"/>
-      <c r="J411" s="39"/>
-      <c r="K411" s="23"/>
-      <c r="L411" s="23"/>
+      <c r="H411" s="24">
+        <v>7</v>
+      </c>
+      <c r="I411" s="24">
+        <v>2589</v>
+      </c>
+      <c r="J411" s="39">
+        <v>1152.79</v>
+      </c>
+      <c r="K411" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L411" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="412" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A412" s="21" t="s">
@@ -26165,11 +26425,21 @@
       <c r="G412" s="23" t="s">
         <v>605</v>
       </c>
-      <c r="H412" s="23"/>
-      <c r="I412" s="23"/>
-      <c r="J412" s="39"/>
-      <c r="K412" s="23"/>
-      <c r="L412" s="23"/>
+      <c r="H412" s="24">
+        <v>7</v>
+      </c>
+      <c r="I412" s="24">
+        <v>2662</v>
+      </c>
+      <c r="J412" s="39">
+        <v>1184.0999999999999</v>
+      </c>
+      <c r="K412" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L412" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="413" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A413" s="21" t="s">
@@ -26193,11 +26463,21 @@
       <c r="G413" s="27" t="s">
         <v>606</v>
       </c>
-      <c r="H413" s="27"/>
-      <c r="I413" s="27"/>
-      <c r="J413" s="40"/>
-      <c r="K413" s="27"/>
-      <c r="L413" s="27"/>
+      <c r="H413" s="27">
+        <v>7</v>
+      </c>
+      <c r="I413" s="27">
+        <v>2726</v>
+      </c>
+      <c r="J413" s="40">
+        <v>1262.95</v>
+      </c>
+      <c r="K413" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L413" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="414" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A414" s="21" t="s">
@@ -26221,11 +26501,21 @@
       <c r="G414" s="32" t="s">
         <v>607</v>
       </c>
-      <c r="H414" s="32"/>
-      <c r="I414" s="32"/>
-      <c r="J414" s="38"/>
-      <c r="K414" s="32"/>
-      <c r="L414" s="32"/>
+      <c r="H414" s="32">
+        <v>5</v>
+      </c>
+      <c r="I414" s="32">
+        <v>2596</v>
+      </c>
+      <c r="J414" s="38">
+        <v>1197.74</v>
+      </c>
+      <c r="K414" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L414" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="415" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A415" s="21" t="s">
@@ -26249,11 +26539,21 @@
       <c r="G415" s="23" t="s">
         <v>608</v>
       </c>
-      <c r="H415" s="23"/>
-      <c r="I415" s="23"/>
-      <c r="J415" s="39"/>
-      <c r="K415" s="23"/>
-      <c r="L415" s="23"/>
+      <c r="H415" s="24">
+        <v>5</v>
+      </c>
+      <c r="I415" s="24">
+        <v>2620</v>
+      </c>
+      <c r="J415" s="39">
+        <v>1196.56</v>
+      </c>
+      <c r="K415" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L415" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="416" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A416" s="21" t="s">
@@ -26277,11 +26577,21 @@
       <c r="G416" s="23" t="s">
         <v>609</v>
       </c>
-      <c r="H416" s="23"/>
-      <c r="I416" s="23"/>
-      <c r="J416" s="39"/>
-      <c r="K416" s="23"/>
-      <c r="L416" s="23"/>
+      <c r="H416" s="24">
+        <v>5</v>
+      </c>
+      <c r="I416" s="24">
+        <v>2601</v>
+      </c>
+      <c r="J416" s="39">
+        <v>1187.74</v>
+      </c>
+      <c r="K416" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L416" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="417" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A417" s="21" t="s">
@@ -26305,11 +26615,21 @@
       <c r="G417" s="27" t="s">
         <v>610</v>
       </c>
-      <c r="H417" s="27"/>
-      <c r="I417" s="27"/>
-      <c r="J417" s="40"/>
-      <c r="K417" s="27"/>
-      <c r="L417" s="27"/>
+      <c r="H417" s="27">
+        <v>5</v>
+      </c>
+      <c r="I417" s="27">
+        <v>2480</v>
+      </c>
+      <c r="J417" s="40">
+        <v>1063.96</v>
+      </c>
+      <c r="K417" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L417" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="418" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A418" s="21" t="s">

</xml_diff>

<commit_message>
starter region 7 results
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5046" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5140" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -4684,7 +4684,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
+      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6333,7 +6333,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomRight" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10500,8 +10500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C390" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H418" sqref="H418"/>
+    <sheetView tabSelected="1" topLeftCell="C415" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H450" sqref="H450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26653,11 +26653,21 @@
       <c r="G418" s="32" t="s">
         <v>642</v>
       </c>
-      <c r="H418" s="32"/>
-      <c r="I418" s="32"/>
-      <c r="J418" s="38"/>
-      <c r="K418" s="32"/>
-      <c r="L418" s="32"/>
+      <c r="H418" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I418" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J418" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K418" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L418" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="419" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A419" s="21" t="s">
@@ -26681,11 +26691,21 @@
       <c r="G419" s="23" t="s">
         <v>643</v>
       </c>
-      <c r="H419" s="23"/>
-      <c r="I419" s="23"/>
-      <c r="J419" s="39"/>
-      <c r="K419" s="23"/>
-      <c r="L419" s="23"/>
+      <c r="H419" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I419" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J419" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K419" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L419" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="420" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A420" s="21" t="s">
@@ -26709,11 +26729,21 @@
       <c r="G420" s="23" t="s">
         <v>644</v>
       </c>
-      <c r="H420" s="23"/>
-      <c r="I420" s="23"/>
-      <c r="J420" s="39"/>
-      <c r="K420" s="23"/>
-      <c r="L420" s="23"/>
+      <c r="H420" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I420" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J420" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K420" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L420" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="421" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A421" s="21" t="s">
@@ -26737,11 +26767,21 @@
       <c r="G421" s="27" t="s">
         <v>645</v>
       </c>
-      <c r="H421" s="27"/>
-      <c r="I421" s="27"/>
-      <c r="J421" s="40"/>
-      <c r="K421" s="27"/>
-      <c r="L421" s="27"/>
+      <c r="H421" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I421" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J421" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K421" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L421" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="422" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A422" s="21" t="s">
@@ -26765,11 +26805,21 @@
       <c r="G422" s="32" t="s">
         <v>646</v>
       </c>
-      <c r="H422" s="32"/>
-      <c r="I422" s="32"/>
-      <c r="J422" s="38"/>
-      <c r="K422" s="32"/>
-      <c r="L422" s="32"/>
+      <c r="H422" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I422" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J422" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K422" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L422" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="423" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A423" s="21" t="s">
@@ -26793,11 +26843,21 @@
       <c r="G423" s="23" t="s">
         <v>615</v>
       </c>
-      <c r="H423" s="23"/>
-      <c r="I423" s="23"/>
-      <c r="J423" s="39"/>
-      <c r="K423" s="23"/>
-      <c r="L423" s="23"/>
+      <c r="H423" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I423" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J423" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K423" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L423" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="424" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A424" s="21" t="s">
@@ -26821,11 +26881,21 @@
       <c r="G424" s="23" t="s">
         <v>616</v>
       </c>
-      <c r="H424" s="23"/>
-      <c r="I424" s="23"/>
-      <c r="J424" s="39"/>
-      <c r="K424" s="23"/>
-      <c r="L424" s="23"/>
+      <c r="H424" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I424" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J424" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K424" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L424" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="425" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A425" s="21" t="s">
@@ -26849,11 +26919,21 @@
       <c r="G425" s="27" t="s">
         <v>617</v>
       </c>
-      <c r="H425" s="27"/>
-      <c r="I425" s="27"/>
-      <c r="J425" s="40"/>
-      <c r="K425" s="27"/>
-      <c r="L425" s="27"/>
+      <c r="H425" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I425" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J425" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K425" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L425" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="426" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A426" s="21" t="s">
@@ -26877,11 +26957,21 @@
       <c r="G426" s="32" t="s">
         <v>618</v>
       </c>
-      <c r="H426" s="32"/>
-      <c r="I426" s="32"/>
-      <c r="J426" s="38"/>
-      <c r="K426" s="32"/>
-      <c r="L426" s="32"/>
+      <c r="H426" s="32">
+        <v>14</v>
+      </c>
+      <c r="I426" s="32">
+        <v>4224</v>
+      </c>
+      <c r="J426" s="38">
+        <v>2142.79</v>
+      </c>
+      <c r="K426" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L426" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="427" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A427" s="21" t="s">
@@ -26905,11 +26995,21 @@
       <c r="G427" s="23" t="s">
         <v>619</v>
       </c>
-      <c r="H427" s="23"/>
-      <c r="I427" s="23"/>
-      <c r="J427" s="39"/>
-      <c r="K427" s="23"/>
-      <c r="L427" s="23"/>
+      <c r="H427" s="23">
+        <v>15</v>
+      </c>
+      <c r="I427" s="23">
+        <v>5042</v>
+      </c>
+      <c r="J427" s="39">
+        <v>2791.05</v>
+      </c>
+      <c r="K427" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L427" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="428" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A428" s="21" t="s">
@@ -26933,11 +27033,21 @@
       <c r="G428" s="23" t="s">
         <v>620</v>
       </c>
-      <c r="H428" s="23"/>
-      <c r="I428" s="23"/>
-      <c r="J428" s="39"/>
-      <c r="K428" s="23"/>
-      <c r="L428" s="23"/>
+      <c r="H428" s="23">
+        <v>15</v>
+      </c>
+      <c r="I428" s="23">
+        <v>4634</v>
+      </c>
+      <c r="J428" s="39">
+        <v>2418.66</v>
+      </c>
+      <c r="K428" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L428" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="429" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A429" s="21" t="s">
@@ -26961,11 +27071,21 @@
       <c r="G429" s="27" t="s">
         <v>621</v>
       </c>
-      <c r="H429" s="27"/>
-      <c r="I429" s="27"/>
-      <c r="J429" s="40"/>
-      <c r="K429" s="27"/>
-      <c r="L429" s="27"/>
+      <c r="H429" s="27">
+        <v>15</v>
+      </c>
+      <c r="I429" s="27">
+        <v>4496</v>
+      </c>
+      <c r="J429" s="40">
+        <v>2350.69</v>
+      </c>
+      <c r="K429" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L429" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="430" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A430" s="21" t="s">
@@ -26989,11 +27109,21 @@
       <c r="G430" s="32" t="s">
         <v>622</v>
       </c>
-      <c r="H430" s="32"/>
-      <c r="I430" s="32"/>
-      <c r="J430" s="38"/>
-      <c r="K430" s="32"/>
-      <c r="L430" s="32"/>
+      <c r="H430" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I430" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J430" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K430" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L430" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="431" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A431" s="21" t="s">
@@ -27017,11 +27147,21 @@
       <c r="G431" s="23" t="s">
         <v>623</v>
       </c>
-      <c r="H431" s="23"/>
-      <c r="I431" s="23"/>
-      <c r="J431" s="39"/>
-      <c r="K431" s="23"/>
-      <c r="L431" s="23"/>
+      <c r="H431" s="24">
+        <v>13</v>
+      </c>
+      <c r="I431" s="24">
+        <v>4264</v>
+      </c>
+      <c r="J431" s="39">
+        <v>2181.91</v>
+      </c>
+      <c r="K431" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L431" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="432" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A432" s="21" t="s">
@@ -27045,11 +27185,21 @@
       <c r="G432" s="23" t="s">
         <v>624</v>
       </c>
-      <c r="H432" s="23"/>
-      <c r="I432" s="23"/>
-      <c r="J432" s="39"/>
-      <c r="K432" s="23"/>
-      <c r="L432" s="23"/>
+      <c r="H432" s="24">
+        <v>13</v>
+      </c>
+      <c r="I432" s="24">
+        <v>4214</v>
+      </c>
+      <c r="J432" s="39">
+        <v>2169.1</v>
+      </c>
+      <c r="K432" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L432" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="433" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A433" s="21" t="s">
@@ -27073,11 +27223,21 @@
       <c r="G433" s="27" t="s">
         <v>625</v>
       </c>
-      <c r="H433" s="27"/>
-      <c r="I433" s="27"/>
-      <c r="J433" s="40"/>
-      <c r="K433" s="27"/>
-      <c r="L433" s="27"/>
+      <c r="H433" s="27">
+        <v>13</v>
+      </c>
+      <c r="I433" s="27">
+        <v>4420</v>
+      </c>
+      <c r="J433" s="40">
+        <v>2293.14</v>
+      </c>
+      <c r="K433" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L433" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="434" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A434" s="21" t="s">
@@ -27101,11 +27261,21 @@
       <c r="G434" s="32" t="s">
         <v>626</v>
       </c>
-      <c r="H434" s="32"/>
-      <c r="I434" s="32"/>
-      <c r="J434" s="38"/>
-      <c r="K434" s="32"/>
-      <c r="L434" s="32"/>
+      <c r="H434" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I434" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J434" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K434" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L434" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="435" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A435" s="21" t="s">
@@ -27129,11 +27299,21 @@
       <c r="G435" s="23" t="s">
         <v>627</v>
       </c>
-      <c r="H435" s="23"/>
-      <c r="I435" s="23"/>
-      <c r="J435" s="39"/>
-      <c r="K435" s="23"/>
-      <c r="L435" s="23"/>
+      <c r="H435" s="24">
+        <v>10</v>
+      </c>
+      <c r="I435" s="24">
+        <v>4168</v>
+      </c>
+      <c r="J435" s="39">
+        <v>2096.67</v>
+      </c>
+      <c r="K435" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L435" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="436" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A436" s="21" t="s">
@@ -27157,11 +27337,21 @@
       <c r="G436" s="23" t="s">
         <v>628</v>
       </c>
-      <c r="H436" s="23"/>
-      <c r="I436" s="23"/>
-      <c r="J436" s="39"/>
-      <c r="K436" s="23"/>
-      <c r="L436" s="23"/>
+      <c r="H436" s="24">
+        <v>11</v>
+      </c>
+      <c r="I436" s="24">
+        <v>4383</v>
+      </c>
+      <c r="J436" s="39">
+        <v>2307.62</v>
+      </c>
+      <c r="K436" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L436" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="437" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A437" s="21" t="s">
@@ -27185,11 +27375,21 @@
       <c r="G437" s="27" t="s">
         <v>629</v>
       </c>
-      <c r="H437" s="27"/>
-      <c r="I437" s="27"/>
-      <c r="J437" s="40"/>
-      <c r="K437" s="27"/>
-      <c r="L437" s="27"/>
+      <c r="H437" s="27">
+        <v>10</v>
+      </c>
+      <c r="I437" s="27">
+        <v>4278</v>
+      </c>
+      <c r="J437" s="40">
+        <v>2166.5500000000002</v>
+      </c>
+      <c r="K437" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L437" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="438" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A438" s="21" t="s">
@@ -27213,11 +27413,21 @@
       <c r="G438" s="32" t="s">
         <v>630</v>
       </c>
-      <c r="H438" s="32"/>
-      <c r="I438" s="32"/>
-      <c r="J438" s="38"/>
-      <c r="K438" s="32"/>
-      <c r="L438" s="32"/>
+      <c r="H438" s="32">
+        <v>7</v>
+      </c>
+      <c r="I438" s="32">
+        <v>3800</v>
+      </c>
+      <c r="J438" s="38">
+        <v>1815.98</v>
+      </c>
+      <c r="K438" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L438" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="439" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A439" s="21" t="s">
@@ -27241,11 +27451,21 @@
       <c r="G439" s="23" t="s">
         <v>631</v>
       </c>
-      <c r="H439" s="23"/>
-      <c r="I439" s="23"/>
-      <c r="J439" s="39"/>
-      <c r="K439" s="23"/>
-      <c r="L439" s="23"/>
+      <c r="H439" s="24">
+        <v>8</v>
+      </c>
+      <c r="I439" s="24">
+        <v>4006</v>
+      </c>
+      <c r="J439" s="39">
+        <v>1991.47</v>
+      </c>
+      <c r="K439" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L439" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="440" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A440" s="21" t="s">
@@ -27269,11 +27489,21 @@
       <c r="G440" s="23" t="s">
         <v>632</v>
       </c>
-      <c r="H440" s="23"/>
-      <c r="I440" s="23"/>
-      <c r="J440" s="39"/>
-      <c r="K440" s="23"/>
-      <c r="L440" s="23"/>
+      <c r="H440" s="24">
+        <v>8</v>
+      </c>
+      <c r="I440" s="24">
+        <v>3873</v>
+      </c>
+      <c r="J440" s="39">
+        <v>1860.47</v>
+      </c>
+      <c r="K440" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L440" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="441" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A441" s="21" t="s">
@@ -27297,11 +27527,21 @@
       <c r="G441" s="27" t="s">
         <v>633</v>
       </c>
-      <c r="H441" s="27"/>
-      <c r="I441" s="27"/>
-      <c r="J441" s="40"/>
-      <c r="K441" s="27"/>
-      <c r="L441" s="27"/>
+      <c r="H441" s="27">
+        <v>8</v>
+      </c>
+      <c r="I441" s="27">
+        <v>3760</v>
+      </c>
+      <c r="J441" s="40">
+        <v>1816.56</v>
+      </c>
+      <c r="K441" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L441" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="442" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A442" s="21" t="s">
@@ -27325,11 +27565,21 @@
       <c r="G442" s="32" t="s">
         <v>634</v>
       </c>
-      <c r="H442" s="32"/>
-      <c r="I442" s="32"/>
-      <c r="J442" s="38"/>
-      <c r="K442" s="32"/>
-      <c r="L442" s="32"/>
+      <c r="H442" s="32">
+        <v>9</v>
+      </c>
+      <c r="I442" s="32">
+        <v>4172</v>
+      </c>
+      <c r="J442" s="38">
+        <v>2044.94</v>
+      </c>
+      <c r="K442" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L442" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="443" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A443" s="21" t="s">
@@ -27353,11 +27603,21 @@
       <c r="G443" s="23" t="s">
         <v>635</v>
       </c>
-      <c r="H443" s="23"/>
-      <c r="I443" s="23"/>
-      <c r="J443" s="39"/>
-      <c r="K443" s="23"/>
-      <c r="L443" s="23"/>
+      <c r="H443" s="24">
+        <v>10</v>
+      </c>
+      <c r="I443" s="24">
+        <v>4320</v>
+      </c>
+      <c r="J443" s="39">
+        <v>2235.61</v>
+      </c>
+      <c r="K443" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L443" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="444" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A444" s="21" t="s">
@@ -27381,11 +27641,21 @@
       <c r="G444" s="23" t="s">
         <v>636</v>
       </c>
-      <c r="H444" s="23"/>
-      <c r="I444" s="23"/>
-      <c r="J444" s="39"/>
-      <c r="K444" s="23"/>
-      <c r="L444" s="23"/>
+      <c r="H444" s="24">
+        <v>11</v>
+      </c>
+      <c r="I444" s="24">
+        <v>4563</v>
+      </c>
+      <c r="J444" s="39">
+        <v>2373.1999999999998</v>
+      </c>
+      <c r="K444" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L444" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="445" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A445" s="21" t="s">
@@ -27409,11 +27679,21 @@
       <c r="G445" s="27" t="s">
         <v>637</v>
       </c>
-      <c r="H445" s="27"/>
-      <c r="I445" s="27"/>
-      <c r="J445" s="40"/>
-      <c r="K445" s="27"/>
-      <c r="L445" s="27"/>
+      <c r="H445" s="27">
+        <v>10</v>
+      </c>
+      <c r="I445" s="27">
+        <v>4127</v>
+      </c>
+      <c r="J445" s="40">
+        <v>2091.7800000000002</v>
+      </c>
+      <c r="K445" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L445" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="446" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A446" s="21" t="s">
@@ -27437,11 +27717,21 @@
       <c r="G446" s="32" t="s">
         <v>638</v>
       </c>
-      <c r="H446" s="32"/>
-      <c r="I446" s="32"/>
-      <c r="J446" s="38"/>
-      <c r="K446" s="32"/>
-      <c r="L446" s="32"/>
+      <c r="H446" s="32">
+        <v>7</v>
+      </c>
+      <c r="I446" s="32">
+        <v>3709</v>
+      </c>
+      <c r="J446" s="38">
+        <v>1758.34</v>
+      </c>
+      <c r="K446" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L446" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="447" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A447" s="21" t="s">
@@ -27465,11 +27755,21 @@
       <c r="G447" s="23" t="s">
         <v>639</v>
       </c>
-      <c r="H447" s="23"/>
-      <c r="I447" s="23"/>
-      <c r="J447" s="39"/>
-      <c r="K447" s="23"/>
-      <c r="L447" s="23"/>
+      <c r="H447" s="24">
+        <v>8</v>
+      </c>
+      <c r="I447" s="24">
+        <v>4142</v>
+      </c>
+      <c r="J447" s="39">
+        <v>2094.38</v>
+      </c>
+      <c r="K447" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L447" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="448" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A448" s="21" t="s">
@@ -27493,11 +27793,21 @@
       <c r="G448" s="23" t="s">
         <v>640</v>
       </c>
-      <c r="H448" s="23"/>
-      <c r="I448" s="23"/>
-      <c r="J448" s="39"/>
-      <c r="K448" s="23"/>
-      <c r="L448" s="23"/>
+      <c r="H448" s="24">
+        <v>8</v>
+      </c>
+      <c r="I448" s="24">
+        <v>3865</v>
+      </c>
+      <c r="J448" s="39">
+        <v>1843.47</v>
+      </c>
+      <c r="K448" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L448" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="449" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A449" s="21" t="s">
@@ -27521,11 +27831,21 @@
       <c r="G449" s="27" t="s">
         <v>641</v>
       </c>
-      <c r="H449" s="27"/>
-      <c r="I449" s="27"/>
-      <c r="J449" s="40"/>
-      <c r="K449" s="27"/>
-      <c r="L449" s="27"/>
+      <c r="H449" s="27">
+        <v>7</v>
+      </c>
+      <c r="I449" s="27">
+        <v>3675</v>
+      </c>
+      <c r="J449" s="40">
+        <v>1748.65</v>
+      </c>
+      <c r="K449" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L449" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="450" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A450" s="21" t="s">

</xml_diff>

<commit_message>
starter region 8 results
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5140" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5228" uniqueCount="690">
   <si>
     <t>shift</t>
   </si>
@@ -4684,7 +4684,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
+      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10500,8 +10500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C415" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H450" sqref="H450"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27869,11 +27869,21 @@
       <c r="G450" s="32" t="s">
         <v>683</v>
       </c>
-      <c r="H450" s="32"/>
-      <c r="I450" s="32"/>
-      <c r="J450" s="38"/>
-      <c r="K450" s="32"/>
-      <c r="L450" s="32"/>
+      <c r="H450" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I450" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J450" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K450" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L450" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="451" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A451" s="21" t="s">
@@ -27897,11 +27907,21 @@
       <c r="G451" s="23" t="s">
         <v>684</v>
       </c>
-      <c r="H451" s="23"/>
-      <c r="I451" s="23"/>
-      <c r="J451" s="39"/>
-      <c r="K451" s="23"/>
-      <c r="L451" s="23"/>
+      <c r="H451" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I451" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J451" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K451" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L451" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="452" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A452" s="21" t="s">
@@ -27925,11 +27945,21 @@
       <c r="G452" s="23" t="s">
         <v>685</v>
       </c>
-      <c r="H452" s="23"/>
-      <c r="I452" s="23"/>
-      <c r="J452" s="39"/>
-      <c r="K452" s="23"/>
-      <c r="L452" s="23"/>
+      <c r="H452" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I452" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J452" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K452" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L452" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="453" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A453" s="21" t="s">
@@ -27953,11 +27983,21 @@
       <c r="G453" s="27" t="s">
         <v>686</v>
       </c>
-      <c r="H453" s="27"/>
-      <c r="I453" s="27"/>
-      <c r="J453" s="40"/>
-      <c r="K453" s="27"/>
-      <c r="L453" s="27"/>
+      <c r="H453" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I453" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J453" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K453" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L453" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="454" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A454" s="21" t="s">
@@ -27981,11 +28021,21 @@
       <c r="G454" s="32" t="s">
         <v>687</v>
       </c>
-      <c r="H454" s="32"/>
-      <c r="I454" s="32"/>
-      <c r="J454" s="38"/>
-      <c r="K454" s="32"/>
-      <c r="L454" s="32"/>
+      <c r="H454" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I454" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J454" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K454" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L454" s="32" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="455" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A455" s="21" t="s">
@@ -28009,11 +28059,21 @@
       <c r="G455" s="23" t="s">
         <v>688</v>
       </c>
-      <c r="H455" s="23"/>
-      <c r="I455" s="23"/>
-      <c r="J455" s="39"/>
-      <c r="K455" s="23"/>
-      <c r="L455" s="23"/>
+      <c r="H455" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I455" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J455" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K455" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L455" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="456" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A456" s="21" t="s">
@@ -28037,11 +28097,21 @@
       <c r="G456" s="23" t="s">
         <v>647</v>
       </c>
-      <c r="H456" s="23"/>
-      <c r="I456" s="23"/>
-      <c r="J456" s="39"/>
-      <c r="K456" s="23"/>
-      <c r="L456" s="23"/>
+      <c r="H456" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I456" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J456" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K456" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L456" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="457" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A457" s="21" t="s">
@@ -28065,11 +28135,21 @@
       <c r="G457" s="27" t="s">
         <v>648</v>
       </c>
-      <c r="H457" s="27"/>
-      <c r="I457" s="27"/>
-      <c r="J457" s="40"/>
-      <c r="K457" s="27"/>
-      <c r="L457" s="27"/>
+      <c r="H457" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I457" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J457" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K457" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L457" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="458" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A458" s="21" t="s">
@@ -28093,11 +28173,21 @@
       <c r="G458" s="32" t="s">
         <v>649</v>
       </c>
-      <c r="H458" s="32"/>
-      <c r="I458" s="32"/>
-      <c r="J458" s="38"/>
-      <c r="K458" s="32"/>
-      <c r="L458" s="32"/>
+      <c r="H458" s="32">
+        <v>12</v>
+      </c>
+      <c r="I458" s="32">
+        <v>3073</v>
+      </c>
+      <c r="J458" s="38">
+        <v>1599.48</v>
+      </c>
+      <c r="K458" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L458" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="459" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A459" s="21" t="s">
@@ -28121,11 +28211,21 @@
       <c r="G459" s="23" t="s">
         <v>650</v>
       </c>
-      <c r="H459" s="23"/>
-      <c r="I459" s="23"/>
-      <c r="J459" s="39"/>
-      <c r="K459" s="23"/>
-      <c r="L459" s="23"/>
+      <c r="H459" s="23">
+        <v>13</v>
+      </c>
+      <c r="I459" s="23">
+        <v>2691</v>
+      </c>
+      <c r="J459" s="39">
+        <v>1275.74</v>
+      </c>
+      <c r="K459" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L459" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="460" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A460" s="21" t="s">
@@ -28149,11 +28249,21 @@
       <c r="G460" s="23" t="s">
         <v>651</v>
       </c>
-      <c r="H460" s="23"/>
-      <c r="I460" s="23"/>
-      <c r="J460" s="39"/>
-      <c r="K460" s="23"/>
-      <c r="L460" s="23"/>
+      <c r="H460" s="23">
+        <v>12</v>
+      </c>
+      <c r="I460" s="23">
+        <v>3020</v>
+      </c>
+      <c r="J460" s="39">
+        <v>1495.68</v>
+      </c>
+      <c r="K460" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L460" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="461" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A461" s="21" t="s">
@@ -28177,11 +28287,21 @@
       <c r="G461" s="27" t="s">
         <v>652</v>
       </c>
-      <c r="H461" s="27"/>
-      <c r="I461" s="27"/>
-      <c r="J461" s="40"/>
-      <c r="K461" s="27"/>
-      <c r="L461" s="27"/>
+      <c r="H461" s="27">
+        <v>12</v>
+      </c>
+      <c r="I461" s="27">
+        <v>2965</v>
+      </c>
+      <c r="J461" s="40">
+        <v>1454.82</v>
+      </c>
+      <c r="K461" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L461" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="462" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A462" s="21" t="s">
@@ -28205,11 +28325,21 @@
       <c r="G462" s="32" t="s">
         <v>653</v>
       </c>
-      <c r="H462" s="32"/>
-      <c r="I462" s="32"/>
-      <c r="J462" s="38"/>
-      <c r="K462" s="32"/>
-      <c r="L462" s="32"/>
+      <c r="H462" s="32">
+        <v>12</v>
+      </c>
+      <c r="I462" s="32">
+        <v>3073</v>
+      </c>
+      <c r="J462" s="38">
+        <v>1599.48</v>
+      </c>
+      <c r="K462" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L462" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="463" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A463" s="21" t="s">
@@ -28233,11 +28363,21 @@
       <c r="G463" s="23" t="s">
         <v>654</v>
       </c>
-      <c r="H463" s="23"/>
-      <c r="I463" s="23"/>
-      <c r="J463" s="39"/>
-      <c r="K463" s="23"/>
-      <c r="L463" s="23"/>
+      <c r="H463" s="24">
+        <v>13</v>
+      </c>
+      <c r="I463" s="24">
+        <v>2691</v>
+      </c>
+      <c r="J463" s="39">
+        <v>1275.71</v>
+      </c>
+      <c r="K463" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L463" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="464" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A464" s="21" t="s">
@@ -28261,11 +28401,21 @@
       <c r="G464" s="23" t="s">
         <v>655</v>
       </c>
-      <c r="H464" s="23"/>
-      <c r="I464" s="23"/>
-      <c r="J464" s="39"/>
-      <c r="K464" s="23"/>
-      <c r="L464" s="23"/>
+      <c r="H464" s="24">
+        <v>12</v>
+      </c>
+      <c r="I464" s="24">
+        <v>3116</v>
+      </c>
+      <c r="J464" s="39">
+        <v>1585.86</v>
+      </c>
+      <c r="K464" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L464" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="465" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A465" s="21" t="s">
@@ -28289,11 +28439,21 @@
       <c r="G465" s="27" t="s">
         <v>656</v>
       </c>
-      <c r="H465" s="27"/>
-      <c r="I465" s="27"/>
-      <c r="J465" s="40"/>
-      <c r="K465" s="27"/>
-      <c r="L465" s="27"/>
+      <c r="H465" s="27">
+        <v>12</v>
+      </c>
+      <c r="I465" s="27">
+        <v>2965</v>
+      </c>
+      <c r="J465" s="40">
+        <v>1454.82</v>
+      </c>
+      <c r="K465" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L465" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="466" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A466" s="21" t="s">
@@ -28317,11 +28477,21 @@
       <c r="G466" s="32" t="s">
         <v>657</v>
       </c>
-      <c r="H466" s="32"/>
-      <c r="I466" s="32"/>
-      <c r="J466" s="38"/>
-      <c r="K466" s="32"/>
-      <c r="L466" s="32"/>
+      <c r="H466" s="32">
+        <v>5</v>
+      </c>
+      <c r="I466" s="32">
+        <v>2277</v>
+      </c>
+      <c r="J466" s="38">
+        <v>821.07</v>
+      </c>
+      <c r="K466" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L466" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="467" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A467" s="21" t="s">
@@ -28345,11 +28515,21 @@
       <c r="G467" s="23" t="s">
         <v>658</v>
       </c>
-      <c r="H467" s="23"/>
-      <c r="I467" s="23"/>
-      <c r="J467" s="39"/>
-      <c r="K467" s="23"/>
-      <c r="L467" s="23"/>
+      <c r="H467" s="24">
+        <v>5</v>
+      </c>
+      <c r="I467" s="24">
+        <v>2245</v>
+      </c>
+      <c r="J467" s="39">
+        <v>790.34</v>
+      </c>
+      <c r="K467" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L467" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="468" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A468" s="21" t="s">
@@ -28373,11 +28553,21 @@
       <c r="G468" s="23" t="s">
         <v>659</v>
       </c>
-      <c r="H468" s="23"/>
-      <c r="I468" s="23"/>
-      <c r="J468" s="39"/>
-      <c r="K468" s="23"/>
-      <c r="L468" s="23"/>
+      <c r="H468" s="24">
+        <v>6</v>
+      </c>
+      <c r="I468" s="24">
+        <v>2394</v>
+      </c>
+      <c r="J468" s="39">
+        <v>889.45</v>
+      </c>
+      <c r="K468" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L468" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="469" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A469" s="21" t="s">
@@ -28401,11 +28591,21 @@
       <c r="G469" s="27" t="s">
         <v>660</v>
       </c>
-      <c r="H469" s="27"/>
-      <c r="I469" s="27"/>
-      <c r="J469" s="40"/>
-      <c r="K469" s="27"/>
-      <c r="L469" s="27"/>
+      <c r="H469" s="27">
+        <v>6</v>
+      </c>
+      <c r="I469" s="27">
+        <v>2456</v>
+      </c>
+      <c r="J469" s="40">
+        <v>985.54</v>
+      </c>
+      <c r="K469" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L469" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="470" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A470" s="21" t="s">
@@ -28429,11 +28629,21 @@
       <c r="G470" s="32" t="s">
         <v>661</v>
       </c>
-      <c r="H470" s="32"/>
-      <c r="I470" s="32"/>
-      <c r="J470" s="38"/>
-      <c r="K470" s="32"/>
-      <c r="L470" s="32"/>
+      <c r="H470" s="32">
+        <v>4</v>
+      </c>
+      <c r="I470" s="32">
+        <v>2190</v>
+      </c>
+      <c r="J470" s="38">
+        <v>774.24</v>
+      </c>
+      <c r="K470" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L470" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="471" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A471" s="21" t="s">
@@ -28457,11 +28667,21 @@
       <c r="G471" s="23" t="s">
         <v>662</v>
       </c>
-      <c r="H471" s="23"/>
-      <c r="I471" s="23"/>
-      <c r="J471" s="39"/>
-      <c r="K471" s="23"/>
-      <c r="L471" s="23"/>
+      <c r="H471" s="24">
+        <v>5</v>
+      </c>
+      <c r="I471" s="24">
+        <v>2447</v>
+      </c>
+      <c r="J471" s="39">
+        <v>949.89</v>
+      </c>
+      <c r="K471" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L471" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="472" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A472" s="21" t="s">
@@ -28485,11 +28705,21 @@
       <c r="G472" s="23" t="s">
         <v>663</v>
       </c>
-      <c r="H472" s="23"/>
-      <c r="I472" s="23"/>
-      <c r="J472" s="39"/>
-      <c r="K472" s="23"/>
-      <c r="L472" s="23"/>
+      <c r="H472" s="24">
+        <v>5</v>
+      </c>
+      <c r="I472" s="24">
+        <v>2258</v>
+      </c>
+      <c r="J472" s="39">
+        <v>840.19</v>
+      </c>
+      <c r="K472" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L472" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="473" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A473" s="21" t="s">
@@ -28513,11 +28743,21 @@
       <c r="G473" s="27" t="s">
         <v>664</v>
       </c>
-      <c r="H473" s="27"/>
-      <c r="I473" s="27"/>
-      <c r="J473" s="40"/>
-      <c r="K473" s="27"/>
-      <c r="L473" s="27"/>
+      <c r="H473" s="27">
+        <v>4</v>
+      </c>
+      <c r="I473" s="27">
+        <v>2132</v>
+      </c>
+      <c r="J473" s="40">
+        <v>721.2</v>
+      </c>
+      <c r="K473" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L473" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="474" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A474" s="21" t="s">
@@ -28541,11 +28781,21 @@
       <c r="G474" s="32" t="s">
         <v>665</v>
       </c>
-      <c r="H474" s="32"/>
-      <c r="I474" s="32"/>
-      <c r="J474" s="38"/>
-      <c r="K474" s="32"/>
-      <c r="L474" s="32"/>
+      <c r="H474" s="32">
+        <v>5</v>
+      </c>
+      <c r="I474" s="32">
+        <v>2296</v>
+      </c>
+      <c r="J474" s="38">
+        <v>832.52</v>
+      </c>
+      <c r="K474" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L474" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="475" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A475" s="21" t="s">
@@ -28569,11 +28819,21 @@
       <c r="G475" s="23" t="s">
         <v>666</v>
       </c>
-      <c r="H475" s="23"/>
-      <c r="I475" s="23"/>
-      <c r="J475" s="39"/>
-      <c r="K475" s="23"/>
-      <c r="L475" s="23"/>
+      <c r="H475" s="24">
+        <v>5</v>
+      </c>
+      <c r="I475" s="24">
+        <v>2228</v>
+      </c>
+      <c r="J475" s="36">
+        <v>783.03</v>
+      </c>
+      <c r="K475" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L475" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="476" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A476" s="21" t="s">
@@ -28597,11 +28857,21 @@
       <c r="G476" s="23" t="s">
         <v>667</v>
       </c>
-      <c r="H476" s="23"/>
-      <c r="I476" s="23"/>
-      <c r="J476" s="39"/>
-      <c r="K476" s="23"/>
-      <c r="L476" s="23"/>
+      <c r="H476" s="24">
+        <v>6</v>
+      </c>
+      <c r="I476" s="24">
+        <v>2259</v>
+      </c>
+      <c r="J476" s="39">
+        <v>854.93</v>
+      </c>
+      <c r="K476" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L476" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="477" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A477" s="21" t="s">
@@ -28625,11 +28895,21 @@
       <c r="G477" s="27" t="s">
         <v>668</v>
       </c>
-      <c r="H477" s="27"/>
-      <c r="I477" s="27"/>
-      <c r="J477" s="40"/>
-      <c r="K477" s="27"/>
-      <c r="L477" s="27"/>
+      <c r="H477" s="27">
+        <v>6</v>
+      </c>
+      <c r="I477" s="27">
+        <v>2402</v>
+      </c>
+      <c r="J477" s="40">
+        <v>935.61</v>
+      </c>
+      <c r="K477" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L477" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="478" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A478" s="21" t="s">
@@ -28653,11 +28933,21 @@
       <c r="G478" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="H478" s="32"/>
-      <c r="I478" s="32"/>
-      <c r="J478" s="38"/>
-      <c r="K478" s="32"/>
-      <c r="L478" s="32"/>
+      <c r="H478" s="32">
+        <v>4</v>
+      </c>
+      <c r="I478" s="32">
+        <v>2175</v>
+      </c>
+      <c r="J478" s="38">
+        <v>759.52</v>
+      </c>
+      <c r="K478" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="L478" s="32" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="479" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A479" s="21" t="s">
@@ -28681,11 +28971,21 @@
       <c r="G479" s="23" t="s">
         <v>670</v>
       </c>
-      <c r="H479" s="23"/>
-      <c r="I479" s="23"/>
-      <c r="J479" s="39"/>
-      <c r="K479" s="23"/>
-      <c r="L479" s="23"/>
+      <c r="H479" s="24">
+        <v>4</v>
+      </c>
+      <c r="I479" s="24">
+        <v>2249</v>
+      </c>
+      <c r="J479" s="39">
+        <v>822.85</v>
+      </c>
+      <c r="K479" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L479" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="480" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A480" s="21" t="s">
@@ -28709,11 +29009,21 @@
       <c r="G480" s="23" t="s">
         <v>671</v>
       </c>
-      <c r="H480" s="23"/>
-      <c r="I480" s="23"/>
-      <c r="J480" s="39"/>
-      <c r="K480" s="23"/>
-      <c r="L480" s="23"/>
+      <c r="H480" s="24">
+        <v>4</v>
+      </c>
+      <c r="I480" s="24">
+        <v>2259</v>
+      </c>
+      <c r="J480" s="39">
+        <v>799.63</v>
+      </c>
+      <c r="K480" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="L480" s="24" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="481" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A481" s="21" t="s">
@@ -28737,11 +29047,21 @@
       <c r="G481" s="27" t="s">
         <v>672</v>
       </c>
-      <c r="H481" s="27"/>
-      <c r="I481" s="27"/>
-      <c r="J481" s="40"/>
-      <c r="K481" s="27"/>
-      <c r="L481" s="27"/>
+      <c r="H481" s="27">
+        <v>4</v>
+      </c>
+      <c r="I481" s="27">
+        <v>2189</v>
+      </c>
+      <c r="J481" s="40">
+        <v>761.56</v>
+      </c>
+      <c r="K481" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="L481" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B33">

</xml_diff>

<commit_message>
updated results for idl5 & str6 - recreated solution text files
</commit_message>
<xml_diff>
--- a/vrp_results_tracker.xlsx
+++ b/vrp_results_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21037EE-275E-44A9-84EA-5138C970A531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11539E0-B282-4FB7-B901-C84BE056111D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="870" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2124,18 +2124,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -2254,7 +2248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2298,18 +2292,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6904,50 +6892,50 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="I1" s="41" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="I1" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41" t="s">
+      <c r="E2" s="42"/>
+      <c r="F2" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="J2" s="41" t="s">
+      <c r="G2" s="42"/>
+      <c r="J2" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41" t="s">
+      <c r="K2" s="42"/>
+      <c r="L2" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41" t="s">
+      <c r="M2" s="42"/>
+      <c r="N2" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="41"/>
+      <c r="O2" s="42"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -7179,50 +7167,50 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="I8" s="41" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="I8" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41" t="s">
+      <c r="C9" s="42"/>
+      <c r="D9" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41" t="s">
+      <c r="E9" s="42"/>
+      <c r="F9" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="41"/>
-      <c r="J9" s="41" t="s">
+      <c r="G9" s="42"/>
+      <c r="J9" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41" t="s">
+      <c r="K9" s="42"/>
+      <c r="L9" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41" t="s">
+      <c r="M9" s="42"/>
+      <c r="N9" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="O9" s="41"/>
+      <c r="O9" s="42"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
@@ -7454,50 +7442,50 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="I15" s="41" t="s">
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="I15" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41" t="s">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41" t="s">
+      <c r="E16" s="42"/>
+      <c r="F16" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="41"/>
-      <c r="J16" s="41" t="s">
+      <c r="G16" s="42"/>
+      <c r="J16" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41" t="s">
+      <c r="K16" s="42"/>
+      <c r="L16" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41" t="s">
+      <c r="M16" s="42"/>
+      <c r="N16" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="O16" s="41"/>
+      <c r="O16" s="42"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
@@ -7729,50 +7717,50 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="I22" s="41" t="s">
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="I22" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41" t="s">
+      <c r="C23" s="42"/>
+      <c r="D23" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41" t="s">
+      <c r="E23" s="42"/>
+      <c r="F23" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="41"/>
-      <c r="J23" s="41" t="s">
+      <c r="G23" s="42"/>
+      <c r="J23" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41" t="s">
+      <c r="K23" s="42"/>
+      <c r="L23" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41" t="s">
+      <c r="M23" s="42"/>
+      <c r="N23" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="O23" s="41"/>
+      <c r="O23" s="42"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
@@ -8005,50 +7993,50 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="I29" s="41" t="s">
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="I29" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41" t="s">
+      <c r="C30" s="42"/>
+      <c r="D30" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41" t="s">
+      <c r="E30" s="42"/>
+      <c r="F30" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="G30" s="41"/>
-      <c r="J30" s="41" t="s">
+      <c r="G30" s="42"/>
+      <c r="J30" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41" t="s">
+      <c r="K30" s="42"/>
+      <c r="L30" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41" t="s">
+      <c r="M30" s="42"/>
+      <c r="N30" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="O30" s="41"/>
+      <c r="O30" s="42"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
@@ -8281,50 +8269,50 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="I36" s="41" t="s">
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="I36" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="J36" s="41"/>
-      <c r="K36" s="41"/>
-      <c r="L36" s="41"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="41"/>
-      <c r="O36" s="41"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="42"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="42"/>
+      <c r="O36" s="42"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41" t="s">
+      <c r="C37" s="42"/>
+      <c r="D37" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41" t="s">
+      <c r="E37" s="42"/>
+      <c r="F37" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="G37" s="41"/>
-      <c r="J37" s="41" t="s">
+      <c r="G37" s="42"/>
+      <c r="J37" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41" t="s">
+      <c r="K37" s="42"/>
+      <c r="L37" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="M37" s="41"/>
-      <c r="N37" s="41" t="s">
+      <c r="M37" s="42"/>
+      <c r="N37" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="O37" s="41"/>
+      <c r="O37" s="42"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
@@ -8557,50 +8545,50 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41"/>
-      <c r="I43" s="41" t="s">
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="I43" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="J43" s="41"/>
-      <c r="K43" s="41"/>
-      <c r="L43" s="41"/>
-      <c r="M43" s="41"/>
-      <c r="N43" s="41"/>
-      <c r="O43" s="41"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="42"/>
+      <c r="M43" s="42"/>
+      <c r="N43" s="42"/>
+      <c r="O43" s="42"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41" t="s">
+      <c r="C44" s="42"/>
+      <c r="D44" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41" t="s">
+      <c r="E44" s="42"/>
+      <c r="F44" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="G44" s="41"/>
-      <c r="J44" s="41" t="s">
+      <c r="G44" s="42"/>
+      <c r="J44" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="K44" s="41"/>
-      <c r="L44" s="41" t="s">
+      <c r="K44" s="42"/>
+      <c r="L44" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="M44" s="41"/>
-      <c r="N44" s="41" t="s">
+      <c r="M44" s="42"/>
+      <c r="N44" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="O44" s="41"/>
+      <c r="O44" s="42"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
@@ -8834,41 +8822,41 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A50" s="42"/>
-      <c r="B50" s="42"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="I50" s="41" t="s">
+      <c r="A50" s="41"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="I50" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="J50" s="41"/>
-      <c r="K50" s="41"/>
-      <c r="L50" s="41"/>
-      <c r="M50" s="41"/>
-      <c r="N50" s="41"/>
-      <c r="O50" s="41"/>
+      <c r="J50" s="42"/>
+      <c r="K50" s="42"/>
+      <c r="L50" s="42"/>
+      <c r="M50" s="42"/>
+      <c r="N50" s="42"/>
+      <c r="O50" s="42"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
-      <c r="J51" s="41" t="s">
+      <c r="B51" s="42"/>
+      <c r="C51" s="42"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="42"/>
+      <c r="J51" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="K51" s="41"/>
-      <c r="L51" s="41" t="s">
+      <c r="K51" s="42"/>
+      <c r="L51" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="M51" s="41"/>
-      <c r="N51" s="41" t="s">
+      <c r="M51" s="42"/>
+      <c r="N51" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="O51" s="41"/>
+      <c r="O51" s="42"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J52" t="s">
@@ -8999,6 +8987,62 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="I8:O8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="I15:O15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="I22:O22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="I29:O29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="I36:O36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="I43:O43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="N44:O44"/>
     <mergeCell ref="A50:F50"/>
     <mergeCell ref="I50:O50"/>
     <mergeCell ref="B51:C51"/>
@@ -9007,62 +9051,6 @@
     <mergeCell ref="J51:K51"/>
     <mergeCell ref="L51:M51"/>
     <mergeCell ref="N51:O51"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="I43:O43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="I36:O36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="I29:O29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="I22:O22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="I15:O15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="I8:O8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="L32:L35">
     <cfRule type="colorScale" priority="60">
@@ -10513,8 +10501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A481" sqref="A481"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154:B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15701,10 +15689,10 @@
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A130" s="45" t="s">
+      <c r="A130" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B130" s="46" t="s">
+      <c r="B130" s="33" t="s">
         <v>171</v>
       </c>
       <c r="C130" s="3" t="s">
@@ -15739,10 +15727,10 @@
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A131" s="43" t="s">
+      <c r="A131" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B131" s="44" t="s">
+      <c r="B131" s="13" t="s">
         <v>172</v>
       </c>
       <c r="C131" s="6" t="s">
@@ -15777,10 +15765,10 @@
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A132" s="43" t="s">
+      <c r="A132" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B132" s="44" t="s">
+      <c r="B132" s="13" t="s">
         <v>173</v>
       </c>
       <c r="C132" s="6" t="s">
@@ -15815,10 +15803,10 @@
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A133" s="47" t="s">
+      <c r="A133" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B133" s="48" t="s">
+      <c r="B133" s="15" t="s">
         <v>174</v>
       </c>
       <c r="C133" s="9" t="s">
@@ -15853,10 +15841,10 @@
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A134" s="45" t="s">
+      <c r="A134" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B134" s="46" t="s">
+      <c r="B134" s="33" t="s">
         <v>175</v>
       </c>
       <c r="C134" s="3" t="s">
@@ -15891,10 +15879,10 @@
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A135" s="43" t="s">
+      <c r="A135" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B135" s="44" t="s">
+      <c r="B135" s="13" t="s">
         <v>176</v>
       </c>
       <c r="C135" s="6" t="s">
@@ -15929,10 +15917,10 @@
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A136" s="43" t="s">
+      <c r="A136" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B136" s="44" t="s">
+      <c r="B136" s="13" t="s">
         <v>177</v>
       </c>
       <c r="C136" s="6" t="s">
@@ -15967,10 +15955,10 @@
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A137" s="47" t="s">
+      <c r="A137" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B137" s="48" t="s">
+      <c r="B137" s="15" t="s">
         <v>178</v>
       </c>
       <c r="C137" s="9" t="s">
@@ -16005,10 +15993,10 @@
       </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A138" s="45" t="s">
+      <c r="A138" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B138" s="46" t="s">
+      <c r="B138" s="33" t="s">
         <v>179</v>
       </c>
       <c r="C138" s="3" t="s">
@@ -16043,10 +16031,10 @@
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A139" s="43" t="s">
+      <c r="A139" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B139" s="44" t="s">
+      <c r="B139" s="13" t="s">
         <v>180</v>
       </c>
       <c r="C139" s="6" t="s">
@@ -16081,10 +16069,10 @@
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A140" s="43" t="s">
+      <c r="A140" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B140" s="44" t="s">
+      <c r="B140" s="13" t="s">
         <v>181</v>
       </c>
       <c r="C140" s="6" t="s">
@@ -16119,10 +16107,10 @@
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A141" s="47" t="s">
+      <c r="A141" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B141" s="48" t="s">
+      <c r="B141" s="15" t="s">
         <v>182</v>
       </c>
       <c r="C141" s="9" t="s">
@@ -16157,10 +16145,10 @@
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A142" s="45" t="s">
+      <c r="A142" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B142" s="46" t="s">
+      <c r="B142" s="33" t="s">
         <v>183</v>
       </c>
       <c r="C142" s="3" t="s">
@@ -16195,10 +16183,10 @@
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A143" s="43" t="s">
+      <c r="A143" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B143" s="44" t="s">
+      <c r="B143" s="13" t="s">
         <v>184</v>
       </c>
       <c r="C143" s="6" t="s">
@@ -16233,10 +16221,10 @@
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A144" s="43" t="s">
+      <c r="A144" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B144" s="44" t="s">
+      <c r="B144" s="13" t="s">
         <v>185</v>
       </c>
       <c r="C144" s="6" t="s">
@@ -16271,10 +16259,10 @@
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A145" s="47" t="s">
+      <c r="A145" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B145" s="48" t="s">
+      <c r="B145" s="15" t="s">
         <v>186</v>
       </c>
       <c r="C145" s="9" t="s">
@@ -16309,10 +16297,10 @@
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A146" s="45" t="s">
+      <c r="A146" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B146" s="46" t="s">
+      <c r="B146" s="33" t="s">
         <v>187</v>
       </c>
       <c r="C146" s="3" t="s">
@@ -16331,13 +16319,13 @@
         <v>345</v>
       </c>
       <c r="H146" s="32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I146" s="32">
-        <v>2471</v>
+        <v>2343</v>
       </c>
       <c r="J146" s="38">
-        <v>1087.55</v>
+        <v>984.22</v>
       </c>
       <c r="K146" s="32" t="s">
         <v>689</v>
@@ -16347,10 +16335,10 @@
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A147" s="43" t="s">
+      <c r="A147" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B147" s="44" t="s">
+      <c r="B147" s="13" t="s">
         <v>188</v>
       </c>
       <c r="C147" s="6" t="s">
@@ -16372,10 +16360,10 @@
         <v>6</v>
       </c>
       <c r="I147" s="23">
-        <v>2580</v>
+        <v>2407</v>
       </c>
       <c r="J147" s="36">
-        <v>1120.95</v>
+        <v>1042.43</v>
       </c>
       <c r="K147" s="24" t="s">
         <v>689</v>
@@ -16385,10 +16373,10 @@
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A148" s="43" t="s">
+      <c r="A148" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B148" s="44" t="s">
+      <c r="B148" s="13" t="s">
         <v>189</v>
       </c>
       <c r="C148" s="6" t="s">
@@ -16410,10 +16398,10 @@
         <v>6</v>
       </c>
       <c r="I148" s="23">
-        <v>2506</v>
+        <v>2462</v>
       </c>
       <c r="J148" s="36">
-        <v>1088.67</v>
+        <v>1042.8</v>
       </c>
       <c r="K148" s="24" t="s">
         <v>689</v>
@@ -16423,10 +16411,10 @@
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A149" s="47" t="s">
+      <c r="A149" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B149" s="48" t="s">
+      <c r="B149" s="15" t="s">
         <v>190</v>
       </c>
       <c r="C149" s="9" t="s">
@@ -16448,10 +16436,10 @@
         <v>6</v>
       </c>
       <c r="I149" s="27">
-        <v>2534</v>
+        <v>2455</v>
       </c>
       <c r="J149" s="40">
-        <v>1113.17</v>
+        <v>1022.54</v>
       </c>
       <c r="K149" s="27" t="s">
         <v>689</v>
@@ -16461,10 +16449,10 @@
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A150" s="45" t="s">
+      <c r="A150" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B150" s="46" t="s">
+      <c r="B150" s="33" t="s">
         <v>191</v>
       </c>
       <c r="C150" s="3" t="s">
@@ -16486,10 +16474,10 @@
         <v>4</v>
       </c>
       <c r="I150" s="32">
-        <v>2353</v>
+        <v>2207</v>
       </c>
       <c r="J150" s="38">
-        <v>1007.94</v>
+        <v>911.65</v>
       </c>
       <c r="K150" s="32" t="s">
         <v>689</v>
@@ -16499,10 +16487,10 @@
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A151" s="43" t="s">
+      <c r="A151" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B151" s="44" t="s">
+      <c r="B151" s="13" t="s">
         <v>192</v>
       </c>
       <c r="C151" s="6" t="s">
@@ -16524,10 +16512,10 @@
         <v>5</v>
       </c>
       <c r="I151" s="24">
-        <v>2434</v>
+        <v>2254</v>
       </c>
       <c r="J151" s="36">
-        <v>1009.44</v>
+        <v>917.96</v>
       </c>
       <c r="K151" s="24" t="s">
         <v>689</v>
@@ -16537,10 +16525,10 @@
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A152" s="43" t="s">
+      <c r="A152" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B152" s="44" t="s">
+      <c r="B152" s="13" t="s">
         <v>193</v>
       </c>
       <c r="C152" s="6" t="s">
@@ -16562,10 +16550,10 @@
         <v>5</v>
       </c>
       <c r="I152" s="24">
-        <v>2547</v>
+        <v>2440</v>
       </c>
       <c r="J152" s="36">
-        <v>1150.0899999999999</v>
+        <v>1081.1199999999999</v>
       </c>
       <c r="K152" s="24" t="s">
         <v>689</v>
@@ -16575,10 +16563,10 @@
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A153" s="47" t="s">
+      <c r="A153" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B153" s="48" t="s">
+      <c r="B153" s="15" t="s">
         <v>194</v>
       </c>
       <c r="C153" s="9" t="s">
@@ -16597,13 +16585,13 @@
         <v>352</v>
       </c>
       <c r="H153" s="27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I153" s="27">
-        <v>2562</v>
+        <v>2266</v>
       </c>
       <c r="J153" s="40">
-        <v>1156.81</v>
+        <v>939.95</v>
       </c>
       <c r="K153" s="27" t="s">
         <v>689</v>
@@ -16613,10 +16601,10 @@
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A154" s="45" t="s">
+      <c r="A154" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B154" s="46" t="s">
+      <c r="B154" s="33" t="s">
         <v>195</v>
       </c>
       <c r="C154" s="3" t="s">
@@ -16635,13 +16623,13 @@
         <v>353</v>
       </c>
       <c r="H154" s="32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I154" s="32">
-        <v>2471</v>
+        <v>2343</v>
       </c>
       <c r="J154" s="38">
-        <v>1087.55</v>
+        <v>984.22</v>
       </c>
       <c r="K154" s="32" t="s">
         <v>689</v>
@@ -16651,10 +16639,10 @@
       </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A155" s="43" t="s">
+      <c r="A155" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B155" s="44" t="s">
+      <c r="B155" s="13" t="s">
         <v>196</v>
       </c>
       <c r="C155" s="6" t="s">
@@ -16676,10 +16664,10 @@
         <v>6</v>
       </c>
       <c r="I155" s="24">
-        <v>2551</v>
+        <v>2407</v>
       </c>
       <c r="J155" s="36">
-        <v>1121.22</v>
+        <v>1042.43</v>
       </c>
       <c r="K155" s="24" t="s">
         <v>689</v>
@@ -16689,10 +16677,10 @@
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A156" s="43" t="s">
+      <c r="A156" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B156" s="44" t="s">
+      <c r="B156" s="13" t="s">
         <v>197</v>
       </c>
       <c r="C156" s="6" t="s">
@@ -16714,10 +16702,10 @@
         <v>6</v>
       </c>
       <c r="I156" s="24">
-        <v>2506</v>
+        <v>2462</v>
       </c>
       <c r="J156" s="36">
-        <v>1088.67</v>
+        <v>1042.8</v>
       </c>
       <c r="K156" s="24" t="s">
         <v>689</v>
@@ -16727,10 +16715,10 @@
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A157" s="47" t="s">
+      <c r="A157" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B157" s="48" t="s">
+      <c r="B157" s="15" t="s">
         <v>198</v>
       </c>
       <c r="C157" s="9" t="s">
@@ -16752,10 +16740,10 @@
         <v>6</v>
       </c>
       <c r="I157" s="27">
-        <v>2526</v>
+        <v>2455</v>
       </c>
       <c r="J157" s="40">
-        <v>1108.9100000000001</v>
+        <v>1022.54</v>
       </c>
       <c r="K157" s="27" t="s">
         <v>689</v>
@@ -16765,10 +16753,10 @@
       </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A158" s="45" t="s">
+      <c r="A158" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B158" s="46" t="s">
+      <c r="B158" s="33" t="s">
         <v>199</v>
       </c>
       <c r="C158" s="3" t="s">
@@ -16790,10 +16778,10 @@
         <v>4</v>
       </c>
       <c r="I158" s="32">
-        <v>2353</v>
+        <v>2207</v>
       </c>
       <c r="J158" s="38">
-        <v>1007.94</v>
+        <v>911.65</v>
       </c>
       <c r="K158" s="32" t="s">
         <v>689</v>
@@ -16803,10 +16791,10 @@
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A159" s="43" t="s">
+      <c r="A159" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B159" s="44" t="s">
+      <c r="B159" s="13" t="s">
         <v>200</v>
       </c>
       <c r="C159" s="6" t="s">
@@ -16828,10 +16816,10 @@
         <v>5</v>
       </c>
       <c r="I159" s="24">
-        <v>2434</v>
+        <v>2254</v>
       </c>
       <c r="J159" s="36">
-        <v>1009.34</v>
+        <v>917.96</v>
       </c>
       <c r="K159" s="24" t="s">
         <v>689</v>
@@ -16841,10 +16829,10 @@
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A160" s="43" t="s">
+      <c r="A160" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B160" s="44" t="s">
+      <c r="B160" s="13" t="s">
         <v>201</v>
       </c>
       <c r="C160" s="6" t="s">
@@ -16866,10 +16854,10 @@
         <v>5</v>
       </c>
       <c r="I160" s="24">
-        <v>2451</v>
+        <v>2428</v>
       </c>
       <c r="J160" s="36">
-        <v>1068.5999999999999</v>
+        <v>1057.33</v>
       </c>
       <c r="K160" s="24" t="s">
         <v>689</v>
@@ -16879,10 +16867,10 @@
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A161" s="47" t="s">
+      <c r="A161" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B161" s="48" t="s">
+      <c r="B161" s="15" t="s">
         <v>202</v>
       </c>
       <c r="C161" s="9" t="s">
@@ -16901,13 +16889,13 @@
         <v>360</v>
       </c>
       <c r="H161" s="27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I161" s="27">
-        <v>2530</v>
+        <v>2293</v>
       </c>
       <c r="J161" s="40">
-        <v>1131.48</v>
+        <v>961.4</v>
       </c>
       <c r="K161" s="27" t="s">
         <v>689</v>
@@ -16917,10 +16905,10 @@
       </c>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A162" s="43" t="s">
+      <c r="A162" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B162" s="44" t="s">
+      <c r="B162" s="13" t="s">
         <v>171</v>
       </c>
       <c r="C162" s="3" t="s">
@@ -16955,10 +16943,10 @@
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A163" s="43" t="s">
+      <c r="A163" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B163" s="44" t="s">
+      <c r="B163" s="13" t="s">
         <v>172</v>
       </c>
       <c r="C163" s="6" t="s">
@@ -16993,10 +16981,10 @@
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A164" s="43" t="s">
+      <c r="A164" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B164" s="44" t="s">
+      <c r="B164" s="13" t="s">
         <v>173</v>
       </c>
       <c r="C164" s="6" t="s">
@@ -17031,10 +17019,10 @@
       </c>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A165" s="43" t="s">
+      <c r="A165" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B165" s="44" t="s">
+      <c r="B165" s="13" t="s">
         <v>174</v>
       </c>
       <c r="C165" s="9" t="s">
@@ -25429,10 +25417,10 @@
       </c>
     </row>
     <row r="386" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A386" s="45" t="s">
+      <c r="A386" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B386" s="46" t="s">
+      <c r="B386" s="33" t="s">
         <v>171</v>
       </c>
       <c r="C386" s="3" t="s">
@@ -25467,10 +25455,10 @@
       </c>
     </row>
     <row r="387" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A387" s="43" t="s">
+      <c r="A387" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B387" s="44" t="s">
+      <c r="B387" s="13" t="s">
         <v>172</v>
       </c>
       <c r="C387" s="6" t="s">
@@ -25505,10 +25493,10 @@
       </c>
     </row>
     <row r="388" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A388" s="43" t="s">
+      <c r="A388" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B388" s="44" t="s">
+      <c r="B388" s="13" t="s">
         <v>173</v>
       </c>
       <c r="C388" s="6" t="s">
@@ -25543,10 +25531,10 @@
       </c>
     </row>
     <row r="389" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A389" s="47" t="s">
+      <c r="A389" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B389" s="48" t="s">
+      <c r="B389" s="15" t="s">
         <v>174</v>
       </c>
       <c r="C389" s="9" t="s">
@@ -25581,10 +25569,10 @@
       </c>
     </row>
     <row r="390" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A390" s="45" t="s">
+      <c r="A390" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B390" s="46" t="s">
+      <c r="B390" s="33" t="s">
         <v>175</v>
       </c>
       <c r="C390" s="3" t="s">
@@ -25619,10 +25607,10 @@
       </c>
     </row>
     <row r="391" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A391" s="43" t="s">
+      <c r="A391" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B391" s="44" t="s">
+      <c r="B391" s="13" t="s">
         <v>176</v>
       </c>
       <c r="C391" s="6" t="s">
@@ -25657,10 +25645,10 @@
       </c>
     </row>
     <row r="392" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A392" s="43" t="s">
+      <c r="A392" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B392" s="44" t="s">
+      <c r="B392" s="13" t="s">
         <v>177</v>
       </c>
       <c r="C392" s="6" t="s">
@@ -25695,10 +25683,10 @@
       </c>
     </row>
     <row r="393" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A393" s="47" t="s">
+      <c r="A393" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B393" s="48" t="s">
+      <c r="B393" s="15" t="s">
         <v>178</v>
       </c>
       <c r="C393" s="9" t="s">
@@ -25733,10 +25721,10 @@
       </c>
     </row>
     <row r="394" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A394" s="45" t="s">
+      <c r="A394" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B394" s="46" t="s">
+      <c r="B394" s="33" t="s">
         <v>179</v>
       </c>
       <c r="C394" s="3" t="s">
@@ -25771,10 +25759,10 @@
       </c>
     </row>
     <row r="395" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A395" s="43" t="s">
+      <c r="A395" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B395" s="44" t="s">
+      <c r="B395" s="13" t="s">
         <v>180</v>
       </c>
       <c r="C395" s="6" t="s">
@@ -25809,10 +25797,10 @@
       </c>
     </row>
     <row r="396" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A396" s="43" t="s">
+      <c r="A396" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B396" s="44" t="s">
+      <c r="B396" s="13" t="s">
         <v>181</v>
       </c>
       <c r="C396" s="6" t="s">
@@ -25847,10 +25835,10 @@
       </c>
     </row>
     <row r="397" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A397" s="47" t="s">
+      <c r="A397" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B397" s="48" t="s">
+      <c r="B397" s="15" t="s">
         <v>182</v>
       </c>
       <c r="C397" s="9" t="s">
@@ -25885,10 +25873,10 @@
       </c>
     </row>
     <row r="398" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A398" s="45" t="s">
+      <c r="A398" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B398" s="46" t="s">
+      <c r="B398" s="33" t="s">
         <v>183</v>
       </c>
       <c r="C398" s="3" t="s">
@@ -25923,10 +25911,10 @@
       </c>
     </row>
     <row r="399" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A399" s="43" t="s">
+      <c r="A399" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B399" s="44" t="s">
+      <c r="B399" s="13" t="s">
         <v>184</v>
       </c>
       <c r="C399" s="6" t="s">
@@ -25961,10 +25949,10 @@
       </c>
     </row>
     <row r="400" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A400" s="43" t="s">
+      <c r="A400" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B400" s="44" t="s">
+      <c r="B400" s="13" t="s">
         <v>185</v>
       </c>
       <c r="C400" s="6" t="s">
@@ -25999,10 +25987,10 @@
       </c>
     </row>
     <row r="401" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A401" s="47" t="s">
+      <c r="A401" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B401" s="48" t="s">
+      <c r="B401" s="15" t="s">
         <v>186</v>
       </c>
       <c r="C401" s="9" t="s">
@@ -26037,10 +26025,10 @@
       </c>
     </row>
     <row r="402" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A402" s="45" t="s">
+      <c r="A402" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B402" s="46" t="s">
+      <c r="B402" s="33" t="s">
         <v>187</v>
       </c>
       <c r="C402" s="3" t="s">
@@ -26062,10 +26050,10 @@
         <v>6</v>
       </c>
       <c r="I402" s="32">
-        <v>2673</v>
+        <v>2502</v>
       </c>
       <c r="J402" s="38">
-        <v>1220.53</v>
+        <v>1087.9000000000001</v>
       </c>
       <c r="K402" s="32" t="s">
         <v>689</v>
@@ -26075,10 +26063,10 @@
       </c>
     </row>
     <row r="403" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A403" s="43" t="s">
+      <c r="A403" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B403" s="44" t="s">
+      <c r="B403" s="13" t="s">
         <v>188</v>
       </c>
       <c r="C403" s="6" t="s">
@@ -26097,13 +26085,13 @@
         <v>596</v>
       </c>
       <c r="H403" s="23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I403" s="23">
-        <v>2955</v>
+        <v>2484</v>
       </c>
       <c r="J403" s="39">
-        <v>1405.63</v>
+        <v>1078.6600000000001</v>
       </c>
       <c r="K403" s="24" t="s">
         <v>689</v>
@@ -26113,10 +26101,10 @@
       </c>
     </row>
     <row r="404" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A404" s="43" t="s">
+      <c r="A404" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B404" s="44" t="s">
+      <c r="B404" s="13" t="s">
         <v>189</v>
       </c>
       <c r="C404" s="6" t="s">
@@ -26135,13 +26123,13 @@
         <v>597</v>
       </c>
       <c r="H404" s="23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I404" s="23">
-        <v>2719</v>
+        <v>2554</v>
       </c>
       <c r="J404" s="39">
-        <v>1252.6600000000001</v>
+        <v>1144.72</v>
       </c>
       <c r="K404" s="24" t="s">
         <v>689</v>
@@ -26151,10 +26139,10 @@
       </c>
     </row>
     <row r="405" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A405" s="47" t="s">
+      <c r="A405" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B405" s="48" t="s">
+      <c r="B405" s="15" t="s">
         <v>190</v>
       </c>
       <c r="C405" s="9" t="s">
@@ -26176,10 +26164,10 @@
         <v>7</v>
       </c>
       <c r="I405" s="27">
-        <v>2751</v>
+        <v>2674</v>
       </c>
       <c r="J405" s="40">
-        <v>1262.0899999999999</v>
+        <v>1250.21</v>
       </c>
       <c r="K405" s="24" t="s">
         <v>689</v>
@@ -26189,10 +26177,10 @@
       </c>
     </row>
     <row r="406" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A406" s="45" t="s">
+      <c r="A406" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B406" s="46" t="s">
+      <c r="B406" s="33" t="s">
         <v>191</v>
       </c>
       <c r="C406" s="3" t="s">
@@ -26214,10 +26202,10 @@
         <v>5</v>
       </c>
       <c r="I406" s="32">
-        <v>2566</v>
+        <v>2504</v>
       </c>
       <c r="J406" s="38">
-        <v>1136.72</v>
+        <v>1129.75</v>
       </c>
       <c r="K406" s="32" t="s">
         <v>689</v>
@@ -26227,10 +26215,10 @@
       </c>
     </row>
     <row r="407" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A407" s="43" t="s">
+      <c r="A407" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B407" s="44" t="s">
+      <c r="B407" s="13" t="s">
         <v>192</v>
       </c>
       <c r="C407" s="6" t="s">
@@ -26249,13 +26237,13 @@
         <v>600</v>
       </c>
       <c r="H407" s="24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I407" s="24">
-        <v>2856</v>
+        <v>2450</v>
       </c>
       <c r="J407" s="39">
-        <v>1315.37</v>
+        <v>1053.47</v>
       </c>
       <c r="K407" s="24" t="s">
         <v>689</v>
@@ -26265,10 +26253,10 @@
       </c>
     </row>
     <row r="408" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A408" s="43" t="s">
+      <c r="A408" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B408" s="44" t="s">
+      <c r="B408" s="13" t="s">
         <v>193</v>
       </c>
       <c r="C408" s="6" t="s">
@@ -26290,10 +26278,10 @@
         <v>5</v>
       </c>
       <c r="I408" s="24">
-        <v>2574</v>
+        <v>2460</v>
       </c>
       <c r="J408" s="39">
-        <v>1151.22</v>
+        <v>1076.2</v>
       </c>
       <c r="K408" s="24" t="s">
         <v>689</v>
@@ -26303,10 +26291,10 @@
       </c>
     </row>
     <row r="409" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A409" s="47" t="s">
+      <c r="A409" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B409" s="48" t="s">
+      <c r="B409" s="15" t="s">
         <v>194</v>
       </c>
       <c r="C409" s="9" t="s">
@@ -26328,10 +26316,10 @@
         <v>5</v>
       </c>
       <c r="I409" s="27">
-        <v>2470</v>
+        <v>2495</v>
       </c>
       <c r="J409" s="40">
-        <v>1094.18</v>
+        <v>1113.44</v>
       </c>
       <c r="K409" s="24" t="s">
         <v>689</v>
@@ -26341,10 +26329,10 @@
       </c>
     </row>
     <row r="410" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A410" s="45" t="s">
+      <c r="A410" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B410" s="46" t="s">
+      <c r="B410" s="33" t="s">
         <v>195</v>
       </c>
       <c r="C410" s="3" t="s">
@@ -26366,10 +26354,10 @@
         <v>6</v>
       </c>
       <c r="I410" s="32">
-        <v>2594</v>
+        <v>2586</v>
       </c>
       <c r="J410" s="38">
-        <v>1195.67</v>
+        <v>1181.01</v>
       </c>
       <c r="K410" s="32" t="s">
         <v>689</v>
@@ -26379,10 +26367,10 @@
       </c>
     </row>
     <row r="411" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A411" s="43" t="s">
+      <c r="A411" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B411" s="44" t="s">
+      <c r="B411" s="13" t="s">
         <v>196</v>
       </c>
       <c r="C411" s="6" t="s">
@@ -26401,13 +26389,13 @@
         <v>604</v>
       </c>
       <c r="H411" s="24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I411" s="24">
-        <v>2589</v>
+        <v>2470</v>
       </c>
       <c r="J411" s="39">
-        <v>1152.79</v>
+        <v>1068.5</v>
       </c>
       <c r="K411" s="24" t="s">
         <v>689</v>
@@ -26417,10 +26405,10 @@
       </c>
     </row>
     <row r="412" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A412" s="43" t="s">
+      <c r="A412" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B412" s="44" t="s">
+      <c r="B412" s="13" t="s">
         <v>197</v>
       </c>
       <c r="C412" s="6" t="s">
@@ -26439,13 +26427,13 @@
         <v>605</v>
       </c>
       <c r="H412" s="24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I412" s="24">
-        <v>2662</v>
+        <v>2582</v>
       </c>
       <c r="J412" s="39">
-        <v>1184.0999999999999</v>
+        <v>1156.49</v>
       </c>
       <c r="K412" s="24" t="s">
         <v>689</v>
@@ -26455,10 +26443,10 @@
       </c>
     </row>
     <row r="413" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A413" s="47" t="s">
+      <c r="A413" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B413" s="48" t="s">
+      <c r="B413" s="15" t="s">
         <v>198</v>
       </c>
       <c r="C413" s="9" t="s">
@@ -26480,10 +26468,10 @@
         <v>7</v>
       </c>
       <c r="I413" s="27">
-        <v>2726</v>
+        <v>2572</v>
       </c>
       <c r="J413" s="40">
-        <v>1262.95</v>
+        <v>1230.54</v>
       </c>
       <c r="K413" s="24" t="s">
         <v>689</v>
@@ -26493,10 +26481,10 @@
       </c>
     </row>
     <row r="414" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A414" s="45" t="s">
+      <c r="A414" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B414" s="46" t="s">
+      <c r="B414" s="33" t="s">
         <v>199</v>
       </c>
       <c r="C414" s="3" t="s">
@@ -26515,13 +26503,13 @@
         <v>607</v>
       </c>
       <c r="H414" s="32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I414" s="32">
-        <v>2596</v>
+        <v>2299</v>
       </c>
       <c r="J414" s="38">
-        <v>1197.74</v>
+        <v>995.63</v>
       </c>
       <c r="K414" s="32" t="s">
         <v>689</v>
@@ -26531,10 +26519,10 @@
       </c>
     </row>
     <row r="415" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A415" s="43" t="s">
+      <c r="A415" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B415" s="44" t="s">
+      <c r="B415" s="13" t="s">
         <v>200</v>
       </c>
       <c r="C415" s="6" t="s">
@@ -26556,10 +26544,10 @@
         <v>5</v>
       </c>
       <c r="I415" s="24">
-        <v>2620</v>
+        <v>2559</v>
       </c>
       <c r="J415" s="39">
-        <v>1196.56</v>
+        <v>1151.3399999999999</v>
       </c>
       <c r="K415" s="24" t="s">
         <v>689</v>
@@ -26569,10 +26557,10 @@
       </c>
     </row>
     <row r="416" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A416" s="43" t="s">
+      <c r="A416" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B416" s="44" t="s">
+      <c r="B416" s="13" t="s">
         <v>201</v>
       </c>
       <c r="C416" s="6" t="s">
@@ -26594,10 +26582,10 @@
         <v>5</v>
       </c>
       <c r="I416" s="24">
-        <v>2601</v>
+        <v>2460</v>
       </c>
       <c r="J416" s="39">
-        <v>1187.74</v>
+        <v>1091.71</v>
       </c>
       <c r="K416" s="24" t="s">
         <v>689</v>
@@ -26607,10 +26595,10 @@
       </c>
     </row>
     <row r="417" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A417" s="47" t="s">
+      <c r="A417" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B417" s="48" t="s">
+      <c r="B417" s="15" t="s">
         <v>202</v>
       </c>
       <c r="C417" s="9" t="s">
@@ -26632,10 +26620,10 @@
         <v>5</v>
       </c>
       <c r="I417" s="27">
-        <v>2480</v>
+        <v>2347</v>
       </c>
       <c r="J417" s="40">
-        <v>1063.96</v>
+        <v>1013.35</v>
       </c>
       <c r="K417" s="24" t="s">
         <v>689</v>

</xml_diff>